<commit_message>
Mon Oct 20 03:19:10 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{ABF20E2A-5E5A-4692-8E92-C1241AD96863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{4ADC3E5C-1086-4165-82FC-9A7AAABC7AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>161.22</v>
+        <v>160.47</v>
       </c>
       <c r="E8" s="10">
-        <v>158.03</v>
+        <v>157.9</v>
       </c>
       <c r="F8" s="10">
-        <v>168.03</v>
+        <v>167.9</v>
       </c>
       <c r="G8" s="10">
-        <v>158.19</v>
+        <v>158.06</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>161.22</v>
+        <v>160.47</v>
       </c>
       <c r="E9" s="13">
-        <v>158.03</v>
+        <v>157.9</v>
       </c>
       <c r="F9" s="13">
-        <v>168.03</v>
+        <v>167.9</v>
       </c>
       <c r="G9" s="13">
-        <v>158.19</v>
+        <v>158.06</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>163.59</v>
+        <v>162.69</v>
       </c>
       <c r="E10" s="10">
-        <v>160.41</v>
+        <v>160.26</v>
       </c>
       <c r="F10" s="10">
-        <v>170.41</v>
+        <v>170.26</v>
       </c>
       <c r="G10" s="10">
-        <v>160.88</v>
+        <v>160.72999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>161.93</v>
+        <v>161.22</v>
       </c>
       <c r="E11" s="13">
-        <v>158.1</v>
+        <v>158.03</v>
       </c>
       <c r="F11" s="13">
-        <v>168.1</v>
+        <v>168.03</v>
       </c>
       <c r="G11" s="13">
-        <v>158.26</v>
+        <v>158.19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>161.93</v>
+        <v>161.22</v>
       </c>
       <c r="E12" s="10">
-        <v>158.1</v>
+        <v>158.03</v>
       </c>
       <c r="F12" s="10">
-        <v>168.1</v>
+        <v>168.03</v>
       </c>
       <c r="G12" s="10">
-        <v>158.26</v>
+        <v>158.19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>164.28</v>
+        <v>163.59</v>
       </c>
       <c r="E13" s="13">
-        <v>160.36000000000001</v>
+        <v>160.41</v>
       </c>
       <c r="F13" s="13">
-        <v>170.36</v>
+        <v>170.41</v>
       </c>
       <c r="G13" s="13">
-        <v>160.83000000000001</v>
+        <v>160.88</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>166.9</v>
+        <v>166.12</v>
       </c>
       <c r="E17" s="10">
-        <v>163.22</v>
+        <v>163.09</v>
       </c>
       <c r="F17" s="10">
-        <v>173.22</v>
+        <v>173.09</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>167.59</v>
+        <v>166.9</v>
       </c>
       <c r="E18" s="13">
-        <v>163.18</v>
+        <v>163.22</v>
       </c>
       <c r="F18" s="13">
-        <v>173.18</v>
+        <v>173.22</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>162.25</v>
+        <v>161.38999999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>159.30000000000001</v>
+        <v>159.15</v>
       </c>
       <c r="F22" s="10">
-        <v>168.9</v>
+        <v>168.75</v>
       </c>
       <c r="G22" s="10">
-        <v>160.47999999999999</v>
+        <v>160.32</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>168.25</v>
+        <v>167.46</v>
       </c>
       <c r="E23" s="13">
-        <v>164.01</v>
+        <v>163.86</v>
       </c>
       <c r="F23" s="13">
-        <v>174.01</v>
+        <v>173.86</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>168.05</v>
+        <v>167.26</v>
       </c>
       <c r="E24" s="10">
-        <v>164.23</v>
+        <v>164.07</v>
       </c>
       <c r="F24" s="10">
-        <v>174.23</v>
+        <v>174.07</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>168.88</v>
+        <v>168.1</v>
       </c>
       <c r="E25" s="13">
-        <v>163.62</v>
+        <v>163.46</v>
       </c>
       <c r="F25" s="13">
-        <v>173.62</v>
+        <v>173.46</v>
       </c>
       <c r="G25" s="13">
-        <v>163.44999999999999</v>
+        <v>163.29</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>167.6</v>
+        <v>166.81</v>
       </c>
       <c r="E26" s="10">
-        <v>165.16</v>
+        <v>165</v>
       </c>
       <c r="F26" s="10">
-        <v>175.16</v>
+        <v>175</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>162.84</v>
+        <v>162.25</v>
       </c>
       <c r="E27" s="13">
-        <v>159.26</v>
+        <v>159.30000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>168.86</v>
+        <v>168.9</v>
       </c>
       <c r="G27" s="13">
-        <v>160.43</v>
+        <v>160.47999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>168.94</v>
+        <v>168.25</v>
       </c>
       <c r="E28" s="22">
-        <v>163.96</v>
+        <v>164.01</v>
       </c>
       <c r="F28" s="22">
-        <v>173.96</v>
+        <v>174.01</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>168.75</v>
+        <v>168.05</v>
       </c>
       <c r="E29" s="13">
-        <v>164.18</v>
+        <v>164.23</v>
       </c>
       <c r="F29" s="13">
-        <v>174.18</v>
+        <v>174.23</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>169.58</v>
+        <v>168.88</v>
       </c>
       <c r="E30" s="22">
-        <v>163.57</v>
+        <v>163.62</v>
       </c>
       <c r="F30" s="22">
-        <v>173.57</v>
+        <v>173.62</v>
       </c>
       <c r="G30" s="22">
-        <v>163.4</v>
+        <v>163.44999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>168.29</v>
+        <v>167.6</v>
       </c>
       <c r="E31" s="13">
-        <v>165.11</v>
+        <v>165.16</v>
       </c>
       <c r="F31" s="13">
-        <v>175.11</v>
+        <v>175.16</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>161.94999999999999</v>
+        <v>161.05000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>157.52000000000001</v>
+        <v>157.36000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>166.52</v>
+        <v>166.36</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>162.53</v>
+        <v>161.94999999999999</v>
       </c>
       <c r="E36" s="13">
-        <v>157.47</v>
+        <v>157.52000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>166.47</v>
+        <v>166.52</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>167.39</v>
+        <v>166.6</v>
       </c>
       <c r="E40" s="10">
-        <v>162.99</v>
+        <v>162.84</v>
       </c>
       <c r="F40" s="10">
-        <v>172.99</v>
+        <v>172.84</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>167.1</v>
+        <v>166.31</v>
       </c>
       <c r="E41" s="13">
-        <v>163.41</v>
+        <v>163.26</v>
       </c>
       <c r="F41" s="13">
-        <v>173.41</v>
+        <v>173.26</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>168.08</v>
+        <v>167.39</v>
       </c>
       <c r="E42" s="10">
-        <v>162.94</v>
+        <v>162.99</v>
       </c>
       <c r="F42" s="10">
-        <v>172.94</v>
+        <v>172.99</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>167.79</v>
+        <v>167.1</v>
       </c>
       <c r="E43" s="13">
-        <v>163.36000000000001</v>
+        <v>163.41</v>
       </c>
       <c r="F43" s="13">
-        <v>173.36</v>
+        <v>173.41</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>162.05000000000001</v>
+        <v>161.34</v>
       </c>
       <c r="E47" s="10">
-        <v>159.28</v>
+        <v>159.06</v>
       </c>
       <c r="F47" s="10">
-        <v>169.28</v>
+        <v>169.06</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>162.03</v>
+        <v>161.32</v>
       </c>
       <c r="E48" s="13">
-        <v>159.44999999999999</v>
+        <v>159.22999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>169.45</v>
+        <v>169.23</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>162.47</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="E49" s="10">
-        <v>159.35</v>
+        <v>159.28</v>
       </c>
       <c r="F49" s="10">
-        <v>169.35</v>
+        <v>169.28</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>162.44999999999999</v>
+        <v>162.03</v>
       </c>
       <c r="E50" s="13">
-        <v>159.52000000000001</v>
+        <v>159.44999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>169.52</v>
+        <v>169.45</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>177.54</v>
+        <v>176.77</v>
       </c>
       <c r="E54" s="10">
-        <v>173.34</v>
+        <v>173.16</v>
       </c>
       <c r="F54" s="10">
-        <v>183.34</v>
+        <v>183.16</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>165.22</v>
+        <v>164.43</v>
       </c>
       <c r="E55" s="13">
-        <v>170.78</v>
+        <v>170.52</v>
       </c>
       <c r="F55" s="13">
-        <v>180.78</v>
+        <v>180.52</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>167.72</v>
+        <v>166.82</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>167.37</v>
+        <v>166.48</v>
       </c>
       <c r="E57" s="13">
-        <v>165.05</v>
+        <v>164.79</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>163.28</v>
+        <v>162.38999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>161.1</v>
+        <v>160.84</v>
       </c>
       <c r="F58" s="10">
-        <v>171.1</v>
+        <v>170.84</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>169.88</v>
+        <v>169.1</v>
       </c>
       <c r="E59" s="13">
-        <v>171.5</v>
+        <v>171.33</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>178.21</v>
+        <v>177.54</v>
       </c>
       <c r="E60" s="10">
-        <v>173.29</v>
+        <v>173.34</v>
       </c>
       <c r="F60" s="10">
-        <v>183.29</v>
+        <v>183.34</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>165.91</v>
+        <v>165.22</v>
       </c>
       <c r="E61" s="13">
-        <v>170.63</v>
+        <v>170.78</v>
       </c>
       <c r="F61" s="13">
-        <v>180.63</v>
+        <v>180.78</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>168.3</v>
+        <v>167.72</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>167.96</v>
+        <v>167.37</v>
       </c>
       <c r="E63" s="13">
-        <v>164.9</v>
+        <v>165.05</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>163.86</v>
+        <v>163.28</v>
       </c>
       <c r="E64" s="10">
-        <v>160.94999999999999</v>
+        <v>161.1</v>
       </c>
       <c r="F64" s="10">
-        <v>170.95</v>
+        <v>171.1</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>170.58</v>
+        <v>169.88</v>
       </c>
       <c r="E65" s="13">
-        <v>171.44</v>
+        <v>171.5</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1866,6 +1866,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2125,15 +2134,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
@@ -2153,6 +2153,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2172,14 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Tue Oct 21 02:45:39 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{4ADC3E5C-1086-4165-82FC-9A7AAABC7AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{39AC5FA7-C6BD-4CC0-ABDC-13FE02E11861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>160.47</v>
+        <v>160.06</v>
       </c>
       <c r="E8" s="10">
-        <v>157.9</v>
+        <v>157.88999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>167.9</v>
+        <v>167.89</v>
       </c>
       <c r="G8" s="10">
-        <v>158.06</v>
+        <v>158.05000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>160.47</v>
+        <v>160.06</v>
       </c>
       <c r="E9" s="13">
-        <v>157.9</v>
+        <v>157.88999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>167.9</v>
+        <v>167.89</v>
       </c>
       <c r="G9" s="13">
-        <v>158.06</v>
+        <v>158.05000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>162.69</v>
+        <v>162.28</v>
       </c>
       <c r="E10" s="10">
-        <v>160.26</v>
+        <v>160.22999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>170.26</v>
+        <v>170.23</v>
       </c>
       <c r="G10" s="10">
-        <v>160.72999999999999</v>
+        <v>160.69999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>161.22</v>
+        <v>160.47</v>
       </c>
       <c r="E11" s="13">
-        <v>158.03</v>
+        <v>157.9</v>
       </c>
       <c r="F11" s="13">
-        <v>168.03</v>
+        <v>167.9</v>
       </c>
       <c r="G11" s="13">
-        <v>158.19</v>
+        <v>158.06</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>161.22</v>
+        <v>160.47</v>
       </c>
       <c r="E12" s="10">
-        <v>158.03</v>
+        <v>157.9</v>
       </c>
       <c r="F12" s="10">
-        <v>168.03</v>
+        <v>167.9</v>
       </c>
       <c r="G12" s="10">
-        <v>158.19</v>
+        <v>158.06</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>163.59</v>
+        <v>162.69</v>
       </c>
       <c r="E13" s="13">
-        <v>160.41</v>
+        <v>160.26</v>
       </c>
       <c r="F13" s="13">
-        <v>170.41</v>
+        <v>170.26</v>
       </c>
       <c r="G13" s="13">
-        <v>160.88</v>
+        <v>160.72999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>166.12</v>
+        <v>165.7</v>
       </c>
       <c r="E17" s="10">
-        <v>163.09</v>
+        <v>163.07</v>
       </c>
       <c r="F17" s="10">
-        <v>173.09</v>
+        <v>173.07</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>166.9</v>
+        <v>166.12</v>
       </c>
       <c r="E18" s="13">
-        <v>163.22</v>
+        <v>163.09</v>
       </c>
       <c r="F18" s="13">
-        <v>173.22</v>
+        <v>173.09</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>161.38999999999999</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>159.15</v>
+        <v>159.12</v>
       </c>
       <c r="F22" s="10">
-        <v>168.75</v>
+        <v>168.72</v>
       </c>
       <c r="G22" s="10">
-        <v>160.32</v>
+        <v>160.30000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>167.46</v>
+        <v>167.04</v>
       </c>
       <c r="E23" s="13">
-        <v>163.86</v>
+        <v>163.83000000000001</v>
       </c>
       <c r="F23" s="13">
-        <v>173.86</v>
+        <v>173.83</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>167.26</v>
+        <v>166.85</v>
       </c>
       <c r="E24" s="10">
-        <v>164.07</v>
+        <v>164.04</v>
       </c>
       <c r="F24" s="10">
-        <v>174.07</v>
+        <v>174.04</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>168.1</v>
+        <v>167.68</v>
       </c>
       <c r="E25" s="13">
-        <v>163.46</v>
+        <v>163.43</v>
       </c>
       <c r="F25" s="13">
-        <v>173.46</v>
+        <v>173.43</v>
       </c>
       <c r="G25" s="13">
-        <v>163.29</v>
+        <v>163.26</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>166.81</v>
+        <v>166.4</v>
       </c>
       <c r="E26" s="10">
-        <v>165</v>
+        <v>164.97</v>
       </c>
       <c r="F26" s="10">
-        <v>175</v>
+        <v>174.97</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>162.25</v>
+        <v>161.38999999999999</v>
       </c>
       <c r="E27" s="13">
-        <v>159.30000000000001</v>
+        <v>159.15</v>
       </c>
       <c r="F27" s="13">
-        <v>168.9</v>
+        <v>168.75</v>
       </c>
       <c r="G27" s="13">
-        <v>160.47999999999999</v>
+        <v>160.32</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>168.25</v>
+        <v>167.46</v>
       </c>
       <c r="E28" s="22">
-        <v>164.01</v>
+        <v>163.86</v>
       </c>
       <c r="F28" s="22">
-        <v>174.01</v>
+        <v>173.86</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>168.05</v>
+        <v>167.26</v>
       </c>
       <c r="E29" s="13">
-        <v>164.23</v>
+        <v>164.07</v>
       </c>
       <c r="F29" s="13">
-        <v>174.23</v>
+        <v>174.07</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>168.88</v>
+        <v>168.1</v>
       </c>
       <c r="E30" s="22">
-        <v>163.62</v>
+        <v>163.46</v>
       </c>
       <c r="F30" s="22">
-        <v>173.62</v>
+        <v>173.46</v>
       </c>
       <c r="G30" s="22">
-        <v>163.44999999999999</v>
+        <v>163.29</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>167.6</v>
+        <v>166.81</v>
       </c>
       <c r="E31" s="13">
-        <v>165.16</v>
+        <v>165</v>
       </c>
       <c r="F31" s="13">
-        <v>175.16</v>
+        <v>175</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>161.05000000000001</v>
+        <v>160.52000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>157.36000000000001</v>
+        <v>157.33000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>166.36</v>
+        <v>166.33</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>161.94999999999999</v>
+        <v>161.05000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>157.52000000000001</v>
+        <v>157.36000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>166.52</v>
+        <v>166.36</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>166.6</v>
+        <v>166.17</v>
       </c>
       <c r="E40" s="10">
-        <v>162.84</v>
+        <v>162.81</v>
       </c>
       <c r="F40" s="10">
-        <v>172.84</v>
+        <v>172.81</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>166.31</v>
+        <v>165.89</v>
       </c>
       <c r="E41" s="13">
-        <v>163.26</v>
+        <v>163.22999999999999</v>
       </c>
       <c r="F41" s="13">
-        <v>173.26</v>
+        <v>173.23</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>167.39</v>
+        <v>166.6</v>
       </c>
       <c r="E42" s="10">
-        <v>162.99</v>
+        <v>162.84</v>
       </c>
       <c r="F42" s="10">
-        <v>172.99</v>
+        <v>172.84</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>167.1</v>
+        <v>166.31</v>
       </c>
       <c r="E43" s="13">
-        <v>163.41</v>
+        <v>163.26</v>
       </c>
       <c r="F43" s="13">
-        <v>173.41</v>
+        <v>173.26</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>161.34</v>
+        <v>160.86000000000001</v>
       </c>
       <c r="E47" s="10">
-        <v>159.06</v>
+        <v>159.02000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>169.06</v>
+        <v>169.02</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>161.32</v>
+        <v>160.84</v>
       </c>
       <c r="E48" s="13">
-        <v>159.22999999999999</v>
+        <v>159.19</v>
       </c>
       <c r="F48" s="13">
-        <v>169.23</v>
+        <v>169.19</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>162.05000000000001</v>
+        <v>161.34</v>
       </c>
       <c r="E49" s="10">
-        <v>159.28</v>
+        <v>159.06</v>
       </c>
       <c r="F49" s="10">
-        <v>169.28</v>
+        <v>169.06</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>162.03</v>
+        <v>161.32</v>
       </c>
       <c r="E50" s="13">
-        <v>159.44999999999999</v>
+        <v>159.22999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>169.45</v>
+        <v>169.23</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>176.77</v>
+        <v>176.36</v>
       </c>
       <c r="E54" s="10">
-        <v>173.16</v>
+        <v>173.11</v>
       </c>
       <c r="F54" s="10">
-        <v>183.16</v>
+        <v>183.11</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>164.43</v>
+        <v>164.01</v>
       </c>
       <c r="E55" s="13">
-        <v>170.52</v>
+        <v>170.5</v>
       </c>
       <c r="F55" s="13">
-        <v>180.52</v>
+        <v>180.5</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>166.82</v>
+        <v>166.3</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>166.48</v>
+        <v>165.96</v>
       </c>
       <c r="E57" s="13">
-        <v>164.79</v>
+        <v>164.77</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>162.38999999999999</v>
+        <v>161.87</v>
       </c>
       <c r="E58" s="10">
-        <v>160.84</v>
+        <v>160.82</v>
       </c>
       <c r="F58" s="10">
-        <v>170.84</v>
+        <v>170.82</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>169.1</v>
+        <v>168.69</v>
       </c>
       <c r="E59" s="13">
-        <v>171.33</v>
+        <v>171.29</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>177.54</v>
+        <v>176.77</v>
       </c>
       <c r="E60" s="10">
-        <v>173.34</v>
+        <v>173.16</v>
       </c>
       <c r="F60" s="10">
-        <v>183.34</v>
+        <v>183.16</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>165.22</v>
+        <v>164.43</v>
       </c>
       <c r="E61" s="13">
-        <v>170.78</v>
+        <v>170.52</v>
       </c>
       <c r="F61" s="13">
-        <v>180.78</v>
+        <v>180.52</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>167.72</v>
+        <v>166.82</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>167.37</v>
+        <v>166.48</v>
       </c>
       <c r="E63" s="13">
-        <v>165.05</v>
+        <v>164.79</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>163.28</v>
+        <v>162.38999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>161.1</v>
+        <v>160.84</v>
       </c>
       <c r="F64" s="10">
-        <v>171.1</v>
+        <v>170.84</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45948</v>
+        <v>45951</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>169.88</v>
+        <v>169.1</v>
       </c>
       <c r="E65" s="13">
-        <v>171.5</v>
+        <v>171.33</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1863,15 +1872,6 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,6 +2135,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2148,14 +2156,6 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Wed Oct 22 02:49:59 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{39AC5FA7-C6BD-4CC0-ABDC-13FE02E11861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{08B7B102-25F3-4832-B455-52F9B4336971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>160.06</v>
+        <v>159.62</v>
       </c>
       <c r="E8" s="10">
-        <v>157.88999999999999</v>
+        <v>157.68</v>
       </c>
       <c r="F8" s="10">
-        <v>167.89</v>
+        <v>167.68</v>
       </c>
       <c r="G8" s="10">
-        <v>158.05000000000001</v>
+        <v>157.83000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>160.06</v>
+        <v>159.62</v>
       </c>
       <c r="E9" s="13">
-        <v>157.88999999999999</v>
+        <v>157.68</v>
       </c>
       <c r="F9" s="13">
-        <v>167.89</v>
+        <v>167.68</v>
       </c>
       <c r="G9" s="13">
-        <v>158.05000000000001</v>
+        <v>157.83000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>162.28</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="E10" s="10">
-        <v>160.22999999999999</v>
+        <v>159.75</v>
       </c>
       <c r="F10" s="10">
-        <v>170.23</v>
+        <v>169.75</v>
       </c>
       <c r="G10" s="10">
-        <v>160.69999999999999</v>
+        <v>160.22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>160.47</v>
+        <v>160.06</v>
       </c>
       <c r="E11" s="13">
-        <v>157.9</v>
+        <v>157.88999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>167.9</v>
+        <v>167.89</v>
       </c>
       <c r="G11" s="13">
-        <v>158.06</v>
+        <v>158.05000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>160.47</v>
+        <v>160.06</v>
       </c>
       <c r="E12" s="10">
-        <v>157.9</v>
+        <v>157.88999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>167.9</v>
+        <v>167.89</v>
       </c>
       <c r="G12" s="10">
-        <v>158.06</v>
+        <v>158.05000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>162.69</v>
+        <v>162.28</v>
       </c>
       <c r="E13" s="13">
-        <v>160.26</v>
+        <v>160.22999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>170.26</v>
+        <v>170.23</v>
       </c>
       <c r="G13" s="13">
-        <v>160.72999999999999</v>
+        <v>160.69999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>165.7</v>
+        <v>165.32</v>
       </c>
       <c r="E17" s="10">
-        <v>163.07</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="F17" s="10">
-        <v>173.07</v>
+        <v>172.8</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>166.12</v>
+        <v>165.7</v>
       </c>
       <c r="E18" s="13">
-        <v>163.09</v>
+        <v>163.07</v>
       </c>
       <c r="F18" s="13">
-        <v>173.09</v>
+        <v>173.07</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>160.97999999999999</v>
+        <v>160.54</v>
       </c>
       <c r="E22" s="10">
-        <v>159.12</v>
+        <v>158.75</v>
       </c>
       <c r="F22" s="10">
-        <v>168.72</v>
+        <v>168.35</v>
       </c>
       <c r="G22" s="10">
-        <v>160.30000000000001</v>
+        <v>159.93</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>167.04</v>
+        <v>166.65</v>
       </c>
       <c r="E23" s="13">
-        <v>163.83000000000001</v>
+        <v>163.57</v>
       </c>
       <c r="F23" s="13">
-        <v>173.83</v>
+        <v>173.57</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>166.85</v>
+        <v>166.46</v>
       </c>
       <c r="E24" s="10">
-        <v>164.04</v>
+        <v>163.78</v>
       </c>
       <c r="F24" s="10">
-        <v>174.04</v>
+        <v>173.78</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>167.68</v>
+        <v>167.29</v>
       </c>
       <c r="E25" s="13">
-        <v>163.43</v>
+        <v>163.16999999999999</v>
       </c>
       <c r="F25" s="13">
-        <v>173.43</v>
+        <v>173.17</v>
       </c>
       <c r="G25" s="13">
-        <v>163.26</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>166.4</v>
+        <v>166.01</v>
       </c>
       <c r="E26" s="10">
-        <v>164.97</v>
+        <v>164.71</v>
       </c>
       <c r="F26" s="10">
-        <v>174.97</v>
+        <v>174.71</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>161.38999999999999</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="E27" s="13">
-        <v>159.15</v>
+        <v>159.12</v>
       </c>
       <c r="F27" s="13">
-        <v>168.75</v>
+        <v>168.72</v>
       </c>
       <c r="G27" s="13">
-        <v>160.32</v>
+        <v>160.30000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>167.46</v>
+        <v>167.04</v>
       </c>
       <c r="E28" s="22">
-        <v>163.86</v>
+        <v>163.83000000000001</v>
       </c>
       <c r="F28" s="22">
-        <v>173.86</v>
+        <v>173.83</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>167.26</v>
+        <v>166.85</v>
       </c>
       <c r="E29" s="13">
-        <v>164.07</v>
+        <v>164.04</v>
       </c>
       <c r="F29" s="13">
-        <v>174.07</v>
+        <v>174.04</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>168.1</v>
+        <v>167.68</v>
       </c>
       <c r="E30" s="22">
-        <v>163.46</v>
+        <v>163.43</v>
       </c>
       <c r="F30" s="22">
-        <v>173.46</v>
+        <v>173.43</v>
       </c>
       <c r="G30" s="22">
-        <v>163.29</v>
+        <v>163.26</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>166.81</v>
+        <v>166.4</v>
       </c>
       <c r="E31" s="13">
-        <v>165</v>
+        <v>164.97</v>
       </c>
       <c r="F31" s="13">
-        <v>175</v>
+        <v>174.97</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>160.52000000000001</v>
+        <v>160.13</v>
       </c>
       <c r="E35" s="10">
-        <v>157.33000000000001</v>
+        <v>157.07</v>
       </c>
       <c r="F35" s="10">
-        <v>166.33</v>
+        <v>166.07</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>161.05000000000001</v>
+        <v>160.52000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>157.36000000000001</v>
+        <v>157.33000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>166.36</v>
+        <v>166.33</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>166.17</v>
+        <v>165.78</v>
       </c>
       <c r="E40" s="10">
-        <v>162.81</v>
+        <v>162.54</v>
       </c>
       <c r="F40" s="10">
-        <v>172.81</v>
+        <v>172.54</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>165.89</v>
+        <v>165.5</v>
       </c>
       <c r="E41" s="13">
-        <v>163.22999999999999</v>
+        <v>162.96</v>
       </c>
       <c r="F41" s="13">
-        <v>173.23</v>
+        <v>172.96</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>166.6</v>
+        <v>166.17</v>
       </c>
       <c r="E42" s="10">
-        <v>162.84</v>
+        <v>162.81</v>
       </c>
       <c r="F42" s="10">
-        <v>172.84</v>
+        <v>172.81</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>166.31</v>
+        <v>165.89</v>
       </c>
       <c r="E43" s="13">
-        <v>163.26</v>
+        <v>163.22999999999999</v>
       </c>
       <c r="F43" s="13">
-        <v>173.26</v>
+        <v>173.23</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>160.86000000000001</v>
+        <v>160.19999999999999</v>
       </c>
       <c r="E47" s="10">
-        <v>159.02000000000001</v>
+        <v>158.82</v>
       </c>
       <c r="F47" s="10">
-        <v>169.02</v>
+        <v>168.82</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>160.84</v>
+        <v>160.18</v>
       </c>
       <c r="E48" s="13">
-        <v>159.19</v>
+        <v>158.99</v>
       </c>
       <c r="F48" s="13">
-        <v>169.19</v>
+        <v>168.99</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>161.34</v>
+        <v>160.86000000000001</v>
       </c>
       <c r="E49" s="10">
-        <v>159.06</v>
+        <v>159.02000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>169.06</v>
+        <v>169.02</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>161.32</v>
+        <v>160.84</v>
       </c>
       <c r="E50" s="13">
-        <v>159.22999999999999</v>
+        <v>159.19</v>
       </c>
       <c r="F50" s="13">
-        <v>169.23</v>
+        <v>169.19</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>176.36</v>
+        <v>175.96</v>
       </c>
       <c r="E54" s="10">
-        <v>173.11</v>
+        <v>172.84</v>
       </c>
       <c r="F54" s="10">
-        <v>183.11</v>
+        <v>182.84</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>164.01</v>
+        <v>163.63</v>
       </c>
       <c r="E55" s="13">
-        <v>170.5</v>
+        <v>170.13</v>
       </c>
       <c r="F55" s="13">
-        <v>180.5</v>
+        <v>180.13</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>166.3</v>
+        <v>165.91</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>165.96</v>
+        <v>165.58</v>
       </c>
       <c r="E57" s="13">
-        <v>164.77</v>
+        <v>164.4</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>161.87</v>
+        <v>161.47999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>160.82</v>
+        <v>160.44999999999999</v>
       </c>
       <c r="F58" s="10">
-        <v>170.82</v>
+        <v>170.45</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>168.69</v>
+        <v>168.3</v>
       </c>
       <c r="E59" s="13">
-        <v>171.29</v>
+        <v>171.03</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>176.77</v>
+        <v>176.36</v>
       </c>
       <c r="E60" s="10">
-        <v>173.16</v>
+        <v>173.11</v>
       </c>
       <c r="F60" s="10">
-        <v>183.16</v>
+        <v>183.11</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>164.43</v>
+        <v>164.01</v>
       </c>
       <c r="E61" s="13">
-        <v>170.52</v>
+        <v>170.5</v>
       </c>
       <c r="F61" s="13">
-        <v>180.52</v>
+        <v>180.5</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>166.82</v>
+        <v>166.3</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>166.48</v>
+        <v>165.96</v>
       </c>
       <c r="E63" s="13">
-        <v>164.79</v>
+        <v>164.77</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>162.38999999999999</v>
+        <v>161.87</v>
       </c>
       <c r="E64" s="10">
-        <v>160.84</v>
+        <v>160.82</v>
       </c>
       <c r="F64" s="10">
-        <v>170.84</v>
+        <v>170.82</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>169.1</v>
+        <v>168.69</v>
       </c>
       <c r="E65" s="13">
-        <v>171.33</v>
+        <v>171.29</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1872,6 +1863,15 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,14 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2156,6 +2148,14 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Thu Oct 23 02:43:47 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{08B7B102-25F3-4832-B455-52F9B4336971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{47456A31-F02F-4C40-A590-5839DCEE9A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>159.62</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="E8" s="10">
-        <v>157.68</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>167.68</v>
+        <v>167.7</v>
       </c>
       <c r="G8" s="10">
-        <v>157.83000000000001</v>
+        <v>157.86000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>159.62</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="E9" s="13">
-        <v>157.68</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>167.68</v>
+        <v>167.7</v>
       </c>
       <c r="G9" s="13">
-        <v>157.83000000000001</v>
+        <v>157.86000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>161.88999999999999</v>
+        <v>162.16</v>
       </c>
       <c r="E10" s="10">
-        <v>159.75</v>
+        <v>159.91</v>
       </c>
       <c r="F10" s="10">
-        <v>169.75</v>
+        <v>169.91</v>
       </c>
       <c r="G10" s="10">
-        <v>160.22</v>
+        <v>160.38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>160.06</v>
+        <v>159.62</v>
       </c>
       <c r="E11" s="13">
-        <v>157.88999999999999</v>
+        <v>157.68</v>
       </c>
       <c r="F11" s="13">
-        <v>167.89</v>
+        <v>167.68</v>
       </c>
       <c r="G11" s="13">
-        <v>158.05000000000001</v>
+        <v>157.83000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>160.06</v>
+        <v>159.62</v>
       </c>
       <c r="E12" s="10">
-        <v>157.88999999999999</v>
+        <v>157.68</v>
       </c>
       <c r="F12" s="10">
-        <v>167.89</v>
+        <v>167.68</v>
       </c>
       <c r="G12" s="10">
-        <v>158.05000000000001</v>
+        <v>157.83000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>162.28</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="E13" s="13">
-        <v>160.22999999999999</v>
+        <v>159.75</v>
       </c>
       <c r="F13" s="13">
-        <v>170.23</v>
+        <v>169.75</v>
       </c>
       <c r="G13" s="13">
-        <v>160.69999999999999</v>
+        <v>160.22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>165.32</v>
+        <v>165.59</v>
       </c>
       <c r="E17" s="10">
-        <v>162.80000000000001</v>
+        <v>162.78</v>
       </c>
       <c r="F17" s="10">
-        <v>172.8</v>
+        <v>172.78</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>165.7</v>
+        <v>165.32</v>
       </c>
       <c r="E18" s="13">
-        <v>163.07</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="F18" s="13">
-        <v>173.07</v>
+        <v>172.8</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>160.54</v>
+        <v>160.88999999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>158.75</v>
+        <v>158.81</v>
       </c>
       <c r="F22" s="10">
-        <v>168.35</v>
+        <v>168.41</v>
       </c>
       <c r="G22" s="10">
-        <v>159.93</v>
+        <v>159.99</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>166.65</v>
+        <v>166.93</v>
       </c>
       <c r="E23" s="13">
-        <v>163.57</v>
+        <v>163.63</v>
       </c>
       <c r="F23" s="13">
-        <v>173.57</v>
+        <v>173.63</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>166.46</v>
+        <v>166.73</v>
       </c>
       <c r="E24" s="10">
-        <v>163.78</v>
+        <v>163.84</v>
       </c>
       <c r="F24" s="10">
-        <v>173.78</v>
+        <v>173.84</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>167.29</v>
+        <v>167.56</v>
       </c>
       <c r="E25" s="13">
-        <v>163.16999999999999</v>
+        <v>163.22999999999999</v>
       </c>
       <c r="F25" s="13">
-        <v>173.17</v>
+        <v>173.23</v>
       </c>
       <c r="G25" s="13">
-        <v>163</v>
+        <v>163.05000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>166.01</v>
+        <v>166.28</v>
       </c>
       <c r="E26" s="10">
-        <v>164.71</v>
+        <v>164.76</v>
       </c>
       <c r="F26" s="10">
-        <v>174.71</v>
+        <v>174.76</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>160.97999999999999</v>
+        <v>160.54</v>
       </c>
       <c r="E27" s="13">
-        <v>159.12</v>
+        <v>158.75</v>
       </c>
       <c r="F27" s="13">
-        <v>168.72</v>
+        <v>168.35</v>
       </c>
       <c r="G27" s="13">
-        <v>160.30000000000001</v>
+        <v>159.93</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>167.04</v>
+        <v>166.65</v>
       </c>
       <c r="E28" s="22">
-        <v>163.83000000000001</v>
+        <v>163.57</v>
       </c>
       <c r="F28" s="22">
-        <v>173.83</v>
+        <v>173.57</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>166.85</v>
+        <v>166.46</v>
       </c>
       <c r="E29" s="13">
-        <v>164.04</v>
+        <v>163.78</v>
       </c>
       <c r="F29" s="13">
-        <v>174.04</v>
+        <v>173.78</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>167.68</v>
+        <v>167.29</v>
       </c>
       <c r="E30" s="22">
-        <v>163.43</v>
+        <v>163.16999999999999</v>
       </c>
       <c r="F30" s="22">
-        <v>173.43</v>
+        <v>173.17</v>
       </c>
       <c r="G30" s="22">
-        <v>163.26</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>166.4</v>
+        <v>166.01</v>
       </c>
       <c r="E31" s="13">
-        <v>164.97</v>
+        <v>164.71</v>
       </c>
       <c r="F31" s="13">
-        <v>174.97</v>
+        <v>174.71</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>160.13</v>
+        <v>160.4</v>
       </c>
       <c r="E35" s="10">
-        <v>157.07</v>
+        <v>157.13</v>
       </c>
       <c r="F35" s="10">
-        <v>166.07</v>
+        <v>166.13</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>160.52000000000001</v>
+        <v>160.13</v>
       </c>
       <c r="E36" s="13">
-        <v>157.33000000000001</v>
+        <v>157.07</v>
       </c>
       <c r="F36" s="13">
-        <v>166.33</v>
+        <v>166.07</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>165.78</v>
+        <v>166.05</v>
       </c>
       <c r="E40" s="10">
-        <v>162.54</v>
+        <v>162.51</v>
       </c>
       <c r="F40" s="10">
-        <v>172.54</v>
+        <v>172.51</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>165.5</v>
+        <v>165.77</v>
       </c>
       <c r="E41" s="13">
-        <v>162.96</v>
+        <v>162.93</v>
       </c>
       <c r="F41" s="13">
-        <v>172.96</v>
+        <v>172.93</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>166.17</v>
+        <v>165.78</v>
       </c>
       <c r="E42" s="10">
-        <v>162.81</v>
+        <v>162.54</v>
       </c>
       <c r="F42" s="10">
-        <v>172.81</v>
+        <v>172.54</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>165.89</v>
+        <v>165.5</v>
       </c>
       <c r="E43" s="13">
-        <v>163.22999999999999</v>
+        <v>162.96</v>
       </c>
       <c r="F43" s="13">
-        <v>173.23</v>
+        <v>172.96</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>160.19999999999999</v>
+        <v>159.88</v>
       </c>
       <c r="E47" s="10">
-        <v>158.82</v>
+        <v>158.61000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>168.82</v>
+        <v>168.61</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>160.18</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="E48" s="13">
-        <v>158.99</v>
+        <v>158.78</v>
       </c>
       <c r="F48" s="13">
-        <v>168.99</v>
+        <v>168.78</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>160.86000000000001</v>
+        <v>160.19999999999999</v>
       </c>
       <c r="E49" s="10">
-        <v>159.02000000000001</v>
+        <v>158.82</v>
       </c>
       <c r="F49" s="10">
-        <v>169.02</v>
+        <v>168.82</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>160.84</v>
+        <v>160.18</v>
       </c>
       <c r="E50" s="13">
-        <v>159.19</v>
+        <v>158.99</v>
       </c>
       <c r="F50" s="13">
-        <v>169.19</v>
+        <v>168.99</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>175.96</v>
+        <v>176.24</v>
       </c>
       <c r="E54" s="10">
-        <v>172.84</v>
+        <v>172.88</v>
       </c>
       <c r="F54" s="10">
-        <v>182.84</v>
+        <v>182.88</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>163.63</v>
+        <v>163.9</v>
       </c>
       <c r="E55" s="13">
-        <v>170.13</v>
+        <v>170.3</v>
       </c>
       <c r="F55" s="13">
-        <v>180.13</v>
+        <v>180.3</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>165.91</v>
+        <v>166.18</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>165.58</v>
+        <v>165.85</v>
       </c>
       <c r="E57" s="13">
-        <v>164.4</v>
+        <v>164.57</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>161.47999999999999</v>
+        <v>161.76</v>
       </c>
       <c r="E58" s="10">
-        <v>160.44999999999999</v>
+        <v>160.62</v>
       </c>
       <c r="F58" s="10">
-        <v>170.45</v>
+        <v>170.62</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>168.3</v>
+        <v>168.58</v>
       </c>
       <c r="E59" s="13">
-        <v>171.03</v>
+        <v>171.08</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>176.36</v>
+        <v>175.96</v>
       </c>
       <c r="E60" s="10">
-        <v>173.11</v>
+        <v>172.84</v>
       </c>
       <c r="F60" s="10">
-        <v>183.11</v>
+        <v>182.84</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>164.01</v>
+        <v>163.63</v>
       </c>
       <c r="E61" s="13">
-        <v>170.5</v>
+        <v>170.13</v>
       </c>
       <c r="F61" s="13">
-        <v>180.5</v>
+        <v>180.13</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>166.3</v>
+        <v>165.91</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>165.96</v>
+        <v>165.58</v>
       </c>
       <c r="E63" s="13">
-        <v>164.77</v>
+        <v>164.4</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>161.87</v>
+        <v>161.47999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>160.82</v>
+        <v>160.44999999999999</v>
       </c>
       <c r="F64" s="10">
-        <v>170.82</v>
+        <v>170.45</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>168.69</v>
+        <v>168.3</v>
       </c>
       <c r="E65" s="13">
-        <v>171.29</v>
+        <v>171.03</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,26 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,33 +2114,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,6 +2154,32 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Fri Oct 24 02:40:24 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{47456A31-F02F-4C40-A590-5839DCEE9A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{011B189F-149B-402C-A264-9BE1E7DB7502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>159.86000000000001</v>
+        <v>161.32</v>
       </c>
       <c r="E8" s="10">
-        <v>157.69999999999999</v>
+        <v>158.15</v>
       </c>
       <c r="F8" s="10">
-        <v>167.7</v>
+        <v>168.15</v>
       </c>
       <c r="G8" s="10">
-        <v>157.86000000000001</v>
+        <v>158.31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>159.86000000000001</v>
+        <v>161.32</v>
       </c>
       <c r="E9" s="13">
-        <v>157.69999999999999</v>
+        <v>158.15</v>
       </c>
       <c r="F9" s="13">
-        <v>167.7</v>
+        <v>168.15</v>
       </c>
       <c r="G9" s="13">
-        <v>157.86000000000001</v>
+        <v>158.31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>162.16</v>
+        <v>163.72</v>
       </c>
       <c r="E10" s="10">
-        <v>159.91</v>
+        <v>160.49</v>
       </c>
       <c r="F10" s="10">
-        <v>169.91</v>
+        <v>170.49</v>
       </c>
       <c r="G10" s="10">
-        <v>160.38</v>
+        <v>160.96</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>159.62</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="E11" s="13">
-        <v>157.68</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>167.68</v>
+        <v>167.7</v>
       </c>
       <c r="G11" s="13">
-        <v>157.83000000000001</v>
+        <v>157.86000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>159.62</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="E12" s="10">
-        <v>157.68</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>167.68</v>
+        <v>167.7</v>
       </c>
       <c r="G12" s="10">
-        <v>157.83000000000001</v>
+        <v>157.86000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>161.88999999999999</v>
+        <v>162.16</v>
       </c>
       <c r="E13" s="13">
-        <v>159.75</v>
+        <v>159.91</v>
       </c>
       <c r="F13" s="13">
-        <v>169.75</v>
+        <v>169.91</v>
       </c>
       <c r="G13" s="13">
-        <v>160.22</v>
+        <v>160.38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>165.59</v>
+        <v>167.16</v>
       </c>
       <c r="E17" s="10">
-        <v>162.78</v>
+        <v>163.29</v>
       </c>
       <c r="F17" s="10">
-        <v>172.78</v>
+        <v>173.29</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>165.32</v>
+        <v>165.59</v>
       </c>
       <c r="E18" s="13">
-        <v>162.80000000000001</v>
+        <v>162.78</v>
       </c>
       <c r="F18" s="13">
-        <v>172.8</v>
+        <v>172.78</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>160.88999999999999</v>
+        <v>162.44999999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>158.81</v>
+        <v>159.5</v>
       </c>
       <c r="F22" s="10">
-        <v>168.41</v>
+        <v>169.1</v>
       </c>
       <c r="G22" s="10">
-        <v>159.99</v>
+        <v>160.66999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>166.93</v>
+        <v>168.49</v>
       </c>
       <c r="E23" s="13">
-        <v>163.63</v>
+        <v>164.21</v>
       </c>
       <c r="F23" s="13">
-        <v>173.63</v>
+        <v>174.21</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>166.73</v>
+        <v>168.29</v>
       </c>
       <c r="E24" s="10">
-        <v>163.84</v>
+        <v>164.41</v>
       </c>
       <c r="F24" s="10">
-        <v>173.84</v>
+        <v>174.41</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>167.56</v>
+        <v>169.12</v>
       </c>
       <c r="E25" s="13">
-        <v>163.22999999999999</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="F25" s="13">
-        <v>173.23</v>
+        <v>173.8</v>
       </c>
       <c r="G25" s="13">
-        <v>163.05000000000001</v>
+        <v>163.63</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>166.28</v>
+        <v>167.85</v>
       </c>
       <c r="E26" s="10">
-        <v>164.76</v>
+        <v>165.34</v>
       </c>
       <c r="F26" s="10">
-        <v>174.76</v>
+        <v>175.34</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>160.54</v>
+        <v>160.88999999999999</v>
       </c>
       <c r="E27" s="13">
-        <v>158.75</v>
+        <v>158.81</v>
       </c>
       <c r="F27" s="13">
-        <v>168.35</v>
+        <v>168.41</v>
       </c>
       <c r="G27" s="13">
-        <v>159.93</v>
+        <v>159.99</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>166.65</v>
+        <v>166.93</v>
       </c>
       <c r="E28" s="22">
-        <v>163.57</v>
+        <v>163.63</v>
       </c>
       <c r="F28" s="22">
-        <v>173.57</v>
+        <v>173.63</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>166.46</v>
+        <v>166.73</v>
       </c>
       <c r="E29" s="13">
-        <v>163.78</v>
+        <v>163.84</v>
       </c>
       <c r="F29" s="13">
-        <v>173.78</v>
+        <v>173.84</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>167.29</v>
+        <v>167.56</v>
       </c>
       <c r="E30" s="22">
-        <v>163.16999999999999</v>
+        <v>163.22999999999999</v>
       </c>
       <c r="F30" s="22">
-        <v>173.17</v>
+        <v>173.23</v>
       </c>
       <c r="G30" s="22">
-        <v>163</v>
+        <v>163.05000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>166.01</v>
+        <v>166.28</v>
       </c>
       <c r="E31" s="13">
-        <v>164.71</v>
+        <v>164.76</v>
       </c>
       <c r="F31" s="13">
-        <v>174.71</v>
+        <v>174.76</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>160.4</v>
+        <v>161.97</v>
       </c>
       <c r="E35" s="10">
-        <v>157.13</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>166.13</v>
+        <v>166.71</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>160.13</v>
+        <v>160.4</v>
       </c>
       <c r="E36" s="13">
-        <v>157.07</v>
+        <v>157.13</v>
       </c>
       <c r="F36" s="13">
-        <v>166.07</v>
+        <v>166.13</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>166.05</v>
+        <v>167.61</v>
       </c>
       <c r="E40" s="10">
-        <v>162.51</v>
+        <v>163.01</v>
       </c>
       <c r="F40" s="10">
-        <v>172.51</v>
+        <v>173.01</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>165.77</v>
+        <v>167.33</v>
       </c>
       <c r="E41" s="13">
-        <v>162.93</v>
+        <v>163.43</v>
       </c>
       <c r="F41" s="13">
-        <v>172.93</v>
+        <v>173.43</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>165.78</v>
+        <v>166.05</v>
       </c>
       <c r="E42" s="10">
-        <v>162.54</v>
+        <v>162.51</v>
       </c>
       <c r="F42" s="10">
-        <v>172.54</v>
+        <v>172.51</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>165.5</v>
+        <v>165.77</v>
       </c>
       <c r="E43" s="13">
-        <v>162.96</v>
+        <v>162.93</v>
       </c>
       <c r="F43" s="13">
-        <v>172.96</v>
+        <v>172.93</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>159.88</v>
+        <v>160.61000000000001</v>
       </c>
       <c r="E47" s="10">
-        <v>158.61000000000001</v>
+        <v>159.08000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>168.61</v>
+        <v>169.08</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>159.86000000000001</v>
+        <v>160.59</v>
       </c>
       <c r="E48" s="13">
-        <v>158.78</v>
+        <v>159.25</v>
       </c>
       <c r="F48" s="13">
-        <v>168.78</v>
+        <v>169.25</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>160.19999999999999</v>
+        <v>159.88</v>
       </c>
       <c r="E49" s="10">
-        <v>158.82</v>
+        <v>158.61000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>168.82</v>
+        <v>168.61</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>160.18</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="E50" s="13">
-        <v>158.99</v>
+        <v>158.78</v>
       </c>
       <c r="F50" s="13">
-        <v>168.99</v>
+        <v>168.78</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>176.24</v>
+        <v>177.81</v>
       </c>
       <c r="E54" s="10">
-        <v>172.88</v>
+        <v>173.44</v>
       </c>
       <c r="F54" s="10">
-        <v>182.88</v>
+        <v>183.44</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>163.9</v>
+        <v>165.46</v>
       </c>
       <c r="E55" s="13">
-        <v>170.3</v>
+        <v>170.77</v>
       </c>
       <c r="F55" s="13">
-        <v>180.3</v>
+        <v>180.77</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>166.18</v>
+        <v>167.74</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>165.85</v>
+        <v>167.42</v>
       </c>
       <c r="E57" s="13">
-        <v>164.57</v>
+        <v>165.04</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>161.76</v>
+        <v>163.32</v>
       </c>
       <c r="E58" s="10">
-        <v>160.62</v>
+        <v>161.09</v>
       </c>
       <c r="F58" s="10">
-        <v>170.62</v>
+        <v>171.09</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>168.58</v>
+        <v>170.15</v>
       </c>
       <c r="E59" s="13">
-        <v>171.08</v>
+        <v>171.65</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>175.96</v>
+        <v>176.24</v>
       </c>
       <c r="E60" s="10">
-        <v>172.84</v>
+        <v>172.88</v>
       </c>
       <c r="F60" s="10">
-        <v>182.84</v>
+        <v>182.88</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>163.63</v>
+        <v>163.9</v>
       </c>
       <c r="E61" s="13">
-        <v>170.13</v>
+        <v>170.3</v>
       </c>
       <c r="F61" s="13">
-        <v>180.13</v>
+        <v>180.3</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>165.91</v>
+        <v>166.18</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>165.58</v>
+        <v>165.85</v>
       </c>
       <c r="E63" s="13">
-        <v>164.4</v>
+        <v>164.57</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>161.47999999999999</v>
+        <v>161.76</v>
       </c>
       <c r="E64" s="10">
-        <v>160.44999999999999</v>
+        <v>160.62</v>
       </c>
       <c r="F64" s="10">
-        <v>170.45</v>
+        <v>170.62</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>168.3</v>
+        <v>168.58</v>
       </c>
       <c r="E65" s="13">
-        <v>171.03</v>
+        <v>171.08</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,42 +2134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2161,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Mon Oct 27 02:57:51 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{011B189F-149B-402C-A264-9BE1E7DB7502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{603108A9-C355-43B8-AFBE-77122574D313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>161.32</v>
+        <v>163.75</v>
       </c>
       <c r="E8" s="10">
-        <v>158.15</v>
+        <v>159.53</v>
       </c>
       <c r="F8" s="10">
-        <v>168.15</v>
+        <v>169.53</v>
       </c>
       <c r="G8" s="10">
-        <v>158.31</v>
+        <v>159.69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>161.32</v>
+        <v>163.75</v>
       </c>
       <c r="E9" s="13">
-        <v>158.15</v>
+        <v>159.53</v>
       </c>
       <c r="F9" s="13">
-        <v>168.15</v>
+        <v>169.53</v>
       </c>
       <c r="G9" s="13">
-        <v>158.31</v>
+        <v>159.69</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>163.72</v>
+        <v>166.18</v>
       </c>
       <c r="E10" s="10">
-        <v>160.49</v>
+        <v>161.81</v>
       </c>
       <c r="F10" s="10">
-        <v>170.49</v>
+        <v>171.81</v>
       </c>
       <c r="G10" s="10">
-        <v>160.96</v>
+        <v>162.28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>159.86000000000001</v>
+        <v>161.32</v>
       </c>
       <c r="E11" s="13">
-        <v>157.69999999999999</v>
+        <v>158.15</v>
       </c>
       <c r="F11" s="13">
-        <v>167.7</v>
+        <v>168.15</v>
       </c>
       <c r="G11" s="13">
-        <v>157.86000000000001</v>
+        <v>158.31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>159.86000000000001</v>
+        <v>161.32</v>
       </c>
       <c r="E12" s="10">
-        <v>157.69999999999999</v>
+        <v>158.15</v>
       </c>
       <c r="F12" s="10">
-        <v>167.7</v>
+        <v>168.15</v>
       </c>
       <c r="G12" s="10">
-        <v>157.86000000000001</v>
+        <v>158.31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>162.16</v>
+        <v>163.72</v>
       </c>
       <c r="E13" s="13">
-        <v>159.91</v>
+        <v>160.49</v>
       </c>
       <c r="F13" s="13">
-        <v>169.91</v>
+        <v>170.49</v>
       </c>
       <c r="G13" s="13">
-        <v>160.38</v>
+        <v>160.96</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>167.16</v>
+        <v>169.63</v>
       </c>
       <c r="E17" s="10">
-        <v>163.29</v>
+        <v>164.59</v>
       </c>
       <c r="F17" s="10">
-        <v>173.29</v>
+        <v>174.59</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>165.59</v>
+        <v>167.16</v>
       </c>
       <c r="E18" s="13">
-        <v>162.78</v>
+        <v>163.29</v>
       </c>
       <c r="F18" s="13">
-        <v>172.78</v>
+        <v>173.29</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>162.44999999999999</v>
+        <v>165.11</v>
       </c>
       <c r="E22" s="10">
-        <v>159.5</v>
+        <v>160.81</v>
       </c>
       <c r="F22" s="10">
-        <v>169.1</v>
+        <v>170.41</v>
       </c>
       <c r="G22" s="10">
-        <v>160.66999999999999</v>
+        <v>161.99</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>168.49</v>
+        <v>170.95</v>
       </c>
       <c r="E23" s="13">
-        <v>164.21</v>
+        <v>165.53</v>
       </c>
       <c r="F23" s="13">
-        <v>174.21</v>
+        <v>175.53</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>168.29</v>
+        <v>170.76</v>
       </c>
       <c r="E24" s="10">
-        <v>164.41</v>
+        <v>165.73</v>
       </c>
       <c r="F24" s="10">
-        <v>174.41</v>
+        <v>175.73</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>169.12</v>
+        <v>171.59</v>
       </c>
       <c r="E25" s="13">
-        <v>163.80000000000001</v>
+        <v>165.12</v>
       </c>
       <c r="F25" s="13">
-        <v>173.8</v>
+        <v>175.12</v>
       </c>
       <c r="G25" s="13">
-        <v>163.63</v>
+        <v>164.95</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>167.85</v>
+        <v>170.31</v>
       </c>
       <c r="E26" s="10">
-        <v>165.34</v>
+        <v>166.68</v>
       </c>
       <c r="F26" s="10">
-        <v>175.34</v>
+        <v>176.68</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>160.88999999999999</v>
+        <v>162.44999999999999</v>
       </c>
       <c r="E27" s="13">
-        <v>158.81</v>
+        <v>159.5</v>
       </c>
       <c r="F27" s="13">
-        <v>168.41</v>
+        <v>169.1</v>
       </c>
       <c r="G27" s="13">
-        <v>159.99</v>
+        <v>160.66999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>166.93</v>
+        <v>168.49</v>
       </c>
       <c r="E28" s="22">
-        <v>163.63</v>
+        <v>164.21</v>
       </c>
       <c r="F28" s="22">
-        <v>173.63</v>
+        <v>174.21</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>166.73</v>
+        <v>168.29</v>
       </c>
       <c r="E29" s="13">
-        <v>163.84</v>
+        <v>164.41</v>
       </c>
       <c r="F29" s="13">
-        <v>173.84</v>
+        <v>174.41</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>167.56</v>
+        <v>169.12</v>
       </c>
       <c r="E30" s="22">
-        <v>163.22999999999999</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="F30" s="22">
-        <v>173.23</v>
+        <v>173.8</v>
       </c>
       <c r="G30" s="22">
-        <v>163.05000000000001</v>
+        <v>163.63</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>166.28</v>
+        <v>167.85</v>
       </c>
       <c r="E31" s="13">
-        <v>164.76</v>
+        <v>165.34</v>
       </c>
       <c r="F31" s="13">
-        <v>174.76</v>
+        <v>175.34</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>161.97</v>
+        <v>164.43</v>
       </c>
       <c r="E35" s="10">
-        <v>157.69999999999999</v>
+        <v>159.02000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>166.71</v>
+        <v>168.02</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>160.4</v>
+        <v>161.97</v>
       </c>
       <c r="E36" s="13">
-        <v>157.13</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>166.13</v>
+        <v>166.71</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>167.61</v>
+        <v>170.08</v>
       </c>
       <c r="E40" s="10">
-        <v>163.01</v>
+        <v>164.3</v>
       </c>
       <c r="F40" s="10">
-        <v>173.01</v>
+        <v>174.3</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>167.33</v>
+        <v>169.79</v>
       </c>
       <c r="E41" s="13">
-        <v>163.43</v>
+        <v>164.72</v>
       </c>
       <c r="F41" s="13">
-        <v>173.43</v>
+        <v>174.72</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>166.05</v>
+        <v>167.61</v>
       </c>
       <c r="E42" s="10">
-        <v>162.51</v>
+        <v>163.01</v>
       </c>
       <c r="F42" s="10">
-        <v>172.51</v>
+        <v>173.01</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>165.77</v>
+        <v>167.33</v>
       </c>
       <c r="E43" s="13">
-        <v>162.93</v>
+        <v>163.43</v>
       </c>
       <c r="F43" s="13">
-        <v>172.93</v>
+        <v>173.43</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>160.61000000000001</v>
+        <v>161.88</v>
       </c>
       <c r="E47" s="10">
-        <v>159.08000000000001</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>169.08</v>
+        <v>169.86</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>160.59</v>
+        <v>161.87</v>
       </c>
       <c r="E48" s="13">
-        <v>159.25</v>
+        <v>160.04</v>
       </c>
       <c r="F48" s="13">
-        <v>169.25</v>
+        <v>170.04</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>159.88</v>
+        <v>160.61000000000001</v>
       </c>
       <c r="E49" s="10">
-        <v>158.61000000000001</v>
+        <v>159.08000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>168.61</v>
+        <v>169.08</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>159.86000000000001</v>
+        <v>160.59</v>
       </c>
       <c r="E50" s="13">
-        <v>158.78</v>
+        <v>159.25</v>
       </c>
       <c r="F50" s="13">
-        <v>168.78</v>
+        <v>169.25</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>177.81</v>
+        <v>180.28</v>
       </c>
       <c r="E54" s="10">
-        <v>173.44</v>
+        <v>174.75</v>
       </c>
       <c r="F54" s="10">
-        <v>183.44</v>
+        <v>184.75</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>165.46</v>
+        <v>167.93</v>
       </c>
       <c r="E55" s="13">
-        <v>170.77</v>
+        <v>171.98</v>
       </c>
       <c r="F55" s="13">
-        <v>180.77</v>
+        <v>181.98</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>167.74</v>
+        <v>170.2</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>167.42</v>
+        <v>169.88</v>
       </c>
       <c r="E57" s="13">
-        <v>165.04</v>
+        <v>166.25</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>163.32</v>
+        <v>165.78</v>
       </c>
       <c r="E58" s="10">
-        <v>161.09</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>171.09</v>
+        <v>172.3</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>170.15</v>
+        <v>172.61</v>
       </c>
       <c r="E59" s="13">
-        <v>171.65</v>
+        <v>172.96</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>176.24</v>
+        <v>177.81</v>
       </c>
       <c r="E60" s="10">
-        <v>172.88</v>
+        <v>173.44</v>
       </c>
       <c r="F60" s="10">
-        <v>182.88</v>
+        <v>183.44</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>163.9</v>
+        <v>165.46</v>
       </c>
       <c r="E61" s="13">
-        <v>170.3</v>
+        <v>170.77</v>
       </c>
       <c r="F61" s="13">
-        <v>180.3</v>
+        <v>180.77</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>166.18</v>
+        <v>167.74</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>165.85</v>
+        <v>167.42</v>
       </c>
       <c r="E63" s="13">
-        <v>164.57</v>
+        <v>165.04</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>161.76</v>
+        <v>163.32</v>
       </c>
       <c r="E64" s="10">
-        <v>160.62</v>
+        <v>161.09</v>
       </c>
       <c r="F64" s="10">
-        <v>170.62</v>
+        <v>171.09</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>168.58</v>
+        <v>170.15</v>
       </c>
       <c r="E65" s="13">
-        <v>171.08</v>
+        <v>171.65</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,26 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,10 +2114,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2161,21 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Oct 28 02:46:40 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{603108A9-C355-43B8-AFBE-77122574D313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5A3604A1-8CF4-48AD-BEEA-A07B10B7D5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>163.75</v>
+        <v>164.26</v>
       </c>
       <c r="E8" s="10">
-        <v>159.53</v>
+        <v>159.51</v>
       </c>
       <c r="F8" s="10">
-        <v>169.53</v>
+        <v>169.51</v>
       </c>
       <c r="G8" s="10">
-        <v>159.69</v>
+        <v>159.66999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>163.75</v>
+        <v>164.26</v>
       </c>
       <c r="E9" s="13">
-        <v>159.53</v>
+        <v>159.51</v>
       </c>
       <c r="F9" s="13">
-        <v>169.53</v>
+        <v>169.51</v>
       </c>
       <c r="G9" s="13">
-        <v>159.69</v>
+        <v>159.66999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>166.18</v>
+        <v>167.11</v>
       </c>
       <c r="E10" s="10">
-        <v>161.81</v>
+        <v>162.22</v>
       </c>
       <c r="F10" s="10">
-        <v>171.81</v>
+        <v>172.22</v>
       </c>
       <c r="G10" s="10">
-        <v>162.28</v>
+        <v>162.69</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>161.32</v>
+        <v>163.75</v>
       </c>
       <c r="E11" s="13">
-        <v>158.15</v>
+        <v>159.53</v>
       </c>
       <c r="F11" s="13">
-        <v>168.15</v>
+        <v>169.53</v>
       </c>
       <c r="G11" s="13">
-        <v>158.31</v>
+        <v>159.69</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>161.32</v>
+        <v>163.75</v>
       </c>
       <c r="E12" s="10">
-        <v>158.15</v>
+        <v>159.53</v>
       </c>
       <c r="F12" s="10">
-        <v>168.15</v>
+        <v>169.53</v>
       </c>
       <c r="G12" s="10">
-        <v>158.31</v>
+        <v>159.69</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>163.72</v>
+        <v>166.18</v>
       </c>
       <c r="E13" s="13">
-        <v>160.49</v>
+        <v>161.81</v>
       </c>
       <c r="F13" s="13">
-        <v>170.49</v>
+        <v>171.81</v>
       </c>
       <c r="G13" s="13">
-        <v>160.96</v>
+        <v>162.28</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>169.63</v>
+        <v>170.56</v>
       </c>
       <c r="E17" s="10">
-        <v>164.59</v>
+        <v>165.08</v>
       </c>
       <c r="F17" s="10">
-        <v>174.59</v>
+        <v>175.08</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>167.16</v>
+        <v>169.63</v>
       </c>
       <c r="E18" s="13">
-        <v>163.29</v>
+        <v>164.59</v>
       </c>
       <c r="F18" s="13">
-        <v>173.29</v>
+        <v>174.59</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>165.11</v>
+        <v>166.05</v>
       </c>
       <c r="E22" s="10">
-        <v>160.81</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>170.41</v>
+        <v>170.83</v>
       </c>
       <c r="G22" s="10">
-        <v>161.99</v>
+        <v>162.4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>170.95</v>
+        <v>171.88</v>
       </c>
       <c r="E23" s="13">
-        <v>165.53</v>
+        <v>165.94</v>
       </c>
       <c r="F23" s="13">
-        <v>175.53</v>
+        <v>175.94</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>170.76</v>
+        <v>171.69</v>
       </c>
       <c r="E24" s="10">
-        <v>165.73</v>
+        <v>166.14</v>
       </c>
       <c r="F24" s="10">
-        <v>175.73</v>
+        <v>176.14</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>171.59</v>
+        <v>172.51</v>
       </c>
       <c r="E25" s="13">
-        <v>165.12</v>
+        <v>165.53</v>
       </c>
       <c r="F25" s="13">
-        <v>175.12</v>
+        <v>175.53</v>
       </c>
       <c r="G25" s="13">
-        <v>164.95</v>
+        <v>165.36</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>170.31</v>
+        <v>171.24</v>
       </c>
       <c r="E26" s="10">
-        <v>166.68</v>
+        <v>167.08</v>
       </c>
       <c r="F26" s="10">
-        <v>176.68</v>
+        <v>177.08</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>162.44999999999999</v>
+        <v>165.11</v>
       </c>
       <c r="E27" s="13">
-        <v>159.5</v>
+        <v>160.81</v>
       </c>
       <c r="F27" s="13">
-        <v>169.1</v>
+        <v>170.41</v>
       </c>
       <c r="G27" s="13">
-        <v>160.66999999999999</v>
+        <v>161.99</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>168.49</v>
+        <v>170.95</v>
       </c>
       <c r="E28" s="22">
-        <v>164.21</v>
+        <v>165.53</v>
       </c>
       <c r="F28" s="22">
-        <v>174.21</v>
+        <v>175.53</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>168.29</v>
+        <v>170.76</v>
       </c>
       <c r="E29" s="13">
-        <v>164.41</v>
+        <v>165.73</v>
       </c>
       <c r="F29" s="13">
-        <v>174.41</v>
+        <v>175.73</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>169.12</v>
+        <v>171.59</v>
       </c>
       <c r="E30" s="22">
-        <v>163.80000000000001</v>
+        <v>165.12</v>
       </c>
       <c r="F30" s="22">
-        <v>173.8</v>
+        <v>175.12</v>
       </c>
       <c r="G30" s="22">
-        <v>163.63</v>
+        <v>164.95</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>167.85</v>
+        <v>170.31</v>
       </c>
       <c r="E31" s="13">
-        <v>165.34</v>
+        <v>166.68</v>
       </c>
       <c r="F31" s="13">
-        <v>175.34</v>
+        <v>176.68</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>164.43</v>
+        <v>165.35</v>
       </c>
       <c r="E35" s="10">
-        <v>159.02000000000001</v>
+        <v>159.43</v>
       </c>
       <c r="F35" s="10">
-        <v>168.02</v>
+        <v>168.43</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>161.97</v>
+        <v>164.43</v>
       </c>
       <c r="E36" s="13">
-        <v>157.69999999999999</v>
+        <v>159.02000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>166.71</v>
+        <v>168.02</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>170.08</v>
+        <v>170.99</v>
       </c>
       <c r="E40" s="10">
-        <v>164.3</v>
+        <v>164.77</v>
       </c>
       <c r="F40" s="10">
-        <v>174.3</v>
+        <v>174.77</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>169.79</v>
+        <v>170.7</v>
       </c>
       <c r="E41" s="13">
-        <v>164.72</v>
+        <v>165.19</v>
       </c>
       <c r="F41" s="13">
-        <v>174.72</v>
+        <v>175.19</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>167.61</v>
+        <v>170.08</v>
       </c>
       <c r="E42" s="10">
-        <v>163.01</v>
+        <v>164.3</v>
       </c>
       <c r="F42" s="10">
-        <v>173.01</v>
+        <v>174.3</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>167.33</v>
+        <v>169.79</v>
       </c>
       <c r="E43" s="13">
-        <v>163.43</v>
+        <v>164.72</v>
       </c>
       <c r="F43" s="13">
-        <v>173.43</v>
+        <v>174.72</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>161.88</v>
+        <v>163.63999999999999</v>
       </c>
       <c r="E47" s="10">
-        <v>159.86000000000001</v>
+        <v>160.38</v>
       </c>
       <c r="F47" s="10">
-        <v>169.86</v>
+        <v>170.38</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>161.87</v>
+        <v>163.63</v>
       </c>
       <c r="E48" s="13">
-        <v>160.04</v>
+        <v>160.55000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>170.04</v>
+        <v>170.55</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>160.61000000000001</v>
+        <v>161.88</v>
       </c>
       <c r="E49" s="10">
-        <v>159.08000000000001</v>
+        <v>159.86000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>169.08</v>
+        <v>169.86</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>160.59</v>
+        <v>161.87</v>
       </c>
       <c r="E50" s="13">
-        <v>159.25</v>
+        <v>160.04</v>
       </c>
       <c r="F50" s="13">
-        <v>169.25</v>
+        <v>170.04</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>180.28</v>
+        <v>181.2</v>
       </c>
       <c r="E54" s="10">
-        <v>174.75</v>
+        <v>175.11</v>
       </c>
       <c r="F54" s="10">
-        <v>184.75</v>
+        <v>185.11</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>167.93</v>
+        <v>168.85</v>
       </c>
       <c r="E55" s="13">
-        <v>171.98</v>
+        <v>172.62</v>
       </c>
       <c r="F55" s="13">
-        <v>181.98</v>
+        <v>182.62</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>170.2</v>
+        <v>171.12</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>169.88</v>
+        <v>170.82</v>
       </c>
       <c r="E57" s="13">
-        <v>166.25</v>
+        <v>166.89</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>165.78</v>
+        <v>166.72</v>
       </c>
       <c r="E58" s="10">
-        <v>162.30000000000001</v>
+        <v>162.94</v>
       </c>
       <c r="F58" s="10">
-        <v>172.3</v>
+        <v>172.94</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>172.61</v>
+        <v>173.55</v>
       </c>
       <c r="E59" s="13">
-        <v>172.96</v>
+        <v>173.34</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>177.81</v>
+        <v>180.28</v>
       </c>
       <c r="E60" s="10">
-        <v>173.44</v>
+        <v>174.75</v>
       </c>
       <c r="F60" s="10">
-        <v>183.44</v>
+        <v>184.75</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>165.46</v>
+        <v>167.93</v>
       </c>
       <c r="E61" s="13">
-        <v>170.77</v>
+        <v>171.98</v>
       </c>
       <c r="F61" s="13">
-        <v>180.77</v>
+        <v>181.98</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>167.74</v>
+        <v>170.2</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>167.42</v>
+        <v>169.88</v>
       </c>
       <c r="E63" s="13">
-        <v>165.04</v>
+        <v>166.25</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>163.32</v>
+        <v>165.78</v>
       </c>
       <c r="E64" s="10">
-        <v>161.09</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>171.09</v>
+        <v>172.3</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45955</v>
+        <v>45958</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>170.15</v>
+        <v>172.61</v>
       </c>
       <c r="E65" s="13">
-        <v>171.65</v>
+        <v>172.96</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,27 +2134,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2154,32 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Wed Oct 29 02:54:18 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5A3604A1-8CF4-48AD-BEEA-A07B10B7D5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8448416C-61B0-4954-A38F-04FEF26881E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>164.26</v>
+        <v>165.97</v>
       </c>
       <c r="E8" s="10">
-        <v>159.51</v>
+        <v>160.19</v>
       </c>
       <c r="F8" s="10">
-        <v>169.51</v>
+        <v>170.19</v>
       </c>
       <c r="G8" s="10">
-        <v>159.66999999999999</v>
+        <v>160.34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>164.26</v>
+        <v>165.97</v>
       </c>
       <c r="E9" s="13">
-        <v>159.51</v>
+        <v>160.19</v>
       </c>
       <c r="F9" s="13">
-        <v>169.51</v>
+        <v>170.19</v>
       </c>
       <c r="G9" s="13">
-        <v>159.66999999999999</v>
+        <v>160.34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>167.11</v>
+        <v>168.85</v>
       </c>
       <c r="E10" s="10">
-        <v>162.22</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>172.22</v>
+        <v>172.95</v>
       </c>
       <c r="G10" s="10">
-        <v>162.69</v>
+        <v>163.41999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>163.75</v>
+        <v>164.26</v>
       </c>
       <c r="E11" s="13">
-        <v>159.53</v>
+        <v>159.51</v>
       </c>
       <c r="F11" s="13">
-        <v>169.53</v>
+        <v>169.51</v>
       </c>
       <c r="G11" s="13">
-        <v>159.69</v>
+        <v>159.66999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>163.75</v>
+        <v>164.26</v>
       </c>
       <c r="E12" s="10">
-        <v>159.53</v>
+        <v>159.51</v>
       </c>
       <c r="F12" s="10">
-        <v>169.53</v>
+        <v>169.51</v>
       </c>
       <c r="G12" s="10">
-        <v>159.69</v>
+        <v>159.66999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>166.18</v>
+        <v>167.11</v>
       </c>
       <c r="E13" s="13">
-        <v>161.81</v>
+        <v>162.22</v>
       </c>
       <c r="F13" s="13">
-        <v>171.81</v>
+        <v>172.22</v>
       </c>
       <c r="G13" s="13">
-        <v>162.28</v>
+        <v>162.69</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>170.56</v>
+        <v>172.33</v>
       </c>
       <c r="E17" s="10">
-        <v>165.08</v>
+        <v>165.82</v>
       </c>
       <c r="F17" s="10">
-        <v>175.08</v>
+        <v>175.82</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>169.63</v>
+        <v>170.56</v>
       </c>
       <c r="E18" s="13">
-        <v>164.59</v>
+        <v>165.08</v>
       </c>
       <c r="F18" s="13">
-        <v>174.59</v>
+        <v>175.08</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>166.05</v>
+        <v>167.87</v>
       </c>
       <c r="E22" s="10">
-        <v>161.22999999999999</v>
+        <v>161.97</v>
       </c>
       <c r="F22" s="10">
-        <v>170.83</v>
+        <v>171.56</v>
       </c>
       <c r="G22" s="10">
-        <v>162.4</v>
+        <v>163.13999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>171.88</v>
+        <v>173.62</v>
       </c>
       <c r="E23" s="13">
-        <v>165.94</v>
+        <v>166.68</v>
       </c>
       <c r="F23" s="13">
-        <v>175.94</v>
+        <v>176.68</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>171.69</v>
+        <v>173.43</v>
       </c>
       <c r="E24" s="10">
-        <v>166.14</v>
+        <v>166.86</v>
       </c>
       <c r="F24" s="10">
-        <v>176.14</v>
+        <v>176.86</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>172.51</v>
+        <v>174.26</v>
       </c>
       <c r="E25" s="13">
-        <v>165.53</v>
+        <v>166.25</v>
       </c>
       <c r="F25" s="13">
-        <v>175.53</v>
+        <v>176.25</v>
       </c>
       <c r="G25" s="13">
-        <v>165.36</v>
+        <v>166.08</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>171.24</v>
+        <v>172.99</v>
       </c>
       <c r="E26" s="10">
-        <v>167.08</v>
+        <v>167.81</v>
       </c>
       <c r="F26" s="10">
-        <v>177.08</v>
+        <v>177.82</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>165.11</v>
+        <v>166.05</v>
       </c>
       <c r="E27" s="13">
-        <v>160.81</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>170.41</v>
+        <v>170.83</v>
       </c>
       <c r="G27" s="13">
-        <v>161.99</v>
+        <v>162.4</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>170.95</v>
+        <v>171.88</v>
       </c>
       <c r="E28" s="22">
-        <v>165.53</v>
+        <v>165.94</v>
       </c>
       <c r="F28" s="22">
-        <v>175.53</v>
+        <v>175.94</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>170.76</v>
+        <v>171.69</v>
       </c>
       <c r="E29" s="13">
-        <v>165.73</v>
+        <v>166.14</v>
       </c>
       <c r="F29" s="13">
-        <v>175.73</v>
+        <v>176.14</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>171.59</v>
+        <v>172.51</v>
       </c>
       <c r="E30" s="22">
-        <v>165.12</v>
+        <v>165.53</v>
       </c>
       <c r="F30" s="22">
-        <v>175.12</v>
+        <v>175.53</v>
       </c>
       <c r="G30" s="22">
-        <v>164.95</v>
+        <v>165.36</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>170.31</v>
+        <v>171.24</v>
       </c>
       <c r="E31" s="13">
-        <v>166.68</v>
+        <v>167.08</v>
       </c>
       <c r="F31" s="13">
-        <v>176.68</v>
+        <v>177.08</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>165.35</v>
+        <v>167.1</v>
       </c>
       <c r="E35" s="10">
-        <v>159.43</v>
+        <v>160.16999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>168.43</v>
+        <v>169.17</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>164.43</v>
+        <v>165.35</v>
       </c>
       <c r="E36" s="13">
-        <v>159.02000000000001</v>
+        <v>159.43</v>
       </c>
       <c r="F36" s="13">
-        <v>168.02</v>
+        <v>168.43</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>170.99</v>
+        <v>172.72</v>
       </c>
       <c r="E40" s="10">
-        <v>164.77</v>
+        <v>165.48</v>
       </c>
       <c r="F40" s="10">
-        <v>174.77</v>
+        <v>175.48</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>170.7</v>
+        <v>172.43</v>
       </c>
       <c r="E41" s="13">
-        <v>165.19</v>
+        <v>165.9</v>
       </c>
       <c r="F41" s="13">
-        <v>175.19</v>
+        <v>175.9</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>170.08</v>
+        <v>170.99</v>
       </c>
       <c r="E42" s="10">
-        <v>164.3</v>
+        <v>164.77</v>
       </c>
       <c r="F42" s="10">
-        <v>174.3</v>
+        <v>174.77</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>169.79</v>
+        <v>170.7</v>
       </c>
       <c r="E43" s="13">
-        <v>164.72</v>
+        <v>165.19</v>
       </c>
       <c r="F43" s="13">
-        <v>174.72</v>
+        <v>175.19</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>163.63999999999999</v>
+        <v>165.14</v>
       </c>
       <c r="E47" s="10">
-        <v>160.38</v>
+        <v>160.96</v>
       </c>
       <c r="F47" s="10">
-        <v>170.38</v>
+        <v>170.96</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>163.63</v>
+        <v>165.14</v>
       </c>
       <c r="E48" s="13">
-        <v>160.55000000000001</v>
+        <v>161.13999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>170.55</v>
+        <v>171.14</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>161.88</v>
+        <v>163.63999999999999</v>
       </c>
       <c r="E49" s="10">
-        <v>159.86000000000001</v>
+        <v>160.38</v>
       </c>
       <c r="F49" s="10">
-        <v>169.86</v>
+        <v>170.38</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>161.87</v>
+        <v>163.63</v>
       </c>
       <c r="E50" s="13">
-        <v>160.04</v>
+        <v>160.55000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>170.04</v>
+        <v>170.55</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>181.2</v>
+        <v>182.95</v>
       </c>
       <c r="E54" s="10">
-        <v>175.11</v>
+        <v>175.77</v>
       </c>
       <c r="F54" s="10">
-        <v>185.11</v>
+        <v>185.77</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>168.85</v>
+        <v>170.6</v>
       </c>
       <c r="E55" s="13">
-        <v>172.62</v>
+        <v>173.26</v>
       </c>
       <c r="F55" s="13">
-        <v>182.62</v>
+        <v>183.26</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>171.12</v>
+        <v>172.86</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>170.82</v>
+        <v>172.58</v>
       </c>
       <c r="E57" s="13">
-        <v>166.89</v>
+        <v>167.53</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>166.72</v>
+        <v>168.49</v>
       </c>
       <c r="E58" s="10">
-        <v>162.94</v>
+        <v>163.58000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>172.94</v>
+        <v>173.58</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>173.55</v>
+        <v>175.32</v>
       </c>
       <c r="E59" s="13">
-        <v>173.34</v>
+        <v>174.04</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>180.28</v>
+        <v>181.2</v>
       </c>
       <c r="E60" s="10">
-        <v>174.75</v>
+        <v>175.11</v>
       </c>
       <c r="F60" s="10">
-        <v>184.75</v>
+        <v>185.11</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>167.93</v>
+        <v>168.85</v>
       </c>
       <c r="E61" s="13">
-        <v>171.98</v>
+        <v>172.62</v>
       </c>
       <c r="F61" s="13">
-        <v>181.98</v>
+        <v>182.62</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>170.2</v>
+        <v>171.12</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>169.88</v>
+        <v>170.82</v>
       </c>
       <c r="E63" s="13">
-        <v>166.25</v>
+        <v>166.89</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>165.78</v>
+        <v>166.72</v>
       </c>
       <c r="E64" s="10">
-        <v>162.30000000000001</v>
+        <v>162.94</v>
       </c>
       <c r="F64" s="10">
-        <v>172.3</v>
+        <v>172.94</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>172.61</v>
+        <v>173.55</v>
       </c>
       <c r="E65" s="13">
-        <v>172.96</v>
+        <v>173.34</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1863,15 +1872,6 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,6 +2135,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2148,14 +2156,6 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Thu Oct 30 02:50:33 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8448416C-61B0-4954-A38F-04FEF26881E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{81B0372F-AA36-45F2-ADD5-5A5B1521226C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>165.97</v>
+        <v>167.32</v>
       </c>
       <c r="E8" s="10">
-        <v>160.19</v>
+        <v>160.94</v>
       </c>
       <c r="F8" s="10">
-        <v>170.19</v>
+        <v>170.94</v>
       </c>
       <c r="G8" s="10">
-        <v>160.34</v>
+        <v>161.09</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>165.97</v>
+        <v>167.32</v>
       </c>
       <c r="E9" s="13">
-        <v>160.19</v>
+        <v>160.94</v>
       </c>
       <c r="F9" s="13">
-        <v>170.19</v>
+        <v>170.94</v>
       </c>
       <c r="G9" s="13">
-        <v>160.34</v>
+        <v>161.09</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>168.85</v>
+        <v>169.79</v>
       </c>
       <c r="E10" s="10">
-        <v>162.94999999999999</v>
+        <v>163.41999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>172.95</v>
+        <v>173.42</v>
       </c>
       <c r="G10" s="10">
-        <v>163.41999999999999</v>
+        <v>163.89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>164.26</v>
+        <v>165.97</v>
       </c>
       <c r="E11" s="13">
-        <v>159.51</v>
+        <v>160.19</v>
       </c>
       <c r="F11" s="13">
-        <v>169.51</v>
+        <v>170.19</v>
       </c>
       <c r="G11" s="13">
-        <v>159.66999999999999</v>
+        <v>160.34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>164.26</v>
+        <v>165.97</v>
       </c>
       <c r="E12" s="10">
-        <v>159.51</v>
+        <v>160.19</v>
       </c>
       <c r="F12" s="10">
-        <v>169.51</v>
+        <v>170.19</v>
       </c>
       <c r="G12" s="10">
-        <v>159.66999999999999</v>
+        <v>160.34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>167.11</v>
+        <v>168.85</v>
       </c>
       <c r="E13" s="13">
-        <v>162.22</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>172.22</v>
+        <v>172.95</v>
       </c>
       <c r="G13" s="13">
-        <v>162.69</v>
+        <v>163.41999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>172.33</v>
+        <v>173.29</v>
       </c>
       <c r="E17" s="10">
-        <v>165.82</v>
+        <v>166.35</v>
       </c>
       <c r="F17" s="10">
-        <v>175.82</v>
+        <v>176.35</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>170.56</v>
+        <v>172.33</v>
       </c>
       <c r="E18" s="13">
-        <v>165.08</v>
+        <v>165.82</v>
       </c>
       <c r="F18" s="13">
-        <v>175.08</v>
+        <v>175.82</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>167.87</v>
+        <v>169</v>
       </c>
       <c r="E22" s="10">
-        <v>161.97</v>
+        <v>162.44</v>
       </c>
       <c r="F22" s="10">
-        <v>171.56</v>
+        <v>172.04</v>
       </c>
       <c r="G22" s="10">
-        <v>163.13999999999999</v>
+        <v>163.62</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>173.62</v>
+        <v>174.56</v>
       </c>
       <c r="E23" s="13">
-        <v>166.68</v>
+        <v>167.15</v>
       </c>
       <c r="F23" s="13">
-        <v>176.68</v>
+        <v>177.15</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>173.43</v>
+        <v>174.37</v>
       </c>
       <c r="E24" s="10">
-        <v>166.86</v>
+        <v>167.32</v>
       </c>
       <c r="F24" s="10">
-        <v>176.86</v>
+        <v>177.32</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>174.26</v>
+        <v>175.2</v>
       </c>
       <c r="E25" s="13">
-        <v>166.25</v>
+        <v>166.71</v>
       </c>
       <c r="F25" s="13">
-        <v>176.25</v>
+        <v>176.71</v>
       </c>
       <c r="G25" s="13">
-        <v>166.08</v>
+        <v>166.54</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>172.99</v>
+        <v>173.94</v>
       </c>
       <c r="E26" s="10">
-        <v>167.81</v>
+        <v>168.28</v>
       </c>
       <c r="F26" s="10">
-        <v>177.82</v>
+        <v>178.28</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>166.05</v>
+        <v>167.87</v>
       </c>
       <c r="E27" s="13">
-        <v>161.22999999999999</v>
+        <v>161.97</v>
       </c>
       <c r="F27" s="13">
-        <v>170.83</v>
+        <v>171.56</v>
       </c>
       <c r="G27" s="13">
-        <v>162.4</v>
+        <v>163.13999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>171.88</v>
+        <v>173.62</v>
       </c>
       <c r="E28" s="22">
-        <v>165.94</v>
+        <v>166.68</v>
       </c>
       <c r="F28" s="22">
-        <v>175.94</v>
+        <v>176.68</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>171.69</v>
+        <v>173.43</v>
       </c>
       <c r="E29" s="13">
-        <v>166.14</v>
+        <v>166.86</v>
       </c>
       <c r="F29" s="13">
-        <v>176.14</v>
+        <v>176.86</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>172.51</v>
+        <v>174.26</v>
       </c>
       <c r="E30" s="22">
-        <v>165.53</v>
+        <v>166.25</v>
       </c>
       <c r="F30" s="22">
-        <v>175.53</v>
+        <v>176.25</v>
       </c>
       <c r="G30" s="22">
-        <v>165.36</v>
+        <v>166.08</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>171.24</v>
+        <v>172.99</v>
       </c>
       <c r="E31" s="13">
-        <v>167.08</v>
+        <v>167.81</v>
       </c>
       <c r="F31" s="13">
-        <v>177.08</v>
+        <v>177.82</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>167.1</v>
+        <v>168.04</v>
       </c>
       <c r="E35" s="10">
-        <v>160.16999999999999</v>
+        <v>160.63</v>
       </c>
       <c r="F35" s="10">
-        <v>169.17</v>
+        <v>169.63</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>165.35</v>
+        <v>167.1</v>
       </c>
       <c r="E36" s="13">
-        <v>159.43</v>
+        <v>160.16999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>168.43</v>
+        <v>169.17</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>172.72</v>
+        <v>173.64</v>
       </c>
       <c r="E40" s="10">
-        <v>165.48</v>
+        <v>165.98</v>
       </c>
       <c r="F40" s="10">
-        <v>175.48</v>
+        <v>175.98</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>172.43</v>
+        <v>173.35</v>
       </c>
       <c r="E41" s="13">
-        <v>165.9</v>
+        <v>166.4</v>
       </c>
       <c r="F41" s="13">
-        <v>175.9</v>
+        <v>176.4</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>170.99</v>
+        <v>172.72</v>
       </c>
       <c r="E42" s="10">
-        <v>164.77</v>
+        <v>165.48</v>
       </c>
       <c r="F42" s="10">
-        <v>174.77</v>
+        <v>175.48</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>170.7</v>
+        <v>172.43</v>
       </c>
       <c r="E43" s="13">
-        <v>165.19</v>
+        <v>165.9</v>
       </c>
       <c r="F43" s="13">
-        <v>175.19</v>
+        <v>175.9</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>165.14</v>
+        <v>166.31</v>
       </c>
       <c r="E47" s="10">
-        <v>160.96</v>
+        <v>161.08000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>170.96</v>
+        <v>171.08</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>165.14</v>
+        <v>166.31</v>
       </c>
       <c r="E48" s="13">
-        <v>161.13999999999999</v>
+        <v>161.26</v>
       </c>
       <c r="F48" s="13">
-        <v>171.14</v>
+        <v>171.26</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>163.63999999999999</v>
+        <v>165.14</v>
       </c>
       <c r="E49" s="10">
-        <v>160.38</v>
+        <v>160.96</v>
       </c>
       <c r="F49" s="10">
-        <v>170.38</v>
+        <v>170.96</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>163.63</v>
+        <v>165.14</v>
       </c>
       <c r="E50" s="13">
-        <v>160.55000000000001</v>
+        <v>161.13999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>170.55</v>
+        <v>171.14</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>182.95</v>
+        <v>183.88</v>
       </c>
       <c r="E54" s="10">
-        <v>175.77</v>
+        <v>176.17</v>
       </c>
       <c r="F54" s="10">
-        <v>185.77</v>
+        <v>186.17</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>170.6</v>
+        <v>171.53</v>
       </c>
       <c r="E55" s="13">
-        <v>173.26</v>
+        <v>173.86</v>
       </c>
       <c r="F55" s="13">
-        <v>183.26</v>
+        <v>183.86</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>172.86</v>
+        <v>173.91</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>172.58</v>
+        <v>173.65</v>
       </c>
       <c r="E57" s="13">
-        <v>167.53</v>
+        <v>168.13</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>168.49</v>
+        <v>169.56</v>
       </c>
       <c r="E58" s="10">
-        <v>163.58000000000001</v>
+        <v>164.18</v>
       </c>
       <c r="F58" s="10">
-        <v>173.58</v>
+        <v>174.18</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>175.32</v>
+        <v>176.29</v>
       </c>
       <c r="E59" s="13">
-        <v>174.04</v>
+        <v>174.46</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>181.2</v>
+        <v>182.95</v>
       </c>
       <c r="E60" s="10">
-        <v>175.11</v>
+        <v>175.77</v>
       </c>
       <c r="F60" s="10">
-        <v>185.11</v>
+        <v>185.77</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>168.85</v>
+        <v>170.6</v>
       </c>
       <c r="E61" s="13">
-        <v>172.62</v>
+        <v>173.26</v>
       </c>
       <c r="F61" s="13">
-        <v>182.62</v>
+        <v>183.26</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>171.12</v>
+        <v>172.86</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>170.82</v>
+        <v>172.58</v>
       </c>
       <c r="E63" s="13">
-        <v>166.89</v>
+        <v>167.53</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>166.72</v>
+        <v>168.49</v>
       </c>
       <c r="E64" s="10">
-        <v>162.94</v>
+        <v>163.58000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>172.94</v>
+        <v>173.58</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>173.55</v>
+        <v>175.32</v>
       </c>
       <c r="E65" s="13">
-        <v>173.34</v>
+        <v>174.04</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1872,6 +1863,15 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,14 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2156,6 +2148,14 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fri Oct 31 02:49:49 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{81B0372F-AA36-45F2-ADD5-5A5B1521226C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{86F8D0A0-A1BC-4F43-8591-ED7427850EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>167.32</v>
+        <v>167.82</v>
       </c>
       <c r="E8" s="10">
-        <v>160.94</v>
+        <v>161.06</v>
       </c>
       <c r="F8" s="10">
-        <v>170.94</v>
+        <v>171.06</v>
       </c>
       <c r="G8" s="10">
-        <v>161.09</v>
+        <v>161.22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>167.32</v>
+        <v>167.82</v>
       </c>
       <c r="E9" s="13">
-        <v>160.94</v>
+        <v>161.06</v>
       </c>
       <c r="F9" s="13">
-        <v>170.94</v>
+        <v>171.06</v>
       </c>
       <c r="G9" s="13">
-        <v>161.09</v>
+        <v>161.22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>169.79</v>
+        <v>169.92</v>
       </c>
       <c r="E10" s="10">
-        <v>163.41999999999999</v>
+        <v>163.41</v>
       </c>
       <c r="F10" s="10">
-        <v>173.42</v>
+        <v>173.41</v>
       </c>
       <c r="G10" s="10">
-        <v>163.89</v>
+        <v>163.9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>165.97</v>
+        <v>167.32</v>
       </c>
       <c r="E11" s="13">
-        <v>160.19</v>
+        <v>160.94</v>
       </c>
       <c r="F11" s="13">
-        <v>170.19</v>
+        <v>170.94</v>
       </c>
       <c r="G11" s="13">
-        <v>160.34</v>
+        <v>161.09</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>165.97</v>
+        <v>167.32</v>
       </c>
       <c r="E12" s="10">
-        <v>160.19</v>
+        <v>160.94</v>
       </c>
       <c r="F12" s="10">
-        <v>170.19</v>
+        <v>170.94</v>
       </c>
       <c r="G12" s="10">
-        <v>160.34</v>
+        <v>161.09</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>168.85</v>
+        <v>169.79</v>
       </c>
       <c r="E13" s="13">
-        <v>162.94999999999999</v>
+        <v>163.41999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>172.95</v>
+        <v>173.42</v>
       </c>
       <c r="G13" s="13">
-        <v>163.41999999999999</v>
+        <v>163.89</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>173.29</v>
+        <v>173.43</v>
       </c>
       <c r="E17" s="10">
-        <v>166.35</v>
+        <v>166.39</v>
       </c>
       <c r="F17" s="10">
-        <v>176.35</v>
+        <v>176.39</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>172.33</v>
+        <v>173.29</v>
       </c>
       <c r="E18" s="13">
-        <v>165.82</v>
+        <v>166.35</v>
       </c>
       <c r="F18" s="13">
-        <v>175.82</v>
+        <v>176.35</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>169</v>
+        <v>169.06</v>
       </c>
       <c r="E22" s="10">
-        <v>162.44</v>
+        <v>162.43</v>
       </c>
       <c r="F22" s="10">
-        <v>172.04</v>
+        <v>172.03</v>
       </c>
       <c r="G22" s="10">
-        <v>163.62</v>
+        <v>163.72</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>174.56</v>
+        <v>174.69</v>
       </c>
       <c r="E23" s="13">
-        <v>167.15</v>
+        <v>167.14</v>
       </c>
       <c r="F23" s="13">
-        <v>177.15</v>
+        <v>177.14</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>174.37</v>
+        <v>174.51</v>
       </c>
       <c r="E24" s="10">
-        <v>167.32</v>
+        <v>167.31</v>
       </c>
       <c r="F24" s="10">
-        <v>177.32</v>
+        <v>177.31</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>175.2</v>
+        <v>175.34</v>
       </c>
       <c r="E25" s="13">
-        <v>166.71</v>
+        <v>166.7</v>
       </c>
       <c r="F25" s="13">
-        <v>176.71</v>
+        <v>176.7</v>
       </c>
       <c r="G25" s="13">
-        <v>166.54</v>
+        <v>166.74</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>173.94</v>
+        <v>174.08</v>
       </c>
       <c r="E26" s="10">
-        <v>168.28</v>
+        <v>168.26</v>
       </c>
       <c r="F26" s="10">
-        <v>178.28</v>
+        <v>178.26</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>167.87</v>
+        <v>169</v>
       </c>
       <c r="E27" s="13">
-        <v>161.97</v>
+        <v>162.44</v>
       </c>
       <c r="F27" s="13">
-        <v>171.56</v>
+        <v>172.04</v>
       </c>
       <c r="G27" s="13">
-        <v>163.13999999999999</v>
+        <v>163.62</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>173.62</v>
+        <v>174.56</v>
       </c>
       <c r="E28" s="22">
-        <v>166.68</v>
+        <v>167.15</v>
       </c>
       <c r="F28" s="22">
-        <v>176.68</v>
+        <v>177.15</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>173.43</v>
+        <v>174.37</v>
       </c>
       <c r="E29" s="13">
-        <v>166.86</v>
+        <v>167.32</v>
       </c>
       <c r="F29" s="13">
-        <v>176.86</v>
+        <v>177.32</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>174.26</v>
+        <v>175.2</v>
       </c>
       <c r="E30" s="22">
-        <v>166.25</v>
+        <v>166.71</v>
       </c>
       <c r="F30" s="22">
-        <v>176.25</v>
+        <v>176.71</v>
       </c>
       <c r="G30" s="22">
-        <v>166.08</v>
+        <v>166.54</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>172.99</v>
+        <v>173.94</v>
       </c>
       <c r="E31" s="13">
-        <v>167.81</v>
+        <v>168.28</v>
       </c>
       <c r="F31" s="13">
-        <v>177.82</v>
+        <v>178.28</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,14 +1300,14 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>168.04</v>
+        <v>168.29</v>
       </c>
       <c r="E35" s="10">
         <v>160.63</v>
@@ -1319,20 +1319,20 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>167.1</v>
+        <v>168.04</v>
       </c>
       <c r="E36" s="13">
-        <v>160.16999999999999</v>
+        <v>160.63</v>
       </c>
       <c r="F36" s="13">
-        <v>169.17</v>
+        <v>169.63</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>173.64</v>
+        <v>173.77</v>
       </c>
       <c r="E40" s="10">
-        <v>165.98</v>
+        <v>166.01</v>
       </c>
       <c r="F40" s="10">
-        <v>175.98</v>
+        <v>176.01</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>173.35</v>
+        <v>173.48</v>
       </c>
       <c r="E41" s="13">
-        <v>166.4</v>
+        <v>166.43</v>
       </c>
       <c r="F41" s="13">
-        <v>176.4</v>
+        <v>176.43</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>172.72</v>
+        <v>173.64</v>
       </c>
       <c r="E42" s="10">
-        <v>165.48</v>
+        <v>165.98</v>
       </c>
       <c r="F42" s="10">
-        <v>175.48</v>
+        <v>175.98</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>172.43</v>
+        <v>173.35</v>
       </c>
       <c r="E43" s="13">
-        <v>165.9</v>
+        <v>166.4</v>
       </c>
       <c r="F43" s="13">
-        <v>175.9</v>
+        <v>176.4</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>166.31</v>
+        <v>167.91</v>
       </c>
       <c r="E47" s="10">
-        <v>161.08000000000001</v>
+        <v>161.74</v>
       </c>
       <c r="F47" s="10">
-        <v>171.08</v>
+        <v>171.74</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>166.31</v>
+        <v>167.92</v>
       </c>
       <c r="E48" s="13">
-        <v>161.26</v>
+        <v>161.91999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>171.26</v>
+        <v>171.92</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>165.14</v>
+        <v>166.31</v>
       </c>
       <c r="E49" s="10">
-        <v>160.96</v>
+        <v>161.08000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>170.96</v>
+        <v>171.08</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>165.14</v>
+        <v>166.31</v>
       </c>
       <c r="E50" s="13">
-        <v>161.13999999999999</v>
+        <v>161.26</v>
       </c>
       <c r="F50" s="13">
-        <v>171.14</v>
+        <v>171.26</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,33 +1607,33 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>183.88</v>
+        <v>184</v>
       </c>
       <c r="E54" s="10">
-        <v>176.17</v>
+        <v>176.13</v>
       </c>
       <c r="F54" s="10">
-        <v>186.17</v>
+        <v>186.13</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>171.53</v>
+        <v>171.66</v>
       </c>
       <c r="E55" s="13">
         <v>173.86</v>
@@ -1645,14 +1645,14 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>173.91</v>
+        <v>174.04</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,14 +1664,14 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>173.65</v>
+        <v>173.8</v>
       </c>
       <c r="E57" s="13">
         <v>168.13</v>
@@ -1683,14 +1683,14 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>169.56</v>
+        <v>169.71</v>
       </c>
       <c r="E58" s="10">
         <v>164.18</v>
@@ -1702,17 +1702,17 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>176.29</v>
+        <v>176.44</v>
       </c>
       <c r="E59" s="13">
-        <v>174.46</v>
+        <v>174.43</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>182.95</v>
+        <v>183.88</v>
       </c>
       <c r="E60" s="10">
-        <v>175.77</v>
+        <v>176.17</v>
       </c>
       <c r="F60" s="10">
-        <v>185.77</v>
+        <v>186.17</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>170.6</v>
+        <v>171.53</v>
       </c>
       <c r="E61" s="13">
-        <v>173.26</v>
+        <v>173.86</v>
       </c>
       <c r="F61" s="13">
-        <v>183.26</v>
+        <v>183.86</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>172.86</v>
+        <v>173.91</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>172.58</v>
+        <v>173.65</v>
       </c>
       <c r="E63" s="13">
-        <v>167.53</v>
+        <v>168.13</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>168.49</v>
+        <v>169.56</v>
       </c>
       <c r="E64" s="10">
-        <v>163.58000000000001</v>
+        <v>164.18</v>
       </c>
       <c r="F64" s="10">
-        <v>173.58</v>
+        <v>174.18</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>175.32</v>
+        <v>176.29</v>
       </c>
       <c r="E65" s="13">
-        <v>174.04</v>
+        <v>174.46</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1863,15 +1872,6 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,6 +2135,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2148,14 +2156,6 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Mon Nov  3 02:55:48 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{86F8D0A0-A1BC-4F43-8591-ED7427850EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{6FA3AF58-7F19-4BC7-A086-F57B0C031C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>167.82</v>
+        <v>168.08</v>
       </c>
       <c r="E8" s="10">
-        <v>161.06</v>
+        <v>160.96</v>
       </c>
       <c r="F8" s="10">
-        <v>171.06</v>
+        <v>170.96</v>
       </c>
       <c r="G8" s="10">
-        <v>161.22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>167.82</v>
+        <v>168.08</v>
       </c>
       <c r="E9" s="13">
-        <v>161.06</v>
+        <v>160.96</v>
       </c>
       <c r="F9" s="13">
-        <v>171.06</v>
+        <v>170.96</v>
       </c>
       <c r="G9" s="13">
-        <v>161.22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>169.92</v>
+        <v>170.01</v>
       </c>
       <c r="E10" s="10">
-        <v>163.41</v>
+        <v>163.04</v>
       </c>
       <c r="F10" s="10">
-        <v>173.41</v>
+        <v>173.04</v>
       </c>
       <c r="G10" s="10">
-        <v>163.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>167.32</v>
+        <v>167.82</v>
       </c>
       <c r="E11" s="13">
-        <v>160.94</v>
+        <v>161.06</v>
       </c>
       <c r="F11" s="13">
-        <v>170.94</v>
+        <v>171.06</v>
       </c>
       <c r="G11" s="13">
-        <v>161.09</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>167.32</v>
+        <v>167.82</v>
       </c>
       <c r="E12" s="10">
-        <v>160.94</v>
+        <v>161.06</v>
       </c>
       <c r="F12" s="10">
-        <v>170.94</v>
+        <v>171.06</v>
       </c>
       <c r="G12" s="10">
-        <v>161.09</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>169.79</v>
+        <v>169.92</v>
       </c>
       <c r="E13" s="13">
-        <v>163.41999999999999</v>
+        <v>163.41</v>
       </c>
       <c r="F13" s="13">
-        <v>173.42</v>
+        <v>173.41</v>
       </c>
       <c r="G13" s="13">
-        <v>163.89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>173.43</v>
+        <v>173.52</v>
       </c>
       <c r="E17" s="10">
-        <v>166.39</v>
+        <v>166.04</v>
       </c>
       <c r="F17" s="10">
-        <v>176.39</v>
+        <v>176.04</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>173.29</v>
+        <v>173.43</v>
       </c>
       <c r="E18" s="13">
-        <v>166.35</v>
+        <v>166.39</v>
       </c>
       <c r="F18" s="13">
-        <v>176.35</v>
+        <v>176.39</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>169.06</v>
+        <v>169.21</v>
       </c>
       <c r="E22" s="10">
-        <v>162.43</v>
+        <v>162.07</v>
       </c>
       <c r="F22" s="10">
-        <v>172.03</v>
+        <v>171.66</v>
       </c>
       <c r="G22" s="10">
-        <v>163.72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>174.69</v>
+        <v>174.78</v>
       </c>
       <c r="E23" s="13">
-        <v>167.14</v>
+        <v>166.77</v>
       </c>
       <c r="F23" s="13">
-        <v>177.14</v>
+        <v>176.77</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>174.51</v>
+        <v>174.6</v>
       </c>
       <c r="E24" s="10">
-        <v>167.31</v>
+        <v>166.93</v>
       </c>
       <c r="F24" s="10">
-        <v>177.31</v>
+        <v>176.93</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>175.34</v>
+        <v>175.42</v>
       </c>
       <c r="E25" s="13">
-        <v>166.7</v>
+        <v>166.32</v>
       </c>
       <c r="F25" s="13">
-        <v>176.7</v>
+        <v>176.32</v>
       </c>
       <c r="G25" s="13">
-        <v>166.74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166.36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>174.08</v>
+        <v>174.16</v>
       </c>
       <c r="E26" s="10">
-        <v>168.26</v>
+        <v>167.88</v>
       </c>
       <c r="F26" s="10">
-        <v>178.26</v>
+        <v>177.88</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>169</v>
+        <v>169.06</v>
       </c>
       <c r="E27" s="13">
-        <v>162.44</v>
+        <v>162.43</v>
       </c>
       <c r="F27" s="13">
-        <v>172.04</v>
+        <v>172.03</v>
       </c>
       <c r="G27" s="13">
-        <v>163.62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>174.56</v>
+        <v>174.69</v>
       </c>
       <c r="E28" s="22">
-        <v>167.15</v>
+        <v>167.14</v>
       </c>
       <c r="F28" s="22">
-        <v>177.15</v>
+        <v>177.14</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>174.37</v>
+        <v>174.51</v>
       </c>
       <c r="E29" s="13">
-        <v>167.32</v>
+        <v>167.31</v>
       </c>
       <c r="F29" s="13">
-        <v>177.32</v>
+        <v>177.31</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>175.2</v>
+        <v>175.34</v>
       </c>
       <c r="E30" s="22">
-        <v>166.71</v>
+        <v>166.7</v>
       </c>
       <c r="F30" s="22">
-        <v>176.71</v>
+        <v>176.7</v>
       </c>
       <c r="G30" s="22">
-        <v>166.54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166.74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>173.94</v>
+        <v>174.08</v>
       </c>
       <c r="E31" s="13">
-        <v>168.28</v>
+        <v>168.26</v>
       </c>
       <c r="F31" s="13">
-        <v>178.28</v>
+        <v>178.26</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,35 +1298,35 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>168.29</v>
+        <v>168.49</v>
       </c>
       <c r="E35" s="10">
-        <v>160.63</v>
+        <v>160.25</v>
       </c>
       <c r="F35" s="10">
-        <v>169.63</v>
+        <v>169.25</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>168.04</v>
+        <v>168.29</v>
       </c>
       <c r="E36" s="13">
         <v>160.63</v>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>173.77</v>
+        <v>173.86</v>
       </c>
       <c r="E40" s="10">
-        <v>166.01</v>
+        <v>165.66</v>
       </c>
       <c r="F40" s="10">
-        <v>176.01</v>
+        <v>175.66</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>173.48</v>
+        <v>173.56</v>
       </c>
       <c r="E41" s="13">
-        <v>166.43</v>
+        <v>166.08</v>
       </c>
       <c r="F41" s="13">
-        <v>176.43</v>
+        <v>176.08</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>173.64</v>
+        <v>173.77</v>
       </c>
       <c r="E42" s="10">
-        <v>165.98</v>
+        <v>166.01</v>
       </c>
       <c r="F42" s="10">
-        <v>175.98</v>
+        <v>176.01</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>173.35</v>
+        <v>173.48</v>
       </c>
       <c r="E43" s="13">
-        <v>166.4</v>
+        <v>166.43</v>
       </c>
       <c r="F43" s="13">
-        <v>176.4</v>
+        <v>176.43</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>167.91</v>
+        <v>168.99</v>
       </c>
       <c r="E47" s="10">
-        <v>161.74</v>
+        <v>162.21</v>
       </c>
       <c r="F47" s="10">
-        <v>171.74</v>
+        <v>172.21</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>167.92</v>
+        <v>169</v>
       </c>
       <c r="E48" s="13">
-        <v>161.91999999999999</v>
+        <v>162.4</v>
       </c>
       <c r="F48" s="13">
-        <v>171.92</v>
+        <v>172.4</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>166.31</v>
+        <v>167.91</v>
       </c>
       <c r="E49" s="10">
-        <v>161.08000000000001</v>
+        <v>161.74</v>
       </c>
       <c r="F49" s="10">
-        <v>171.08</v>
+        <v>171.74</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>166.31</v>
+        <v>167.92</v>
       </c>
       <c r="E50" s="13">
-        <v>161.26</v>
+        <v>161.91999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>171.26</v>
+        <v>171.92</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>184</v>
+        <v>184.08</v>
       </c>
       <c r="E54" s="10">
-        <v>176.13</v>
+        <v>175.74</v>
       </c>
       <c r="F54" s="10">
-        <v>186.13</v>
+        <v>185.74</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>171.66</v>
+        <v>171.75</v>
       </c>
       <c r="E55" s="13">
-        <v>173.86</v>
+        <v>173.6</v>
       </c>
       <c r="F55" s="13">
-        <v>183.86</v>
+        <v>183.6</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>174.04</v>
+        <v>174.23</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,92 +1662,92 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>173.8</v>
+        <v>174</v>
       </c>
       <c r="E57" s="13">
-        <v>168.13</v>
+        <v>167.87</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>169.71</v>
+        <v>169.91</v>
       </c>
       <c r="E58" s="10">
-        <v>164.18</v>
+        <v>163.92</v>
       </c>
       <c r="F58" s="10">
-        <v>174.18</v>
+        <v>173.92</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>176.44</v>
+        <v>176.53</v>
       </c>
       <c r="E59" s="13">
-        <v>174.43</v>
+        <v>174.04</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>183.88</v>
+        <v>184</v>
       </c>
       <c r="E60" s="10">
-        <v>176.17</v>
+        <v>176.13</v>
       </c>
       <c r="F60" s="10">
-        <v>186.17</v>
+        <v>186.13</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>171.53</v>
+        <v>171.66</v>
       </c>
       <c r="E61" s="13">
         <v>173.86</v>
@@ -1757,16 +1757,16 @@
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>173.91</v>
+        <v>174.04</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,16 +1776,16 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>173.65</v>
+        <v>173.8</v>
       </c>
       <c r="E63" s="13">
         <v>168.13</v>
@@ -1795,16 +1795,16 @@
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>169.56</v>
+        <v>169.71</v>
       </c>
       <c r="E64" s="10">
         <v>164.18</v>
@@ -1814,19 +1814,19 @@
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>45961</v>
+        <v>45962</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>176.29</v>
+        <v>176.44</v>
       </c>
       <c r="E65" s="13">
-        <v>174.46</v>
+        <v>174.43</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,26 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,10 +2114,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2161,21 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Nov  4 02:49:38 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{6FA3AF58-7F19-4BC7-A086-F57B0C031C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{3DF8B5D8-9F34-4205-822D-9E85F0CD3A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>168.08</v>
+        <v>168.21</v>
       </c>
       <c r="E8" s="10">
-        <v>160.96</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="F8" s="10">
-        <v>170.96</v>
+        <v>170.83</v>
       </c>
       <c r="G8" s="10">
-        <v>161.13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>168.08</v>
+        <v>168.21</v>
       </c>
       <c r="E9" s="13">
-        <v>160.96</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="F9" s="13">
-        <v>170.96</v>
+        <v>170.83</v>
       </c>
       <c r="G9" s="13">
-        <v>161.13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>170.01</v>
+        <v>170.13</v>
       </c>
       <c r="E10" s="10">
-        <v>163.04</v>
+        <v>163.01</v>
       </c>
       <c r="F10" s="10">
-        <v>173.04</v>
+        <v>173.01</v>
       </c>
       <c r="G10" s="10">
-        <v>163.53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>167.82</v>
+        <v>168.08</v>
       </c>
       <c r="E11" s="13">
-        <v>161.06</v>
+        <v>160.96</v>
       </c>
       <c r="F11" s="13">
-        <v>171.06</v>
+        <v>170.96</v>
       </c>
       <c r="G11" s="13">
-        <v>161.22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>167.82</v>
+        <v>168.08</v>
       </c>
       <c r="E12" s="10">
-        <v>161.06</v>
+        <v>160.96</v>
       </c>
       <c r="F12" s="10">
-        <v>171.06</v>
+        <v>170.96</v>
       </c>
       <c r="G12" s="10">
-        <v>161.22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>169.92</v>
+        <v>170.01</v>
       </c>
       <c r="E13" s="13">
-        <v>163.41</v>
+        <v>163.04</v>
       </c>
       <c r="F13" s="13">
-        <v>173.41</v>
+        <v>173.04</v>
       </c>
       <c r="G13" s="13">
-        <v>163.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>173.52</v>
+        <v>173.64</v>
       </c>
       <c r="E17" s="10">
-        <v>166.04</v>
+        <v>165.97</v>
       </c>
       <c r="F17" s="10">
-        <v>176.04</v>
+        <v>175.97</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>173.43</v>
+        <v>173.52</v>
       </c>
       <c r="E18" s="13">
-        <v>166.39</v>
+        <v>166.04</v>
       </c>
       <c r="F18" s="13">
-        <v>176.39</v>
+        <v>176.04</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>169.21</v>
+        <v>169.34</v>
       </c>
       <c r="E22" s="10">
-        <v>162.07</v>
+        <v>162.04</v>
       </c>
       <c r="F22" s="10">
-        <v>171.66</v>
+        <v>171.64</v>
       </c>
       <c r="G22" s="10">
-        <v>163.35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.33000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>174.78</v>
+        <v>174.9</v>
       </c>
       <c r="E23" s="13">
-        <v>166.77</v>
+        <v>166.74</v>
       </c>
       <c r="F23" s="13">
-        <v>176.77</v>
+        <v>176.74</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>174.6</v>
+        <v>174.72</v>
       </c>
       <c r="E24" s="10">
-        <v>166.93</v>
+        <v>166.91</v>
       </c>
       <c r="F24" s="10">
-        <v>176.93</v>
+        <v>176.91</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>175.42</v>
+        <v>175.55</v>
       </c>
       <c r="E25" s="13">
-        <v>166.32</v>
+        <v>166.3</v>
       </c>
       <c r="F25" s="13">
-        <v>176.32</v>
+        <v>176.3</v>
       </c>
       <c r="G25" s="13">
-        <v>166.36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>166.34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>174.16</v>
+        <v>174.29</v>
       </c>
       <c r="E26" s="10">
-        <v>167.88</v>
+        <v>167.86</v>
       </c>
       <c r="F26" s="10">
-        <v>177.88</v>
+        <v>177.86</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>169.06</v>
+        <v>169.21</v>
       </c>
       <c r="E27" s="13">
-        <v>162.43</v>
+        <v>162.07</v>
       </c>
       <c r="F27" s="13">
-        <v>172.03</v>
+        <v>171.66</v>
       </c>
       <c r="G27" s="13">
-        <v>163.72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>174.69</v>
+        <v>174.78</v>
       </c>
       <c r="E28" s="22">
-        <v>167.14</v>
+        <v>166.77</v>
       </c>
       <c r="F28" s="22">
-        <v>177.14</v>
+        <v>176.77</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>174.51</v>
+        <v>174.6</v>
       </c>
       <c r="E29" s="13">
-        <v>167.31</v>
+        <v>166.93</v>
       </c>
       <c r="F29" s="13">
-        <v>177.31</v>
+        <v>176.93</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>175.34</v>
+        <v>175.42</v>
       </c>
       <c r="E30" s="22">
-        <v>166.7</v>
+        <v>166.32</v>
       </c>
       <c r="F30" s="22">
-        <v>176.7</v>
+        <v>176.32</v>
       </c>
       <c r="G30" s="22">
-        <v>166.74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>166.36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>174.08</v>
+        <v>174.16</v>
       </c>
       <c r="E31" s="13">
-        <v>168.26</v>
+        <v>167.88</v>
       </c>
       <c r="F31" s="13">
-        <v>178.26</v>
+        <v>177.88</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>168.49</v>
+        <v>168.61</v>
       </c>
       <c r="E35" s="10">
-        <v>160.25</v>
+        <v>160.22999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>169.25</v>
+        <v>169.23</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>168.29</v>
+        <v>168.49</v>
       </c>
       <c r="E36" s="13">
-        <v>160.63</v>
+        <v>160.25</v>
       </c>
       <c r="F36" s="13">
-        <v>169.63</v>
+        <v>169.25</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>173.86</v>
+        <v>173.98</v>
       </c>
       <c r="E40" s="10">
-        <v>165.66</v>
+        <v>165.59</v>
       </c>
       <c r="F40" s="10">
-        <v>175.66</v>
+        <v>175.59</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>173.56</v>
+        <v>173.69</v>
       </c>
       <c r="E41" s="13">
-        <v>166.08</v>
+        <v>166.01</v>
       </c>
       <c r="F41" s="13">
-        <v>176.08</v>
+        <v>176.01</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>173.77</v>
+        <v>173.86</v>
       </c>
       <c r="E42" s="10">
-        <v>166.01</v>
+        <v>165.66</v>
       </c>
       <c r="F42" s="10">
-        <v>176.01</v>
+        <v>175.66</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>173.48</v>
+        <v>173.56</v>
       </c>
       <c r="E43" s="13">
-        <v>166.43</v>
+        <v>166.08</v>
       </c>
       <c r="F43" s="13">
-        <v>176.43</v>
+        <v>176.08</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>168.99</v>
+        <v>168.62</v>
       </c>
       <c r="E47" s="10">
-        <v>162.21</v>
+        <v>161.96</v>
       </c>
       <c r="F47" s="10">
-        <v>172.21</v>
+        <v>171.96</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>169</v>
+        <v>168.63</v>
       </c>
       <c r="E48" s="13">
-        <v>162.4</v>
+        <v>162.15</v>
       </c>
       <c r="F48" s="13">
-        <v>172.4</v>
+        <v>172.15</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>167.91</v>
+        <v>168.99</v>
       </c>
       <c r="E49" s="10">
-        <v>161.74</v>
+        <v>162.21</v>
       </c>
       <c r="F49" s="10">
-        <v>171.74</v>
+        <v>172.21</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>167.92</v>
+        <v>169</v>
       </c>
       <c r="E50" s="13">
-        <v>161.91999999999999</v>
+        <v>162.4</v>
       </c>
       <c r="F50" s="13">
-        <v>171.92</v>
+        <v>172.4</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,16 +1605,16 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>184.08</v>
+        <v>184.2</v>
       </c>
       <c r="E54" s="10">
         <v>175.74</v>
@@ -1624,35 +1624,35 @@
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>171.75</v>
+        <v>171.87</v>
       </c>
       <c r="E55" s="13">
-        <v>173.6</v>
+        <v>173.58</v>
       </c>
       <c r="F55" s="13">
-        <v>183.6</v>
+        <v>183.58</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>174.23</v>
+        <v>174.36</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>174</v>
+        <v>174.12</v>
       </c>
       <c r="E57" s="13">
-        <v>167.87</v>
+        <v>167.84</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>169.91</v>
+        <v>170.03</v>
       </c>
       <c r="E58" s="10">
-        <v>163.92</v>
+        <v>163.9</v>
       </c>
       <c r="F58" s="10">
-        <v>173.92</v>
+        <v>173.9</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>176.53</v>
+        <v>176.65</v>
       </c>
       <c r="E59" s="13">
-        <v>174.04</v>
+        <v>174.03</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>184</v>
+        <v>184.08</v>
       </c>
       <c r="E60" s="10">
-        <v>176.13</v>
+        <v>175.74</v>
       </c>
       <c r="F60" s="10">
-        <v>186.13</v>
+        <v>185.74</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>171.66</v>
+        <v>171.75</v>
       </c>
       <c r="E61" s="13">
-        <v>173.86</v>
+        <v>173.6</v>
       </c>
       <c r="F61" s="13">
-        <v>183.86</v>
+        <v>183.6</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>174.04</v>
+        <v>174.23</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>173.8</v>
+        <v>174</v>
       </c>
       <c r="E63" s="13">
-        <v>168.13</v>
+        <v>167.87</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>169.71</v>
+        <v>169.91</v>
       </c>
       <c r="E64" s="10">
-        <v>164.18</v>
+        <v>163.92</v>
       </c>
       <c r="F64" s="10">
-        <v>174.18</v>
+        <v>173.92</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45962</v>
+        <v>45965</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>176.44</v>
+        <v>176.53</v>
       </c>
       <c r="E65" s="13">
-        <v>174.43</v>
+        <v>174.04</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,17 +2125,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,6 +2135,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2154,24 +2172,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Wed Nov  5 02:50:34 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{3DF8B5D8-9F34-4205-822D-9E85F0CD3A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8E39DC7C-3465-4FEF-AE67-9616E741D446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>168.21</v>
+        <v>168.28</v>
       </c>
       <c r="E8" s="10">
-        <v>160.83000000000001</v>
+        <v>160.72999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>170.83</v>
+        <v>170.73</v>
       </c>
       <c r="G8" s="10">
-        <v>161</v>
+        <v>160.9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>168.21</v>
+        <v>168.28</v>
       </c>
       <c r="E9" s="13">
-        <v>160.83000000000001</v>
+        <v>160.72999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>170.83</v>
+        <v>170.73</v>
       </c>
       <c r="G9" s="13">
-        <v>161</v>
+        <v>160.9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>170.13</v>
+        <v>170.11</v>
       </c>
       <c r="E10" s="10">
-        <v>163.01</v>
+        <v>162.91999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>173.01</v>
+        <v>172.92</v>
       </c>
       <c r="G10" s="10">
-        <v>163.51</v>
+        <v>163.41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>168.08</v>
+        <v>168.21</v>
       </c>
       <c r="E11" s="13">
-        <v>160.96</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="F11" s="13">
-        <v>170.96</v>
+        <v>170.83</v>
       </c>
       <c r="G11" s="13">
-        <v>161.13</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>168.08</v>
+        <v>168.21</v>
       </c>
       <c r="E12" s="10">
-        <v>160.96</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="F12" s="10">
-        <v>170.96</v>
+        <v>170.83</v>
       </c>
       <c r="G12" s="10">
-        <v>161.13</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>170.01</v>
+        <v>170.13</v>
       </c>
       <c r="E13" s="13">
-        <v>163.04</v>
+        <v>163.01</v>
       </c>
       <c r="F13" s="13">
-        <v>173.04</v>
+        <v>173.01</v>
       </c>
       <c r="G13" s="13">
-        <v>163.53</v>
+        <v>163.51</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>173.64</v>
+        <v>173.61</v>
       </c>
       <c r="E17" s="10">
-        <v>165.97</v>
+        <v>165.89</v>
       </c>
       <c r="F17" s="10">
-        <v>175.97</v>
+        <v>175.89</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>173.52</v>
+        <v>173.64</v>
       </c>
       <c r="E18" s="13">
-        <v>166.04</v>
+        <v>165.97</v>
       </c>
       <c r="F18" s="13">
-        <v>176.04</v>
+        <v>175.97</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>169.34</v>
+        <v>169.31</v>
       </c>
       <c r="E22" s="10">
-        <v>162.04</v>
+        <v>161.94999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>171.64</v>
+        <v>171.55</v>
       </c>
       <c r="G22" s="10">
-        <v>163.33000000000001</v>
+        <v>163.22999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>174.9</v>
+        <v>174.88</v>
       </c>
       <c r="E23" s="13">
-        <v>166.74</v>
+        <v>166.65</v>
       </c>
       <c r="F23" s="13">
-        <v>176.74</v>
+        <v>176.65</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>174.72</v>
+        <v>174.69</v>
       </c>
       <c r="E24" s="10">
-        <v>166.91</v>
+        <v>166.82</v>
       </c>
       <c r="F24" s="10">
-        <v>176.91</v>
+        <v>176.82</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>175.55</v>
+        <v>175.52</v>
       </c>
       <c r="E25" s="13">
-        <v>166.3</v>
+        <v>166.21</v>
       </c>
       <c r="F25" s="13">
-        <v>176.3</v>
+        <v>176.21</v>
       </c>
       <c r="G25" s="13">
-        <v>166.34</v>
+        <v>166.25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>174.29</v>
+        <v>174.26</v>
       </c>
       <c r="E26" s="10">
-        <v>167.86</v>
+        <v>167.77</v>
       </c>
       <c r="F26" s="10">
-        <v>177.86</v>
+        <v>177.77</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>169.21</v>
+        <v>169.34</v>
       </c>
       <c r="E27" s="13">
-        <v>162.07</v>
+        <v>162.04</v>
       </c>
       <c r="F27" s="13">
-        <v>171.66</v>
+        <v>171.64</v>
       </c>
       <c r="G27" s="13">
-        <v>163.35</v>
+        <v>163.33000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>174.78</v>
+        <v>174.9</v>
       </c>
       <c r="E28" s="22">
-        <v>166.77</v>
+        <v>166.74</v>
       </c>
       <c r="F28" s="22">
-        <v>176.77</v>
+        <v>176.74</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>174.6</v>
+        <v>174.72</v>
       </c>
       <c r="E29" s="13">
-        <v>166.93</v>
+        <v>166.91</v>
       </c>
       <c r="F29" s="13">
-        <v>176.93</v>
+        <v>176.91</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>175.42</v>
+        <v>175.55</v>
       </c>
       <c r="E30" s="22">
-        <v>166.32</v>
+        <v>166.3</v>
       </c>
       <c r="F30" s="22">
-        <v>176.32</v>
+        <v>176.3</v>
       </c>
       <c r="G30" s="22">
-        <v>166.36</v>
+        <v>166.34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>174.16</v>
+        <v>174.29</v>
       </c>
       <c r="E31" s="13">
-        <v>167.88</v>
+        <v>167.86</v>
       </c>
       <c r="F31" s="13">
-        <v>177.88</v>
+        <v>177.86</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>168.61</v>
+        <v>168.69</v>
       </c>
       <c r="E35" s="10">
-        <v>160.22999999999999</v>
+        <v>160.13999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>169.23</v>
+        <v>169.14</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>168.49</v>
+        <v>168.61</v>
       </c>
       <c r="E36" s="13">
-        <v>160.25</v>
+        <v>160.22999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>169.25</v>
+        <v>169.23</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>173.98</v>
+        <v>173.96</v>
       </c>
       <c r="E40" s="10">
-        <v>165.59</v>
+        <v>165.52</v>
       </c>
       <c r="F40" s="10">
-        <v>175.59</v>
+        <v>175.52</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>173.69</v>
+        <v>173.67</v>
       </c>
       <c r="E41" s="13">
-        <v>166.01</v>
+        <v>165.94</v>
       </c>
       <c r="F41" s="13">
-        <v>176.01</v>
+        <v>175.95</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>173.86</v>
+        <v>173.98</v>
       </c>
       <c r="E42" s="10">
-        <v>165.66</v>
+        <v>165.59</v>
       </c>
       <c r="F42" s="10">
-        <v>175.66</v>
+        <v>175.59</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>173.56</v>
+        <v>173.69</v>
       </c>
       <c r="E43" s="13">
-        <v>166.08</v>
+        <v>166.01</v>
       </c>
       <c r="F43" s="13">
-        <v>176.08</v>
+        <v>176.01</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>168.62</v>
+        <v>168.34</v>
       </c>
       <c r="E47" s="10">
-        <v>161.96</v>
+        <v>161.63999999999999</v>
       </c>
       <c r="F47" s="10">
-        <v>171.96</v>
+        <v>171.64</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>168.63</v>
+        <v>168.36</v>
       </c>
       <c r="E48" s="13">
-        <v>162.15</v>
+        <v>161.83000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>172.15</v>
+        <v>171.83</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>168.99</v>
+        <v>168.62</v>
       </c>
       <c r="E49" s="10">
-        <v>162.21</v>
+        <v>161.96</v>
       </c>
       <c r="F49" s="10">
-        <v>172.21</v>
+        <v>171.96</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>169</v>
+        <v>168.63</v>
       </c>
       <c r="E50" s="13">
-        <v>162.4</v>
+        <v>162.15</v>
       </c>
       <c r="F50" s="13">
-        <v>172.4</v>
+        <v>172.15</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>184.2</v>
+        <v>184.18</v>
       </c>
       <c r="E54" s="10">
-        <v>175.74</v>
+        <v>175.67</v>
       </c>
       <c r="F54" s="10">
-        <v>185.74</v>
+        <v>185.67</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>171.87</v>
+        <v>171.85</v>
       </c>
       <c r="E55" s="13">
-        <v>173.58</v>
+        <v>173.59</v>
       </c>
       <c r="F55" s="13">
-        <v>183.58</v>
+        <v>183.59</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>174.36</v>
+        <v>174.33</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>174.12</v>
+        <v>174.09</v>
       </c>
       <c r="E57" s="13">
-        <v>167.84</v>
+        <v>167.85</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>170.03</v>
+        <v>170</v>
       </c>
       <c r="E58" s="10">
-        <v>163.9</v>
+        <v>163.91</v>
       </c>
       <c r="F58" s="10">
-        <v>173.9</v>
+        <v>173.91</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>176.65</v>
+        <v>176.61</v>
       </c>
       <c r="E59" s="13">
-        <v>174.03</v>
+        <v>173.95</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,14 +1721,14 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>184.08</v>
+        <v>184.2</v>
       </c>
       <c r="E60" s="10">
         <v>175.74</v>
@@ -1740,33 +1740,33 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>171.75</v>
+        <v>171.87</v>
       </c>
       <c r="E61" s="13">
-        <v>173.6</v>
+        <v>173.58</v>
       </c>
       <c r="F61" s="13">
-        <v>183.6</v>
+        <v>183.58</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>174.23</v>
+        <v>174.36</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>174</v>
+        <v>174.12</v>
       </c>
       <c r="E63" s="13">
-        <v>167.87</v>
+        <v>167.84</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>169.91</v>
+        <v>170.03</v>
       </c>
       <c r="E64" s="10">
-        <v>163.92</v>
+        <v>163.9</v>
       </c>
       <c r="F64" s="10">
-        <v>173.92</v>
+        <v>173.9</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>176.53</v>
+        <v>176.65</v>
       </c>
       <c r="E65" s="13">
-        <v>174.04</v>
+        <v>174.03</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,17 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2125,6 +2114,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,24 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2172,6 +2154,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Thu Nov  6 02:52:28 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8E39DC7C-3465-4FEF-AE67-9616E741D446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{01627818-19E9-41EB-8E15-A15F335F634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>168.28</v>
+        <v>168.74</v>
       </c>
       <c r="E8" s="10">
-        <v>160.72999999999999</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>170.73</v>
+        <v>170.7</v>
       </c>
       <c r="G8" s="10">
-        <v>160.9</v>
+        <v>160.86000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>168.28</v>
+        <v>168.74</v>
       </c>
       <c r="E9" s="13">
-        <v>160.72999999999999</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>170.73</v>
+        <v>170.7</v>
       </c>
       <c r="G9" s="13">
-        <v>160.9</v>
+        <v>160.86000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>170.11</v>
+        <v>170.96</v>
       </c>
       <c r="E10" s="10">
-        <v>162.91999999999999</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>172.92</v>
+        <v>172.95</v>
       </c>
       <c r="G10" s="10">
-        <v>163.41</v>
+        <v>163.44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>168.21</v>
+        <v>168.28</v>
       </c>
       <c r="E11" s="13">
-        <v>160.83000000000001</v>
+        <v>160.72999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>170.83</v>
+        <v>170.73</v>
       </c>
       <c r="G11" s="13">
-        <v>161</v>
+        <v>160.9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>168.21</v>
+        <v>168.28</v>
       </c>
       <c r="E12" s="10">
-        <v>160.83000000000001</v>
+        <v>160.72999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>170.83</v>
+        <v>170.73</v>
       </c>
       <c r="G12" s="10">
-        <v>161</v>
+        <v>160.9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>170.13</v>
+        <v>170.11</v>
       </c>
       <c r="E13" s="13">
-        <v>163.01</v>
+        <v>162.91999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>173.01</v>
+        <v>172.92</v>
       </c>
       <c r="G13" s="13">
-        <v>163.51</v>
+        <v>163.41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>173.61</v>
+        <v>174.44</v>
       </c>
       <c r="E17" s="10">
-        <v>165.89</v>
+        <v>165.92</v>
       </c>
       <c r="F17" s="10">
-        <v>175.89</v>
+        <v>175.92</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>173.64</v>
+        <v>173.61</v>
       </c>
       <c r="E18" s="13">
-        <v>165.97</v>
+        <v>165.89</v>
       </c>
       <c r="F18" s="13">
-        <v>175.97</v>
+        <v>175.89</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>169.31</v>
+        <v>170.09</v>
       </c>
       <c r="E22" s="10">
-        <v>161.94999999999999</v>
+        <v>161.96</v>
       </c>
       <c r="F22" s="10">
-        <v>171.55</v>
+        <v>171.56</v>
       </c>
       <c r="G22" s="10">
-        <v>163.22999999999999</v>
+        <v>163.25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>174.88</v>
+        <v>175.73</v>
       </c>
       <c r="E23" s="13">
-        <v>166.65</v>
+        <v>166.67</v>
       </c>
       <c r="F23" s="13">
-        <v>176.65</v>
+        <v>176.67</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>174.69</v>
+        <v>175.54</v>
       </c>
       <c r="E24" s="10">
-        <v>166.82</v>
+        <v>166.85</v>
       </c>
       <c r="F24" s="10">
-        <v>176.82</v>
+        <v>176.85</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>175.52</v>
+        <v>176.37</v>
       </c>
       <c r="E25" s="13">
-        <v>166.21</v>
+        <v>166.25</v>
       </c>
       <c r="F25" s="13">
-        <v>176.21</v>
+        <v>176.25</v>
       </c>
       <c r="G25" s="13">
-        <v>166.25</v>
+        <v>166.29</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>174.26</v>
+        <v>175.1</v>
       </c>
       <c r="E26" s="10">
-        <v>167.77</v>
+        <v>167.81</v>
       </c>
       <c r="F26" s="10">
-        <v>177.77</v>
+        <v>177.81</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>169.34</v>
+        <v>169.31</v>
       </c>
       <c r="E27" s="13">
-        <v>162.04</v>
+        <v>161.94999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>171.64</v>
+        <v>171.55</v>
       </c>
       <c r="G27" s="13">
-        <v>163.33000000000001</v>
+        <v>163.22999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>174.9</v>
+        <v>174.88</v>
       </c>
       <c r="E28" s="22">
-        <v>166.74</v>
+        <v>166.65</v>
       </c>
       <c r="F28" s="22">
-        <v>176.74</v>
+        <v>176.65</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>174.72</v>
+        <v>174.69</v>
       </c>
       <c r="E29" s="13">
-        <v>166.91</v>
+        <v>166.82</v>
       </c>
       <c r="F29" s="13">
-        <v>176.91</v>
+        <v>176.82</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>175.55</v>
+        <v>175.52</v>
       </c>
       <c r="E30" s="22">
-        <v>166.3</v>
+        <v>166.21</v>
       </c>
       <c r="F30" s="22">
-        <v>176.3</v>
+        <v>176.21</v>
       </c>
       <c r="G30" s="22">
-        <v>166.34</v>
+        <v>166.25</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>174.29</v>
+        <v>174.26</v>
       </c>
       <c r="E31" s="13">
-        <v>167.86</v>
+        <v>167.77</v>
       </c>
       <c r="F31" s="13">
-        <v>177.86</v>
+        <v>177.77</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>168.69</v>
+        <v>169.43</v>
       </c>
       <c r="E35" s="10">
-        <v>160.13999999999999</v>
+        <v>160.16</v>
       </c>
       <c r="F35" s="10">
-        <v>169.14</v>
+        <v>169.16</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>168.61</v>
+        <v>168.69</v>
       </c>
       <c r="E36" s="13">
-        <v>160.22999999999999</v>
+        <v>160.13999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>169.23</v>
+        <v>169.14</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>173.96</v>
+        <v>174.83</v>
       </c>
       <c r="E40" s="10">
-        <v>165.52</v>
+        <v>165.58</v>
       </c>
       <c r="F40" s="10">
-        <v>175.52</v>
+        <v>175.58</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>173.67</v>
+        <v>174.53</v>
       </c>
       <c r="E41" s="13">
-        <v>165.94</v>
+        <v>166</v>
       </c>
       <c r="F41" s="13">
-        <v>175.95</v>
+        <v>176</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>173.98</v>
+        <v>173.96</v>
       </c>
       <c r="E42" s="10">
-        <v>165.59</v>
+        <v>165.52</v>
       </c>
       <c r="F42" s="10">
-        <v>175.59</v>
+        <v>175.52</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>173.69</v>
+        <v>173.67</v>
       </c>
       <c r="E43" s="13">
-        <v>166.01</v>
+        <v>165.94</v>
       </c>
       <c r="F43" s="13">
-        <v>176.01</v>
+        <v>175.95</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>168.34</v>
+        <v>168.28</v>
       </c>
       <c r="E47" s="10">
-        <v>161.63999999999999</v>
+        <v>161.47999999999999</v>
       </c>
       <c r="F47" s="10">
-        <v>171.64</v>
+        <v>171.48</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>168.36</v>
+        <v>168.29</v>
       </c>
       <c r="E48" s="13">
-        <v>161.83000000000001</v>
+        <v>161.66999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>171.83</v>
+        <v>171.67</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>168.62</v>
+        <v>168.34</v>
       </c>
       <c r="E49" s="10">
-        <v>161.96</v>
+        <v>161.63999999999999</v>
       </c>
       <c r="F49" s="10">
-        <v>171.96</v>
+        <v>171.64</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>168.63</v>
+        <v>168.36</v>
       </c>
       <c r="E50" s="13">
-        <v>162.15</v>
+        <v>161.83000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>172.15</v>
+        <v>171.83</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>184.18</v>
+        <v>185.04</v>
       </c>
       <c r="E54" s="10">
-        <v>175.67</v>
+        <v>175.76</v>
       </c>
       <c r="F54" s="10">
-        <v>185.67</v>
+        <v>185.76</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>171.85</v>
+        <v>172.7</v>
       </c>
       <c r="E55" s="13">
-        <v>173.59</v>
+        <v>173.48</v>
       </c>
       <c r="F55" s="13">
-        <v>183.59</v>
+        <v>183.48</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>174.33</v>
+        <v>175.19</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>174.09</v>
+        <v>174.91</v>
       </c>
       <c r="E57" s="13">
-        <v>167.85</v>
+        <v>167.75</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>170</v>
+        <v>170.82</v>
       </c>
       <c r="E58" s="10">
-        <v>163.91</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>173.91</v>
+        <v>173.8</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>176.61</v>
+        <v>177.44</v>
       </c>
       <c r="E59" s="13">
-        <v>173.95</v>
+        <v>174.02</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>184.2</v>
+        <v>184.18</v>
       </c>
       <c r="E60" s="10">
-        <v>175.74</v>
+        <v>175.67</v>
       </c>
       <c r="F60" s="10">
-        <v>185.74</v>
+        <v>185.67</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>171.87</v>
+        <v>171.85</v>
       </c>
       <c r="E61" s="13">
-        <v>173.58</v>
+        <v>173.59</v>
       </c>
       <c r="F61" s="13">
-        <v>183.58</v>
+        <v>183.59</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>174.36</v>
+        <v>174.33</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>174.12</v>
+        <v>174.09</v>
       </c>
       <c r="E63" s="13">
-        <v>167.84</v>
+        <v>167.85</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>170.03</v>
+        <v>170</v>
       </c>
       <c r="E64" s="10">
-        <v>163.9</v>
+        <v>163.91</v>
       </c>
       <c r="F64" s="10">
-        <v>173.9</v>
+        <v>173.91</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>176.65</v>
+        <v>176.61</v>
       </c>
       <c r="E65" s="13">
-        <v>174.03</v>
+        <v>173.95</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,17 +2125,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,6 +2135,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2154,24 +2172,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fri Nov  7 02:49:47 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{01627818-19E9-41EB-8E15-A15F335F634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{F3AF17E4-B89E-45FC-BB02-37DB80F0FF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>168.74</v>
+        <v>169.5</v>
       </c>
       <c r="E8" s="10">
-        <v>160.69999999999999</v>
+        <v>160.18</v>
       </c>
       <c r="F8" s="10">
-        <v>170.7</v>
+        <v>170.18</v>
       </c>
       <c r="G8" s="10">
-        <v>160.86000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>168.74</v>
+        <v>169.5</v>
       </c>
       <c r="E9" s="13">
-        <v>160.69999999999999</v>
+        <v>160.18</v>
       </c>
       <c r="F9" s="13">
-        <v>170.7</v>
+        <v>170.18</v>
       </c>
       <c r="G9" s="13">
-        <v>160.86000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>170.96</v>
+        <v>171.66</v>
       </c>
       <c r="E10" s="10">
-        <v>162.94999999999999</v>
+        <v>162.91</v>
       </c>
       <c r="F10" s="10">
-        <v>172.95</v>
+        <v>172.91</v>
       </c>
       <c r="G10" s="10">
-        <v>163.44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>168.28</v>
+        <v>168.74</v>
       </c>
       <c r="E11" s="13">
-        <v>160.72999999999999</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>170.73</v>
+        <v>170.7</v>
       </c>
       <c r="G11" s="13">
-        <v>160.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.86000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>168.28</v>
+        <v>168.74</v>
       </c>
       <c r="E12" s="10">
-        <v>160.72999999999999</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>170.73</v>
+        <v>170.7</v>
       </c>
       <c r="G12" s="10">
-        <v>160.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.86000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>170.11</v>
+        <v>170.96</v>
       </c>
       <c r="E13" s="13">
-        <v>162.91999999999999</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>172.92</v>
+        <v>172.95</v>
       </c>
       <c r="G13" s="13">
-        <v>163.41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>174.44</v>
+        <v>175.13</v>
       </c>
       <c r="E17" s="10">
-        <v>165.92</v>
+        <v>165.89</v>
       </c>
       <c r="F17" s="10">
-        <v>175.92</v>
+        <v>175.89</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>173.61</v>
+        <v>174.44</v>
       </c>
       <c r="E18" s="13">
-        <v>165.89</v>
+        <v>165.92</v>
       </c>
       <c r="F18" s="13">
-        <v>175.89</v>
+        <v>175.92</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>170.09</v>
+        <v>170.74</v>
       </c>
       <c r="E22" s="10">
-        <v>161.96</v>
+        <v>161.91999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>171.56</v>
+        <v>171.52</v>
       </c>
       <c r="G22" s="10">
-        <v>163.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>175.73</v>
+        <v>176.43</v>
       </c>
       <c r="E23" s="13">
-        <v>166.67</v>
+        <v>166.64</v>
       </c>
       <c r="F23" s="13">
-        <v>176.67</v>
+        <v>176.64</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>175.54</v>
+        <v>176.24</v>
       </c>
       <c r="E24" s="10">
-        <v>166.85</v>
+        <v>166.82</v>
       </c>
       <c r="F24" s="10">
-        <v>176.85</v>
+        <v>176.82</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>176.37</v>
+        <v>177.07</v>
       </c>
       <c r="E25" s="13">
-        <v>166.25</v>
+        <v>166.22</v>
       </c>
       <c r="F25" s="13">
-        <v>176.25</v>
+        <v>176.22</v>
       </c>
       <c r="G25" s="13">
-        <v>166.29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166.26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>175.1</v>
+        <v>175.8</v>
       </c>
       <c r="E26" s="10">
-        <v>167.81</v>
+        <v>167.78</v>
       </c>
       <c r="F26" s="10">
-        <v>177.81</v>
+        <v>177.78</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>169.31</v>
+        <v>170.09</v>
       </c>
       <c r="E27" s="13">
-        <v>161.94999999999999</v>
+        <v>161.96</v>
       </c>
       <c r="F27" s="13">
-        <v>171.55</v>
+        <v>171.56</v>
       </c>
       <c r="G27" s="13">
-        <v>163.22999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>174.88</v>
+        <v>175.73</v>
       </c>
       <c r="E28" s="22">
-        <v>166.65</v>
+        <v>166.67</v>
       </c>
       <c r="F28" s="22">
-        <v>176.65</v>
+        <v>176.67</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>174.69</v>
+        <v>175.54</v>
       </c>
       <c r="E29" s="13">
-        <v>166.82</v>
+        <v>166.85</v>
       </c>
       <c r="F29" s="13">
-        <v>176.82</v>
+        <v>176.85</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>175.52</v>
+        <v>176.37</v>
       </c>
       <c r="E30" s="22">
-        <v>166.21</v>
+        <v>166.25</v>
       </c>
       <c r="F30" s="22">
-        <v>176.21</v>
+        <v>176.25</v>
       </c>
       <c r="G30" s="22">
-        <v>166.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166.29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>174.26</v>
+        <v>175.1</v>
       </c>
       <c r="E31" s="13">
-        <v>167.77</v>
+        <v>167.81</v>
       </c>
       <c r="F31" s="13">
-        <v>177.77</v>
+        <v>177.81</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>169.43</v>
+        <v>170.12</v>
       </c>
       <c r="E35" s="10">
-        <v>160.16</v>
+        <v>160.13</v>
       </c>
       <c r="F35" s="10">
-        <v>169.16</v>
+        <v>169.13</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>168.69</v>
+        <v>169.43</v>
       </c>
       <c r="E36" s="13">
-        <v>160.13999999999999</v>
+        <v>160.16</v>
       </c>
       <c r="F36" s="13">
-        <v>169.14</v>
+        <v>169.16</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>174.83</v>
+        <v>175.53</v>
       </c>
       <c r="E40" s="10">
-        <v>165.58</v>
+        <v>165.57</v>
       </c>
       <c r="F40" s="10">
-        <v>175.58</v>
+        <v>175.57</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>174.53</v>
+        <v>175.24</v>
       </c>
       <c r="E41" s="13">
-        <v>166</v>
+        <v>165.99</v>
       </c>
       <c r="F41" s="13">
-        <v>176</v>
+        <v>175.99</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>173.96</v>
+        <v>174.83</v>
       </c>
       <c r="E42" s="10">
-        <v>165.52</v>
+        <v>165.58</v>
       </c>
       <c r="F42" s="10">
-        <v>175.52</v>
+        <v>175.58</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>173.67</v>
+        <v>174.53</v>
       </c>
       <c r="E43" s="13">
-        <v>165.94</v>
+        <v>166</v>
       </c>
       <c r="F43" s="13">
-        <v>175.95</v>
+        <v>176</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,35 +1490,35 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>168.28</v>
+        <v>169.24</v>
       </c>
       <c r="E47" s="10">
-        <v>161.47999999999999</v>
+        <v>161.49</v>
       </c>
       <c r="F47" s="10">
-        <v>171.48</v>
+        <v>171.49</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>168.29</v>
+        <v>169.25</v>
       </c>
       <c r="E48" s="13">
         <v>161.66999999999999</v>
@@ -1528,45 +1528,45 @@
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>168.34</v>
+        <v>168.28</v>
       </c>
       <c r="E49" s="10">
-        <v>161.63999999999999</v>
+        <v>161.47999999999999</v>
       </c>
       <c r="F49" s="10">
-        <v>171.64</v>
+        <v>171.48</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>168.36</v>
+        <v>168.29</v>
       </c>
       <c r="E50" s="13">
-        <v>161.83000000000001</v>
+        <v>161.66999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>171.83</v>
+        <v>171.67</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>185.04</v>
+        <v>185.75</v>
       </c>
       <c r="E54" s="10">
-        <v>175.76</v>
+        <v>175.77</v>
       </c>
       <c r="F54" s="10">
-        <v>185.76</v>
+        <v>185.77</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>172.7</v>
+        <v>173.4</v>
       </c>
       <c r="E55" s="13">
-        <v>173.48</v>
+        <v>173.43</v>
       </c>
       <c r="F55" s="13">
-        <v>183.48</v>
+        <v>183.43</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>175.19</v>
+        <v>175.89</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>174.91</v>
+        <v>175.59</v>
       </c>
       <c r="E57" s="13">
-        <v>167.75</v>
+        <v>167.7</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>170.82</v>
+        <v>171.5</v>
       </c>
       <c r="E58" s="10">
-        <v>163.80000000000001</v>
+        <v>163.75</v>
       </c>
       <c r="F58" s="10">
-        <v>173.8</v>
+        <v>173.75</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>177.44</v>
+        <v>178.12</v>
       </c>
       <c r="E59" s="13">
-        <v>174.02</v>
+        <v>174.01</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>184.18</v>
+        <v>185.04</v>
       </c>
       <c r="E60" s="10">
-        <v>175.67</v>
+        <v>175.76</v>
       </c>
       <c r="F60" s="10">
-        <v>185.67</v>
+        <v>185.76</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>171.85</v>
+        <v>172.7</v>
       </c>
       <c r="E61" s="13">
-        <v>173.59</v>
+        <v>173.48</v>
       </c>
       <c r="F61" s="13">
-        <v>183.59</v>
+        <v>183.48</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>174.33</v>
+        <v>175.19</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>174.09</v>
+        <v>174.91</v>
       </c>
       <c r="E63" s="13">
-        <v>167.85</v>
+        <v>167.75</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>170</v>
+        <v>170.82</v>
       </c>
       <c r="E64" s="10">
-        <v>163.91</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>173.91</v>
+        <v>173.8</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>176.61</v>
+        <v>177.44</v>
       </c>
       <c r="E65" s="13">
-        <v>173.95</v>
+        <v>174.02</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Mon Nov 10 02:57:11 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F3AF17E4-B89E-45FC-BB02-37DB80F0FF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{2A21E62C-D5DD-4026-A824-799920448C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11160" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>169.5</v>
+        <v>169.58</v>
       </c>
       <c r="E8" s="10">
-        <v>160.18</v>
+        <v>160.28</v>
       </c>
       <c r="F8" s="10">
-        <v>170.18</v>
+        <v>170.28</v>
       </c>
       <c r="G8" s="10">
-        <v>160.35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>169.5</v>
+        <v>169.58</v>
       </c>
       <c r="E9" s="13">
-        <v>160.18</v>
+        <v>160.28</v>
       </c>
       <c r="F9" s="13">
-        <v>170.18</v>
+        <v>170.28</v>
       </c>
       <c r="G9" s="13">
-        <v>160.35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>171.66</v>
+        <v>172.63</v>
       </c>
       <c r="E10" s="10">
-        <v>162.91</v>
+        <v>163.22999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>172.91</v>
+        <v>173.23</v>
       </c>
       <c r="G10" s="10">
-        <v>163.41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>168.74</v>
+        <v>169.5</v>
       </c>
       <c r="E11" s="13">
-        <v>160.69999999999999</v>
+        <v>160.18</v>
       </c>
       <c r="F11" s="13">
-        <v>170.7</v>
+        <v>170.18</v>
       </c>
       <c r="G11" s="13">
-        <v>160.86000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>168.74</v>
+        <v>169.5</v>
       </c>
       <c r="E12" s="10">
-        <v>160.69999999999999</v>
+        <v>160.18</v>
       </c>
       <c r="F12" s="10">
-        <v>170.7</v>
+        <v>170.18</v>
       </c>
       <c r="G12" s="10">
-        <v>160.86000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>170.96</v>
+        <v>171.66</v>
       </c>
       <c r="E13" s="13">
-        <v>162.94999999999999</v>
+        <v>162.91</v>
       </c>
       <c r="F13" s="13">
-        <v>172.95</v>
+        <v>172.91</v>
       </c>
       <c r="G13" s="13">
-        <v>163.44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>175.13</v>
+        <v>176.07</v>
       </c>
       <c r="E17" s="10">
-        <v>165.89</v>
+        <v>166.2</v>
       </c>
       <c r="F17" s="10">
-        <v>175.89</v>
+        <v>176.2</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>174.44</v>
+        <v>175.13</v>
       </c>
       <c r="E18" s="13">
-        <v>165.92</v>
+        <v>165.89</v>
       </c>
       <c r="F18" s="13">
-        <v>175.92</v>
+        <v>175.89</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>170.74</v>
+        <v>171.59</v>
       </c>
       <c r="E22" s="10">
-        <v>161.91999999999999</v>
+        <v>162.22</v>
       </c>
       <c r="F22" s="10">
-        <v>171.52</v>
+        <v>171.82</v>
       </c>
       <c r="G22" s="10">
-        <v>163.21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>176.43</v>
+        <v>177.4</v>
       </c>
       <c r="E23" s="13">
-        <v>166.64</v>
+        <v>166.95</v>
       </c>
       <c r="F23" s="13">
-        <v>176.64</v>
+        <v>176.95</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>176.24</v>
+        <v>177.21</v>
       </c>
       <c r="E24" s="10">
-        <v>166.82</v>
+        <v>167.15</v>
       </c>
       <c r="F24" s="10">
-        <v>176.82</v>
+        <v>177.15</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>177.07</v>
+        <v>178.04</v>
       </c>
       <c r="E25" s="13">
-        <v>166.22</v>
+        <v>166.54</v>
       </c>
       <c r="F25" s="13">
-        <v>176.22</v>
+        <v>176.54</v>
       </c>
       <c r="G25" s="13">
-        <v>166.26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>166.58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>175.8</v>
+        <v>176.76</v>
       </c>
       <c r="E26" s="10">
-        <v>167.78</v>
+        <v>168.11</v>
       </c>
       <c r="F26" s="10">
-        <v>177.78</v>
+        <v>178.11</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>170.09</v>
+        <v>170.74</v>
       </c>
       <c r="E27" s="13">
-        <v>161.96</v>
+        <v>161.91999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>171.56</v>
+        <v>171.52</v>
       </c>
       <c r="G27" s="13">
-        <v>163.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>175.73</v>
+        <v>176.43</v>
       </c>
       <c r="E28" s="22">
-        <v>166.67</v>
+        <v>166.64</v>
       </c>
       <c r="F28" s="22">
-        <v>176.67</v>
+        <v>176.64</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>175.54</v>
+        <v>176.24</v>
       </c>
       <c r="E29" s="13">
-        <v>166.85</v>
+        <v>166.82</v>
       </c>
       <c r="F29" s="13">
-        <v>176.85</v>
+        <v>176.82</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>176.37</v>
+        <v>177.07</v>
       </c>
       <c r="E30" s="22">
-        <v>166.25</v>
+        <v>166.22</v>
       </c>
       <c r="F30" s="22">
-        <v>176.25</v>
+        <v>176.22</v>
       </c>
       <c r="G30" s="22">
-        <v>166.29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>166.26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>175.1</v>
+        <v>175.8</v>
       </c>
       <c r="E31" s="13">
-        <v>167.81</v>
+        <v>167.78</v>
       </c>
       <c r="F31" s="13">
-        <v>177.81</v>
+        <v>177.78</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>170.12</v>
+        <v>170.98</v>
       </c>
       <c r="E35" s="10">
-        <v>160.13</v>
+        <v>160.44</v>
       </c>
       <c r="F35" s="10">
-        <v>169.13</v>
+        <v>169.44</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>169.43</v>
+        <v>170.12</v>
       </c>
       <c r="E36" s="13">
-        <v>160.16</v>
+        <v>160.13</v>
       </c>
       <c r="F36" s="13">
-        <v>169.16</v>
+        <v>169.13</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>175.53</v>
+        <v>176.53</v>
       </c>
       <c r="E40" s="10">
-        <v>165.57</v>
+        <v>165.93</v>
       </c>
       <c r="F40" s="10">
-        <v>175.57</v>
+        <v>175.93</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>175.24</v>
+        <v>176.24</v>
       </c>
       <c r="E41" s="13">
-        <v>165.99</v>
+        <v>166.35</v>
       </c>
       <c r="F41" s="13">
-        <v>175.99</v>
+        <v>176.35</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>174.83</v>
+        <v>175.53</v>
       </c>
       <c r="E42" s="10">
-        <v>165.58</v>
+        <v>165.57</v>
       </c>
       <c r="F42" s="10">
-        <v>175.58</v>
+        <v>175.57</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>174.53</v>
+        <v>175.24</v>
       </c>
       <c r="E43" s="13">
-        <v>166</v>
+        <v>165.99</v>
       </c>
       <c r="F43" s="13">
-        <v>176</v>
+        <v>175.99</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,73 +1490,73 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>169.24</v>
+        <v>170.02</v>
       </c>
       <c r="E47" s="10">
-        <v>161.49</v>
+        <v>162.52000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>171.49</v>
+        <v>172.52</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>169.25</v>
+        <v>170.02</v>
       </c>
       <c r="E48" s="13">
-        <v>161.66999999999999</v>
+        <v>162.69999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>171.67</v>
+        <v>172.7</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>168.28</v>
+        <v>169.24</v>
       </c>
       <c r="E49" s="10">
-        <v>161.47999999999999</v>
+        <v>161.49</v>
       </c>
       <c r="F49" s="10">
-        <v>171.48</v>
+        <v>171.49</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>168.29</v>
+        <v>169.25</v>
       </c>
       <c r="E50" s="13">
         <v>161.66999999999999</v>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>185.75</v>
+        <v>186.73</v>
       </c>
       <c r="E54" s="10">
-        <v>175.77</v>
+        <v>176.2</v>
       </c>
       <c r="F54" s="10">
-        <v>185.77</v>
+        <v>186.2</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>173.4</v>
+        <v>174.38</v>
       </c>
       <c r="E55" s="13">
-        <v>173.43</v>
+        <v>173.71</v>
       </c>
       <c r="F55" s="13">
-        <v>183.43</v>
+        <v>183.71</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>175.89</v>
+        <v>176.76</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>175.59</v>
+        <v>176.41</v>
       </c>
       <c r="E57" s="13">
-        <v>167.7</v>
+        <v>167.98</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>171.5</v>
+        <v>172.32</v>
       </c>
       <c r="E58" s="10">
-        <v>163.75</v>
+        <v>164.03</v>
       </c>
       <c r="F58" s="10">
-        <v>173.75</v>
+        <v>174.03</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>178.12</v>
+        <v>179.05</v>
       </c>
       <c r="E59" s="13">
-        <v>174.01</v>
+        <v>174.4</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>185.04</v>
+        <v>185.75</v>
       </c>
       <c r="E60" s="10">
-        <v>175.76</v>
+        <v>175.77</v>
       </c>
       <c r="F60" s="10">
-        <v>185.76</v>
+        <v>185.77</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>172.7</v>
+        <v>173.4</v>
       </c>
       <c r="E61" s="13">
-        <v>173.48</v>
+        <v>173.43</v>
       </c>
       <c r="F61" s="13">
-        <v>183.48</v>
+        <v>183.43</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>175.19</v>
+        <v>175.89</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>174.91</v>
+        <v>175.59</v>
       </c>
       <c r="E63" s="13">
-        <v>167.75</v>
+        <v>167.7</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>170.82</v>
+        <v>171.5</v>
       </c>
       <c r="E64" s="10">
-        <v>163.80000000000001</v>
+        <v>163.75</v>
       </c>
       <c r="F64" s="10">
-        <v>173.8</v>
+        <v>173.75</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45968</v>
+        <v>45969</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>177.44</v>
+        <v>178.12</v>
       </c>
       <c r="E65" s="13">
-        <v>174.02</v>
+        <v>174.01</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,14 +1855,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2126,28 +2124,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2163,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Nov 11 02:52:36 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{2A21E62C-D5DD-4026-A824-799920448C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D1BD1A6B-8BBF-459B-BB53-A81D5CE5AA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11160" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>169.58</v>
+        <v>170.76</v>
       </c>
       <c r="E8" s="10">
-        <v>160.28</v>
+        <v>160.49</v>
       </c>
       <c r="F8" s="10">
-        <v>170.28</v>
+        <v>170.49</v>
       </c>
       <c r="G8" s="10">
-        <v>160.44</v>
+        <v>160.66</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>169.58</v>
+        <v>170.76</v>
       </c>
       <c r="E9" s="13">
-        <v>160.28</v>
+        <v>160.49</v>
       </c>
       <c r="F9" s="13">
-        <v>170.28</v>
+        <v>170.49</v>
       </c>
       <c r="G9" s="13">
-        <v>160.44</v>
+        <v>160.66</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>172.63</v>
+        <v>173.14</v>
       </c>
       <c r="E10" s="10">
-        <v>163.22999999999999</v>
+        <v>163.41999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>173.23</v>
+        <v>173.42</v>
       </c>
       <c r="G10" s="10">
-        <v>163.72</v>
+        <v>163.91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>169.5</v>
+        <v>169.58</v>
       </c>
       <c r="E11" s="13">
-        <v>160.18</v>
+        <v>160.28</v>
       </c>
       <c r="F11" s="13">
-        <v>170.18</v>
+        <v>170.28</v>
       </c>
       <c r="G11" s="13">
-        <v>160.35</v>
+        <v>160.44</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>169.5</v>
+        <v>169.58</v>
       </c>
       <c r="E12" s="10">
-        <v>160.18</v>
+        <v>160.28</v>
       </c>
       <c r="F12" s="10">
-        <v>170.18</v>
+        <v>170.28</v>
       </c>
       <c r="G12" s="10">
-        <v>160.35</v>
+        <v>160.44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>171.66</v>
+        <v>172.63</v>
       </c>
       <c r="E13" s="13">
-        <v>162.91</v>
+        <v>163.22999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>172.91</v>
+        <v>173.23</v>
       </c>
       <c r="G13" s="13">
-        <v>163.41</v>
+        <v>163.72</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>176.07</v>
+        <v>176.55</v>
       </c>
       <c r="E17" s="10">
-        <v>166.2</v>
+        <v>166.39</v>
       </c>
       <c r="F17" s="10">
-        <v>176.2</v>
+        <v>176.39</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>175.13</v>
+        <v>176.07</v>
       </c>
       <c r="E18" s="13">
-        <v>165.89</v>
+        <v>166.2</v>
       </c>
       <c r="F18" s="13">
-        <v>175.89</v>
+        <v>176.2</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>171.59</v>
+        <v>172</v>
       </c>
       <c r="E22" s="10">
-        <v>162.22</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>171.82</v>
+        <v>171.9</v>
       </c>
       <c r="G22" s="10">
-        <v>163.51</v>
+        <v>163.58000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>177.4</v>
+        <v>177.92</v>
       </c>
       <c r="E23" s="13">
-        <v>166.95</v>
+        <v>167.14</v>
       </c>
       <c r="F23" s="13">
-        <v>176.95</v>
+        <v>177.14</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>177.21</v>
+        <v>177.72</v>
       </c>
       <c r="E24" s="10">
-        <v>167.15</v>
+        <v>167.35</v>
       </c>
       <c r="F24" s="10">
-        <v>177.15</v>
+        <v>177.35</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>178.04</v>
+        <v>178.55</v>
       </c>
       <c r="E25" s="13">
-        <v>166.54</v>
+        <v>166.75</v>
       </c>
       <c r="F25" s="13">
-        <v>176.54</v>
+        <v>176.75</v>
       </c>
       <c r="G25" s="13">
-        <v>166.58</v>
+        <v>166.79</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>176.76</v>
+        <v>177.27</v>
       </c>
       <c r="E26" s="10">
-        <v>168.11</v>
+        <v>168.32</v>
       </c>
       <c r="F26" s="10">
-        <v>178.11</v>
+        <v>178.32</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>170.74</v>
+        <v>171.59</v>
       </c>
       <c r="E27" s="13">
-        <v>161.91999999999999</v>
+        <v>162.22</v>
       </c>
       <c r="F27" s="13">
-        <v>171.52</v>
+        <v>171.82</v>
       </c>
       <c r="G27" s="13">
-        <v>163.21</v>
+        <v>163.51</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>176.43</v>
+        <v>177.4</v>
       </c>
       <c r="E28" s="22">
-        <v>166.64</v>
+        <v>166.95</v>
       </c>
       <c r="F28" s="22">
-        <v>176.64</v>
+        <v>176.95</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>176.24</v>
+        <v>177.21</v>
       </c>
       <c r="E29" s="13">
-        <v>166.82</v>
+        <v>167.15</v>
       </c>
       <c r="F29" s="13">
-        <v>176.82</v>
+        <v>177.15</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>177.07</v>
+        <v>178.04</v>
       </c>
       <c r="E30" s="22">
-        <v>166.22</v>
+        <v>166.54</v>
       </c>
       <c r="F30" s="22">
-        <v>176.22</v>
+        <v>176.54</v>
       </c>
       <c r="G30" s="22">
-        <v>166.26</v>
+        <v>166.58</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>175.8</v>
+        <v>176.76</v>
       </c>
       <c r="E31" s="13">
-        <v>167.78</v>
+        <v>168.11</v>
       </c>
       <c r="F31" s="13">
-        <v>177.78</v>
+        <v>178.11</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>170.98</v>
+        <v>171.5</v>
       </c>
       <c r="E35" s="10">
-        <v>160.44</v>
+        <v>160.63</v>
       </c>
       <c r="F35" s="10">
-        <v>169.44</v>
+        <v>169.63</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>170.12</v>
+        <v>170.98</v>
       </c>
       <c r="E36" s="13">
-        <v>160.13</v>
+        <v>160.44</v>
       </c>
       <c r="F36" s="13">
-        <v>169.13</v>
+        <v>169.44</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>176.53</v>
+        <v>177.07</v>
       </c>
       <c r="E40" s="10">
-        <v>165.93</v>
+        <v>166.17</v>
       </c>
       <c r="F40" s="10">
-        <v>175.93</v>
+        <v>176.17</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>176.24</v>
+        <v>176.77</v>
       </c>
       <c r="E41" s="13">
-        <v>166.35</v>
+        <v>166.59</v>
       </c>
       <c r="F41" s="13">
-        <v>176.35</v>
+        <v>176.59</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>175.53</v>
+        <v>176.53</v>
       </c>
       <c r="E42" s="10">
-        <v>165.57</v>
+        <v>165.93</v>
       </c>
       <c r="F42" s="10">
-        <v>175.57</v>
+        <v>175.93</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>175.24</v>
+        <v>176.24</v>
       </c>
       <c r="E43" s="13">
-        <v>165.99</v>
+        <v>166.35</v>
       </c>
       <c r="F43" s="13">
-        <v>175.99</v>
+        <v>176.35</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>170.02</v>
+        <v>170.8</v>
       </c>
       <c r="E47" s="10">
-        <v>162.52000000000001</v>
+        <v>162.63999999999999</v>
       </c>
       <c r="F47" s="10">
-        <v>172.52</v>
+        <v>172.64</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>170.02</v>
+        <v>170.8</v>
       </c>
       <c r="E48" s="13">
-        <v>162.69999999999999</v>
+        <v>162.81</v>
       </c>
       <c r="F48" s="13">
-        <v>172.7</v>
+        <v>172.81</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>169.24</v>
+        <v>170.02</v>
       </c>
       <c r="E49" s="10">
-        <v>161.49</v>
+        <v>162.52000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>171.49</v>
+        <v>172.52</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>169.25</v>
+        <v>170.02</v>
       </c>
       <c r="E50" s="13">
-        <v>161.66999999999999</v>
+        <v>162.69999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>171.67</v>
+        <v>172.7</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>186.73</v>
+        <v>187.24</v>
       </c>
       <c r="E54" s="10">
-        <v>176.2</v>
+        <v>176.52</v>
       </c>
       <c r="F54" s="10">
-        <v>186.2</v>
+        <v>186.52</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>174.38</v>
+        <v>174.89</v>
       </c>
       <c r="E55" s="13">
-        <v>173.71</v>
+        <v>173.76</v>
       </c>
       <c r="F55" s="13">
-        <v>183.71</v>
+        <v>183.76</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>176.76</v>
+        <v>177.28</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>176.41</v>
+        <v>176.88</v>
       </c>
       <c r="E57" s="13">
-        <v>167.98</v>
+        <v>168.03</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>172.32</v>
+        <v>172.79</v>
       </c>
       <c r="E58" s="10">
-        <v>164.03</v>
+        <v>164.08</v>
       </c>
       <c r="F58" s="10">
-        <v>174.03</v>
+        <v>174.08</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>179.05</v>
+        <v>179.53</v>
       </c>
       <c r="E59" s="13">
-        <v>174.4</v>
+        <v>174.66</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>185.75</v>
+        <v>186.73</v>
       </c>
       <c r="E60" s="10">
-        <v>175.77</v>
+        <v>176.2</v>
       </c>
       <c r="F60" s="10">
-        <v>185.77</v>
+        <v>186.2</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>173.4</v>
+        <v>174.38</v>
       </c>
       <c r="E61" s="13">
-        <v>173.43</v>
+        <v>173.71</v>
       </c>
       <c r="F61" s="13">
-        <v>183.43</v>
+        <v>183.71</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>175.89</v>
+        <v>176.76</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>175.59</v>
+        <v>176.41</v>
       </c>
       <c r="E63" s="13">
-        <v>167.7</v>
+        <v>167.98</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>171.5</v>
+        <v>172.32</v>
       </c>
       <c r="E64" s="10">
-        <v>163.75</v>
+        <v>164.03</v>
       </c>
       <c r="F64" s="10">
-        <v>173.75</v>
+        <v>174.03</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45969</v>
+        <v>45972</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>178.12</v>
+        <v>179.05</v>
       </c>
       <c r="E65" s="13">
-        <v>174.01</v>
+        <v>174.4</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,12 +1855,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2124,20 +2126,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2163,19 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Wed Nov 12 02:51:24 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D1BD1A6B-8BBF-459B-BB53-A81D5CE5AA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{1668E664-3F67-4745-B351-413A462D3EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>170.76</v>
+        <v>171.51</v>
       </c>
       <c r="E8" s="10">
-        <v>160.49</v>
+        <v>160.94</v>
       </c>
       <c r="F8" s="10">
-        <v>170.49</v>
+        <v>170.94</v>
       </c>
       <c r="G8" s="10">
-        <v>160.66</v>
+        <v>161.1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>170.76</v>
+        <v>171.51</v>
       </c>
       <c r="E9" s="13">
-        <v>160.49</v>
+        <v>160.94</v>
       </c>
       <c r="F9" s="13">
-        <v>170.49</v>
+        <v>170.94</v>
       </c>
       <c r="G9" s="13">
-        <v>160.66</v>
+        <v>161.1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>173.14</v>
+        <v>173.97</v>
       </c>
       <c r="E10" s="10">
-        <v>163.41999999999999</v>
+        <v>163.94</v>
       </c>
       <c r="F10" s="10">
-        <v>173.42</v>
+        <v>173.94</v>
       </c>
       <c r="G10" s="10">
-        <v>163.91</v>
+        <v>164.43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>169.58</v>
+        <v>170.76</v>
       </c>
       <c r="E11" s="13">
-        <v>160.28</v>
+        <v>160.49</v>
       </c>
       <c r="F11" s="13">
-        <v>170.28</v>
+        <v>170.49</v>
       </c>
       <c r="G11" s="13">
-        <v>160.44</v>
+        <v>160.66</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>169.58</v>
+        <v>170.76</v>
       </c>
       <c r="E12" s="10">
-        <v>160.28</v>
+        <v>160.49</v>
       </c>
       <c r="F12" s="10">
-        <v>170.28</v>
+        <v>170.49</v>
       </c>
       <c r="G12" s="10">
-        <v>160.44</v>
+        <v>160.66</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>172.63</v>
+        <v>173.14</v>
       </c>
       <c r="E13" s="13">
-        <v>163.22999999999999</v>
+        <v>163.41999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>173.23</v>
+        <v>173.42</v>
       </c>
       <c r="G13" s="13">
-        <v>163.72</v>
+        <v>163.91</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>176.55</v>
+        <v>177.35</v>
       </c>
       <c r="E17" s="10">
-        <v>166.39</v>
+        <v>166.8</v>
       </c>
       <c r="F17" s="10">
-        <v>176.39</v>
+        <v>176.8</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>176.07</v>
+        <v>176.55</v>
       </c>
       <c r="E18" s="13">
-        <v>166.2</v>
+        <v>166.39</v>
       </c>
       <c r="F18" s="13">
-        <v>176.2</v>
+        <v>176.39</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>172</v>
+        <v>172.75</v>
       </c>
       <c r="E22" s="10">
-        <v>162.30000000000001</v>
+        <v>163.03</v>
       </c>
       <c r="F22" s="10">
-        <v>171.9</v>
+        <v>172.63</v>
       </c>
       <c r="G22" s="10">
-        <v>163.58000000000001</v>
+        <v>164.31</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>177.92</v>
+        <v>178.75</v>
       </c>
       <c r="E23" s="13">
-        <v>167.14</v>
+        <v>167.66</v>
       </c>
       <c r="F23" s="13">
-        <v>177.14</v>
+        <v>177.66</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>177.72</v>
+        <v>178.55</v>
       </c>
       <c r="E24" s="10">
-        <v>167.35</v>
+        <v>167.88</v>
       </c>
       <c r="F24" s="10">
-        <v>177.35</v>
+        <v>177.88</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>178.55</v>
+        <v>179.38</v>
       </c>
       <c r="E25" s="13">
-        <v>166.75</v>
+        <v>167.28</v>
       </c>
       <c r="F25" s="13">
-        <v>176.75</v>
+        <v>177.28</v>
       </c>
       <c r="G25" s="13">
-        <v>166.79</v>
+        <v>167.32</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>177.27</v>
+        <v>178.09</v>
       </c>
       <c r="E26" s="10">
-        <v>168.32</v>
+        <v>168.85</v>
       </c>
       <c r="F26" s="10">
-        <v>178.32</v>
+        <v>178.85</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>171.59</v>
+        <v>172</v>
       </c>
       <c r="E27" s="13">
-        <v>162.22</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>171.82</v>
+        <v>171.9</v>
       </c>
       <c r="G27" s="13">
-        <v>163.51</v>
+        <v>163.58000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>177.4</v>
+        <v>177.92</v>
       </c>
       <c r="E28" s="22">
-        <v>166.95</v>
+        <v>167.14</v>
       </c>
       <c r="F28" s="22">
-        <v>176.95</v>
+        <v>177.14</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>177.21</v>
+        <v>177.72</v>
       </c>
       <c r="E29" s="13">
-        <v>167.15</v>
+        <v>167.35</v>
       </c>
       <c r="F29" s="13">
-        <v>177.15</v>
+        <v>177.35</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>178.04</v>
+        <v>178.55</v>
       </c>
       <c r="E30" s="22">
-        <v>166.54</v>
+        <v>166.75</v>
       </c>
       <c r="F30" s="22">
-        <v>176.54</v>
+        <v>176.75</v>
       </c>
       <c r="G30" s="22">
-        <v>166.58</v>
+        <v>166.79</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>176.76</v>
+        <v>177.27</v>
       </c>
       <c r="E31" s="13">
-        <v>168.11</v>
+        <v>168.32</v>
       </c>
       <c r="F31" s="13">
-        <v>178.11</v>
+        <v>178.32</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>171.5</v>
+        <v>172.44</v>
       </c>
       <c r="E35" s="10">
-        <v>160.63</v>
+        <v>161.15</v>
       </c>
       <c r="F35" s="10">
-        <v>169.63</v>
+        <v>170.15</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>170.98</v>
+        <v>171.5</v>
       </c>
       <c r="E36" s="13">
-        <v>160.44</v>
+        <v>160.63</v>
       </c>
       <c r="F36" s="13">
-        <v>169.44</v>
+        <v>169.63</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>177.07</v>
+        <v>177.92</v>
       </c>
       <c r="E40" s="10">
-        <v>166.17</v>
+        <v>166.63</v>
       </c>
       <c r="F40" s="10">
-        <v>176.17</v>
+        <v>176.63</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>176.77</v>
+        <v>177.63</v>
       </c>
       <c r="E41" s="13">
-        <v>166.59</v>
+        <v>167.05</v>
       </c>
       <c r="F41" s="13">
-        <v>176.59</v>
+        <v>177.05</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>176.53</v>
+        <v>177.07</v>
       </c>
       <c r="E42" s="10">
-        <v>165.93</v>
+        <v>166.17</v>
       </c>
       <c r="F42" s="10">
-        <v>175.93</v>
+        <v>176.17</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>176.24</v>
+        <v>176.77</v>
       </c>
       <c r="E43" s="13">
-        <v>166.35</v>
+        <v>166.59</v>
       </c>
       <c r="F43" s="13">
-        <v>176.35</v>
+        <v>176.59</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>170.8</v>
+        <v>171.39</v>
       </c>
       <c r="E47" s="10">
-        <v>162.63999999999999</v>
+        <v>162.29</v>
       </c>
       <c r="F47" s="10">
-        <v>172.64</v>
+        <v>172.29</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>170.8</v>
+        <v>171.38</v>
       </c>
       <c r="E48" s="13">
-        <v>162.81</v>
+        <v>162.46</v>
       </c>
       <c r="F48" s="13">
-        <v>172.81</v>
+        <v>172.46</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>170.02</v>
+        <v>170.8</v>
       </c>
       <c r="E49" s="10">
-        <v>162.52000000000001</v>
+        <v>162.63999999999999</v>
       </c>
       <c r="F49" s="10">
-        <v>172.52</v>
+        <v>172.64</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>170.02</v>
+        <v>170.8</v>
       </c>
       <c r="E50" s="13">
-        <v>162.69999999999999</v>
+        <v>162.81</v>
       </c>
       <c r="F50" s="13">
-        <v>172.7</v>
+        <v>172.81</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>187.24</v>
+        <v>188.06</v>
       </c>
       <c r="E54" s="10">
-        <v>176.52</v>
+        <v>177.14</v>
       </c>
       <c r="F54" s="10">
-        <v>186.52</v>
+        <v>187.14</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>174.89</v>
+        <v>175.73</v>
       </c>
       <c r="E55" s="13">
-        <v>173.76</v>
+        <v>174.36</v>
       </c>
       <c r="F55" s="13">
-        <v>183.76</v>
+        <v>184.36</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>177.28</v>
+        <v>178.22</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>176.88</v>
+        <v>177.79</v>
       </c>
       <c r="E57" s="13">
-        <v>168.03</v>
+        <v>168.63</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>172.79</v>
+        <v>173.7</v>
       </c>
       <c r="E58" s="10">
-        <v>164.08</v>
+        <v>164.68</v>
       </c>
       <c r="F58" s="10">
-        <v>174.08</v>
+        <v>174.68</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>179.53</v>
+        <v>180.33</v>
       </c>
       <c r="E59" s="13">
-        <v>174.66</v>
+        <v>175.24</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>186.73</v>
+        <v>187.24</v>
       </c>
       <c r="E60" s="10">
-        <v>176.2</v>
+        <v>176.52</v>
       </c>
       <c r="F60" s="10">
-        <v>186.2</v>
+        <v>186.52</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>174.38</v>
+        <v>174.89</v>
       </c>
       <c r="E61" s="13">
-        <v>173.71</v>
+        <v>173.76</v>
       </c>
       <c r="F61" s="13">
-        <v>183.71</v>
+        <v>183.76</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>176.76</v>
+        <v>177.28</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>176.41</v>
+        <v>176.88</v>
       </c>
       <c r="E63" s="13">
-        <v>167.98</v>
+        <v>168.03</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>172.32</v>
+        <v>172.79</v>
       </c>
       <c r="E64" s="10">
-        <v>164.03</v>
+        <v>164.08</v>
       </c>
       <c r="F64" s="10">
-        <v>174.03</v>
+        <v>174.08</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>179.05</v>
+        <v>179.53</v>
       </c>
       <c r="E65" s="13">
-        <v>174.4</v>
+        <v>174.66</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,17 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2125,6 +2114,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,24 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2172,6 +2154,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Thu Nov 13 02:53:36 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1668E664-3F67-4745-B351-413A462D3EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{0D4328D9-8BB4-45CD-AAB9-B358A3A6D501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>171.51</v>
+        <v>172.24</v>
       </c>
       <c r="E8" s="10">
-        <v>160.94</v>
+        <v>161.46</v>
       </c>
       <c r="F8" s="10">
-        <v>170.94</v>
+        <v>171.46</v>
       </c>
       <c r="G8" s="10">
-        <v>161.1</v>
+        <v>161.63</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>171.51</v>
+        <v>172.24</v>
       </c>
       <c r="E9" s="13">
-        <v>160.94</v>
+        <v>161.46</v>
       </c>
       <c r="F9" s="13">
-        <v>170.94</v>
+        <v>171.46</v>
       </c>
       <c r="G9" s="13">
-        <v>161.1</v>
+        <v>161.63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>173.97</v>
+        <v>174.8</v>
       </c>
       <c r="E10" s="10">
-        <v>163.94</v>
+        <v>164.66</v>
       </c>
       <c r="F10" s="10">
-        <v>173.94</v>
+        <v>174.66</v>
       </c>
       <c r="G10" s="10">
-        <v>164.43</v>
+        <v>165.16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>170.76</v>
+        <v>171.51</v>
       </c>
       <c r="E11" s="13">
-        <v>160.49</v>
+        <v>160.94</v>
       </c>
       <c r="F11" s="13">
-        <v>170.49</v>
+        <v>170.94</v>
       </c>
       <c r="G11" s="13">
-        <v>160.66</v>
+        <v>161.1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>170.76</v>
+        <v>171.51</v>
       </c>
       <c r="E12" s="10">
-        <v>160.49</v>
+        <v>160.94</v>
       </c>
       <c r="F12" s="10">
-        <v>170.49</v>
+        <v>170.94</v>
       </c>
       <c r="G12" s="10">
-        <v>160.66</v>
+        <v>161.1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>173.14</v>
+        <v>173.97</v>
       </c>
       <c r="E13" s="13">
-        <v>163.41999999999999</v>
+        <v>163.94</v>
       </c>
       <c r="F13" s="13">
-        <v>173.42</v>
+        <v>173.94</v>
       </c>
       <c r="G13" s="13">
-        <v>163.91</v>
+        <v>164.43</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>177.35</v>
+        <v>178.16</v>
       </c>
       <c r="E17" s="10">
-        <v>166.8</v>
+        <v>167.49</v>
       </c>
       <c r="F17" s="10">
-        <v>176.8</v>
+        <v>177.49</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>176.55</v>
+        <v>177.35</v>
       </c>
       <c r="E18" s="13">
-        <v>166.39</v>
+        <v>166.8</v>
       </c>
       <c r="F18" s="13">
-        <v>176.39</v>
+        <v>176.8</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>172.75</v>
+        <v>173.59</v>
       </c>
       <c r="E22" s="10">
-        <v>163.03</v>
+        <v>163.74</v>
       </c>
       <c r="F22" s="10">
-        <v>172.63</v>
+        <v>173.34</v>
       </c>
       <c r="G22" s="10">
-        <v>164.31</v>
+        <v>165.03</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>178.75</v>
+        <v>179.58</v>
       </c>
       <c r="E23" s="13">
-        <v>167.66</v>
+        <v>168.27</v>
       </c>
       <c r="F23" s="13">
-        <v>177.66</v>
+        <v>178.27</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>178.55</v>
+        <v>179.38</v>
       </c>
       <c r="E24" s="10">
-        <v>167.88</v>
+        <v>168.5</v>
       </c>
       <c r="F24" s="10">
-        <v>177.88</v>
+        <v>178.5</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>179.38</v>
+        <v>180.21</v>
       </c>
       <c r="E25" s="13">
-        <v>167.28</v>
+        <v>167.91</v>
       </c>
       <c r="F25" s="13">
-        <v>177.28</v>
+        <v>177.91</v>
       </c>
       <c r="G25" s="13">
-        <v>167.32</v>
+        <v>167.95</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>178.09</v>
+        <v>178.91</v>
       </c>
       <c r="E26" s="10">
-        <v>168.85</v>
+        <v>169.48</v>
       </c>
       <c r="F26" s="10">
-        <v>178.85</v>
+        <v>179.48</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>172</v>
+        <v>172.75</v>
       </c>
       <c r="E27" s="13">
-        <v>162.30000000000001</v>
+        <v>163.03</v>
       </c>
       <c r="F27" s="13">
-        <v>171.9</v>
+        <v>172.63</v>
       </c>
       <c r="G27" s="13">
-        <v>163.58000000000001</v>
+        <v>164.31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>177.92</v>
+        <v>178.75</v>
       </c>
       <c r="E28" s="22">
-        <v>167.14</v>
+        <v>167.66</v>
       </c>
       <c r="F28" s="22">
-        <v>177.14</v>
+        <v>177.66</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>177.72</v>
+        <v>178.55</v>
       </c>
       <c r="E29" s="13">
-        <v>167.35</v>
+        <v>167.88</v>
       </c>
       <c r="F29" s="13">
-        <v>177.35</v>
+        <v>177.88</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>178.55</v>
+        <v>179.38</v>
       </c>
       <c r="E30" s="22">
-        <v>166.75</v>
+        <v>167.28</v>
       </c>
       <c r="F30" s="22">
-        <v>176.75</v>
+        <v>177.28</v>
       </c>
       <c r="G30" s="22">
-        <v>166.79</v>
+        <v>167.32</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>177.27</v>
+        <v>178.09</v>
       </c>
       <c r="E31" s="13">
-        <v>168.32</v>
+        <v>168.85</v>
       </c>
       <c r="F31" s="13">
-        <v>178.32</v>
+        <v>178.85</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>172.44</v>
+        <v>173.16</v>
       </c>
       <c r="E35" s="10">
-        <v>161.15</v>
+        <v>161.76</v>
       </c>
       <c r="F35" s="10">
-        <v>170.15</v>
+        <v>170.76</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>171.5</v>
+        <v>172.44</v>
       </c>
       <c r="E36" s="13">
-        <v>160.63</v>
+        <v>161.15</v>
       </c>
       <c r="F36" s="13">
-        <v>169.63</v>
+        <v>170.15</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>177.92</v>
+        <v>178.77</v>
       </c>
       <c r="E40" s="10">
-        <v>166.63</v>
+        <v>167.35</v>
       </c>
       <c r="F40" s="10">
-        <v>176.63</v>
+        <v>177.35</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>177.63</v>
+        <v>178.48</v>
       </c>
       <c r="E41" s="13">
-        <v>167.05</v>
+        <v>167.77</v>
       </c>
       <c r="F41" s="13">
-        <v>177.05</v>
+        <v>177.77</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>177.07</v>
+        <v>177.92</v>
       </c>
       <c r="E42" s="10">
-        <v>166.17</v>
+        <v>166.63</v>
       </c>
       <c r="F42" s="10">
-        <v>176.17</v>
+        <v>176.63</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>176.77</v>
+        <v>177.63</v>
       </c>
       <c r="E43" s="13">
-        <v>166.59</v>
+        <v>167.05</v>
       </c>
       <c r="F43" s="13">
-        <v>176.59</v>
+        <v>177.05</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>171.39</v>
+        <v>172.16</v>
       </c>
       <c r="E47" s="10">
-        <v>162.29</v>
+        <v>162.59</v>
       </c>
       <c r="F47" s="10">
-        <v>172.29</v>
+        <v>172.59</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>171.38</v>
+        <v>172.14</v>
       </c>
       <c r="E48" s="13">
-        <v>162.46</v>
+        <v>162.75</v>
       </c>
       <c r="F48" s="13">
-        <v>172.46</v>
+        <v>172.75</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>170.8</v>
+        <v>171.39</v>
       </c>
       <c r="E49" s="10">
-        <v>162.63999999999999</v>
+        <v>162.29</v>
       </c>
       <c r="F49" s="10">
-        <v>172.64</v>
+        <v>172.29</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>170.8</v>
+        <v>171.38</v>
       </c>
       <c r="E50" s="13">
-        <v>162.81</v>
+        <v>162.46</v>
       </c>
       <c r="F50" s="13">
-        <v>172.81</v>
+        <v>172.46</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>188.06</v>
+        <v>188.88</v>
       </c>
       <c r="E54" s="10">
-        <v>177.14</v>
+        <v>177.86</v>
       </c>
       <c r="F54" s="10">
-        <v>187.14</v>
+        <v>187.86</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>175.73</v>
+        <v>176.56</v>
       </c>
       <c r="E55" s="13">
-        <v>174.36</v>
+        <v>174.95</v>
       </c>
       <c r="F55" s="13">
-        <v>184.36</v>
+        <v>184.95</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>178.22</v>
+        <v>179.06</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>177.79</v>
+        <v>178.59</v>
       </c>
       <c r="E57" s="13">
-        <v>168.63</v>
+        <v>169.22</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>173.7</v>
+        <v>174.5</v>
       </c>
       <c r="E58" s="10">
-        <v>164.68</v>
+        <v>165.27</v>
       </c>
       <c r="F58" s="10">
-        <v>174.68</v>
+        <v>175.27</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>180.33</v>
+        <v>181.13</v>
       </c>
       <c r="E59" s="13">
-        <v>175.24</v>
+        <v>175.9</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>187.24</v>
+        <v>188.06</v>
       </c>
       <c r="E60" s="10">
-        <v>176.52</v>
+        <v>177.14</v>
       </c>
       <c r="F60" s="10">
-        <v>186.52</v>
+        <v>187.14</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>174.89</v>
+        <v>175.73</v>
       </c>
       <c r="E61" s="13">
-        <v>173.76</v>
+        <v>174.36</v>
       </c>
       <c r="F61" s="13">
-        <v>183.76</v>
+        <v>184.36</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>177.28</v>
+        <v>178.22</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>176.88</v>
+        <v>177.79</v>
       </c>
       <c r="E63" s="13">
-        <v>168.03</v>
+        <v>168.63</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>172.79</v>
+        <v>173.7</v>
       </c>
       <c r="E64" s="10">
-        <v>164.08</v>
+        <v>164.68</v>
       </c>
       <c r="F64" s="10">
-        <v>174.08</v>
+        <v>174.68</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>179.53</v>
+        <v>180.33</v>
       </c>
       <c r="E65" s="13">
-        <v>174.66</v>
+        <v>175.24</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -2115,6 +2115,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -2123,15 +2132,6 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2155,6 +2155,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2172,14 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Fri Nov 14 02:52:19 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{0D4328D9-8BB4-45CD-AAB9-B358A3A6D501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D09B11FF-C9F0-4B6F-BCED-D5E6606659B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>172.24</v>
+        <v>172.4</v>
       </c>
       <c r="E8" s="10">
-        <v>161.46</v>
+        <v>161.6</v>
       </c>
       <c r="F8" s="10">
-        <v>171.46</v>
+        <v>171.6</v>
       </c>
       <c r="G8" s="10">
-        <v>161.63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.77000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>172.24</v>
+        <v>172.4</v>
       </c>
       <c r="E9" s="13">
-        <v>161.46</v>
+        <v>161.6</v>
       </c>
       <c r="F9" s="13">
-        <v>171.46</v>
+        <v>171.6</v>
       </c>
       <c r="G9" s="13">
-        <v>161.63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.77000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>174.8</v>
+        <v>174.69</v>
       </c>
       <c r="E10" s="10">
-        <v>164.66</v>
+        <v>164.64</v>
       </c>
       <c r="F10" s="10">
-        <v>174.66</v>
+        <v>174.64</v>
       </c>
       <c r="G10" s="10">
-        <v>165.16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>165.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>171.51</v>
+        <v>172.24</v>
       </c>
       <c r="E11" s="13">
-        <v>160.94</v>
+        <v>161.46</v>
       </c>
       <c r="F11" s="13">
-        <v>170.94</v>
+        <v>171.46</v>
       </c>
       <c r="G11" s="13">
-        <v>161.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>171.51</v>
+        <v>172.24</v>
       </c>
       <c r="E12" s="10">
-        <v>160.94</v>
+        <v>161.46</v>
       </c>
       <c r="F12" s="10">
-        <v>170.94</v>
+        <v>171.46</v>
       </c>
       <c r="G12" s="10">
-        <v>161.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>173.97</v>
+        <v>174.8</v>
       </c>
       <c r="E13" s="13">
-        <v>163.94</v>
+        <v>164.66</v>
       </c>
       <c r="F13" s="13">
-        <v>173.94</v>
+        <v>174.66</v>
       </c>
       <c r="G13" s="13">
-        <v>164.43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>165.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>178.16</v>
+        <v>178.03</v>
       </c>
       <c r="E17" s="10">
-        <v>167.49</v>
+        <v>167.54</v>
       </c>
       <c r="F17" s="10">
-        <v>177.49</v>
+        <v>177.54</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>177.35</v>
+        <v>178.16</v>
       </c>
       <c r="E18" s="13">
-        <v>166.8</v>
+        <v>167.49</v>
       </c>
       <c r="F18" s="13">
-        <v>176.8</v>
+        <v>177.49</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>173.59</v>
+        <v>173.63</v>
       </c>
       <c r="E22" s="10">
-        <v>163.74</v>
+        <v>163.72</v>
       </c>
       <c r="F22" s="10">
-        <v>173.34</v>
+        <v>173.32</v>
       </c>
       <c r="G22" s="10">
-        <v>165.03</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>165.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>179.58</v>
+        <v>179.48</v>
       </c>
       <c r="E23" s="13">
-        <v>168.27</v>
+        <v>168.25</v>
       </c>
       <c r="F23" s="13">
-        <v>178.27</v>
+        <v>178.25</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>179.38</v>
+        <v>179.27</v>
       </c>
       <c r="E24" s="10">
-        <v>168.5</v>
+        <v>168.49</v>
       </c>
       <c r="F24" s="10">
-        <v>178.5</v>
+        <v>178.49</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>180.21</v>
+        <v>180.1</v>
       </c>
       <c r="E25" s="13">
-        <v>167.91</v>
+        <v>167.9</v>
       </c>
       <c r="F25" s="13">
-        <v>177.91</v>
+        <v>177.9</v>
       </c>
       <c r="G25" s="13">
-        <v>167.95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>167.94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>178.91</v>
+        <v>178.8</v>
       </c>
       <c r="E26" s="10">
-        <v>169.48</v>
+        <v>169.47</v>
       </c>
       <c r="F26" s="10">
-        <v>179.48</v>
+        <v>179.47</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>172.75</v>
+        <v>173.59</v>
       </c>
       <c r="E27" s="13">
-        <v>163.03</v>
+        <v>163.74</v>
       </c>
       <c r="F27" s="13">
-        <v>172.63</v>
+        <v>173.34</v>
       </c>
       <c r="G27" s="13">
-        <v>164.31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>165.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>178.75</v>
+        <v>179.58</v>
       </c>
       <c r="E28" s="22">
-        <v>167.66</v>
+        <v>168.27</v>
       </c>
       <c r="F28" s="22">
-        <v>177.66</v>
+        <v>178.27</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>178.55</v>
+        <v>179.38</v>
       </c>
       <c r="E29" s="13">
-        <v>167.88</v>
+        <v>168.5</v>
       </c>
       <c r="F29" s="13">
-        <v>177.88</v>
+        <v>178.5</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>179.38</v>
+        <v>180.21</v>
       </c>
       <c r="E30" s="22">
-        <v>167.28</v>
+        <v>167.91</v>
       </c>
       <c r="F30" s="22">
-        <v>177.28</v>
+        <v>177.91</v>
       </c>
       <c r="G30" s="22">
-        <v>167.32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>167.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>178.09</v>
+        <v>178.91</v>
       </c>
       <c r="E31" s="13">
-        <v>168.85</v>
+        <v>169.48</v>
       </c>
       <c r="F31" s="13">
-        <v>178.85</v>
+        <v>179.48</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>173.16</v>
+        <v>173.05</v>
       </c>
       <c r="E35" s="10">
-        <v>161.76</v>
+        <v>161.75</v>
       </c>
       <c r="F35" s="10">
-        <v>170.76</v>
+        <v>170.75</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>172.44</v>
+        <v>173.16</v>
       </c>
       <c r="E36" s="13">
-        <v>161.15</v>
+        <v>161.76</v>
       </c>
       <c r="F36" s="13">
-        <v>170.15</v>
+        <v>170.76</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>178.77</v>
+        <v>178.68</v>
       </c>
       <c r="E40" s="10">
-        <v>167.35</v>
+        <v>167.44</v>
       </c>
       <c r="F40" s="10">
-        <v>177.35</v>
+        <v>177.44</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>178.48</v>
+        <v>178.38</v>
       </c>
       <c r="E41" s="13">
-        <v>167.77</v>
+        <v>167.86</v>
       </c>
       <c r="F41" s="13">
-        <v>177.77</v>
+        <v>177.86</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>177.92</v>
+        <v>178.77</v>
       </c>
       <c r="E42" s="10">
-        <v>166.63</v>
+        <v>167.35</v>
       </c>
       <c r="F42" s="10">
-        <v>176.63</v>
+        <v>177.35</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>177.63</v>
+        <v>178.48</v>
       </c>
       <c r="E43" s="13">
-        <v>167.05</v>
+        <v>167.77</v>
       </c>
       <c r="F43" s="13">
-        <v>177.05</v>
+        <v>177.77</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>172.16</v>
+        <v>172.96</v>
       </c>
       <c r="E47" s="10">
-        <v>162.59</v>
+        <v>162.86000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>172.59</v>
+        <v>172.86</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>172.14</v>
+        <v>172.94</v>
       </c>
       <c r="E48" s="13">
-        <v>162.75</v>
+        <v>163.03</v>
       </c>
       <c r="F48" s="13">
-        <v>172.75</v>
+        <v>173.03</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>171.39</v>
+        <v>172.16</v>
       </c>
       <c r="E49" s="10">
-        <v>162.29</v>
+        <v>162.59</v>
       </c>
       <c r="F49" s="10">
-        <v>172.29</v>
+        <v>172.59</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>171.38</v>
+        <v>172.14</v>
       </c>
       <c r="E50" s="13">
-        <v>162.46</v>
+        <v>162.75</v>
       </c>
       <c r="F50" s="13">
-        <v>172.46</v>
+        <v>172.75</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>188.88</v>
+        <v>188.76</v>
       </c>
       <c r="E54" s="10">
-        <v>177.86</v>
+        <v>177.92</v>
       </c>
       <c r="F54" s="10">
-        <v>187.86</v>
+        <v>187.92</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>176.56</v>
+        <v>176.45</v>
       </c>
       <c r="E55" s="13">
-        <v>174.95</v>
+        <v>174.91</v>
       </c>
       <c r="F55" s="13">
-        <v>184.95</v>
+        <v>184.91</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>179.06</v>
+        <v>178.95</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>178.59</v>
+        <v>178.46</v>
       </c>
       <c r="E57" s="13">
-        <v>169.22</v>
+        <v>169.18</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>174.5</v>
+        <v>174.37</v>
       </c>
       <c r="E58" s="10">
-        <v>165.27</v>
+        <v>165.23</v>
       </c>
       <c r="F58" s="10">
-        <v>175.27</v>
+        <v>175.23</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>181.13</v>
+        <v>181</v>
       </c>
       <c r="E59" s="13">
-        <v>175.9</v>
+        <v>175.93</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>188.06</v>
+        <v>188.88</v>
       </c>
       <c r="E60" s="10">
-        <v>177.14</v>
+        <v>177.86</v>
       </c>
       <c r="F60" s="10">
-        <v>187.14</v>
+        <v>187.86</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>175.73</v>
+        <v>176.56</v>
       </c>
       <c r="E61" s="13">
-        <v>174.36</v>
+        <v>174.95</v>
       </c>
       <c r="F61" s="13">
-        <v>184.36</v>
+        <v>184.95</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>178.22</v>
+        <v>179.06</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>177.79</v>
+        <v>178.59</v>
       </c>
       <c r="E63" s="13">
-        <v>168.63</v>
+        <v>169.22</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>173.7</v>
+        <v>174.5</v>
       </c>
       <c r="E64" s="10">
-        <v>164.68</v>
+        <v>165.27</v>
       </c>
       <c r="F64" s="10">
-        <v>174.68</v>
+        <v>175.27</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>180.33</v>
+        <v>181.13</v>
       </c>
       <c r="E65" s="13">
-        <v>175.24</v>
+        <v>175.9</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -2115,15 +2115,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -2132,6 +2123,15 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2155,14 +2155,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2180,6 +2172,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Mon Nov 17 02:54:01 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D09B11FF-C9F0-4B6F-BCED-D5E6606659B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D218C491-B70C-4810-BF2D-CD4C6A5F7912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>172.4</v>
+        <v>171.98</v>
       </c>
       <c r="E8" s="10">
-        <v>161.6</v>
+        <v>161.81</v>
       </c>
       <c r="F8" s="10">
-        <v>171.6</v>
+        <v>171.81</v>
       </c>
       <c r="G8" s="10">
-        <v>161.77000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.97999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>172.4</v>
+        <v>171.98</v>
       </c>
       <c r="E9" s="13">
-        <v>161.6</v>
+        <v>161.81</v>
       </c>
       <c r="F9" s="13">
-        <v>171.6</v>
+        <v>171.81</v>
       </c>
       <c r="G9" s="13">
-        <v>161.77000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.97999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>174.69</v>
+        <v>174.07</v>
       </c>
       <c r="E10" s="10">
-        <v>164.64</v>
+        <v>164.86</v>
       </c>
       <c r="F10" s="10">
-        <v>174.64</v>
+        <v>174.86</v>
       </c>
       <c r="G10" s="10">
-        <v>165.14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>165.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>172.24</v>
+        <v>172.4</v>
       </c>
       <c r="E11" s="13">
-        <v>161.46</v>
+        <v>161.6</v>
       </c>
       <c r="F11" s="13">
-        <v>171.46</v>
+        <v>171.6</v>
       </c>
       <c r="G11" s="13">
-        <v>161.63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.77000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>172.24</v>
+        <v>172.4</v>
       </c>
       <c r="E12" s="10">
-        <v>161.46</v>
+        <v>161.6</v>
       </c>
       <c r="F12" s="10">
-        <v>171.46</v>
+        <v>171.6</v>
       </c>
       <c r="G12" s="10">
-        <v>161.63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.77000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>174.8</v>
+        <v>174.69</v>
       </c>
       <c r="E13" s="13">
-        <v>164.66</v>
+        <v>164.64</v>
       </c>
       <c r="F13" s="13">
-        <v>174.66</v>
+        <v>174.64</v>
       </c>
       <c r="G13" s="13">
-        <v>165.16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>165.14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>178.03</v>
+        <v>177.4</v>
       </c>
       <c r="E17" s="10">
-        <v>167.54</v>
+        <v>167.62</v>
       </c>
       <c r="F17" s="10">
-        <v>177.54</v>
+        <v>177.62</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>178.16</v>
+        <v>178.03</v>
       </c>
       <c r="E18" s="13">
-        <v>167.49</v>
+        <v>167.54</v>
       </c>
       <c r="F18" s="13">
-        <v>177.49</v>
+        <v>177.54</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>173.63</v>
+        <v>172.99</v>
       </c>
       <c r="E22" s="10">
-        <v>163.72</v>
+        <v>163.83000000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>173.32</v>
+        <v>173.43</v>
       </c>
       <c r="G22" s="10">
-        <v>165.01</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>165.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>179.48</v>
+        <v>178.85</v>
       </c>
       <c r="E23" s="13">
-        <v>168.25</v>
+        <v>168.36</v>
       </c>
       <c r="F23" s="13">
-        <v>178.25</v>
+        <v>178.36</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>179.27</v>
+        <v>178.65</v>
       </c>
       <c r="E24" s="10">
-        <v>168.49</v>
+        <v>168.6</v>
       </c>
       <c r="F24" s="10">
-        <v>178.49</v>
+        <v>178.6</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>180.1</v>
+        <v>179.47</v>
       </c>
       <c r="E25" s="13">
-        <v>167.9</v>
+        <v>168.01</v>
       </c>
       <c r="F25" s="13">
-        <v>177.9</v>
+        <v>178.01</v>
       </c>
       <c r="G25" s="13">
-        <v>167.94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>168.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>178.8</v>
+        <v>178.17</v>
       </c>
       <c r="E26" s="10">
-        <v>169.47</v>
+        <v>169.58</v>
       </c>
       <c r="F26" s="10">
-        <v>179.47</v>
+        <v>179.58</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>173.59</v>
+        <v>173.63</v>
       </c>
       <c r="E27" s="13">
-        <v>163.74</v>
+        <v>163.72</v>
       </c>
       <c r="F27" s="13">
-        <v>173.34</v>
+        <v>173.32</v>
       </c>
       <c r="G27" s="13">
-        <v>165.03</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>165.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>179.58</v>
+        <v>179.48</v>
       </c>
       <c r="E28" s="22">
-        <v>168.27</v>
+        <v>168.25</v>
       </c>
       <c r="F28" s="22">
-        <v>178.27</v>
+        <v>178.25</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>179.38</v>
+        <v>179.27</v>
       </c>
       <c r="E29" s="13">
-        <v>168.5</v>
+        <v>168.49</v>
       </c>
       <c r="F29" s="13">
-        <v>178.5</v>
+        <v>178.49</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>180.21</v>
+        <v>180.1</v>
       </c>
       <c r="E30" s="22">
-        <v>167.91</v>
+        <v>167.9</v>
       </c>
       <c r="F30" s="22">
-        <v>177.91</v>
+        <v>177.9</v>
       </c>
       <c r="G30" s="22">
-        <v>167.95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>167.94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>178.91</v>
+        <v>178.8</v>
       </c>
       <c r="E31" s="13">
-        <v>169.48</v>
+        <v>169.47</v>
       </c>
       <c r="F31" s="13">
-        <v>179.48</v>
+        <v>179.47</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>173.05</v>
+        <v>172.54</v>
       </c>
       <c r="E35" s="10">
-        <v>161.75</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>170.75</v>
+        <v>170.86</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>173.16</v>
+        <v>173.05</v>
       </c>
       <c r="E36" s="13">
-        <v>161.76</v>
+        <v>161.75</v>
       </c>
       <c r="F36" s="13">
-        <v>170.76</v>
+        <v>170.75</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>178.68</v>
+        <v>178.05</v>
       </c>
       <c r="E40" s="10">
-        <v>167.44</v>
+        <v>167.54</v>
       </c>
       <c r="F40" s="10">
-        <v>177.44</v>
+        <v>177.54</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>178.38</v>
+        <v>177.75</v>
       </c>
       <c r="E41" s="13">
-        <v>167.86</v>
+        <v>167.95</v>
       </c>
       <c r="F41" s="13">
-        <v>177.86</v>
+        <v>177.95</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>178.77</v>
+        <v>178.68</v>
       </c>
       <c r="E42" s="10">
-        <v>167.35</v>
+        <v>167.44</v>
       </c>
       <c r="F42" s="10">
-        <v>177.35</v>
+        <v>177.44</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>178.48</v>
+        <v>178.38</v>
       </c>
       <c r="E43" s="13">
-        <v>167.77</v>
+        <v>167.86</v>
       </c>
       <c r="F43" s="13">
-        <v>177.77</v>
+        <v>177.86</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>172.96</v>
+        <v>173.34</v>
       </c>
       <c r="E47" s="10">
-        <v>162.86000000000001</v>
+        <v>163.30000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>172.86</v>
+        <v>173.3</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>172.94</v>
+        <v>173.31</v>
       </c>
       <c r="E48" s="13">
-        <v>163.03</v>
+        <v>163.46</v>
       </c>
       <c r="F48" s="13">
-        <v>173.03</v>
+        <v>173.46</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>172.16</v>
+        <v>172.96</v>
       </c>
       <c r="E49" s="10">
-        <v>162.59</v>
+        <v>162.86000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>172.59</v>
+        <v>172.86</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>172.14</v>
+        <v>172.94</v>
       </c>
       <c r="E50" s="13">
-        <v>162.75</v>
+        <v>163.03</v>
       </c>
       <c r="F50" s="13">
-        <v>172.75</v>
+        <v>173.03</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>188.76</v>
+        <v>188.11</v>
       </c>
       <c r="E54" s="10">
-        <v>177.92</v>
+        <v>178.04</v>
       </c>
       <c r="F54" s="10">
-        <v>187.92</v>
+        <v>188.05</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>176.45</v>
+        <v>175.82</v>
       </c>
       <c r="E55" s="13">
-        <v>174.91</v>
+        <v>175.02</v>
       </c>
       <c r="F55" s="13">
-        <v>184.91</v>
+        <v>185.02</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>178.95</v>
+        <v>178.32</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>178.46</v>
+        <v>177.83</v>
       </c>
       <c r="E57" s="13">
-        <v>169.18</v>
+        <v>169.29</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>174.37</v>
+        <v>173.74</v>
       </c>
       <c r="E58" s="10">
-        <v>165.23</v>
+        <v>165.34</v>
       </c>
       <c r="F58" s="10">
-        <v>175.23</v>
+        <v>175.34</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>181</v>
+        <v>180.37</v>
       </c>
       <c r="E59" s="13">
-        <v>175.93</v>
+        <v>176.05</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>188.88</v>
+        <v>188.76</v>
       </c>
       <c r="E60" s="10">
-        <v>177.86</v>
+        <v>177.92</v>
       </c>
       <c r="F60" s="10">
-        <v>187.86</v>
+        <v>187.92</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>176.56</v>
+        <v>176.45</v>
       </c>
       <c r="E61" s="13">
-        <v>174.95</v>
+        <v>174.91</v>
       </c>
       <c r="F61" s="13">
-        <v>184.95</v>
+        <v>184.91</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>179.06</v>
+        <v>178.95</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>178.59</v>
+        <v>178.46</v>
       </c>
       <c r="E63" s="13">
-        <v>169.22</v>
+        <v>169.18</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>174.5</v>
+        <v>174.37</v>
       </c>
       <c r="E64" s="10">
-        <v>165.27</v>
+        <v>165.23</v>
       </c>
       <c r="F64" s="10">
-        <v>175.27</v>
+        <v>175.23</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>181.13</v>
+        <v>181</v>
       </c>
       <c r="E65" s="13">
-        <v>175.9</v>
+        <v>175.93</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,17 +2125,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,6 +2135,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2154,24 +2172,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Tue Nov 18 02:50:45 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D218C491-B70C-4810-BF2D-CD4C6A5F7912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{7EBBE6C8-F999-4BAF-9F03-C09F0133E9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>171.98</v>
+        <v>171.9</v>
       </c>
       <c r="E8" s="10">
-        <v>161.81</v>
+        <v>161.93</v>
       </c>
       <c r="F8" s="10">
-        <v>171.81</v>
+        <v>171.93</v>
       </c>
       <c r="G8" s="10">
-        <v>161.97999999999999</v>
+        <v>162.09</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>171.98</v>
+        <v>171.9</v>
       </c>
       <c r="E9" s="13">
-        <v>161.81</v>
+        <v>161.93</v>
       </c>
       <c r="F9" s="13">
-        <v>171.81</v>
+        <v>171.93</v>
       </c>
       <c r="G9" s="13">
-        <v>161.97999999999999</v>
+        <v>162.09</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>174.07</v>
+        <v>174</v>
       </c>
       <c r="E10" s="10">
-        <v>164.86</v>
+        <v>164.99</v>
       </c>
       <c r="F10" s="10">
-        <v>174.86</v>
+        <v>174.99</v>
       </c>
       <c r="G10" s="10">
-        <v>165.36</v>
+        <v>165.49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>172.4</v>
+        <v>171.98</v>
       </c>
       <c r="E11" s="13">
-        <v>161.6</v>
+        <v>161.81</v>
       </c>
       <c r="F11" s="13">
-        <v>171.6</v>
+        <v>171.81</v>
       </c>
       <c r="G11" s="13">
-        <v>161.77000000000001</v>
+        <v>161.97999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>172.4</v>
+        <v>171.98</v>
       </c>
       <c r="E12" s="10">
-        <v>161.6</v>
+        <v>161.81</v>
       </c>
       <c r="F12" s="10">
-        <v>171.6</v>
+        <v>171.81</v>
       </c>
       <c r="G12" s="10">
-        <v>161.77000000000001</v>
+        <v>161.97999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>174.69</v>
+        <v>174.07</v>
       </c>
       <c r="E13" s="13">
-        <v>164.64</v>
+        <v>164.86</v>
       </c>
       <c r="F13" s="13">
-        <v>174.64</v>
+        <v>174.86</v>
       </c>
       <c r="G13" s="13">
-        <v>165.14</v>
+        <v>165.36</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>177.4</v>
+        <v>177.33</v>
       </c>
       <c r="E17" s="10">
-        <v>167.62</v>
+        <v>167.72</v>
       </c>
       <c r="F17" s="10">
-        <v>177.62</v>
+        <v>177.72</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>178.03</v>
+        <v>177.4</v>
       </c>
       <c r="E18" s="13">
-        <v>167.54</v>
+        <v>167.62</v>
       </c>
       <c r="F18" s="13">
-        <v>177.54</v>
+        <v>177.62</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>172.99</v>
+        <v>172.92</v>
       </c>
       <c r="E22" s="10">
-        <v>163.83000000000001</v>
+        <v>163.96</v>
       </c>
       <c r="F22" s="10">
-        <v>173.43</v>
+        <v>173.56</v>
       </c>
       <c r="G22" s="10">
-        <v>165.12</v>
+        <v>165.24</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>178.85</v>
+        <v>178.78</v>
       </c>
       <c r="E23" s="13">
-        <v>168.36</v>
+        <v>168.49</v>
       </c>
       <c r="F23" s="13">
-        <v>178.36</v>
+        <v>178.49</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>178.65</v>
+        <v>178.58</v>
       </c>
       <c r="E24" s="10">
-        <v>168.6</v>
+        <v>168.73</v>
       </c>
       <c r="F24" s="10">
-        <v>178.6</v>
+        <v>178.73</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>179.47</v>
+        <v>179.41</v>
       </c>
       <c r="E25" s="13">
-        <v>168.01</v>
+        <v>168.14</v>
       </c>
       <c r="F25" s="13">
-        <v>178.01</v>
+        <v>178.14</v>
       </c>
       <c r="G25" s="13">
-        <v>168.05</v>
+        <v>168.18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>178.17</v>
+        <v>178.1</v>
       </c>
       <c r="E26" s="10">
-        <v>169.58</v>
+        <v>169.72</v>
       </c>
       <c r="F26" s="10">
-        <v>179.58</v>
+        <v>179.72</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>173.63</v>
+        <v>172.99</v>
       </c>
       <c r="E27" s="13">
-        <v>163.72</v>
+        <v>163.83000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>173.32</v>
+        <v>173.43</v>
       </c>
       <c r="G27" s="13">
-        <v>165.01</v>
+        <v>165.12</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>179.48</v>
+        <v>178.85</v>
       </c>
       <c r="E28" s="22">
-        <v>168.25</v>
+        <v>168.36</v>
       </c>
       <c r="F28" s="22">
-        <v>178.25</v>
+        <v>178.36</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>179.27</v>
+        <v>178.65</v>
       </c>
       <c r="E29" s="13">
-        <v>168.49</v>
+        <v>168.6</v>
       </c>
       <c r="F29" s="13">
-        <v>178.49</v>
+        <v>178.6</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>180.1</v>
+        <v>179.47</v>
       </c>
       <c r="E30" s="22">
-        <v>167.9</v>
+        <v>168.01</v>
       </c>
       <c r="F30" s="22">
-        <v>177.9</v>
+        <v>178.01</v>
       </c>
       <c r="G30" s="22">
-        <v>167.94</v>
+        <v>168.05</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>178.8</v>
+        <v>178.17</v>
       </c>
       <c r="E31" s="13">
-        <v>169.47</v>
+        <v>169.58</v>
       </c>
       <c r="F31" s="13">
-        <v>179.47</v>
+        <v>179.58</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>172.54</v>
+        <v>172.36</v>
       </c>
       <c r="E35" s="10">
-        <v>161.86000000000001</v>
+        <v>161.99</v>
       </c>
       <c r="F35" s="10">
-        <v>170.86</v>
+        <v>170.99</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>173.05</v>
+        <v>172.54</v>
       </c>
       <c r="E36" s="13">
-        <v>161.75</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>170.75</v>
+        <v>170.86</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>178.05</v>
+        <v>177.99</v>
       </c>
       <c r="E40" s="10">
-        <v>167.54</v>
+        <v>167.64</v>
       </c>
       <c r="F40" s="10">
-        <v>177.54</v>
+        <v>177.64</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>177.75</v>
+        <v>177.69</v>
       </c>
       <c r="E41" s="13">
-        <v>167.95</v>
+        <v>168.06</v>
       </c>
       <c r="F41" s="13">
-        <v>177.95</v>
+        <v>178.06</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>178.68</v>
+        <v>178.05</v>
       </c>
       <c r="E42" s="10">
-        <v>167.44</v>
+        <v>167.54</v>
       </c>
       <c r="F42" s="10">
-        <v>177.44</v>
+        <v>177.54</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>178.38</v>
+        <v>177.75</v>
       </c>
       <c r="E43" s="13">
-        <v>167.86</v>
+        <v>167.95</v>
       </c>
       <c r="F43" s="13">
-        <v>177.86</v>
+        <v>177.95</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>173.34</v>
+        <v>172.7</v>
       </c>
       <c r="E47" s="10">
-        <v>163.30000000000001</v>
+        <v>163.41999999999999</v>
       </c>
       <c r="F47" s="10">
-        <v>173.3</v>
+        <v>173.42</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>173.31</v>
+        <v>172.66</v>
       </c>
       <c r="E48" s="13">
-        <v>163.46</v>
+        <v>163.58000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>173.46</v>
+        <v>173.58</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>172.96</v>
+        <v>173.34</v>
       </c>
       <c r="E49" s="10">
-        <v>162.86000000000001</v>
+        <v>163.30000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>172.86</v>
+        <v>173.3</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>172.94</v>
+        <v>173.31</v>
       </c>
       <c r="E50" s="13">
-        <v>163.03</v>
+        <v>163.46</v>
       </c>
       <c r="F50" s="13">
-        <v>173.03</v>
+        <v>173.46</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>188.11</v>
+        <v>188.05</v>
       </c>
       <c r="E54" s="10">
-        <v>178.04</v>
+        <v>178.19</v>
       </c>
       <c r="F54" s="10">
-        <v>188.05</v>
+        <v>188.19</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>175.82</v>
+        <v>175.75</v>
       </c>
       <c r="E55" s="13">
-        <v>175.02</v>
+        <v>175.14</v>
       </c>
       <c r="F55" s="13">
-        <v>185.02</v>
+        <v>185.14</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>178.32</v>
+        <v>178.26</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>177.83</v>
+        <v>177.76</v>
       </c>
       <c r="E57" s="13">
-        <v>169.29</v>
+        <v>169.41</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>173.74</v>
+        <v>173.67</v>
       </c>
       <c r="E58" s="10">
-        <v>165.34</v>
+        <v>165.46</v>
       </c>
       <c r="F58" s="10">
-        <v>175.34</v>
+        <v>175.46</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>180.37</v>
+        <v>180.29</v>
       </c>
       <c r="E59" s="13">
-        <v>176.05</v>
+        <v>176.19</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>188.76</v>
+        <v>188.11</v>
       </c>
       <c r="E60" s="10">
-        <v>177.92</v>
+        <v>178.04</v>
       </c>
       <c r="F60" s="10">
-        <v>187.92</v>
+        <v>188.05</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>176.45</v>
+        <v>175.82</v>
       </c>
       <c r="E61" s="13">
-        <v>174.91</v>
+        <v>175.02</v>
       </c>
       <c r="F61" s="13">
-        <v>184.91</v>
+        <v>185.02</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>178.95</v>
+        <v>178.32</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>178.46</v>
+        <v>177.83</v>
       </c>
       <c r="E63" s="13">
-        <v>169.18</v>
+        <v>169.29</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>174.37</v>
+        <v>173.74</v>
       </c>
       <c r="E64" s="10">
-        <v>165.23</v>
+        <v>165.34</v>
       </c>
       <c r="F64" s="10">
-        <v>175.23</v>
+        <v>175.34</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45976</v>
+        <v>45979</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>181</v>
+        <v>180.37</v>
       </c>
       <c r="E65" s="13">
-        <v>175.93</v>
+        <v>176.05</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,17 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2125,6 +2114,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,24 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2172,6 +2154,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Wed Nov 19 02:51:11 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{7EBBE6C8-F999-4BAF-9F03-C09F0133E9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{F8125992-F6D7-45D7-9BB3-8C1E9675CD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>171.9</v>
+        <v>172.2</v>
       </c>
       <c r="E8" s="10">
-        <v>161.93</v>
+        <v>162.07</v>
       </c>
       <c r="F8" s="10">
-        <v>171.93</v>
+        <v>172.07</v>
       </c>
       <c r="G8" s="10">
-        <v>162.09</v>
+        <v>162.22999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>171.9</v>
+        <v>172.2</v>
       </c>
       <c r="E9" s="13">
-        <v>161.93</v>
+        <v>162.07</v>
       </c>
       <c r="F9" s="13">
-        <v>171.93</v>
+        <v>172.07</v>
       </c>
       <c r="G9" s="13">
-        <v>162.09</v>
+        <v>162.22999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>174</v>
+        <v>174.24</v>
       </c>
       <c r="E10" s="10">
-        <v>164.99</v>
+        <v>165.06</v>
       </c>
       <c r="F10" s="10">
-        <v>174.99</v>
+        <v>175.06</v>
       </c>
       <c r="G10" s="10">
-        <v>165.49</v>
+        <v>165.55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>171.98</v>
+        <v>171.9</v>
       </c>
       <c r="E11" s="13">
-        <v>161.81</v>
+        <v>161.93</v>
       </c>
       <c r="F11" s="13">
-        <v>171.81</v>
+        <v>171.93</v>
       </c>
       <c r="G11" s="13">
-        <v>161.97999999999999</v>
+        <v>162.09</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>171.98</v>
+        <v>171.9</v>
       </c>
       <c r="E12" s="10">
-        <v>161.81</v>
+        <v>161.93</v>
       </c>
       <c r="F12" s="10">
-        <v>171.81</v>
+        <v>171.93</v>
       </c>
       <c r="G12" s="10">
-        <v>161.97999999999999</v>
+        <v>162.09</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>174.07</v>
+        <v>174</v>
       </c>
       <c r="E13" s="13">
-        <v>164.86</v>
+        <v>164.99</v>
       </c>
       <c r="F13" s="13">
-        <v>174.86</v>
+        <v>174.99</v>
       </c>
       <c r="G13" s="13">
-        <v>165.36</v>
+        <v>165.49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>177.33</v>
+        <v>177.55</v>
       </c>
       <c r="E17" s="10">
-        <v>167.72</v>
+        <v>167.83</v>
       </c>
       <c r="F17" s="10">
-        <v>177.72</v>
+        <v>177.83</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>177.4</v>
+        <v>177.33</v>
       </c>
       <c r="E18" s="13">
-        <v>167.62</v>
+        <v>167.72</v>
       </c>
       <c r="F18" s="13">
-        <v>177.62</v>
+        <v>177.72</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>172.92</v>
+        <v>173.11</v>
       </c>
       <c r="E22" s="10">
-        <v>163.96</v>
+        <v>164.01</v>
       </c>
       <c r="F22" s="10">
-        <v>173.56</v>
+        <v>173.61</v>
       </c>
       <c r="G22" s="10">
-        <v>165.24</v>
+        <v>165.3</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>178.78</v>
+        <v>179.02</v>
       </c>
       <c r="E23" s="13">
-        <v>168.49</v>
+        <v>168.55</v>
       </c>
       <c r="F23" s="13">
-        <v>178.49</v>
+        <v>178.55</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>178.58</v>
+        <v>178.82</v>
       </c>
       <c r="E24" s="10">
-        <v>168.73</v>
+        <v>168.8</v>
       </c>
       <c r="F24" s="10">
-        <v>178.73</v>
+        <v>178.8</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>179.41</v>
+        <v>179.64</v>
       </c>
       <c r="E25" s="13">
-        <v>168.14</v>
+        <v>168.21</v>
       </c>
       <c r="F25" s="13">
-        <v>178.14</v>
+        <v>178.21</v>
       </c>
       <c r="G25" s="13">
-        <v>168.18</v>
+        <v>168.25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>178.1</v>
+        <v>178.34</v>
       </c>
       <c r="E26" s="10">
-        <v>169.72</v>
+        <v>169.78</v>
       </c>
       <c r="F26" s="10">
-        <v>179.72</v>
+        <v>179.78</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>172.99</v>
+        <v>172.92</v>
       </c>
       <c r="E27" s="13">
-        <v>163.83000000000001</v>
+        <v>163.96</v>
       </c>
       <c r="F27" s="13">
-        <v>173.43</v>
+        <v>173.56</v>
       </c>
       <c r="G27" s="13">
-        <v>165.12</v>
+        <v>165.24</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>178.85</v>
+        <v>178.78</v>
       </c>
       <c r="E28" s="22">
-        <v>168.36</v>
+        <v>168.49</v>
       </c>
       <c r="F28" s="22">
-        <v>178.36</v>
+        <v>178.49</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>178.65</v>
+        <v>178.58</v>
       </c>
       <c r="E29" s="13">
-        <v>168.6</v>
+        <v>168.73</v>
       </c>
       <c r="F29" s="13">
-        <v>178.6</v>
+        <v>178.73</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>179.47</v>
+        <v>179.41</v>
       </c>
       <c r="E30" s="22">
-        <v>168.01</v>
+        <v>168.14</v>
       </c>
       <c r="F30" s="22">
-        <v>178.01</v>
+        <v>178.14</v>
       </c>
       <c r="G30" s="22">
-        <v>168.05</v>
+        <v>168.18</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>178.17</v>
+        <v>178.1</v>
       </c>
       <c r="E31" s="13">
-        <v>169.58</v>
+        <v>169.72</v>
       </c>
       <c r="F31" s="13">
-        <v>179.58</v>
+        <v>179.72</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>172.36</v>
+        <v>172.49</v>
       </c>
       <c r="E35" s="10">
-        <v>161.99</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>170.99</v>
+        <v>171.05</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>172.54</v>
+        <v>172.36</v>
       </c>
       <c r="E36" s="13">
-        <v>161.86000000000001</v>
+        <v>161.99</v>
       </c>
       <c r="F36" s="13">
-        <v>170.86</v>
+        <v>170.99</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>177.99</v>
+        <v>178.24</v>
       </c>
       <c r="E40" s="10">
-        <v>167.64</v>
+        <v>167.76</v>
       </c>
       <c r="F40" s="10">
-        <v>177.64</v>
+        <v>177.76</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>177.69</v>
+        <v>177.94</v>
       </c>
       <c r="E41" s="13">
-        <v>168.06</v>
+        <v>168.18</v>
       </c>
       <c r="F41" s="13">
-        <v>178.06</v>
+        <v>178.18</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>178.05</v>
+        <v>177.99</v>
       </c>
       <c r="E42" s="10">
-        <v>167.54</v>
+        <v>167.64</v>
       </c>
       <c r="F42" s="10">
-        <v>177.54</v>
+        <v>177.64</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>177.75</v>
+        <v>177.69</v>
       </c>
       <c r="E43" s="13">
-        <v>167.95</v>
+        <v>168.06</v>
       </c>
       <c r="F43" s="13">
-        <v>177.95</v>
+        <v>178.06</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>172.7</v>
+        <v>171.88</v>
       </c>
       <c r="E47" s="10">
-        <v>163.41999999999999</v>
+        <v>163.43</v>
       </c>
       <c r="F47" s="10">
-        <v>173.42</v>
+        <v>173.43</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>172.66</v>
+        <v>171.84</v>
       </c>
       <c r="E48" s="13">
-        <v>163.58000000000001</v>
+        <v>163.59</v>
       </c>
       <c r="F48" s="13">
-        <v>173.58</v>
+        <v>173.59</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>173.34</v>
+        <v>172.7</v>
       </c>
       <c r="E49" s="10">
-        <v>163.30000000000001</v>
+        <v>163.41999999999999</v>
       </c>
       <c r="F49" s="10">
-        <v>173.3</v>
+        <v>173.42</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>173.31</v>
+        <v>172.66</v>
       </c>
       <c r="E50" s="13">
-        <v>163.46</v>
+        <v>163.58000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>173.46</v>
+        <v>173.58</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>188.05</v>
+        <v>188.29</v>
       </c>
       <c r="E54" s="10">
-        <v>178.19</v>
+        <v>178.3</v>
       </c>
       <c r="F54" s="10">
-        <v>188.19</v>
+        <v>188.3</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>175.75</v>
+        <v>175.99</v>
       </c>
       <c r="E55" s="13">
-        <v>175.14</v>
+        <v>175.08</v>
       </c>
       <c r="F55" s="13">
-        <v>185.14</v>
+        <v>185.08</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>178.26</v>
+        <v>178.39</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>177.76</v>
+        <v>177.87</v>
       </c>
       <c r="E57" s="13">
-        <v>169.41</v>
+        <v>169.35</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>173.67</v>
+        <v>173.78</v>
       </c>
       <c r="E58" s="10">
-        <v>165.46</v>
+        <v>165.4</v>
       </c>
       <c r="F58" s="10">
-        <v>175.46</v>
+        <v>175.4</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>180.29</v>
+        <v>180.52</v>
       </c>
       <c r="E59" s="13">
-        <v>176.19</v>
+        <v>176.27</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>188.11</v>
+        <v>188.05</v>
       </c>
       <c r="E60" s="10">
-        <v>178.04</v>
+        <v>178.19</v>
       </c>
       <c r="F60" s="10">
-        <v>188.05</v>
+        <v>188.19</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>175.82</v>
+        <v>175.75</v>
       </c>
       <c r="E61" s="13">
-        <v>175.02</v>
+        <v>175.14</v>
       </c>
       <c r="F61" s="13">
-        <v>185.02</v>
+        <v>185.14</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>178.32</v>
+        <v>178.26</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>177.83</v>
+        <v>177.76</v>
       </c>
       <c r="E63" s="13">
-        <v>169.29</v>
+        <v>169.41</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>173.74</v>
+        <v>173.67</v>
       </c>
       <c r="E64" s="10">
-        <v>165.34</v>
+        <v>165.46</v>
       </c>
       <c r="F64" s="10">
-        <v>175.34</v>
+        <v>175.46</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>180.37</v>
+        <v>180.29</v>
       </c>
       <c r="E65" s="13">
-        <v>176.05</v>
+        <v>176.19</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,42 +2134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2161,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Thu Nov 20 02:49:29 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F8125992-F6D7-45D7-9BB3-8C1E9675CD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{A079AA28-2FF3-4A06-A7A7-054F7FD0ABD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentManualCount="12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>172.2</v>
+        <v>172.56</v>
       </c>
       <c r="E8" s="10">
-        <v>162.07</v>
+        <v>161.93</v>
       </c>
       <c r="F8" s="10">
-        <v>172.07</v>
+        <v>171.93</v>
       </c>
       <c r="G8" s="10">
-        <v>162.22999999999999</v>
+        <v>162.09</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>172.2</v>
+        <v>172.56</v>
       </c>
       <c r="E9" s="13">
-        <v>162.07</v>
+        <v>161.93</v>
       </c>
       <c r="F9" s="13">
-        <v>172.07</v>
+        <v>171.93</v>
       </c>
       <c r="G9" s="13">
-        <v>162.22999999999999</v>
+        <v>162.09</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>174.24</v>
+        <v>174.61</v>
       </c>
       <c r="E10" s="10">
-        <v>165.06</v>
+        <v>164.6</v>
       </c>
       <c r="F10" s="10">
-        <v>175.06</v>
+        <v>174.6</v>
       </c>
       <c r="G10" s="10">
-        <v>165.55</v>
+        <v>165.09</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>171.9</v>
+        <v>172.2</v>
       </c>
       <c r="E11" s="13">
-        <v>161.93</v>
+        <v>162.07</v>
       </c>
       <c r="F11" s="13">
-        <v>171.93</v>
+        <v>172.07</v>
       </c>
       <c r="G11" s="13">
-        <v>162.09</v>
+        <v>162.22999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>171.9</v>
+        <v>172.2</v>
       </c>
       <c r="E12" s="10">
-        <v>161.93</v>
+        <v>162.07</v>
       </c>
       <c r="F12" s="10">
-        <v>171.93</v>
+        <v>172.07</v>
       </c>
       <c r="G12" s="10">
-        <v>162.09</v>
+        <v>162.22999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>174</v>
+        <v>174.24</v>
       </c>
       <c r="E13" s="13">
-        <v>164.99</v>
+        <v>165.06</v>
       </c>
       <c r="F13" s="13">
-        <v>174.99</v>
+        <v>175.06</v>
       </c>
       <c r="G13" s="13">
-        <v>165.49</v>
+        <v>165.55</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>177.55</v>
+        <v>177.91</v>
       </c>
       <c r="E17" s="10">
-        <v>167.83</v>
+        <v>167.24</v>
       </c>
       <c r="F17" s="10">
-        <v>177.83</v>
+        <v>177.24</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>177.33</v>
+        <v>177.55</v>
       </c>
       <c r="E18" s="13">
-        <v>167.72</v>
+        <v>167.83</v>
       </c>
       <c r="F18" s="13">
-        <v>177.72</v>
+        <v>177.83</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>173.11</v>
+        <v>173.58</v>
       </c>
       <c r="E22" s="10">
-        <v>164.01</v>
+        <v>163.66999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>173.61</v>
+        <v>173.27</v>
       </c>
       <c r="G22" s="10">
-        <v>165.3</v>
+        <v>164.95</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>179.02</v>
+        <v>179.39</v>
       </c>
       <c r="E23" s="13">
-        <v>168.55</v>
+        <v>168.42</v>
       </c>
       <c r="F23" s="13">
-        <v>178.55</v>
+        <v>178.42</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>178.82</v>
+        <v>179.19</v>
       </c>
       <c r="E24" s="10">
-        <v>168.8</v>
+        <v>168.79</v>
       </c>
       <c r="F24" s="10">
-        <v>178.8</v>
+        <v>178.79</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>179.64</v>
+        <v>180.01</v>
       </c>
       <c r="E25" s="13">
-        <v>168.21</v>
+        <v>168.2</v>
       </c>
       <c r="F25" s="13">
-        <v>178.21</v>
+        <v>178.2</v>
       </c>
       <c r="G25" s="13">
-        <v>168.25</v>
+        <v>168.24</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>178.34</v>
+        <v>178.7</v>
       </c>
       <c r="E26" s="10">
-        <v>169.78</v>
+        <v>169.66</v>
       </c>
       <c r="F26" s="10">
-        <v>179.78</v>
+        <v>179.66</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>172.92</v>
+        <v>173.11</v>
       </c>
       <c r="E27" s="13">
-        <v>163.96</v>
+        <v>164.01</v>
       </c>
       <c r="F27" s="13">
-        <v>173.56</v>
+        <v>173.61</v>
       </c>
       <c r="G27" s="13">
-        <v>165.24</v>
+        <v>165.3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>178.78</v>
+        <v>179.02</v>
       </c>
       <c r="E28" s="22">
-        <v>168.49</v>
+        <v>168.55</v>
       </c>
       <c r="F28" s="22">
-        <v>178.49</v>
+        <v>178.55</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>178.58</v>
+        <v>178.82</v>
       </c>
       <c r="E29" s="13">
-        <v>168.73</v>
+        <v>168.8</v>
       </c>
       <c r="F29" s="13">
-        <v>178.73</v>
+        <v>178.8</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>179.41</v>
+        <v>179.64</v>
       </c>
       <c r="E30" s="22">
-        <v>168.14</v>
+        <v>168.21</v>
       </c>
       <c r="F30" s="22">
-        <v>178.14</v>
+        <v>178.21</v>
       </c>
       <c r="G30" s="22">
-        <v>168.18</v>
+        <v>168.25</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>178.1</v>
+        <v>178.34</v>
       </c>
       <c r="E31" s="13">
-        <v>169.72</v>
+        <v>169.78</v>
       </c>
       <c r="F31" s="13">
-        <v>179.72</v>
+        <v>179.78</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>172.49</v>
+        <v>172.85</v>
       </c>
       <c r="E35" s="10">
-        <v>162.05000000000001</v>
+        <v>161.59</v>
       </c>
       <c r="F35" s="10">
-        <v>171.05</v>
+        <v>170.59</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>172.36</v>
+        <v>172.49</v>
       </c>
       <c r="E36" s="13">
-        <v>161.99</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>170.99</v>
+        <v>171.05</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>178.24</v>
+        <v>178.62</v>
       </c>
       <c r="E40" s="10">
-        <v>167.76</v>
+        <v>167.2</v>
       </c>
       <c r="F40" s="10">
-        <v>177.76</v>
+        <v>177.2</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>177.94</v>
+        <v>178.32</v>
       </c>
       <c r="E41" s="13">
-        <v>168.18</v>
+        <v>167.62</v>
       </c>
       <c r="F41" s="13">
-        <v>178.18</v>
+        <v>177.62</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>177.99</v>
+        <v>178.24</v>
       </c>
       <c r="E42" s="10">
-        <v>167.64</v>
+        <v>167.76</v>
       </c>
       <c r="F42" s="10">
-        <v>177.64</v>
+        <v>177.76</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>177.69</v>
+        <v>177.94</v>
       </c>
       <c r="E43" s="13">
-        <v>168.06</v>
+        <v>168.18</v>
       </c>
       <c r="F43" s="13">
-        <v>178.06</v>
+        <v>178.18</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>171.88</v>
+        <v>172.33</v>
       </c>
       <c r="E47" s="10">
-        <v>163.43</v>
+        <v>163.27000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>173.43</v>
+        <v>173.27</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>171.84</v>
+        <v>172.29</v>
       </c>
       <c r="E48" s="13">
-        <v>163.59</v>
+        <v>163.43</v>
       </c>
       <c r="F48" s="13">
-        <v>173.59</v>
+        <v>173.43</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>172.7</v>
+        <v>171.88</v>
       </c>
       <c r="E49" s="10">
-        <v>163.41999999999999</v>
+        <v>163.43</v>
       </c>
       <c r="F49" s="10">
-        <v>173.42</v>
+        <v>173.43</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>172.66</v>
+        <v>171.84</v>
       </c>
       <c r="E50" s="13">
-        <v>163.58000000000001</v>
+        <v>163.59</v>
       </c>
       <c r="F50" s="13">
-        <v>173.58</v>
+        <v>173.59</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>188.29</v>
+        <v>188.66</v>
       </c>
       <c r="E54" s="10">
-        <v>178.3</v>
+        <v>177.89</v>
       </c>
       <c r="F54" s="10">
-        <v>188.3</v>
+        <v>187.89</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>175.99</v>
+        <v>176.36</v>
       </c>
       <c r="E55" s="13">
-        <v>175.08</v>
+        <v>174.62</v>
       </c>
       <c r="F55" s="13">
-        <v>185.08</v>
+        <v>184.62</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>178.39</v>
+        <v>178.76</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>177.87</v>
+        <v>178.23</v>
       </c>
       <c r="E57" s="13">
-        <v>169.35</v>
+        <v>168.88</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>173.78</v>
+        <v>174.14</v>
       </c>
       <c r="E58" s="10">
-        <v>165.4</v>
+        <v>164.94</v>
       </c>
       <c r="F58" s="10">
-        <v>175.4</v>
+        <v>174.94</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>180.52</v>
+        <v>180.87</v>
       </c>
       <c r="E59" s="13">
-        <v>176.27</v>
+        <v>175.84</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>188.05</v>
+        <v>188.29</v>
       </c>
       <c r="E60" s="10">
-        <v>178.19</v>
+        <v>178.3</v>
       </c>
       <c r="F60" s="10">
-        <v>188.19</v>
+        <v>188.3</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>175.75</v>
+        <v>175.99</v>
       </c>
       <c r="E61" s="13">
-        <v>175.14</v>
+        <v>175.08</v>
       </c>
       <c r="F61" s="13">
-        <v>185.14</v>
+        <v>185.08</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>178.26</v>
+        <v>178.39</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>177.76</v>
+        <v>177.87</v>
       </c>
       <c r="E63" s="13">
-        <v>169.41</v>
+        <v>169.35</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>173.67</v>
+        <v>173.78</v>
       </c>
       <c r="E64" s="10">
-        <v>165.46</v>
+        <v>165.4</v>
       </c>
       <c r="F64" s="10">
-        <v>175.46</v>
+        <v>175.4</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>180.29</v>
+        <v>180.52</v>
       </c>
       <c r="E65" s="13">
-        <v>176.19</v>
+        <v>176.27</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1872,6 +1863,15 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,14 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2156,6 +2148,14 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fri Nov 21 02:49:52 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{A079AA28-2FF3-4A06-A7A7-054F7FD0ABD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{9B2F28E4-79DA-4500-B24C-E3B3BC9371B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="12"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>172.56</v>
+        <v>173.3</v>
       </c>
       <c r="E8" s="10">
-        <v>161.93</v>
+        <v>161.74</v>
       </c>
       <c r="F8" s="10">
-        <v>171.93</v>
+        <v>171.74</v>
       </c>
       <c r="G8" s="10">
-        <v>162.09</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>172.56</v>
+        <v>173.3</v>
       </c>
       <c r="E9" s="13">
-        <v>161.93</v>
+        <v>161.74</v>
       </c>
       <c r="F9" s="13">
-        <v>171.93</v>
+        <v>171.74</v>
       </c>
       <c r="G9" s="13">
-        <v>162.09</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>174.61</v>
+        <v>175.43</v>
       </c>
       <c r="E10" s="10">
-        <v>164.6</v>
+        <v>164.39</v>
       </c>
       <c r="F10" s="10">
-        <v>174.6</v>
+        <v>174.39</v>
       </c>
       <c r="G10" s="10">
-        <v>165.09</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>172.2</v>
+        <v>172.56</v>
       </c>
       <c r="E11" s="13">
-        <v>162.07</v>
+        <v>161.93</v>
       </c>
       <c r="F11" s="13">
-        <v>172.07</v>
+        <v>171.93</v>
       </c>
       <c r="G11" s="13">
-        <v>162.22999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>162.09</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>172.2</v>
+        <v>172.56</v>
       </c>
       <c r="E12" s="10">
-        <v>162.07</v>
+        <v>161.93</v>
       </c>
       <c r="F12" s="10">
-        <v>172.07</v>
+        <v>171.93</v>
       </c>
       <c r="G12" s="10">
-        <v>162.22999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>162.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>174.24</v>
+        <v>174.61</v>
       </c>
       <c r="E13" s="13">
-        <v>165.06</v>
+        <v>164.6</v>
       </c>
       <c r="F13" s="13">
-        <v>175.06</v>
+        <v>174.6</v>
       </c>
       <c r="G13" s="13">
-        <v>165.55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>165.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>177.91</v>
+        <v>178.72</v>
       </c>
       <c r="E17" s="10">
-        <v>167.24</v>
+        <v>166.89</v>
       </c>
       <c r="F17" s="10">
-        <v>177.24</v>
+        <v>176.89</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>177.55</v>
+        <v>177.91</v>
       </c>
       <c r="E18" s="13">
-        <v>167.83</v>
+        <v>167.24</v>
       </c>
       <c r="F18" s="13">
-        <v>177.83</v>
+        <v>177.24</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>173.58</v>
+        <v>174.43</v>
       </c>
       <c r="E22" s="10">
-        <v>163.66999999999999</v>
+        <v>163.44</v>
       </c>
       <c r="F22" s="10">
-        <v>173.27</v>
+        <v>173.04</v>
       </c>
       <c r="G22" s="10">
-        <v>164.95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>179.39</v>
+        <v>180.22</v>
       </c>
       <c r="E23" s="13">
-        <v>168.42</v>
+        <v>168.2</v>
       </c>
       <c r="F23" s="13">
-        <v>178.42</v>
+        <v>178.2</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>179.19</v>
+        <v>180.01</v>
       </c>
       <c r="E24" s="10">
-        <v>168.79</v>
+        <v>168.58</v>
       </c>
       <c r="F24" s="10">
-        <v>178.79</v>
+        <v>178.58</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>180.01</v>
+        <v>180.83</v>
       </c>
       <c r="E25" s="13">
-        <v>168.2</v>
+        <v>167.99</v>
       </c>
       <c r="F25" s="13">
-        <v>178.2</v>
+        <v>177.99</v>
       </c>
       <c r="G25" s="13">
-        <v>168.24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>168.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>178.7</v>
+        <v>179.52</v>
       </c>
       <c r="E26" s="10">
-        <v>169.66</v>
+        <v>169.45</v>
       </c>
       <c r="F26" s="10">
-        <v>179.66</v>
+        <v>179.45</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>173.11</v>
+        <v>173.58</v>
       </c>
       <c r="E27" s="13">
-        <v>164.01</v>
+        <v>163.66999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>173.61</v>
+        <v>173.27</v>
       </c>
       <c r="G27" s="13">
-        <v>165.3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>179.02</v>
+        <v>179.39</v>
       </c>
       <c r="E28" s="22">
-        <v>168.55</v>
+        <v>168.42</v>
       </c>
       <c r="F28" s="22">
-        <v>178.55</v>
+        <v>178.42</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>178.82</v>
+        <v>179.19</v>
       </c>
       <c r="E29" s="13">
-        <v>168.8</v>
+        <v>168.79</v>
       </c>
       <c r="F29" s="13">
-        <v>178.8</v>
+        <v>178.79</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>179.64</v>
+        <v>180.01</v>
       </c>
       <c r="E30" s="22">
-        <v>168.21</v>
+        <v>168.2</v>
       </c>
       <c r="F30" s="22">
-        <v>178.21</v>
+        <v>178.2</v>
       </c>
       <c r="G30" s="22">
-        <v>168.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>168.24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>178.34</v>
+        <v>178.7</v>
       </c>
       <c r="E31" s="13">
-        <v>169.78</v>
+        <v>169.66</v>
       </c>
       <c r="F31" s="13">
-        <v>179.78</v>
+        <v>179.66</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>172.85</v>
+        <v>173.67</v>
       </c>
       <c r="E35" s="10">
-        <v>161.59</v>
+        <v>161.38</v>
       </c>
       <c r="F35" s="10">
-        <v>170.59</v>
+        <v>170.38</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>172.49</v>
+        <v>172.85</v>
       </c>
       <c r="E36" s="13">
-        <v>162.05000000000001</v>
+        <v>161.59</v>
       </c>
       <c r="F36" s="13">
-        <v>171.05</v>
+        <v>170.59</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>178.62</v>
+        <v>179.45</v>
       </c>
       <c r="E40" s="10">
-        <v>167.2</v>
+        <v>166.87</v>
       </c>
       <c r="F40" s="10">
-        <v>177.2</v>
+        <v>176.87</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>178.32</v>
+        <v>179.15</v>
       </c>
       <c r="E41" s="13">
-        <v>167.62</v>
+        <v>167.29</v>
       </c>
       <c r="F41" s="13">
-        <v>177.62</v>
+        <v>177.29</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>178.24</v>
+        <v>178.62</v>
       </c>
       <c r="E42" s="10">
-        <v>167.76</v>
+        <v>167.2</v>
       </c>
       <c r="F42" s="10">
-        <v>177.76</v>
+        <v>177.2</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>177.94</v>
+        <v>178.32</v>
       </c>
       <c r="E43" s="13">
-        <v>168.18</v>
+        <v>167.62</v>
       </c>
       <c r="F43" s="13">
-        <v>178.18</v>
+        <v>177.62</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>172.33</v>
+        <v>172.79</v>
       </c>
       <c r="E47" s="10">
-        <v>163.27000000000001</v>
+        <v>162.81</v>
       </c>
       <c r="F47" s="10">
-        <v>173.27</v>
+        <v>172.81</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>172.29</v>
+        <v>172.75</v>
       </c>
       <c r="E48" s="13">
-        <v>163.43</v>
+        <v>162.96</v>
       </c>
       <c r="F48" s="13">
-        <v>173.43</v>
+        <v>172.96</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>171.88</v>
+        <v>172.33</v>
       </c>
       <c r="E49" s="10">
-        <v>163.43</v>
+        <v>163.27000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>173.43</v>
+        <v>173.27</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>171.84</v>
+        <v>172.29</v>
       </c>
       <c r="E50" s="13">
-        <v>163.59</v>
+        <v>163.43</v>
       </c>
       <c r="F50" s="13">
-        <v>173.59</v>
+        <v>173.43</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>188.66</v>
+        <v>189.5</v>
       </c>
       <c r="E54" s="10">
-        <v>177.89</v>
+        <v>177.72</v>
       </c>
       <c r="F54" s="10">
-        <v>187.89</v>
+        <v>187.72</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>176.36</v>
+        <v>177.19</v>
       </c>
       <c r="E55" s="13">
-        <v>174.62</v>
+        <v>174.39</v>
       </c>
       <c r="F55" s="13">
-        <v>184.62</v>
+        <v>184.39</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>178.76</v>
+        <v>179.59</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>178.23</v>
+        <v>179.03</v>
       </c>
       <c r="E57" s="13">
-        <v>168.88</v>
+        <v>168.65</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>174.14</v>
+        <v>174.94</v>
       </c>
       <c r="E58" s="10">
-        <v>164.94</v>
+        <v>164.71</v>
       </c>
       <c r="F58" s="10">
-        <v>174.94</v>
+        <v>174.71</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>180.87</v>
+        <v>181.68</v>
       </c>
       <c r="E59" s="13">
-        <v>175.84</v>
+        <v>175.66</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>188.29</v>
+        <v>188.66</v>
       </c>
       <c r="E60" s="10">
-        <v>178.3</v>
+        <v>177.89</v>
       </c>
       <c r="F60" s="10">
-        <v>188.3</v>
+        <v>187.89</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>175.99</v>
+        <v>176.36</v>
       </c>
       <c r="E61" s="13">
-        <v>175.08</v>
+        <v>174.62</v>
       </c>
       <c r="F61" s="13">
-        <v>185.08</v>
+        <v>184.62</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>178.39</v>
+        <v>178.76</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>177.87</v>
+        <v>178.23</v>
       </c>
       <c r="E63" s="13">
-        <v>169.35</v>
+        <v>168.88</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>173.78</v>
+        <v>174.14</v>
       </c>
       <c r="E64" s="10">
-        <v>165.4</v>
+        <v>164.94</v>
       </c>
       <c r="F64" s="10">
-        <v>175.4</v>
+        <v>174.94</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>180.52</v>
+        <v>180.87</v>
       </c>
       <c r="E65" s="13">
-        <v>176.27</v>
+        <v>175.84</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1866,15 +1866,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,6 +2125,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
@@ -2153,14 +2153,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,6 +2172,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Mon Nov 24 03:01:57 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{9B2F28E4-79DA-4500-B24C-E3B3BC9371B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8CF966FA-FC6F-499E-A679-9834DDA887E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>173.3</v>
+        <v>173.02</v>
       </c>
       <c r="E8" s="10">
-        <v>161.74</v>
+        <v>161.29</v>
       </c>
       <c r="F8" s="10">
-        <v>171.74</v>
+        <v>171.29</v>
       </c>
       <c r="G8" s="10">
-        <v>161.9</v>
+        <v>161.46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>173.3</v>
+        <v>173.02</v>
       </c>
       <c r="E9" s="13">
-        <v>161.74</v>
+        <v>161.29</v>
       </c>
       <c r="F9" s="13">
-        <v>171.74</v>
+        <v>171.29</v>
       </c>
       <c r="G9" s="13">
-        <v>161.9</v>
+        <v>161.46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>175.43</v>
+        <v>174.97</v>
       </c>
       <c r="E10" s="10">
-        <v>164.39</v>
+        <v>163.77000000000001</v>
       </c>
       <c r="F10" s="10">
-        <v>174.39</v>
+        <v>173.77</v>
       </c>
       <c r="G10" s="10">
-        <v>164.88</v>
+        <v>164.26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>172.56</v>
+        <v>173.3</v>
       </c>
       <c r="E11" s="13">
-        <v>161.93</v>
+        <v>161.74</v>
       </c>
       <c r="F11" s="13">
-        <v>171.93</v>
+        <v>171.74</v>
       </c>
       <c r="G11" s="13">
-        <v>162.09</v>
+        <v>161.9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>172.56</v>
+        <v>173.3</v>
       </c>
       <c r="E12" s="10">
-        <v>161.93</v>
+        <v>161.74</v>
       </c>
       <c r="F12" s="10">
-        <v>171.93</v>
+        <v>171.74</v>
       </c>
       <c r="G12" s="10">
-        <v>162.09</v>
+        <v>161.9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>174.61</v>
+        <v>175.43</v>
       </c>
       <c r="E13" s="13">
-        <v>164.6</v>
+        <v>164.39</v>
       </c>
       <c r="F13" s="13">
-        <v>174.6</v>
+        <v>174.39</v>
       </c>
       <c r="G13" s="13">
-        <v>165.09</v>
+        <v>164.88</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>178.72</v>
+        <v>178.25</v>
       </c>
       <c r="E17" s="10">
-        <v>166.89</v>
+        <v>166.26</v>
       </c>
       <c r="F17" s="10">
-        <v>176.89</v>
+        <v>176.26</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>177.91</v>
+        <v>178.72</v>
       </c>
       <c r="E18" s="13">
-        <v>167.24</v>
+        <v>166.89</v>
       </c>
       <c r="F18" s="13">
-        <v>177.24</v>
+        <v>176.89</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>174.43</v>
+        <v>174.14</v>
       </c>
       <c r="E22" s="10">
-        <v>163.44</v>
+        <v>162.83000000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>173.04</v>
+        <v>172.43</v>
       </c>
       <c r="G22" s="10">
-        <v>164.73</v>
+        <v>164.11</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>180.22</v>
+        <v>179.76</v>
       </c>
       <c r="E23" s="13">
-        <v>168.2</v>
+        <v>167.59</v>
       </c>
       <c r="F23" s="13">
-        <v>178.2</v>
+        <v>177.59</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>180.01</v>
+        <v>179.55</v>
       </c>
       <c r="E24" s="10">
-        <v>168.58</v>
+        <v>167.97</v>
       </c>
       <c r="F24" s="10">
-        <v>178.58</v>
+        <v>177.97</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>180.83</v>
+        <v>180.37</v>
       </c>
       <c r="E25" s="13">
-        <v>167.99</v>
+        <v>167.38</v>
       </c>
       <c r="F25" s="13">
-        <v>177.99</v>
+        <v>177.38</v>
       </c>
       <c r="G25" s="13">
-        <v>168.03</v>
+        <v>167.42</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>179.52</v>
+        <v>179.06</v>
       </c>
       <c r="E26" s="10">
-        <v>169.45</v>
+        <v>168.83</v>
       </c>
       <c r="F26" s="10">
-        <v>179.45</v>
+        <v>178.83</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>173.58</v>
+        <v>174.43</v>
       </c>
       <c r="E27" s="13">
-        <v>163.66999999999999</v>
+        <v>163.44</v>
       </c>
       <c r="F27" s="13">
-        <v>173.27</v>
+        <v>173.04</v>
       </c>
       <c r="G27" s="13">
-        <v>164.95</v>
+        <v>164.73</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>179.39</v>
+        <v>180.22</v>
       </c>
       <c r="E28" s="22">
-        <v>168.42</v>
+        <v>168.2</v>
       </c>
       <c r="F28" s="22">
-        <v>178.42</v>
+        <v>178.2</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>179.19</v>
+        <v>180.01</v>
       </c>
       <c r="E29" s="13">
-        <v>168.79</v>
+        <v>168.58</v>
       </c>
       <c r="F29" s="13">
-        <v>178.79</v>
+        <v>178.58</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>180.01</v>
+        <v>180.83</v>
       </c>
       <c r="E30" s="22">
-        <v>168.2</v>
+        <v>167.99</v>
       </c>
       <c r="F30" s="22">
-        <v>178.2</v>
+        <v>177.99</v>
       </c>
       <c r="G30" s="22">
-        <v>168.24</v>
+        <v>168.03</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>178.7</v>
+        <v>179.52</v>
       </c>
       <c r="E31" s="13">
-        <v>169.66</v>
+        <v>169.45</v>
       </c>
       <c r="F31" s="13">
-        <v>179.66</v>
+        <v>179.45</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>173.67</v>
+        <v>173.32</v>
       </c>
       <c r="E35" s="10">
-        <v>161.38</v>
+        <v>160.76</v>
       </c>
       <c r="F35" s="10">
-        <v>170.38</v>
+        <v>169.76</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>172.85</v>
+        <v>173.67</v>
       </c>
       <c r="E36" s="13">
-        <v>161.59</v>
+        <v>161.38</v>
       </c>
       <c r="F36" s="13">
-        <v>170.59</v>
+        <v>170.38</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>179.45</v>
+        <v>179</v>
       </c>
       <c r="E40" s="10">
-        <v>166.87</v>
+        <v>166.26</v>
       </c>
       <c r="F40" s="10">
-        <v>176.87</v>
+        <v>176.26</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>179.15</v>
+        <v>178.7</v>
       </c>
       <c r="E41" s="13">
-        <v>167.29</v>
+        <v>166.68</v>
       </c>
       <c r="F41" s="13">
-        <v>177.29</v>
+        <v>176.68</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>178.62</v>
+        <v>179.45</v>
       </c>
       <c r="E42" s="10">
-        <v>167.2</v>
+        <v>166.87</v>
       </c>
       <c r="F42" s="10">
-        <v>177.2</v>
+        <v>176.87</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>178.32</v>
+        <v>179.15</v>
       </c>
       <c r="E43" s="13">
-        <v>167.62</v>
+        <v>167.29</v>
       </c>
       <c r="F43" s="13">
-        <v>177.62</v>
+        <v>177.29</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>172.79</v>
+        <v>173.02</v>
       </c>
       <c r="E47" s="10">
-        <v>162.81</v>
+        <v>162.59</v>
       </c>
       <c r="F47" s="10">
-        <v>172.81</v>
+        <v>172.59</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>172.75</v>
+        <v>172.98</v>
       </c>
       <c r="E48" s="13">
-        <v>162.96</v>
+        <v>162.74</v>
       </c>
       <c r="F48" s="13">
-        <v>172.96</v>
+        <v>172.74</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>172.33</v>
+        <v>172.79</v>
       </c>
       <c r="E49" s="10">
-        <v>163.27000000000001</v>
+        <v>162.81</v>
       </c>
       <c r="F49" s="10">
-        <v>173.27</v>
+        <v>172.81</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>172.29</v>
+        <v>172.75</v>
       </c>
       <c r="E50" s="13">
-        <v>163.43</v>
+        <v>162.96</v>
       </c>
       <c r="F50" s="13">
-        <v>173.43</v>
+        <v>172.96</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>189.5</v>
+        <v>189.05</v>
       </c>
       <c r="E54" s="10">
-        <v>177.72</v>
+        <v>177.14</v>
       </c>
       <c r="F54" s="10">
-        <v>187.72</v>
+        <v>187.14</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>177.19</v>
+        <v>176.95</v>
       </c>
       <c r="E55" s="13">
-        <v>174.39</v>
+        <v>173.76</v>
       </c>
       <c r="F55" s="13">
-        <v>184.39</v>
+        <v>183.76</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>179.59</v>
+        <v>179.13</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>179.03</v>
+        <v>178.56</v>
       </c>
       <c r="E57" s="13">
-        <v>168.65</v>
+        <v>168.03</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>174.94</v>
+        <v>174.47</v>
       </c>
       <c r="E58" s="10">
-        <v>164.71</v>
+        <v>164.08</v>
       </c>
       <c r="F58" s="10">
-        <v>174.71</v>
+        <v>174.08</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>181.68</v>
+        <v>181.2</v>
       </c>
       <c r="E59" s="13">
-        <v>175.66</v>
+        <v>175.06</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>188.66</v>
+        <v>189.5</v>
       </c>
       <c r="E60" s="10">
-        <v>177.89</v>
+        <v>177.72</v>
       </c>
       <c r="F60" s="10">
-        <v>187.89</v>
+        <v>187.72</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>176.36</v>
+        <v>177.19</v>
       </c>
       <c r="E61" s="13">
-        <v>174.62</v>
+        <v>174.39</v>
       </c>
       <c r="F61" s="13">
-        <v>184.62</v>
+        <v>184.39</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>178.76</v>
+        <v>179.59</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>178.23</v>
+        <v>179.03</v>
       </c>
       <c r="E63" s="13">
-        <v>168.88</v>
+        <v>168.65</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>174.14</v>
+        <v>174.94</v>
       </c>
       <c r="E64" s="10">
-        <v>164.94</v>
+        <v>164.71</v>
       </c>
       <c r="F64" s="10">
-        <v>174.94</v>
+        <v>174.71</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>180.87</v>
+        <v>181.68</v>
       </c>
       <c r="E65" s="13">
-        <v>175.84</v>
+        <v>175.66</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,14 +1855,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2126,28 +2124,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2163,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Nov 25 02:53:45 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8CF966FA-FC6F-499E-A679-9834DDA887E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{64F65E5F-0047-4E93-BFE6-DD381E5DE7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>173.02</v>
+        <v>171.96</v>
       </c>
       <c r="E8" s="10">
-        <v>161.29</v>
+        <v>160.74</v>
       </c>
       <c r="F8" s="10">
-        <v>171.29</v>
+        <v>170.74</v>
       </c>
       <c r="G8" s="10">
-        <v>161.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>173.02</v>
+        <v>171.96</v>
       </c>
       <c r="E9" s="13">
-        <v>161.29</v>
+        <v>160.74</v>
       </c>
       <c r="F9" s="13">
-        <v>171.29</v>
+        <v>170.74</v>
       </c>
       <c r="G9" s="13">
-        <v>161.46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>174.97</v>
+        <v>173.71</v>
       </c>
       <c r="E10" s="10">
-        <v>163.77000000000001</v>
+        <v>163.03</v>
       </c>
       <c r="F10" s="10">
-        <v>173.77</v>
+        <v>173.03</v>
       </c>
       <c r="G10" s="10">
-        <v>164.26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.52000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>173.3</v>
+        <v>173.02</v>
       </c>
       <c r="E11" s="13">
-        <v>161.74</v>
+        <v>161.29</v>
       </c>
       <c r="F11" s="13">
-        <v>171.74</v>
+        <v>171.29</v>
       </c>
       <c r="G11" s="13">
-        <v>161.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>173.3</v>
+        <v>173.02</v>
       </c>
       <c r="E12" s="10">
-        <v>161.74</v>
+        <v>161.29</v>
       </c>
       <c r="F12" s="10">
-        <v>171.74</v>
+        <v>171.29</v>
       </c>
       <c r="G12" s="10">
-        <v>161.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>175.43</v>
+        <v>174.97</v>
       </c>
       <c r="E13" s="13">
-        <v>164.39</v>
+        <v>163.77000000000001</v>
       </c>
       <c r="F13" s="13">
-        <v>174.39</v>
+        <v>173.77</v>
       </c>
       <c r="G13" s="13">
-        <v>164.88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>164.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>178.25</v>
+        <v>176.98</v>
       </c>
       <c r="E17" s="10">
-        <v>166.26</v>
+        <v>165.5</v>
       </c>
       <c r="F17" s="10">
-        <v>176.26</v>
+        <v>175.5</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>178.72</v>
+        <v>178.25</v>
       </c>
       <c r="E18" s="13">
-        <v>166.89</v>
+        <v>166.26</v>
       </c>
       <c r="F18" s="13">
-        <v>176.89</v>
+        <v>176.26</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>174.14</v>
+        <v>173.09</v>
       </c>
       <c r="E22" s="10">
-        <v>162.83000000000001</v>
+        <v>162.19</v>
       </c>
       <c r="F22" s="10">
-        <v>172.43</v>
+        <v>171.79</v>
       </c>
       <c r="G22" s="10">
-        <v>164.11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.47999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>179.76</v>
+        <v>178.5</v>
       </c>
       <c r="E23" s="13">
-        <v>167.59</v>
+        <v>166.95</v>
       </c>
       <c r="F23" s="13">
-        <v>177.59</v>
+        <v>176.95</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>179.55</v>
+        <v>178.28</v>
       </c>
       <c r="E24" s="10">
-        <v>167.97</v>
+        <v>167.23</v>
       </c>
       <c r="F24" s="10">
-        <v>177.97</v>
+        <v>177.23</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>180.37</v>
+        <v>179.11</v>
       </c>
       <c r="E25" s="13">
-        <v>167.38</v>
+        <v>166.63</v>
       </c>
       <c r="F25" s="13">
-        <v>177.38</v>
+        <v>176.63</v>
       </c>
       <c r="G25" s="13">
-        <v>167.42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>166.67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>179.06</v>
+        <v>177.8</v>
       </c>
       <c r="E26" s="10">
-        <v>168.83</v>
+        <v>168.08</v>
       </c>
       <c r="F26" s="10">
-        <v>178.83</v>
+        <v>178.08</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>174.43</v>
+        <v>174.14</v>
       </c>
       <c r="E27" s="13">
-        <v>163.44</v>
+        <v>162.83000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>173.04</v>
+        <v>172.43</v>
       </c>
       <c r="G27" s="13">
-        <v>164.73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>164.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>180.22</v>
+        <v>179.76</v>
       </c>
       <c r="E28" s="22">
-        <v>168.2</v>
+        <v>167.59</v>
       </c>
       <c r="F28" s="22">
-        <v>178.2</v>
+        <v>177.59</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>180.01</v>
+        <v>179.55</v>
       </c>
       <c r="E29" s="13">
-        <v>168.58</v>
+        <v>167.97</v>
       </c>
       <c r="F29" s="13">
-        <v>178.58</v>
+        <v>177.97</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>180.83</v>
+        <v>180.37</v>
       </c>
       <c r="E30" s="22">
-        <v>167.99</v>
+        <v>167.38</v>
       </c>
       <c r="F30" s="22">
-        <v>177.99</v>
+        <v>177.38</v>
       </c>
       <c r="G30" s="22">
-        <v>168.03</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>167.42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>179.52</v>
+        <v>179.06</v>
       </c>
       <c r="E31" s="13">
-        <v>169.45</v>
+        <v>168.83</v>
       </c>
       <c r="F31" s="13">
-        <v>179.45</v>
+        <v>178.83</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>173.32</v>
+        <v>172.06</v>
       </c>
       <c r="E35" s="10">
-        <v>160.76</v>
+        <v>160.01</v>
       </c>
       <c r="F35" s="10">
-        <v>169.76</v>
+        <v>169.02</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>173.67</v>
+        <v>173.32</v>
       </c>
       <c r="E36" s="13">
-        <v>161.38</v>
+        <v>160.76</v>
       </c>
       <c r="F36" s="13">
-        <v>170.38</v>
+        <v>169.76</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>179</v>
+        <v>177.74</v>
       </c>
       <c r="E40" s="10">
-        <v>166.26</v>
+        <v>165.51</v>
       </c>
       <c r="F40" s="10">
-        <v>176.26</v>
+        <v>175.51</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>178.7</v>
+        <v>177.45</v>
       </c>
       <c r="E41" s="13">
-        <v>166.68</v>
+        <v>165.93</v>
       </c>
       <c r="F41" s="13">
-        <v>176.68</v>
+        <v>175.93</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>179.45</v>
+        <v>179</v>
       </c>
       <c r="E42" s="10">
-        <v>166.87</v>
+        <v>166.26</v>
       </c>
       <c r="F42" s="10">
-        <v>176.87</v>
+        <v>176.26</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>179.15</v>
+        <v>178.7</v>
       </c>
       <c r="E43" s="13">
-        <v>167.29</v>
+        <v>166.68</v>
       </c>
       <c r="F43" s="13">
-        <v>177.29</v>
+        <v>176.68</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>173.02</v>
+        <v>173.43</v>
       </c>
       <c r="E47" s="10">
-        <v>162.59</v>
+        <v>162.31</v>
       </c>
       <c r="F47" s="10">
-        <v>172.59</v>
+        <v>172.31</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>172.98</v>
+        <v>173.38</v>
       </c>
       <c r="E48" s="13">
-        <v>162.74</v>
+        <v>162.44999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>172.74</v>
+        <v>172.45</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>172.79</v>
+        <v>173.02</v>
       </c>
       <c r="E49" s="10">
-        <v>162.81</v>
+        <v>162.59</v>
       </c>
       <c r="F49" s="10">
-        <v>172.81</v>
+        <v>172.59</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>172.75</v>
+        <v>172.98</v>
       </c>
       <c r="E50" s="13">
-        <v>162.96</v>
+        <v>162.74</v>
       </c>
       <c r="F50" s="13">
-        <v>172.96</v>
+        <v>172.74</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>189.05</v>
+        <v>187.79</v>
       </c>
       <c r="E54" s="10">
-        <v>177.14</v>
+        <v>176.42</v>
       </c>
       <c r="F54" s="10">
-        <v>187.14</v>
+        <v>186.42</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>176.95</v>
+        <v>175.69</v>
       </c>
       <c r="E55" s="13">
-        <v>173.76</v>
+        <v>173.12</v>
       </c>
       <c r="F55" s="13">
-        <v>183.76</v>
+        <v>183.12</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>179.13</v>
+        <v>177.98</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>178.56</v>
+        <v>177.4</v>
       </c>
       <c r="E57" s="13">
-        <v>168.03</v>
+        <v>167.39</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>174.47</v>
+        <v>173.31</v>
       </c>
       <c r="E58" s="10">
-        <v>164.08</v>
+        <v>163.44</v>
       </c>
       <c r="F58" s="10">
-        <v>174.08</v>
+        <v>173.44</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>181.2</v>
+        <v>179.93</v>
       </c>
       <c r="E59" s="13">
-        <v>175.06</v>
+        <v>174.33</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>189.5</v>
+        <v>189.05</v>
       </c>
       <c r="E60" s="10">
-        <v>177.72</v>
+        <v>177.14</v>
       </c>
       <c r="F60" s="10">
-        <v>187.72</v>
+        <v>187.14</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>177.19</v>
+        <v>176.95</v>
       </c>
       <c r="E61" s="13">
-        <v>174.39</v>
+        <v>173.76</v>
       </c>
       <c r="F61" s="13">
-        <v>184.39</v>
+        <v>183.76</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>179.59</v>
+        <v>179.13</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>179.03</v>
+        <v>178.56</v>
       </c>
       <c r="E63" s="13">
-        <v>168.65</v>
+        <v>168.03</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>174.94</v>
+        <v>174.47</v>
       </c>
       <c r="E64" s="10">
-        <v>164.71</v>
+        <v>164.08</v>
       </c>
       <c r="F64" s="10">
-        <v>174.71</v>
+        <v>174.08</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45983</v>
+        <v>45986</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>181.68</v>
+        <v>181.2</v>
       </c>
       <c r="E65" s="13">
-        <v>175.66</v>
+        <v>175.06</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2123,6 +2114,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2135,14 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2158,6 +2150,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Wed Nov 26 02:53:32 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{64F65E5F-0047-4E93-BFE6-DD381E5DE7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5901F00C-930F-4011-965C-096C7F6DB7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentManualCount="12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>171.96</v>
+        <v>170.56</v>
       </c>
       <c r="E8" s="10">
-        <v>160.74</v>
+        <v>160.32</v>
       </c>
       <c r="F8" s="10">
-        <v>170.74</v>
+        <v>170.32</v>
       </c>
       <c r="G8" s="10">
-        <v>160.91</v>
+        <v>160.47999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>171.96</v>
+        <v>170.56</v>
       </c>
       <c r="E9" s="13">
-        <v>160.74</v>
+        <v>160.32</v>
       </c>
       <c r="F9" s="13">
-        <v>170.74</v>
+        <v>170.32</v>
       </c>
       <c r="G9" s="13">
-        <v>160.91</v>
+        <v>160.47999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>173.71</v>
+        <v>171.98</v>
       </c>
       <c r="E10" s="10">
-        <v>163.03</v>
+        <v>162.4</v>
       </c>
       <c r="F10" s="10">
-        <v>173.03</v>
+        <v>172.4</v>
       </c>
       <c r="G10" s="10">
-        <v>163.52000000000001</v>
+        <v>162.88999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>173.02</v>
+        <v>171.96</v>
       </c>
       <c r="E11" s="13">
-        <v>161.29</v>
+        <v>160.74</v>
       </c>
       <c r="F11" s="13">
-        <v>171.29</v>
+        <v>170.74</v>
       </c>
       <c r="G11" s="13">
-        <v>161.46</v>
+        <v>160.91</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>173.02</v>
+        <v>171.96</v>
       </c>
       <c r="E12" s="10">
-        <v>161.29</v>
+        <v>160.74</v>
       </c>
       <c r="F12" s="10">
-        <v>171.29</v>
+        <v>170.74</v>
       </c>
       <c r="G12" s="10">
-        <v>161.46</v>
+        <v>160.91</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>174.97</v>
+        <v>173.71</v>
       </c>
       <c r="E13" s="13">
-        <v>163.77000000000001</v>
+        <v>163.03</v>
       </c>
       <c r="F13" s="13">
-        <v>173.77</v>
+        <v>173.03</v>
       </c>
       <c r="G13" s="13">
-        <v>164.26</v>
+        <v>163.52000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>176.98</v>
+        <v>175.23</v>
       </c>
       <c r="E17" s="10">
-        <v>165.5</v>
+        <v>164.85</v>
       </c>
       <c r="F17" s="10">
-        <v>175.5</v>
+        <v>174.85</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>178.25</v>
+        <v>176.98</v>
       </c>
       <c r="E18" s="13">
-        <v>166.26</v>
+        <v>165.5</v>
       </c>
       <c r="F18" s="13">
-        <v>176.26</v>
+        <v>175.5</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>173.09</v>
+        <v>171.46</v>
       </c>
       <c r="E22" s="10">
-        <v>162.19</v>
+        <v>161.55000000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>171.79</v>
+        <v>171.15</v>
       </c>
       <c r="G22" s="10">
-        <v>163.47999999999999</v>
+        <v>162.84</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>178.5</v>
+        <v>176.76</v>
       </c>
       <c r="E23" s="13">
-        <v>166.95</v>
+        <v>166.42</v>
       </c>
       <c r="F23" s="13">
-        <v>176.95</v>
+        <v>176.42</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>178.28</v>
+        <v>176.55</v>
       </c>
       <c r="E24" s="10">
-        <v>167.23</v>
+        <v>166.82</v>
       </c>
       <c r="F24" s="10">
-        <v>177.23</v>
+        <v>176.82</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>179.11</v>
+        <v>177.37</v>
       </c>
       <c r="E25" s="13">
-        <v>166.63</v>
+        <v>166.23</v>
       </c>
       <c r="F25" s="13">
-        <v>176.63</v>
+        <v>176.23</v>
       </c>
       <c r="G25" s="13">
-        <v>166.67</v>
+        <v>166.27</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>177.8</v>
+        <v>176.05</v>
       </c>
       <c r="E26" s="10">
-        <v>168.08</v>
+        <v>167.67</v>
       </c>
       <c r="F26" s="10">
-        <v>178.08</v>
+        <v>177.67</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>174.14</v>
+        <v>173.09</v>
       </c>
       <c r="E27" s="13">
-        <v>162.83000000000001</v>
+        <v>162.19</v>
       </c>
       <c r="F27" s="13">
-        <v>172.43</v>
+        <v>171.79</v>
       </c>
       <c r="G27" s="13">
-        <v>164.11</v>
+        <v>163.47999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>179.76</v>
+        <v>178.5</v>
       </c>
       <c r="E28" s="22">
-        <v>167.59</v>
+        <v>166.95</v>
       </c>
       <c r="F28" s="22">
-        <v>177.59</v>
+        <v>176.95</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>179.55</v>
+        <v>178.28</v>
       </c>
       <c r="E29" s="13">
-        <v>167.97</v>
+        <v>167.23</v>
       </c>
       <c r="F29" s="13">
-        <v>177.97</v>
+        <v>177.23</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>180.37</v>
+        <v>179.11</v>
       </c>
       <c r="E30" s="22">
-        <v>167.38</v>
+        <v>166.63</v>
       </c>
       <c r="F30" s="22">
-        <v>177.38</v>
+        <v>176.63</v>
       </c>
       <c r="G30" s="22">
-        <v>167.42</v>
+        <v>166.67</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>179.06</v>
+        <v>177.8</v>
       </c>
       <c r="E31" s="13">
-        <v>168.83</v>
+        <v>168.08</v>
       </c>
       <c r="F31" s="13">
-        <v>178.83</v>
+        <v>178.08</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>172.06</v>
+        <v>170.32</v>
       </c>
       <c r="E35" s="10">
-        <v>160.01</v>
+        <v>159.38</v>
       </c>
       <c r="F35" s="10">
-        <v>169.02</v>
+        <v>168.38</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>173.32</v>
+        <v>172.06</v>
       </c>
       <c r="E36" s="13">
-        <v>160.76</v>
+        <v>160.01</v>
       </c>
       <c r="F36" s="13">
-        <v>169.76</v>
+        <v>169.02</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>177.74</v>
+        <v>176.02</v>
       </c>
       <c r="E40" s="10">
-        <v>165.51</v>
+        <v>164.89</v>
       </c>
       <c r="F40" s="10">
-        <v>175.51</v>
+        <v>174.89</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>177.45</v>
+        <v>175.72</v>
       </c>
       <c r="E41" s="13">
-        <v>165.93</v>
+        <v>165.31</v>
       </c>
       <c r="F41" s="13">
-        <v>175.93</v>
+        <v>175.31</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>179</v>
+        <v>177.74</v>
       </c>
       <c r="E42" s="10">
-        <v>166.26</v>
+        <v>165.51</v>
       </c>
       <c r="F42" s="10">
-        <v>176.26</v>
+        <v>175.51</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>178.7</v>
+        <v>177.45</v>
       </c>
       <c r="E43" s="13">
-        <v>166.68</v>
+        <v>165.93</v>
       </c>
       <c r="F43" s="13">
-        <v>176.68</v>
+        <v>175.93</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>173.43</v>
+        <v>172.37</v>
       </c>
       <c r="E47" s="10">
-        <v>162.31</v>
+        <v>161.69</v>
       </c>
       <c r="F47" s="10">
-        <v>172.31</v>
+        <v>171.69</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>173.38</v>
+        <v>172.31</v>
       </c>
       <c r="E48" s="13">
-        <v>162.44999999999999</v>
+        <v>161.83000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>172.45</v>
+        <v>171.83</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>173.02</v>
+        <v>173.43</v>
       </c>
       <c r="E49" s="10">
-        <v>162.59</v>
+        <v>162.31</v>
       </c>
       <c r="F49" s="10">
-        <v>172.59</v>
+        <v>172.31</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>172.98</v>
+        <v>173.38</v>
       </c>
       <c r="E50" s="13">
-        <v>162.74</v>
+        <v>162.44999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>172.74</v>
+        <v>172.45</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>187.79</v>
+        <v>186.05</v>
       </c>
       <c r="E54" s="10">
-        <v>176.42</v>
+        <v>175.85</v>
       </c>
       <c r="F54" s="10">
-        <v>186.42</v>
+        <v>185.85</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>175.69</v>
+        <v>173.95</v>
       </c>
       <c r="E55" s="13">
-        <v>173.12</v>
+        <v>172.48</v>
       </c>
       <c r="F55" s="13">
-        <v>183.12</v>
+        <v>182.48</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>177.98</v>
+        <v>176.25</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>177.4</v>
+        <v>175.64</v>
       </c>
       <c r="E57" s="13">
-        <v>167.39</v>
+        <v>166.74</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>173.31</v>
+        <v>171.55</v>
       </c>
       <c r="E58" s="10">
-        <v>163.44</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>173.44</v>
+        <v>172.8</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>179.93</v>
+        <v>178.17</v>
       </c>
       <c r="E59" s="13">
-        <v>174.33</v>
+        <v>173.74</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>189.05</v>
+        <v>187.79</v>
       </c>
       <c r="E60" s="10">
-        <v>177.14</v>
+        <v>176.42</v>
       </c>
       <c r="F60" s="10">
-        <v>187.14</v>
+        <v>186.42</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>176.95</v>
+        <v>175.69</v>
       </c>
       <c r="E61" s="13">
-        <v>173.76</v>
+        <v>173.12</v>
       </c>
       <c r="F61" s="13">
-        <v>183.76</v>
+        <v>183.12</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>179.13</v>
+        <v>177.98</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>178.56</v>
+        <v>177.4</v>
       </c>
       <c r="E63" s="13">
-        <v>168.03</v>
+        <v>167.39</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>174.47</v>
+        <v>173.31</v>
       </c>
       <c r="E64" s="10">
-        <v>164.08</v>
+        <v>163.44</v>
       </c>
       <c r="F64" s="10">
-        <v>174.08</v>
+        <v>173.44</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>181.2</v>
+        <v>179.93</v>
       </c>
       <c r="E65" s="13">
-        <v>175.06</v>
+        <v>174.33</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -2115,15 +2115,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -2132,6 +2123,15 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2155,14 +2155,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2180,6 +2172,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Thu Nov 27 02:50:52 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5901F00C-930F-4011-965C-096C7F6DB7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{84134239-DFB4-469C-B006-AFE78B7CCA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="12"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>170.56</v>
+        <v>167.73</v>
       </c>
       <c r="E8" s="10">
-        <v>160.32</v>
+        <v>159.87</v>
       </c>
       <c r="F8" s="10">
-        <v>170.32</v>
+        <v>169.87</v>
       </c>
       <c r="G8" s="10">
-        <v>160.47999999999999</v>
+        <v>160.03</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>170.56</v>
+        <v>167.73</v>
       </c>
       <c r="E9" s="13">
-        <v>160.32</v>
+        <v>159.87</v>
       </c>
       <c r="F9" s="13">
-        <v>170.32</v>
+        <v>169.87</v>
       </c>
       <c r="G9" s="13">
-        <v>160.47999999999999</v>
+        <v>160.03</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>171.98</v>
+        <v>169.16</v>
       </c>
       <c r="E10" s="10">
-        <v>162.4</v>
+        <v>162.41999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>172.4</v>
+        <v>172.42</v>
       </c>
       <c r="G10" s="10">
-        <v>162.88999999999999</v>
+        <v>162.91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>171.96</v>
+        <v>170.56</v>
       </c>
       <c r="E11" s="13">
-        <v>160.74</v>
+        <v>160.32</v>
       </c>
       <c r="F11" s="13">
-        <v>170.74</v>
+        <v>170.32</v>
       </c>
       <c r="G11" s="13">
-        <v>160.91</v>
+        <v>160.47999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>171.96</v>
+        <v>170.56</v>
       </c>
       <c r="E12" s="10">
-        <v>160.74</v>
+        <v>160.32</v>
       </c>
       <c r="F12" s="10">
-        <v>170.74</v>
+        <v>170.32</v>
       </c>
       <c r="G12" s="10">
-        <v>160.91</v>
+        <v>160.47999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>173.71</v>
+        <v>171.98</v>
       </c>
       <c r="E13" s="13">
-        <v>163.03</v>
+        <v>162.4</v>
       </c>
       <c r="F13" s="13">
-        <v>173.03</v>
+        <v>172.4</v>
       </c>
       <c r="G13" s="13">
-        <v>163.52000000000001</v>
+        <v>162.88999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,14 +972,14 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>175.23</v>
+        <v>172.4</v>
       </c>
       <c r="E17" s="10">
         <v>164.85</v>
@@ -991,20 +991,20 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>176.98</v>
+        <v>175.23</v>
       </c>
       <c r="E18" s="13">
-        <v>165.5</v>
+        <v>164.85</v>
       </c>
       <c r="F18" s="13">
-        <v>175.5</v>
+        <v>174.85</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>171.46</v>
+        <v>168.53</v>
       </c>
       <c r="E22" s="10">
-        <v>161.55000000000001</v>
+        <v>161.68</v>
       </c>
       <c r="F22" s="10">
-        <v>171.15</v>
+        <v>171.28</v>
       </c>
       <c r="G22" s="10">
-        <v>162.84</v>
+        <v>162.97</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>176.76</v>
+        <v>173.95</v>
       </c>
       <c r="E23" s="13">
-        <v>166.42</v>
+        <v>166.44</v>
       </c>
       <c r="F23" s="13">
-        <v>176.42</v>
+        <v>176.44</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>176.55</v>
+        <v>173.73</v>
       </c>
       <c r="E24" s="10">
-        <v>166.82</v>
+        <v>166.85</v>
       </c>
       <c r="F24" s="10">
-        <v>176.82</v>
+        <v>176.85</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>177.37</v>
+        <v>174.56</v>
       </c>
       <c r="E25" s="13">
-        <v>166.23</v>
+        <v>166.26</v>
       </c>
       <c r="F25" s="13">
-        <v>176.23</v>
+        <v>176.26</v>
       </c>
       <c r="G25" s="13">
-        <v>166.27</v>
+        <v>166.3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>176.05</v>
+        <v>173.23</v>
       </c>
       <c r="E26" s="10">
-        <v>167.67</v>
+        <v>167.7</v>
       </c>
       <c r="F26" s="10">
-        <v>177.67</v>
+        <v>177.7</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>173.09</v>
+        <v>171.46</v>
       </c>
       <c r="E27" s="13">
-        <v>162.19</v>
+        <v>161.55000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>171.79</v>
+        <v>171.15</v>
       </c>
       <c r="G27" s="13">
-        <v>163.47999999999999</v>
+        <v>162.84</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>178.5</v>
+        <v>176.76</v>
       </c>
       <c r="E28" s="22">
-        <v>166.95</v>
+        <v>166.42</v>
       </c>
       <c r="F28" s="22">
-        <v>176.95</v>
+        <v>176.42</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>178.28</v>
+        <v>176.55</v>
       </c>
       <c r="E29" s="13">
-        <v>167.23</v>
+        <v>166.82</v>
       </c>
       <c r="F29" s="13">
-        <v>177.23</v>
+        <v>176.82</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>179.11</v>
+        <v>177.37</v>
       </c>
       <c r="E30" s="22">
-        <v>166.63</v>
+        <v>166.23</v>
       </c>
       <c r="F30" s="22">
-        <v>176.63</v>
+        <v>176.23</v>
       </c>
       <c r="G30" s="22">
-        <v>166.67</v>
+        <v>166.27</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>177.8</v>
+        <v>176.05</v>
       </c>
       <c r="E31" s="13">
-        <v>168.08</v>
+        <v>167.67</v>
       </c>
       <c r="F31" s="13">
-        <v>178.08</v>
+        <v>177.67</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>170.32</v>
+        <v>167.4</v>
       </c>
       <c r="E35" s="10">
-        <v>159.38</v>
+        <v>159.4</v>
       </c>
       <c r="F35" s="10">
-        <v>168.38</v>
+        <v>168.4</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>172.06</v>
+        <v>170.32</v>
       </c>
       <c r="E36" s="13">
-        <v>160.01</v>
+        <v>159.38</v>
       </c>
       <c r="F36" s="13">
-        <v>169.02</v>
+        <v>168.38</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>176.02</v>
+        <v>173.22</v>
       </c>
       <c r="E40" s="10">
-        <v>164.89</v>
+        <v>164.92</v>
       </c>
       <c r="F40" s="10">
-        <v>174.89</v>
+        <v>174.92</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>175.72</v>
+        <v>172.92</v>
       </c>
       <c r="E41" s="13">
-        <v>165.31</v>
+        <v>165.34</v>
       </c>
       <c r="F41" s="13">
-        <v>175.31</v>
+        <v>175.34</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>177.74</v>
+        <v>176.02</v>
       </c>
       <c r="E42" s="10">
-        <v>165.51</v>
+        <v>164.89</v>
       </c>
       <c r="F42" s="10">
-        <v>175.51</v>
+        <v>174.89</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>177.45</v>
+        <v>175.72</v>
       </c>
       <c r="E43" s="13">
-        <v>165.93</v>
+        <v>165.31</v>
       </c>
       <c r="F43" s="13">
-        <v>175.93</v>
+        <v>175.31</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>172.37</v>
+        <v>170.65</v>
       </c>
       <c r="E47" s="10">
-        <v>161.69</v>
+        <v>161.44</v>
       </c>
       <c r="F47" s="10">
-        <v>171.69</v>
+        <v>171.44</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>172.31</v>
+        <v>170.58</v>
       </c>
       <c r="E48" s="13">
-        <v>161.83000000000001</v>
+        <v>161.58000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>171.83</v>
+        <v>171.58</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>173.43</v>
+        <v>172.37</v>
       </c>
       <c r="E49" s="10">
-        <v>162.31</v>
+        <v>161.69</v>
       </c>
       <c r="F49" s="10">
-        <v>172.31</v>
+        <v>171.69</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>173.38</v>
+        <v>172.31</v>
       </c>
       <c r="E50" s="13">
-        <v>162.44999999999999</v>
+        <v>161.83000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>172.45</v>
+        <v>171.83</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>186.05</v>
+        <v>183.21</v>
       </c>
       <c r="E54" s="10">
-        <v>175.85</v>
+        <v>175.95</v>
       </c>
       <c r="F54" s="10">
-        <v>185.85</v>
+        <v>185.95</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>173.95</v>
+        <v>171.13</v>
       </c>
       <c r="E55" s="13">
-        <v>172.48</v>
+        <v>172.47</v>
       </c>
       <c r="F55" s="13">
-        <v>182.48</v>
+        <v>182.47</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>176.25</v>
+        <v>173.44</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,14 +1664,14 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>175.64</v>
+        <v>172.81</v>
       </c>
       <c r="E57" s="13">
         <v>166.74</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>171.55</v>
+        <v>168.72</v>
       </c>
       <c r="E58" s="10">
-        <v>162.80000000000001</v>
+        <v>162.79</v>
       </c>
       <c r="F58" s="10">
-        <v>172.8</v>
+        <v>172.79</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>178.17</v>
+        <v>175.34</v>
       </c>
       <c r="E59" s="13">
-        <v>173.74</v>
+        <v>173.8</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>187.79</v>
+        <v>186.05</v>
       </c>
       <c r="E60" s="10">
-        <v>176.42</v>
+        <v>175.85</v>
       </c>
       <c r="F60" s="10">
-        <v>186.42</v>
+        <v>185.85</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>175.69</v>
+        <v>173.95</v>
       </c>
       <c r="E61" s="13">
-        <v>173.12</v>
+        <v>172.48</v>
       </c>
       <c r="F61" s="13">
-        <v>183.12</v>
+        <v>182.48</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>177.98</v>
+        <v>176.25</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>177.4</v>
+        <v>175.64</v>
       </c>
       <c r="E63" s="13">
-        <v>167.39</v>
+        <v>166.74</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>173.31</v>
+        <v>171.55</v>
       </c>
       <c r="E64" s="10">
-        <v>163.44</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>173.44</v>
+        <v>172.8</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>179.93</v>
+        <v>178.17</v>
       </c>
       <c r="E65" s="13">
-        <v>174.33</v>
+        <v>173.74</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,42 +2134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2161,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fri Nov 28 02:50:02 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{84134239-DFB4-469C-B006-AFE78B7CCA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{FFA194FD-F452-4AF1-8580-E0DACC17DAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>167.73</v>
+        <v>165.46</v>
       </c>
       <c r="E8" s="10">
-        <v>159.87</v>
+        <v>160.34</v>
       </c>
       <c r="F8" s="10">
-        <v>169.87</v>
+        <v>170.34</v>
       </c>
       <c r="G8" s="10">
-        <v>160.03</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>167.73</v>
+        <v>165.46</v>
       </c>
       <c r="E9" s="13">
-        <v>159.87</v>
+        <v>160.34</v>
       </c>
       <c r="F9" s="13">
-        <v>169.87</v>
+        <v>170.34</v>
       </c>
       <c r="G9" s="13">
-        <v>160.03</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>169.16</v>
+        <v>166.84</v>
       </c>
       <c r="E10" s="10">
-        <v>162.41999999999999</v>
+        <v>162.85</v>
       </c>
       <c r="F10" s="10">
-        <v>172.42</v>
+        <v>172.85</v>
       </c>
       <c r="G10" s="10">
-        <v>162.91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>170.56</v>
+        <v>167.73</v>
       </c>
       <c r="E11" s="13">
-        <v>160.32</v>
+        <v>159.87</v>
       </c>
       <c r="F11" s="13">
-        <v>170.32</v>
+        <v>169.87</v>
       </c>
       <c r="G11" s="13">
-        <v>160.47999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>170.56</v>
+        <v>167.73</v>
       </c>
       <c r="E12" s="10">
-        <v>160.32</v>
+        <v>159.87</v>
       </c>
       <c r="F12" s="10">
-        <v>170.32</v>
+        <v>169.87</v>
       </c>
       <c r="G12" s="10">
-        <v>160.47999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>171.98</v>
+        <v>169.16</v>
       </c>
       <c r="E13" s="13">
-        <v>162.4</v>
+        <v>162.41999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>172.4</v>
+        <v>172.42</v>
       </c>
       <c r="G13" s="13">
-        <v>162.88999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>162.91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,35 +970,35 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>172.4</v>
+        <v>170.02</v>
       </c>
       <c r="E17" s="10">
-        <v>164.85</v>
+        <v>165.22</v>
       </c>
       <c r="F17" s="10">
-        <v>174.85</v>
+        <v>175.22</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>175.23</v>
+        <v>172.4</v>
       </c>
       <c r="E18" s="13">
         <v>164.85</v>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>168.53</v>
+        <v>166.27</v>
       </c>
       <c r="E22" s="10">
-        <v>161.68</v>
+        <v>162.09</v>
       </c>
       <c r="F22" s="10">
-        <v>171.28</v>
+        <v>171.69</v>
       </c>
       <c r="G22" s="10">
-        <v>162.97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163.38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>173.95</v>
+        <v>171.63</v>
       </c>
       <c r="E23" s="13">
-        <v>166.44</v>
+        <v>166.87</v>
       </c>
       <c r="F23" s="13">
-        <v>176.44</v>
+        <v>176.87</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>173.73</v>
+        <v>171.41</v>
       </c>
       <c r="E24" s="10">
-        <v>166.85</v>
+        <v>167.3</v>
       </c>
       <c r="F24" s="10">
-        <v>176.85</v>
+        <v>177.3</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>174.56</v>
+        <v>172.24</v>
       </c>
       <c r="E25" s="13">
-        <v>166.26</v>
+        <v>166.71</v>
       </c>
       <c r="F25" s="13">
-        <v>176.26</v>
+        <v>176.71</v>
       </c>
       <c r="G25" s="13">
-        <v>166.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>173.23</v>
+        <v>170.89</v>
       </c>
       <c r="E26" s="10">
-        <v>167.7</v>
+        <v>168.16</v>
       </c>
       <c r="F26" s="10">
-        <v>177.7</v>
+        <v>178.16</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>171.46</v>
+        <v>168.53</v>
       </c>
       <c r="E27" s="13">
-        <v>161.55000000000001</v>
+        <v>161.68</v>
       </c>
       <c r="F27" s="13">
-        <v>171.15</v>
+        <v>171.28</v>
       </c>
       <c r="G27" s="13">
-        <v>162.84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>162.97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>176.76</v>
+        <v>173.95</v>
       </c>
       <c r="E28" s="22">
-        <v>166.42</v>
+        <v>166.44</v>
       </c>
       <c r="F28" s="22">
-        <v>176.42</v>
+        <v>176.44</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>176.55</v>
+        <v>173.73</v>
       </c>
       <c r="E29" s="13">
-        <v>166.82</v>
+        <v>166.85</v>
       </c>
       <c r="F29" s="13">
-        <v>176.82</v>
+        <v>176.85</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>177.37</v>
+        <v>174.56</v>
       </c>
       <c r="E30" s="22">
-        <v>166.23</v>
+        <v>166.26</v>
       </c>
       <c r="F30" s="22">
-        <v>176.23</v>
+        <v>176.26</v>
       </c>
       <c r="G30" s="22">
-        <v>166.27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>176.05</v>
+        <v>173.23</v>
       </c>
       <c r="E31" s="13">
-        <v>167.67</v>
+        <v>167.7</v>
       </c>
       <c r="F31" s="13">
-        <v>177.67</v>
+        <v>177.7</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>167.4</v>
+        <v>165.2</v>
       </c>
       <c r="E35" s="10">
-        <v>159.4</v>
+        <v>159.84</v>
       </c>
       <c r="F35" s="10">
-        <v>168.4</v>
+        <v>168.84</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>170.32</v>
+        <v>167.4</v>
       </c>
       <c r="E36" s="13">
-        <v>159.38</v>
+        <v>159.4</v>
       </c>
       <c r="F36" s="13">
-        <v>168.38</v>
+        <v>168.4</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>173.22</v>
+        <v>170.94</v>
       </c>
       <c r="E40" s="10">
-        <v>164.92</v>
+        <v>165.4</v>
       </c>
       <c r="F40" s="10">
-        <v>174.92</v>
+        <v>175.4</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>172.92</v>
+        <v>170.65</v>
       </c>
       <c r="E41" s="13">
-        <v>165.34</v>
+        <v>165.82</v>
       </c>
       <c r="F41" s="13">
-        <v>175.34</v>
+        <v>175.82</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>176.02</v>
+        <v>173.22</v>
       </c>
       <c r="E42" s="10">
-        <v>164.89</v>
+        <v>164.92</v>
       </c>
       <c r="F42" s="10">
-        <v>174.89</v>
+        <v>174.92</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>175.72</v>
+        <v>172.92</v>
       </c>
       <c r="E43" s="13">
-        <v>165.31</v>
+        <v>165.34</v>
       </c>
       <c r="F43" s="13">
-        <v>175.31</v>
+        <v>175.34</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>170.65</v>
+        <v>168.41</v>
       </c>
       <c r="E47" s="10">
-        <v>161.44</v>
+        <v>161.24</v>
       </c>
       <c r="F47" s="10">
-        <v>171.44</v>
+        <v>171.24</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>170.58</v>
+        <v>168.33</v>
       </c>
       <c r="E48" s="13">
-        <v>161.58000000000001</v>
+        <v>161.37</v>
       </c>
       <c r="F48" s="13">
-        <v>171.58</v>
+        <v>171.37</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>172.37</v>
+        <v>170.65</v>
       </c>
       <c r="E49" s="10">
-        <v>161.69</v>
+        <v>161.44</v>
       </c>
       <c r="F49" s="10">
-        <v>171.69</v>
+        <v>171.44</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>172.31</v>
+        <v>170.58</v>
       </c>
       <c r="E50" s="13">
-        <v>161.83000000000001</v>
+        <v>161.58000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>171.83</v>
+        <v>171.58</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>183.21</v>
+        <v>180.86</v>
       </c>
       <c r="E54" s="10">
-        <v>175.95</v>
+        <v>176.62</v>
       </c>
       <c r="F54" s="10">
-        <v>185.95</v>
+        <v>186.62</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>171.13</v>
+        <v>168.81</v>
       </c>
       <c r="E55" s="13">
-        <v>172.47</v>
+        <v>172.85</v>
       </c>
       <c r="F55" s="13">
-        <v>182.47</v>
+        <v>182.85</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>173.44</v>
+        <v>171.13</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>172.81</v>
+        <v>170.43</v>
       </c>
       <c r="E57" s="13">
-        <v>166.74</v>
+        <v>167.11</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>168.72</v>
+        <v>166.34</v>
       </c>
       <c r="E58" s="10">
-        <v>162.79</v>
+        <v>163.16999999999999</v>
       </c>
       <c r="F58" s="10">
-        <v>172.79</v>
+        <v>173.17</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>175.34</v>
+        <v>172.95</v>
       </c>
       <c r="E59" s="13">
-        <v>173.8</v>
+        <v>174.36</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>186.05</v>
+        <v>183.21</v>
       </c>
       <c r="E60" s="10">
-        <v>175.85</v>
+        <v>175.95</v>
       </c>
       <c r="F60" s="10">
-        <v>185.85</v>
+        <v>185.95</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>173.95</v>
+        <v>171.13</v>
       </c>
       <c r="E61" s="13">
-        <v>172.48</v>
+        <v>172.47</v>
       </c>
       <c r="F61" s="13">
-        <v>182.48</v>
+        <v>182.47</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>176.25</v>
+        <v>173.44</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,16 +1776,16 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>175.64</v>
+        <v>172.81</v>
       </c>
       <c r="E63" s="13">
         <v>166.74</v>
@@ -1795,38 +1795,38 @@
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>171.55</v>
+        <v>168.72</v>
       </c>
       <c r="E64" s="10">
-        <v>162.80000000000001</v>
+        <v>162.79</v>
       </c>
       <c r="F64" s="10">
-        <v>172.8</v>
+        <v>172.79</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>178.17</v>
+        <v>175.34</v>
       </c>
       <c r="E65" s="13">
-        <v>173.74</v>
+        <v>173.8</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1872,6 +1863,15 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,14 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2156,6 +2148,14 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Mon Dec  1 03:19:12 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{FFA194FD-F452-4AF1-8580-E0DACC17DAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{41B1401D-FFB6-4165-82F6-D9077943C928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>165.46</v>
+        <v>164.35</v>
       </c>
       <c r="E8" s="10">
-        <v>160.34</v>
+        <v>160.5</v>
       </c>
       <c r="F8" s="10">
-        <v>170.34</v>
+        <v>170.5</v>
       </c>
       <c r="G8" s="10">
-        <v>160.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.61000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>165.46</v>
+        <v>164.35</v>
       </c>
       <c r="E9" s="13">
-        <v>160.34</v>
+        <v>160.5</v>
       </c>
       <c r="F9" s="13">
-        <v>170.34</v>
+        <v>170.5</v>
       </c>
       <c r="G9" s="13">
-        <v>160.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.61000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>166.84</v>
+        <v>165.96</v>
       </c>
       <c r="E10" s="10">
-        <v>162.85</v>
+        <v>163.34</v>
       </c>
       <c r="F10" s="10">
-        <v>172.85</v>
+        <v>173.34</v>
       </c>
       <c r="G10" s="10">
-        <v>163.34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>167.73</v>
+        <v>165.46</v>
       </c>
       <c r="E11" s="13">
-        <v>159.87</v>
+        <v>160.34</v>
       </c>
       <c r="F11" s="13">
-        <v>169.87</v>
+        <v>170.34</v>
       </c>
       <c r="G11" s="13">
-        <v>160.03</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>167.73</v>
+        <v>165.46</v>
       </c>
       <c r="E12" s="10">
-        <v>159.87</v>
+        <v>160.34</v>
       </c>
       <c r="F12" s="10">
-        <v>169.87</v>
+        <v>170.34</v>
       </c>
       <c r="G12" s="10">
-        <v>160.03</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>169.16</v>
+        <v>166.84</v>
       </c>
       <c r="E13" s="13">
-        <v>162.41999999999999</v>
+        <v>162.85</v>
       </c>
       <c r="F13" s="13">
-        <v>172.42</v>
+        <v>172.85</v>
       </c>
       <c r="G13" s="13">
-        <v>162.91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>170.02</v>
+        <v>169.08</v>
       </c>
       <c r="E17" s="10">
-        <v>165.22</v>
+        <v>165.68</v>
       </c>
       <c r="F17" s="10">
-        <v>175.22</v>
+        <v>175.68</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>172.4</v>
+        <v>170.02</v>
       </c>
       <c r="E18" s="13">
-        <v>164.85</v>
+        <v>165.22</v>
       </c>
       <c r="F18" s="13">
-        <v>174.85</v>
+        <v>175.22</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>166.27</v>
+        <v>165.37</v>
       </c>
       <c r="E22" s="10">
-        <v>162.09</v>
+        <v>162.57</v>
       </c>
       <c r="F22" s="10">
-        <v>171.69</v>
+        <v>172.17</v>
       </c>
       <c r="G22" s="10">
-        <v>163.38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.72999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>171.63</v>
+        <v>170.75</v>
       </c>
       <c r="E23" s="13">
-        <v>166.87</v>
+        <v>167.36</v>
       </c>
       <c r="F23" s="13">
-        <v>176.87</v>
+        <v>177.36</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>171.41</v>
+        <v>170.52</v>
       </c>
       <c r="E24" s="10">
-        <v>167.3</v>
+        <v>167.81</v>
       </c>
       <c r="F24" s="10">
-        <v>177.3</v>
+        <v>177.81</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>172.24</v>
+        <v>171.35</v>
       </c>
       <c r="E25" s="13">
-        <v>166.71</v>
+        <v>167.23</v>
       </c>
       <c r="F25" s="13">
-        <v>176.71</v>
+        <v>177.23</v>
       </c>
       <c r="G25" s="13">
-        <v>166.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>170.89</v>
+        <v>169.99</v>
       </c>
       <c r="E26" s="10">
-        <v>168.16</v>
+        <v>168.69</v>
       </c>
       <c r="F26" s="10">
-        <v>178.16</v>
+        <v>178.69</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>168.53</v>
+        <v>166.27</v>
       </c>
       <c r="E27" s="13">
-        <v>161.68</v>
+        <v>162.09</v>
       </c>
       <c r="F27" s="13">
-        <v>171.28</v>
+        <v>171.69</v>
       </c>
       <c r="G27" s="13">
-        <v>162.97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>173.95</v>
+        <v>171.63</v>
       </c>
       <c r="E28" s="22">
-        <v>166.44</v>
+        <v>166.87</v>
       </c>
       <c r="F28" s="22">
-        <v>176.44</v>
+        <v>176.87</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>173.73</v>
+        <v>171.41</v>
       </c>
       <c r="E29" s="13">
-        <v>166.85</v>
+        <v>167.3</v>
       </c>
       <c r="F29" s="13">
-        <v>176.85</v>
+        <v>177.3</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>174.56</v>
+        <v>172.24</v>
       </c>
       <c r="E30" s="22">
-        <v>166.26</v>
+        <v>166.71</v>
       </c>
       <c r="F30" s="22">
-        <v>176.26</v>
+        <v>176.71</v>
       </c>
       <c r="G30" s="22">
-        <v>166.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>166.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>173.23</v>
+        <v>170.89</v>
       </c>
       <c r="E31" s="13">
-        <v>167.7</v>
+        <v>168.16</v>
       </c>
       <c r="F31" s="13">
-        <v>177.7</v>
+        <v>178.16</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>165.2</v>
+        <v>164.32</v>
       </c>
       <c r="E35" s="10">
-        <v>159.84</v>
+        <v>160.33000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>168.84</v>
+        <v>169.33</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>167.4</v>
+        <v>165.2</v>
       </c>
       <c r="E36" s="13">
-        <v>159.4</v>
+        <v>159.84</v>
       </c>
       <c r="F36" s="13">
-        <v>168.4</v>
+        <v>168.84</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>170.94</v>
+        <v>170.1</v>
       </c>
       <c r="E40" s="10">
-        <v>165.4</v>
+        <v>165.96</v>
       </c>
       <c r="F40" s="10">
-        <v>175.4</v>
+        <v>175.96</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>170.65</v>
+        <v>169.81</v>
       </c>
       <c r="E41" s="13">
-        <v>165.82</v>
+        <v>166.38</v>
       </c>
       <c r="F41" s="13">
-        <v>175.82</v>
+        <v>176.38</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>173.22</v>
+        <v>170.94</v>
       </c>
       <c r="E42" s="10">
-        <v>164.92</v>
+        <v>165.4</v>
       </c>
       <c r="F42" s="10">
-        <v>174.92</v>
+        <v>175.4</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>172.92</v>
+        <v>170.65</v>
       </c>
       <c r="E43" s="13">
-        <v>165.34</v>
+        <v>165.82</v>
       </c>
       <c r="F43" s="13">
-        <v>175.34</v>
+        <v>175.82</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>168.41</v>
+        <v>165.87</v>
       </c>
       <c r="E47" s="10">
-        <v>161.24</v>
+        <v>161.37</v>
       </c>
       <c r="F47" s="10">
-        <v>171.24</v>
+        <v>171.37</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>168.33</v>
+        <v>165.77</v>
       </c>
       <c r="E48" s="13">
-        <v>161.37</v>
+        <v>161.49</v>
       </c>
       <c r="F48" s="13">
-        <v>171.37</v>
+        <v>171.49</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>170.65</v>
+        <v>168.41</v>
       </c>
       <c r="E49" s="10">
-        <v>161.44</v>
+        <v>161.24</v>
       </c>
       <c r="F49" s="10">
-        <v>171.44</v>
+        <v>171.24</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>170.58</v>
+        <v>168.33</v>
       </c>
       <c r="E50" s="13">
-        <v>161.58000000000001</v>
+        <v>161.37</v>
       </c>
       <c r="F50" s="13">
-        <v>171.58</v>
+        <v>171.37</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>180.86</v>
+        <v>179.93</v>
       </c>
       <c r="E54" s="10">
-        <v>176.62</v>
+        <v>177.34</v>
       </c>
       <c r="F54" s="10">
-        <v>186.62</v>
+        <v>187.34</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>168.81</v>
+        <v>167.93</v>
       </c>
       <c r="E55" s="13">
-        <v>172.85</v>
+        <v>173.28</v>
       </c>
       <c r="F55" s="13">
-        <v>182.85</v>
+        <v>183.28</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>171.13</v>
+        <v>170.26</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>170.43</v>
+        <v>169.48</v>
       </c>
       <c r="E57" s="13">
-        <v>167.11</v>
+        <v>167.55</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>166.34</v>
+        <v>165.39</v>
       </c>
       <c r="E58" s="10">
-        <v>163.16999999999999</v>
+        <v>163.6</v>
       </c>
       <c r="F58" s="10">
-        <v>173.17</v>
+        <v>173.6</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>172.95</v>
+        <v>172</v>
       </c>
       <c r="E59" s="13">
-        <v>174.36</v>
+        <v>174.98</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>183.21</v>
+        <v>180.86</v>
       </c>
       <c r="E60" s="10">
-        <v>175.95</v>
+        <v>176.62</v>
       </c>
       <c r="F60" s="10">
-        <v>185.95</v>
+        <v>186.62</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>171.13</v>
+        <v>168.81</v>
       </c>
       <c r="E61" s="13">
-        <v>172.47</v>
+        <v>172.85</v>
       </c>
       <c r="F61" s="13">
-        <v>182.47</v>
+        <v>182.85</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>173.44</v>
+        <v>171.13</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>172.81</v>
+        <v>170.43</v>
       </c>
       <c r="E63" s="13">
-        <v>166.74</v>
+        <v>167.11</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>168.72</v>
+        <v>166.34</v>
       </c>
       <c r="E64" s="10">
-        <v>162.79</v>
+        <v>163.16999999999999</v>
       </c>
       <c r="F64" s="10">
-        <v>172.79</v>
+        <v>173.17</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45989</v>
+        <v>45990</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>175.34</v>
+        <v>172.95</v>
       </c>
       <c r="E65" s="13">
-        <v>173.8</v>
+        <v>174.36</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1863,15 +1872,6 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2135,6 +2135,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2148,14 +2156,6 @@
     <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
     <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Dec  2 02:56:18 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{41B1401D-FFB6-4165-82F6-D9077943C928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{9648AEDD-5A3D-43C4-8C6F-C16E3B134140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>164.35</v>
+        <v>163.91</v>
       </c>
       <c r="E8" s="10">
-        <v>160.5</v>
+        <v>161.19999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>170.5</v>
+        <v>171.2</v>
       </c>
       <c r="G8" s="10">
-        <v>160.61000000000001</v>
+        <v>161.31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>164.35</v>
+        <v>163.91</v>
       </c>
       <c r="E9" s="13">
-        <v>160.5</v>
+        <v>161.19999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>170.5</v>
+        <v>171.2</v>
       </c>
       <c r="G9" s="13">
-        <v>160.61000000000001</v>
+        <v>161.31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>165.96</v>
+        <v>165.71</v>
       </c>
       <c r="E10" s="10">
-        <v>163.34</v>
+        <v>164</v>
       </c>
       <c r="F10" s="10">
-        <v>173.34</v>
+        <v>174</v>
       </c>
       <c r="G10" s="10">
-        <v>163.86</v>
+        <v>164.51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>165.46</v>
+        <v>164.35</v>
       </c>
       <c r="E11" s="13">
-        <v>160.34</v>
+        <v>160.5</v>
       </c>
       <c r="F11" s="13">
-        <v>170.34</v>
+        <v>170.5</v>
       </c>
       <c r="G11" s="13">
-        <v>160.5</v>
+        <v>160.61000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>165.46</v>
+        <v>164.35</v>
       </c>
       <c r="E12" s="10">
-        <v>160.34</v>
+        <v>160.5</v>
       </c>
       <c r="F12" s="10">
-        <v>170.34</v>
+        <v>170.5</v>
       </c>
       <c r="G12" s="10">
-        <v>160.5</v>
+        <v>160.61000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>166.84</v>
+        <v>165.96</v>
       </c>
       <c r="E13" s="13">
-        <v>162.85</v>
+        <v>163.34</v>
       </c>
       <c r="F13" s="13">
-        <v>172.85</v>
+        <v>173.34</v>
       </c>
       <c r="G13" s="13">
-        <v>163.34</v>
+        <v>163.86</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>169.08</v>
+        <v>168.77</v>
       </c>
       <c r="E17" s="10">
-        <v>165.68</v>
+        <v>166.31</v>
       </c>
       <c r="F17" s="10">
-        <v>175.68</v>
+        <v>176.31</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>170.02</v>
+        <v>169.08</v>
       </c>
       <c r="E18" s="13">
-        <v>165.22</v>
+        <v>165.68</v>
       </c>
       <c r="F18" s="13">
-        <v>175.22</v>
+        <v>175.68</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>165.37</v>
+        <v>164.94</v>
       </c>
       <c r="E22" s="10">
-        <v>162.57</v>
+        <v>163.21</v>
       </c>
       <c r="F22" s="10">
-        <v>172.17</v>
+        <v>172.81</v>
       </c>
       <c r="G22" s="10">
-        <v>163.72999999999999</v>
+        <v>164.37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>170.75</v>
+        <v>170.5</v>
       </c>
       <c r="E23" s="13">
-        <v>167.36</v>
+        <v>168.01</v>
       </c>
       <c r="F23" s="13">
-        <v>177.36</v>
+        <v>178.01</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>170.52</v>
+        <v>170.27</v>
       </c>
       <c r="E24" s="10">
-        <v>167.81</v>
+        <v>168.49</v>
       </c>
       <c r="F24" s="10">
-        <v>177.81</v>
+        <v>178.49</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>171.35</v>
+        <v>171.1</v>
       </c>
       <c r="E25" s="13">
-        <v>167.23</v>
+        <v>167.91</v>
       </c>
       <c r="F25" s="13">
-        <v>177.23</v>
+        <v>177.91</v>
       </c>
       <c r="G25" s="13">
-        <v>167</v>
+        <v>167.68</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>169.99</v>
+        <v>169.72</v>
       </c>
       <c r="E26" s="10">
-        <v>168.69</v>
+        <v>169.37</v>
       </c>
       <c r="F26" s="10">
-        <v>178.69</v>
+        <v>179.37</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>166.27</v>
+        <v>165.37</v>
       </c>
       <c r="E27" s="13">
-        <v>162.09</v>
+        <v>162.57</v>
       </c>
       <c r="F27" s="13">
-        <v>171.69</v>
+        <v>172.17</v>
       </c>
       <c r="G27" s="13">
-        <v>163.38</v>
+        <v>163.72999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>171.63</v>
+        <v>170.75</v>
       </c>
       <c r="E28" s="22">
-        <v>166.87</v>
+        <v>167.36</v>
       </c>
       <c r="F28" s="22">
-        <v>176.87</v>
+        <v>177.36</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>171.41</v>
+        <v>170.52</v>
       </c>
       <c r="E29" s="13">
-        <v>167.3</v>
+        <v>167.81</v>
       </c>
       <c r="F29" s="13">
-        <v>177.3</v>
+        <v>177.81</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>172.24</v>
+        <v>171.35</v>
       </c>
       <c r="E30" s="22">
-        <v>166.71</v>
+        <v>167.23</v>
       </c>
       <c r="F30" s="22">
-        <v>176.71</v>
+        <v>177.23</v>
       </c>
       <c r="G30" s="22">
-        <v>166.75</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>170.89</v>
+        <v>169.99</v>
       </c>
       <c r="E31" s="13">
-        <v>168.16</v>
+        <v>168.69</v>
       </c>
       <c r="F31" s="13">
-        <v>178.16</v>
+        <v>178.69</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>164.32</v>
+        <v>164.07</v>
       </c>
       <c r="E35" s="10">
-        <v>160.33000000000001</v>
+        <v>160.99</v>
       </c>
       <c r="F35" s="10">
-        <v>169.33</v>
+        <v>169.99</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>165.2</v>
+        <v>164.32</v>
       </c>
       <c r="E36" s="13">
-        <v>159.84</v>
+        <v>160.33000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>168.84</v>
+        <v>169.33</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>170.1</v>
+        <v>169.89</v>
       </c>
       <c r="E40" s="10">
-        <v>165.96</v>
+        <v>166.7</v>
       </c>
       <c r="F40" s="10">
-        <v>175.96</v>
+        <v>176.7</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>169.81</v>
+        <v>169.6</v>
       </c>
       <c r="E41" s="13">
-        <v>166.38</v>
+        <v>167.12</v>
       </c>
       <c r="F41" s="13">
-        <v>176.38</v>
+        <v>177.12</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>170.94</v>
+        <v>170.1</v>
       </c>
       <c r="E42" s="10">
-        <v>165.4</v>
+        <v>165.96</v>
       </c>
       <c r="F42" s="10">
-        <v>175.4</v>
+        <v>175.96</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>170.65</v>
+        <v>169.81</v>
       </c>
       <c r="E43" s="13">
-        <v>165.82</v>
+        <v>166.38</v>
       </c>
       <c r="F43" s="13">
-        <v>175.82</v>
+        <v>176.38</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>165.87</v>
+        <v>164.4</v>
       </c>
       <c r="E47" s="10">
-        <v>161.37</v>
+        <v>162.04</v>
       </c>
       <c r="F47" s="10">
-        <v>171.37</v>
+        <v>172.04</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>165.77</v>
+        <v>164.29</v>
       </c>
       <c r="E48" s="13">
-        <v>161.49</v>
+        <v>162.16</v>
       </c>
       <c r="F48" s="13">
-        <v>171.49</v>
+        <v>172.16</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>168.41</v>
+        <v>165.87</v>
       </c>
       <c r="E49" s="10">
-        <v>161.24</v>
+        <v>161.37</v>
       </c>
       <c r="F49" s="10">
-        <v>171.24</v>
+        <v>171.37</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>168.33</v>
+        <v>165.77</v>
       </c>
       <c r="E50" s="13">
-        <v>161.37</v>
+        <v>161.49</v>
       </c>
       <c r="F50" s="13">
-        <v>171.37</v>
+        <v>171.49</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>179.93</v>
+        <v>179.65</v>
       </c>
       <c r="E54" s="10">
-        <v>177.34</v>
+        <v>178.22</v>
       </c>
       <c r="F54" s="10">
-        <v>187.34</v>
+        <v>188.22</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>167.93</v>
+        <v>167.68</v>
       </c>
       <c r="E55" s="13">
-        <v>173.28</v>
+        <v>173.88</v>
       </c>
       <c r="F55" s="13">
-        <v>183.28</v>
+        <v>183.88</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>170.26</v>
+        <v>170.01</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>169.48</v>
+        <v>169.17</v>
       </c>
       <c r="E57" s="13">
-        <v>167.55</v>
+        <v>168.15</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>165.39</v>
+        <v>165.07</v>
       </c>
       <c r="E58" s="10">
-        <v>163.6</v>
+        <v>164.2</v>
       </c>
       <c r="F58" s="10">
-        <v>173.6</v>
+        <v>174.2</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>172</v>
+        <v>171.69</v>
       </c>
       <c r="E59" s="13">
-        <v>174.98</v>
+        <v>175.75</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>180.86</v>
+        <v>179.93</v>
       </c>
       <c r="E60" s="10">
-        <v>176.62</v>
+        <v>177.34</v>
       </c>
       <c r="F60" s="10">
-        <v>186.62</v>
+        <v>187.34</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>168.81</v>
+        <v>167.93</v>
       </c>
       <c r="E61" s="13">
-        <v>172.85</v>
+        <v>173.28</v>
       </c>
       <c r="F61" s="13">
-        <v>182.85</v>
+        <v>183.28</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>171.13</v>
+        <v>170.26</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>170.43</v>
+        <v>169.48</v>
       </c>
       <c r="E63" s="13">
-        <v>167.11</v>
+        <v>167.55</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>166.34</v>
+        <v>165.39</v>
       </c>
       <c r="E64" s="10">
-        <v>163.16999999999999</v>
+        <v>163.6</v>
       </c>
       <c r="F64" s="10">
-        <v>173.17</v>
+        <v>173.6</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45990</v>
+        <v>45993</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>172.95</v>
+        <v>172</v>
       </c>
       <c r="E65" s="13">
-        <v>174.36</v>
+        <v>174.98</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1864,17 +1864,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,6 +2123,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
@@ -2143,24 +2143,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,6 +2162,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Wed Dec  3 02:55:24 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{9648AEDD-5A3D-43C4-8C6F-C16E3B134140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{C0D10CC2-DE7A-41C3-A7A4-69142849BF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-28920" yWindow="60" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>163.91</v>
+        <v>163.51</v>
       </c>
       <c r="E8" s="10">
-        <v>161.19999999999999</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F8" s="10">
-        <v>171.2</v>
+        <v>171.86</v>
       </c>
       <c r="G8" s="10">
-        <v>161.31</v>
+        <v>161.97</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>163.91</v>
+        <v>163.51</v>
       </c>
       <c r="E9" s="13">
-        <v>161.19999999999999</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F9" s="13">
-        <v>171.2</v>
+        <v>171.86</v>
       </c>
       <c r="G9" s="13">
-        <v>161.31</v>
+        <v>161.97</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>165.71</v>
+        <v>165.38</v>
       </c>
       <c r="E10" s="10">
-        <v>164</v>
+        <v>164.6</v>
       </c>
       <c r="F10" s="10">
-        <v>174</v>
+        <v>174.6</v>
       </c>
       <c r="G10" s="10">
-        <v>164.51</v>
+        <v>165.12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>164.35</v>
+        <v>163.91</v>
       </c>
       <c r="E11" s="13">
-        <v>160.5</v>
+        <v>161.19999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>170.5</v>
+        <v>171.2</v>
       </c>
       <c r="G11" s="13">
-        <v>160.61000000000001</v>
+        <v>161.31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>164.35</v>
+        <v>163.91</v>
       </c>
       <c r="E12" s="10">
-        <v>160.5</v>
+        <v>161.19999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>170.5</v>
+        <v>171.2</v>
       </c>
       <c r="G12" s="10">
-        <v>160.61000000000001</v>
+        <v>161.31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>165.96</v>
+        <v>165.71</v>
       </c>
       <c r="E13" s="13">
-        <v>163.34</v>
+        <v>164</v>
       </c>
       <c r="F13" s="13">
-        <v>173.34</v>
+        <v>174</v>
       </c>
       <c r="G13" s="13">
-        <v>163.86</v>
+        <v>164.51</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>168.77</v>
+        <v>168.37</v>
       </c>
       <c r="E17" s="10">
-        <v>166.31</v>
+        <v>167.07</v>
       </c>
       <c r="F17" s="10">
-        <v>176.31</v>
+        <v>177.07</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>169.08</v>
+        <v>168.77</v>
       </c>
       <c r="E18" s="13">
-        <v>165.68</v>
+        <v>166.31</v>
       </c>
       <c r="F18" s="13">
-        <v>175.68</v>
+        <v>176.31</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>164.94</v>
+        <v>164.32</v>
       </c>
       <c r="E22" s="10">
-        <v>163.21</v>
+        <v>163.79</v>
       </c>
       <c r="F22" s="10">
-        <v>172.81</v>
+        <v>173.39</v>
       </c>
       <c r="G22" s="10">
-        <v>164.37</v>
+        <v>164.95</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>170.5</v>
+        <v>170.4</v>
       </c>
       <c r="E23" s="13">
-        <v>168.01</v>
+        <v>168.83</v>
       </c>
       <c r="F23" s="13">
-        <v>178.01</v>
+        <v>178.83</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>170.27</v>
+        <v>170.16</v>
       </c>
       <c r="E24" s="10">
-        <v>168.49</v>
+        <v>169.12</v>
       </c>
       <c r="F24" s="10">
-        <v>178.49</v>
+        <v>179.12</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>171.1</v>
+        <v>170.77</v>
       </c>
       <c r="E25" s="13">
-        <v>167.91</v>
+        <v>168.55</v>
       </c>
       <c r="F25" s="13">
-        <v>177.91</v>
+        <v>178.55</v>
       </c>
       <c r="G25" s="13">
-        <v>167.68</v>
+        <v>168.32</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>169.72</v>
+        <v>169.59</v>
       </c>
       <c r="E26" s="10">
-        <v>169.37</v>
+        <v>170.01</v>
       </c>
       <c r="F26" s="10">
-        <v>179.37</v>
+        <v>180.01</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>165.37</v>
+        <v>164.94</v>
       </c>
       <c r="E27" s="13">
-        <v>162.57</v>
+        <v>163.21</v>
       </c>
       <c r="F27" s="13">
-        <v>172.17</v>
+        <v>172.81</v>
       </c>
       <c r="G27" s="13">
-        <v>163.72999999999999</v>
+        <v>164.37</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>170.75</v>
+        <v>170.5</v>
       </c>
       <c r="E28" s="22">
-        <v>167.36</v>
+        <v>168.01</v>
       </c>
       <c r="F28" s="22">
-        <v>177.36</v>
+        <v>178.01</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>170.52</v>
+        <v>170.27</v>
       </c>
       <c r="E29" s="13">
-        <v>167.81</v>
+        <v>168.49</v>
       </c>
       <c r="F29" s="13">
-        <v>177.81</v>
+        <v>178.49</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>171.35</v>
+        <v>171.1</v>
       </c>
       <c r="E30" s="22">
-        <v>167.23</v>
+        <v>167.91</v>
       </c>
       <c r="F30" s="22">
-        <v>177.23</v>
+        <v>177.91</v>
       </c>
       <c r="G30" s="22">
-        <v>167</v>
+        <v>167.68</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>169.99</v>
+        <v>169.72</v>
       </c>
       <c r="E31" s="13">
-        <v>168.69</v>
+        <v>169.37</v>
       </c>
       <c r="F31" s="13">
-        <v>178.69</v>
+        <v>179.37</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>164.07</v>
+        <v>163.75</v>
       </c>
       <c r="E35" s="10">
-        <v>160.99</v>
+        <v>161.6</v>
       </c>
       <c r="F35" s="10">
-        <v>169.99</v>
+        <v>170.6</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>164.32</v>
+        <v>164.07</v>
       </c>
       <c r="E36" s="13">
-        <v>160.33000000000001</v>
+        <v>160.99</v>
       </c>
       <c r="F36" s="13">
-        <v>169.33</v>
+        <v>169.99</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>169.89</v>
+        <v>169.62</v>
       </c>
       <c r="E40" s="10">
-        <v>166.7</v>
+        <v>167.59</v>
       </c>
       <c r="F40" s="10">
-        <v>176.7</v>
+        <v>177.59</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>169.6</v>
+        <v>169.33</v>
       </c>
       <c r="E41" s="13">
-        <v>167.12</v>
+        <v>168.01</v>
       </c>
       <c r="F41" s="13">
-        <v>177.12</v>
+        <v>178.01</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>170.1</v>
+        <v>169.89</v>
       </c>
       <c r="E42" s="10">
-        <v>165.96</v>
+        <v>166.7</v>
       </c>
       <c r="F42" s="10">
-        <v>175.96</v>
+        <v>176.7</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>169.81</v>
+        <v>169.6</v>
       </c>
       <c r="E43" s="13">
-        <v>166.38</v>
+        <v>167.12</v>
       </c>
       <c r="F43" s="13">
-        <v>176.38</v>
+        <v>177.12</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>164.4</v>
+        <v>164.33</v>
       </c>
       <c r="E47" s="10">
-        <v>162.04</v>
+        <v>162.62</v>
       </c>
       <c r="F47" s="10">
-        <v>172.04</v>
+        <v>172.62</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>164.29</v>
+        <v>164.19</v>
       </c>
       <c r="E48" s="13">
-        <v>162.16</v>
+        <v>162.72999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>172.16</v>
+        <v>172.73</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>165.87</v>
+        <v>164.4</v>
       </c>
       <c r="E49" s="10">
-        <v>161.37</v>
+        <v>162.04</v>
       </c>
       <c r="F49" s="10">
-        <v>171.37</v>
+        <v>172.04</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>165.77</v>
+        <v>164.29</v>
       </c>
       <c r="E50" s="13">
-        <v>161.49</v>
+        <v>162.16</v>
       </c>
       <c r="F50" s="13">
-        <v>171.49</v>
+        <v>172.16</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>179.65</v>
+        <v>179.27</v>
       </c>
       <c r="E54" s="10">
-        <v>178.22</v>
+        <v>179.13</v>
       </c>
       <c r="F54" s="10">
-        <v>188.22</v>
+        <v>189.13</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>167.68</v>
+        <v>167.35</v>
       </c>
       <c r="E55" s="13">
-        <v>173.88</v>
+        <v>174.41</v>
       </c>
       <c r="F55" s="13">
-        <v>183.88</v>
+        <v>184.41</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>170.01</v>
+        <v>169.7</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>169.17</v>
+        <v>168.75</v>
       </c>
       <c r="E57" s="13">
-        <v>168.15</v>
+        <v>168.67</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>165.07</v>
+        <v>164.66</v>
       </c>
       <c r="E58" s="10">
-        <v>164.2</v>
+        <v>164.73</v>
       </c>
       <c r="F58" s="10">
-        <v>174.2</v>
+        <v>174.73</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>171.69</v>
+        <v>171.27</v>
       </c>
       <c r="E59" s="13">
-        <v>175.75</v>
+        <v>176.52</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>179.93</v>
+        <v>179.65</v>
       </c>
       <c r="E60" s="10">
-        <v>177.34</v>
+        <v>178.22</v>
       </c>
       <c r="F60" s="10">
-        <v>187.34</v>
+        <v>188.22</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>167.93</v>
+        <v>167.68</v>
       </c>
       <c r="E61" s="13">
-        <v>173.28</v>
+        <v>173.88</v>
       </c>
       <c r="F61" s="13">
-        <v>183.28</v>
+        <v>183.88</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>170.26</v>
+        <v>170.01</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>169.48</v>
+        <v>169.17</v>
       </c>
       <c r="E63" s="13">
-        <v>167.55</v>
+        <v>168.15</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>165.39</v>
+        <v>165.07</v>
       </c>
       <c r="E64" s="10">
-        <v>163.6</v>
+        <v>164.2</v>
       </c>
       <c r="F64" s="10">
-        <v>173.6</v>
+        <v>174.2</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>172</v>
+        <v>171.69</v>
       </c>
       <c r="E65" s="13">
-        <v>174.98</v>
+        <v>175.75</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,12 +1855,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2124,20 +2126,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2163,19 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Thu Dec  4 02:57:07 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{C0D10CC2-DE7A-41C3-A7A4-69142849BF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{96F55874-43E2-4D22-8711-AE8BA658E9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="60" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>163.51</v>
+        <v>163.05000000000001</v>
       </c>
       <c r="E8" s="10">
-        <v>161.86000000000001</v>
+        <v>161.81</v>
       </c>
       <c r="F8" s="10">
-        <v>171.86</v>
+        <v>171.81</v>
       </c>
       <c r="G8" s="10">
-        <v>161.97</v>
+        <v>161.93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>163.51</v>
+        <v>163.05000000000001</v>
       </c>
       <c r="E9" s="13">
-        <v>161.86000000000001</v>
+        <v>161.81</v>
       </c>
       <c r="F9" s="13">
-        <v>171.86</v>
+        <v>171.81</v>
       </c>
       <c r="G9" s="13">
-        <v>161.97</v>
+        <v>161.93</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>165.38</v>
+        <v>165.14</v>
       </c>
       <c r="E10" s="10">
-        <v>164.6</v>
+        <v>164.43</v>
       </c>
       <c r="F10" s="10">
-        <v>174.6</v>
+        <v>174.43</v>
       </c>
       <c r="G10" s="10">
-        <v>165.12</v>
+        <v>164.95</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>163.91</v>
+        <v>163.51</v>
       </c>
       <c r="E11" s="13">
-        <v>161.19999999999999</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F11" s="13">
-        <v>171.2</v>
+        <v>171.86</v>
       </c>
       <c r="G11" s="13">
-        <v>161.31</v>
+        <v>161.97</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>163.91</v>
+        <v>163.51</v>
       </c>
       <c r="E12" s="10">
-        <v>161.19999999999999</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F12" s="10">
-        <v>171.2</v>
+        <v>171.86</v>
       </c>
       <c r="G12" s="10">
-        <v>161.31</v>
+        <v>161.97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>165.71</v>
+        <v>165.38</v>
       </c>
       <c r="E13" s="13">
-        <v>164</v>
+        <v>164.6</v>
       </c>
       <c r="F13" s="13">
-        <v>174</v>
+        <v>174.6</v>
       </c>
       <c r="G13" s="13">
-        <v>164.51</v>
+        <v>165.12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>168.37</v>
+        <v>168.08</v>
       </c>
       <c r="E17" s="10">
-        <v>167.07</v>
+        <v>167.19</v>
       </c>
       <c r="F17" s="10">
-        <v>177.07</v>
+        <v>177.19</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>168.77</v>
+        <v>168.37</v>
       </c>
       <c r="E18" s="13">
-        <v>166.31</v>
+        <v>167.07</v>
       </c>
       <c r="F18" s="13">
-        <v>176.31</v>
+        <v>177.07</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>164.32</v>
+        <v>164.18</v>
       </c>
       <c r="E22" s="10">
-        <v>163.79</v>
+        <v>163.72</v>
       </c>
       <c r="F22" s="10">
-        <v>173.39</v>
+        <v>173.32</v>
       </c>
       <c r="G22" s="10">
-        <v>164.95</v>
+        <v>164.88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>170.4</v>
+        <v>170.17</v>
       </c>
       <c r="E23" s="13">
-        <v>168.83</v>
+        <v>168.65</v>
       </c>
       <c r="F23" s="13">
-        <v>178.83</v>
+        <v>178.65</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>170.16</v>
+        <v>169.93</v>
       </c>
       <c r="E24" s="10">
-        <v>169.12</v>
+        <v>168.97</v>
       </c>
       <c r="F24" s="10">
-        <v>179.12</v>
+        <v>178.97</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>170.77</v>
+        <v>170.54</v>
       </c>
       <c r="E25" s="13">
-        <v>168.55</v>
+        <v>168.41</v>
       </c>
       <c r="F25" s="13">
-        <v>178.55</v>
+        <v>178.41</v>
       </c>
       <c r="G25" s="13">
-        <v>168.32</v>
+        <v>168.18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>169.59</v>
+        <v>169.34</v>
       </c>
       <c r="E26" s="10">
-        <v>170.01</v>
+        <v>169.87</v>
       </c>
       <c r="F26" s="10">
-        <v>180.01</v>
+        <v>179.87</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>164.94</v>
+        <v>164.32</v>
       </c>
       <c r="E27" s="13">
-        <v>163.21</v>
+        <v>163.79</v>
       </c>
       <c r="F27" s="13">
-        <v>172.81</v>
+        <v>173.39</v>
       </c>
       <c r="G27" s="13">
-        <v>164.37</v>
+        <v>164.95</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>170.5</v>
+        <v>170.4</v>
       </c>
       <c r="E28" s="22">
-        <v>168.01</v>
+        <v>168.83</v>
       </c>
       <c r="F28" s="22">
-        <v>178.01</v>
+        <v>178.83</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>170.27</v>
+        <v>170.16</v>
       </c>
       <c r="E29" s="13">
-        <v>168.49</v>
+        <v>169.12</v>
       </c>
       <c r="F29" s="13">
-        <v>178.49</v>
+        <v>179.12</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>171.1</v>
+        <v>170.77</v>
       </c>
       <c r="E30" s="22">
-        <v>167.91</v>
+        <v>168.55</v>
       </c>
       <c r="F30" s="22">
-        <v>177.91</v>
+        <v>178.55</v>
       </c>
       <c r="G30" s="22">
-        <v>167.68</v>
+        <v>168.32</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>169.72</v>
+        <v>169.59</v>
       </c>
       <c r="E31" s="13">
-        <v>169.37</v>
+        <v>170.01</v>
       </c>
       <c r="F31" s="13">
-        <v>179.37</v>
+        <v>180.01</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>163.75</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>161.6</v>
+        <v>161.43</v>
       </c>
       <c r="F35" s="10">
-        <v>170.6</v>
+        <v>170.43</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>164.07</v>
+        <v>163.75</v>
       </c>
       <c r="E36" s="13">
-        <v>160.99</v>
+        <v>161.6</v>
       </c>
       <c r="F36" s="13">
-        <v>169.99</v>
+        <v>170.6</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>169.62</v>
+        <v>169.43</v>
       </c>
       <c r="E40" s="10">
-        <v>167.59</v>
+        <v>167.81</v>
       </c>
       <c r="F40" s="10">
-        <v>177.59</v>
+        <v>177.81</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>169.33</v>
+        <v>169.14</v>
       </c>
       <c r="E41" s="13">
-        <v>168.01</v>
+        <v>168.23</v>
       </c>
       <c r="F41" s="13">
-        <v>178.01</v>
+        <v>178.23</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>169.89</v>
+        <v>169.62</v>
       </c>
       <c r="E42" s="10">
-        <v>166.7</v>
+        <v>167.59</v>
       </c>
       <c r="F42" s="10">
-        <v>176.7</v>
+        <v>177.59</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>169.6</v>
+        <v>169.33</v>
       </c>
       <c r="E43" s="13">
-        <v>167.12</v>
+        <v>168.01</v>
       </c>
       <c r="F43" s="13">
-        <v>177.12</v>
+        <v>178.01</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>164.33</v>
+        <v>163.68</v>
       </c>
       <c r="E47" s="10">
-        <v>162.62</v>
+        <v>163.33000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>172.62</v>
+        <v>173.33</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>164.19</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="E48" s="13">
-        <v>162.72999999999999</v>
+        <v>163.44</v>
       </c>
       <c r="F48" s="13">
-        <v>172.73</v>
+        <v>173.44</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>164.4</v>
+        <v>164.33</v>
       </c>
       <c r="E49" s="10">
-        <v>162.04</v>
+        <v>162.62</v>
       </c>
       <c r="F49" s="10">
-        <v>172.04</v>
+        <v>172.62</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>164.29</v>
+        <v>164.19</v>
       </c>
       <c r="E50" s="13">
-        <v>162.16</v>
+        <v>162.72999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>172.16</v>
+        <v>172.73</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>179.27</v>
+        <v>179.01</v>
       </c>
       <c r="E54" s="10">
-        <v>179.13</v>
+        <v>179.19</v>
       </c>
       <c r="F54" s="10">
-        <v>189.13</v>
+        <v>189.19</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>167.35</v>
+        <v>167.12</v>
       </c>
       <c r="E55" s="13">
-        <v>174.41</v>
+        <v>174.3</v>
       </c>
       <c r="F55" s="13">
-        <v>184.41</v>
+        <v>184.3</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>169.7</v>
+        <v>169.59</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>168.75</v>
+        <v>168.57</v>
       </c>
       <c r="E57" s="13">
-        <v>168.67</v>
+        <v>168.56</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>164.66</v>
+        <v>164.47</v>
       </c>
       <c r="E58" s="10">
-        <v>164.73</v>
+        <v>164.62</v>
       </c>
       <c r="F58" s="10">
-        <v>174.73</v>
+        <v>174.62</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>171.27</v>
+        <v>170.98</v>
       </c>
       <c r="E59" s="13">
-        <v>176.52</v>
+        <v>176.48</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>179.65</v>
+        <v>179.27</v>
       </c>
       <c r="E60" s="10">
-        <v>178.22</v>
+        <v>179.13</v>
       </c>
       <c r="F60" s="10">
-        <v>188.22</v>
+        <v>189.13</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>167.68</v>
+        <v>167.35</v>
       </c>
       <c r="E61" s="13">
-        <v>173.88</v>
+        <v>174.41</v>
       </c>
       <c r="F61" s="13">
-        <v>183.88</v>
+        <v>184.41</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>170.01</v>
+        <v>169.7</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>169.17</v>
+        <v>168.75</v>
       </c>
       <c r="E63" s="13">
-        <v>168.15</v>
+        <v>168.67</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>165.07</v>
+        <v>164.66</v>
       </c>
       <c r="E64" s="10">
-        <v>164.2</v>
+        <v>164.73</v>
       </c>
       <c r="F64" s="10">
-        <v>174.2</v>
+        <v>174.73</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>171.69</v>
+        <v>171.27</v>
       </c>
       <c r="E65" s="13">
-        <v>175.75</v>
+        <v>176.52</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,17 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2125,6 +2114,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,24 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2172,6 +2154,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fri Dec  5 02:57:08 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{96F55874-43E2-4D22-8711-AE8BA658E9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8CF926B6-62E6-449A-A9CD-0DEAFA464B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>163.05000000000001</v>
+        <v>162.59</v>
       </c>
       <c r="E8" s="10">
-        <v>161.81</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>171.81</v>
+        <v>171.45</v>
       </c>
       <c r="G8" s="10">
-        <v>161.93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>163.05000000000001</v>
+        <v>162.59</v>
       </c>
       <c r="E9" s="13">
-        <v>161.81</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>171.81</v>
+        <v>171.45</v>
       </c>
       <c r="G9" s="13">
-        <v>161.93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>165.14</v>
+        <v>164.79</v>
       </c>
       <c r="E10" s="10">
-        <v>164.43</v>
+        <v>163.95</v>
       </c>
       <c r="F10" s="10">
-        <v>174.43</v>
+        <v>173.95</v>
       </c>
       <c r="G10" s="10">
-        <v>164.95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>163.51</v>
+        <v>163.05000000000001</v>
       </c>
       <c r="E11" s="13">
-        <v>161.86000000000001</v>
+        <v>161.81</v>
       </c>
       <c r="F11" s="13">
-        <v>171.86</v>
+        <v>171.81</v>
       </c>
       <c r="G11" s="13">
-        <v>161.97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>163.51</v>
+        <v>163.05000000000001</v>
       </c>
       <c r="E12" s="10">
-        <v>161.86000000000001</v>
+        <v>161.81</v>
       </c>
       <c r="F12" s="10">
-        <v>171.86</v>
+        <v>171.81</v>
       </c>
       <c r="G12" s="10">
-        <v>161.97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>165.38</v>
+        <v>165.14</v>
       </c>
       <c r="E13" s="13">
-        <v>164.6</v>
+        <v>164.43</v>
       </c>
       <c r="F13" s="13">
-        <v>174.6</v>
+        <v>174.43</v>
       </c>
       <c r="G13" s="13">
-        <v>165.12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>168.08</v>
+        <v>167.71</v>
       </c>
       <c r="E17" s="10">
-        <v>167.19</v>
+        <v>167.02</v>
       </c>
       <c r="F17" s="10">
-        <v>177.19</v>
+        <v>177.02</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>168.37</v>
+        <v>168.08</v>
       </c>
       <c r="E18" s="13">
-        <v>167.07</v>
+        <v>167.19</v>
       </c>
       <c r="F18" s="13">
-        <v>177.07</v>
+        <v>177.19</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>164.18</v>
+        <v>163.84</v>
       </c>
       <c r="E22" s="10">
-        <v>163.72</v>
+        <v>163.24</v>
       </c>
       <c r="F22" s="10">
-        <v>173.32</v>
+        <v>172.84</v>
       </c>
       <c r="G22" s="10">
-        <v>164.88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>170.17</v>
+        <v>169.82</v>
       </c>
       <c r="E23" s="13">
-        <v>168.65</v>
+        <v>168.17</v>
       </c>
       <c r="F23" s="13">
-        <v>178.65</v>
+        <v>178.17</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>169.93</v>
+        <v>169.58</v>
       </c>
       <c r="E24" s="10">
-        <v>168.97</v>
+        <v>168.49</v>
       </c>
       <c r="F24" s="10">
-        <v>178.97</v>
+        <v>178.49</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>170.54</v>
+        <v>170.19</v>
       </c>
       <c r="E25" s="13">
-        <v>168.41</v>
+        <v>167.93</v>
       </c>
       <c r="F25" s="13">
-        <v>178.41</v>
+        <v>177.93</v>
       </c>
       <c r="G25" s="13">
-        <v>168.18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>167.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>169.34</v>
+        <v>168.99</v>
       </c>
       <c r="E26" s="10">
-        <v>169.87</v>
+        <v>169.39</v>
       </c>
       <c r="F26" s="10">
-        <v>179.87</v>
+        <v>179.39</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>164.32</v>
+        <v>164.18</v>
       </c>
       <c r="E27" s="13">
-        <v>163.79</v>
+        <v>163.72</v>
       </c>
       <c r="F27" s="13">
-        <v>173.39</v>
+        <v>173.32</v>
       </c>
       <c r="G27" s="13">
-        <v>164.95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>170.4</v>
+        <v>170.17</v>
       </c>
       <c r="E28" s="22">
-        <v>168.83</v>
+        <v>168.65</v>
       </c>
       <c r="F28" s="22">
-        <v>178.83</v>
+        <v>178.65</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>170.16</v>
+        <v>169.93</v>
       </c>
       <c r="E29" s="13">
-        <v>169.12</v>
+        <v>168.97</v>
       </c>
       <c r="F29" s="13">
-        <v>179.12</v>
+        <v>178.97</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>170.77</v>
+        <v>170.54</v>
       </c>
       <c r="E30" s="22">
-        <v>168.55</v>
+        <v>168.41</v>
       </c>
       <c r="F30" s="22">
-        <v>178.55</v>
+        <v>178.41</v>
       </c>
       <c r="G30" s="22">
-        <v>168.32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>168.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>169.59</v>
+        <v>169.34</v>
       </c>
       <c r="E31" s="13">
-        <v>170.01</v>
+        <v>169.87</v>
       </c>
       <c r="F31" s="13">
-        <v>180.01</v>
+        <v>179.87</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>163.52000000000001</v>
+        <v>163.06</v>
       </c>
       <c r="E35" s="10">
-        <v>161.43</v>
+        <v>160.94999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>170.43</v>
+        <v>169.95</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>163.75</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>161.6</v>
+        <v>161.43</v>
       </c>
       <c r="F36" s="13">
-        <v>170.6</v>
+        <v>170.43</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>169.43</v>
+        <v>169.09</v>
       </c>
       <c r="E40" s="10">
-        <v>167.81</v>
+        <v>167.68</v>
       </c>
       <c r="F40" s="10">
-        <v>177.81</v>
+        <v>177.68</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>169.14</v>
+        <v>168.8</v>
       </c>
       <c r="E41" s="13">
-        <v>168.23</v>
+        <v>168.09</v>
       </c>
       <c r="F41" s="13">
-        <v>178.23</v>
+        <v>178.09</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>169.62</v>
+        <v>169.43</v>
       </c>
       <c r="E42" s="10">
-        <v>167.59</v>
+        <v>167.81</v>
       </c>
       <c r="F42" s="10">
-        <v>177.59</v>
+        <v>177.81</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>169.33</v>
+        <v>169.14</v>
       </c>
       <c r="E43" s="13">
-        <v>168.01</v>
+        <v>168.23</v>
       </c>
       <c r="F43" s="13">
-        <v>178.01</v>
+        <v>178.23</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>163.68</v>
+        <v>163.65</v>
       </c>
       <c r="E47" s="10">
-        <v>163.33000000000001</v>
+        <v>162.9</v>
       </c>
       <c r="F47" s="10">
-        <v>173.33</v>
+        <v>172.9</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>163.52000000000001</v>
+        <v>163.47999999999999</v>
       </c>
       <c r="E48" s="13">
-        <v>163.44</v>
+        <v>162.99</v>
       </c>
       <c r="F48" s="13">
-        <v>173.44</v>
+        <v>172.99</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>164.33</v>
+        <v>163.68</v>
       </c>
       <c r="E49" s="10">
-        <v>162.62</v>
+        <v>163.33000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>172.62</v>
+        <v>173.33</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>164.19</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="E50" s="13">
-        <v>162.72999999999999</v>
+        <v>163.44</v>
       </c>
       <c r="F50" s="13">
-        <v>172.73</v>
+        <v>173.44</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>179.01</v>
+        <v>178.64</v>
       </c>
       <c r="E54" s="10">
-        <v>179.19</v>
+        <v>178.77</v>
       </c>
       <c r="F54" s="10">
-        <v>189.19</v>
+        <v>188.77</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>167.12</v>
+        <v>166.76</v>
       </c>
       <c r="E55" s="13">
-        <v>174.3</v>
+        <v>173.69</v>
       </c>
       <c r="F55" s="13">
-        <v>184.3</v>
+        <v>183.69</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>169.59</v>
+        <v>169.24</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>168.57</v>
+        <v>168.2</v>
       </c>
       <c r="E57" s="13">
-        <v>168.56</v>
+        <v>167.96</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>164.47</v>
+        <v>164.1</v>
       </c>
       <c r="E58" s="10">
-        <v>164.62</v>
+        <v>164.01</v>
       </c>
       <c r="F58" s="10">
-        <v>174.62</v>
+        <v>174.01</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>170.98</v>
+        <v>170.61</v>
       </c>
       <c r="E59" s="13">
-        <v>176.48</v>
+        <v>176.02</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>179.27</v>
+        <v>179.01</v>
       </c>
       <c r="E60" s="10">
-        <v>179.13</v>
+        <v>179.19</v>
       </c>
       <c r="F60" s="10">
-        <v>189.13</v>
+        <v>189.19</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>167.35</v>
+        <v>167.12</v>
       </c>
       <c r="E61" s="13">
-        <v>174.41</v>
+        <v>174.3</v>
       </c>
       <c r="F61" s="13">
-        <v>184.41</v>
+        <v>184.3</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>169.7</v>
+        <v>169.59</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>168.75</v>
+        <v>168.57</v>
       </c>
       <c r="E63" s="13">
-        <v>168.67</v>
+        <v>168.56</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>164.66</v>
+        <v>164.47</v>
       </c>
       <c r="E64" s="10">
-        <v>164.73</v>
+        <v>164.62</v>
       </c>
       <c r="F64" s="10">
-        <v>174.73</v>
+        <v>174.62</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>171.27</v>
+        <v>170.98</v>
       </c>
       <c r="E65" s="13">
-        <v>176.52</v>
+        <v>176.48</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,42 +2134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2161,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Mon Dec  8 02:59:05 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8CF926B6-62E6-449A-A9CD-0DEAFA464B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{96295068-CC9B-4FC8-B4E2-B62DAB326EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-28920" yWindow="60" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>162.59</v>
+        <v>162.22999999999999</v>
       </c>
       <c r="E8" s="10">
-        <v>161.44999999999999</v>
+        <v>160.99</v>
       </c>
       <c r="F8" s="10">
-        <v>171.45</v>
+        <v>170.99</v>
       </c>
       <c r="G8" s="10">
-        <v>161.57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.11000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>162.59</v>
+        <v>162.22999999999999</v>
       </c>
       <c r="E9" s="13">
-        <v>161.44999999999999</v>
+        <v>160.99</v>
       </c>
       <c r="F9" s="13">
-        <v>171.45</v>
+        <v>170.99</v>
       </c>
       <c r="G9" s="13">
-        <v>161.57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.11000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>164.79</v>
+        <v>164.17</v>
       </c>
       <c r="E10" s="10">
-        <v>163.95</v>
+        <v>163.32</v>
       </c>
       <c r="F10" s="10">
-        <v>173.95</v>
+        <v>173.32</v>
       </c>
       <c r="G10" s="10">
-        <v>164.47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>163.05000000000001</v>
+        <v>162.59</v>
       </c>
       <c r="E11" s="13">
-        <v>161.81</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>171.81</v>
+        <v>171.45</v>
       </c>
       <c r="G11" s="13">
-        <v>161.93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>163.05000000000001</v>
+        <v>162.59</v>
       </c>
       <c r="E12" s="10">
-        <v>161.81</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>171.81</v>
+        <v>171.45</v>
       </c>
       <c r="G12" s="10">
-        <v>161.93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>165.14</v>
+        <v>164.79</v>
       </c>
       <c r="E13" s="13">
-        <v>164.43</v>
+        <v>163.95</v>
       </c>
       <c r="F13" s="13">
-        <v>174.43</v>
+        <v>173.95</v>
       </c>
       <c r="G13" s="13">
-        <v>164.95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>164.47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>167.71</v>
+        <v>167.08</v>
       </c>
       <c r="E17" s="10">
-        <v>167.02</v>
+        <v>166.69</v>
       </c>
       <c r="F17" s="10">
-        <v>177.02</v>
+        <v>176.69</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>168.08</v>
+        <v>167.71</v>
       </c>
       <c r="E18" s="13">
-        <v>167.19</v>
+        <v>167.02</v>
       </c>
       <c r="F18" s="13">
-        <v>177.19</v>
+        <v>177.02</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>163.84</v>
+        <v>163.26</v>
       </c>
       <c r="E22" s="10">
-        <v>163.24</v>
+        <v>162.5</v>
       </c>
       <c r="F22" s="10">
-        <v>172.84</v>
+        <v>172.1</v>
       </c>
       <c r="G22" s="10">
-        <v>164.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>163.66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>169.82</v>
+        <v>169.19</v>
       </c>
       <c r="E23" s="13">
-        <v>168.17</v>
+        <v>167.54</v>
       </c>
       <c r="F23" s="13">
-        <v>178.17</v>
+        <v>177.54</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>169.58</v>
+        <v>168.95</v>
       </c>
       <c r="E24" s="10">
-        <v>168.49</v>
+        <v>167.87</v>
       </c>
       <c r="F24" s="10">
-        <v>178.49</v>
+        <v>177.87</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>170.19</v>
+        <v>169.56</v>
       </c>
       <c r="E25" s="13">
-        <v>167.93</v>
+        <v>167.3</v>
       </c>
       <c r="F25" s="13">
-        <v>177.93</v>
+        <v>177.3</v>
       </c>
       <c r="G25" s="13">
-        <v>167.7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>167.07</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>168.99</v>
+        <v>168.36</v>
       </c>
       <c r="E26" s="10">
-        <v>169.39</v>
+        <v>168.75</v>
       </c>
       <c r="F26" s="10">
-        <v>179.39</v>
+        <v>178.75</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>164.18</v>
+        <v>163.84</v>
       </c>
       <c r="E27" s="13">
-        <v>163.72</v>
+        <v>163.24</v>
       </c>
       <c r="F27" s="13">
-        <v>173.32</v>
+        <v>172.84</v>
       </c>
       <c r="G27" s="13">
-        <v>164.88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>170.17</v>
+        <v>169.82</v>
       </c>
       <c r="E28" s="22">
-        <v>168.65</v>
+        <v>168.17</v>
       </c>
       <c r="F28" s="22">
-        <v>178.65</v>
+        <v>178.17</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>169.93</v>
+        <v>169.58</v>
       </c>
       <c r="E29" s="13">
-        <v>168.97</v>
+        <v>168.49</v>
       </c>
       <c r="F29" s="13">
-        <v>178.97</v>
+        <v>178.49</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>170.54</v>
+        <v>170.19</v>
       </c>
       <c r="E30" s="22">
-        <v>168.41</v>
+        <v>167.93</v>
       </c>
       <c r="F30" s="22">
-        <v>178.41</v>
+        <v>177.93</v>
       </c>
       <c r="G30" s="22">
-        <v>168.18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>167.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>169.34</v>
+        <v>168.99</v>
       </c>
       <c r="E31" s="13">
-        <v>169.87</v>
+        <v>169.39</v>
       </c>
       <c r="F31" s="13">
-        <v>179.87</v>
+        <v>179.39</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>163.06</v>
+        <v>162.44</v>
       </c>
       <c r="E35" s="10">
-        <v>160.94999999999999</v>
+        <v>160.33000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>169.95</v>
+        <v>169.33</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>163.52000000000001</v>
+        <v>163.06</v>
       </c>
       <c r="E36" s="13">
-        <v>161.43</v>
+        <v>160.94999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>170.43</v>
+        <v>169.95</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>169.09</v>
+        <v>168.47</v>
       </c>
       <c r="E40" s="10">
-        <v>167.68</v>
+        <v>167.37</v>
       </c>
       <c r="F40" s="10">
-        <v>177.68</v>
+        <v>177.37</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>168.8</v>
+        <v>168.18</v>
       </c>
       <c r="E41" s="13">
-        <v>168.09</v>
+        <v>167.79</v>
       </c>
       <c r="F41" s="13">
-        <v>178.09</v>
+        <v>177.79</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>169.43</v>
+        <v>169.09</v>
       </c>
       <c r="E42" s="10">
-        <v>167.81</v>
+        <v>167.68</v>
       </c>
       <c r="F42" s="10">
-        <v>177.81</v>
+        <v>177.68</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>169.14</v>
+        <v>168.8</v>
       </c>
       <c r="E43" s="13">
-        <v>168.23</v>
+        <v>168.09</v>
       </c>
       <c r="F43" s="13">
-        <v>178.23</v>
+        <v>178.09</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>163.65</v>
+        <v>163.54</v>
       </c>
       <c r="E47" s="10">
-        <v>162.9</v>
+        <v>162.56</v>
       </c>
       <c r="F47" s="10">
-        <v>172.9</v>
+        <v>172.56</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>163.47999999999999</v>
+        <v>163.35</v>
       </c>
       <c r="E48" s="13">
-        <v>162.99</v>
+        <v>162.65</v>
       </c>
       <c r="F48" s="13">
-        <v>172.99</v>
+        <v>172.65</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>163.68</v>
+        <v>163.65</v>
       </c>
       <c r="E49" s="10">
-        <v>163.33000000000001</v>
+        <v>162.9</v>
       </c>
       <c r="F49" s="10">
-        <v>173.33</v>
+        <v>172.9</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>163.52000000000001</v>
+        <v>163.47999999999999</v>
       </c>
       <c r="E50" s="13">
-        <v>163.44</v>
+        <v>162.99</v>
       </c>
       <c r="F50" s="13">
-        <v>173.44</v>
+        <v>172.99</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>178.64</v>
+        <v>177.99</v>
       </c>
       <c r="E54" s="10">
-        <v>178.77</v>
+        <v>178.19</v>
       </c>
       <c r="F54" s="10">
-        <v>188.77</v>
+        <v>188.19</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>166.76</v>
+        <v>166.14</v>
       </c>
       <c r="E55" s="13">
-        <v>173.69</v>
+        <v>173.05</v>
       </c>
       <c r="F55" s="13">
-        <v>183.69</v>
+        <v>183.05</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>169.24</v>
+        <v>168.62</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>168.2</v>
+        <v>167.57</v>
       </c>
       <c r="E57" s="13">
-        <v>167.96</v>
+        <v>167.32</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>164.1</v>
+        <v>163.47</v>
       </c>
       <c r="E58" s="10">
-        <v>164.01</v>
+        <v>163.37</v>
       </c>
       <c r="F58" s="10">
-        <v>174.01</v>
+        <v>173.37</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>170.61</v>
+        <v>169.98</v>
       </c>
       <c r="E59" s="13">
-        <v>176.02</v>
+        <v>175.41</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>179.01</v>
+        <v>178.64</v>
       </c>
       <c r="E60" s="10">
-        <v>179.19</v>
+        <v>178.77</v>
       </c>
       <c r="F60" s="10">
-        <v>189.19</v>
+        <v>188.77</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>167.12</v>
+        <v>166.76</v>
       </c>
       <c r="E61" s="13">
-        <v>174.3</v>
+        <v>173.69</v>
       </c>
       <c r="F61" s="13">
-        <v>184.3</v>
+        <v>183.69</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>169.59</v>
+        <v>169.24</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>168.57</v>
+        <v>168.2</v>
       </c>
       <c r="E63" s="13">
-        <v>168.56</v>
+        <v>167.96</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>164.47</v>
+        <v>164.1</v>
       </c>
       <c r="E64" s="10">
-        <v>164.62</v>
+        <v>164.01</v>
       </c>
       <c r="F64" s="10">
-        <v>174.62</v>
+        <v>174.01</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>170.98</v>
+        <v>170.61</v>
       </c>
       <c r="E65" s="13">
-        <v>176.48</v>
+        <v>176.02</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,26 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,10 +2114,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2161,21 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Dec  9 02:56:33 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{96295068-CC9B-4FC8-B4E2-B62DAB326EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{7984842D-C2DA-490D-99E6-034959EEBF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="60" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>162.22999999999999</v>
+        <v>161.82</v>
       </c>
       <c r="E8" s="10">
-        <v>160.99</v>
+        <v>160.41999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>170.99</v>
+        <v>170.42</v>
       </c>
       <c r="G8" s="10">
-        <v>161.11000000000001</v>
+        <v>160.54</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>162.22999999999999</v>
+        <v>161.82</v>
       </c>
       <c r="E9" s="13">
-        <v>160.99</v>
+        <v>160.41999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>170.99</v>
+        <v>170.42</v>
       </c>
       <c r="G9" s="13">
-        <v>161.11000000000001</v>
+        <v>160.54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>164.17</v>
+        <v>163.65</v>
       </c>
       <c r="E10" s="10">
-        <v>163.32</v>
+        <v>162.63999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>173.32</v>
+        <v>172.64</v>
       </c>
       <c r="G10" s="10">
-        <v>163.84</v>
+        <v>163.16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>162.59</v>
+        <v>162.22999999999999</v>
       </c>
       <c r="E11" s="13">
-        <v>161.44999999999999</v>
+        <v>160.99</v>
       </c>
       <c r="F11" s="13">
-        <v>171.45</v>
+        <v>170.99</v>
       </c>
       <c r="G11" s="13">
-        <v>161.57</v>
+        <v>161.11000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>162.59</v>
+        <v>162.22999999999999</v>
       </c>
       <c r="E12" s="10">
-        <v>161.44999999999999</v>
+        <v>160.99</v>
       </c>
       <c r="F12" s="10">
-        <v>171.45</v>
+        <v>170.99</v>
       </c>
       <c r="G12" s="10">
-        <v>161.57</v>
+        <v>161.11000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>164.79</v>
+        <v>164.17</v>
       </c>
       <c r="E13" s="13">
-        <v>163.95</v>
+        <v>163.32</v>
       </c>
       <c r="F13" s="13">
-        <v>173.95</v>
+        <v>173.32</v>
       </c>
       <c r="G13" s="13">
-        <v>164.47</v>
+        <v>163.84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>167.08</v>
+        <v>166.56</v>
       </c>
       <c r="E17" s="10">
-        <v>166.69</v>
+        <v>166.32</v>
       </c>
       <c r="F17" s="10">
-        <v>176.69</v>
+        <v>176.32</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>167.71</v>
+        <v>167.08</v>
       </c>
       <c r="E18" s="13">
-        <v>167.02</v>
+        <v>166.69</v>
       </c>
       <c r="F18" s="13">
-        <v>177.02</v>
+        <v>176.69</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>163.26</v>
+        <v>162.85</v>
       </c>
       <c r="E22" s="10">
-        <v>162.5</v>
+        <v>161.72</v>
       </c>
       <c r="F22" s="10">
-        <v>172.1</v>
+        <v>171.32</v>
       </c>
       <c r="G22" s="10">
-        <v>163.66</v>
+        <v>162.88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>169.19</v>
+        <v>168.67</v>
       </c>
       <c r="E23" s="13">
-        <v>167.54</v>
+        <v>166.86</v>
       </c>
       <c r="F23" s="13">
-        <v>177.54</v>
+        <v>176.86</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>168.95</v>
+        <v>168.44</v>
       </c>
       <c r="E24" s="10">
-        <v>167.87</v>
+        <v>167.19</v>
       </c>
       <c r="F24" s="10">
-        <v>177.87</v>
+        <v>177.19</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>169.56</v>
+        <v>169.05</v>
       </c>
       <c r="E25" s="13">
-        <v>167.3</v>
+        <v>166.63</v>
       </c>
       <c r="F25" s="13">
-        <v>177.3</v>
+        <v>176.63</v>
       </c>
       <c r="G25" s="13">
-        <v>167.07</v>
+        <v>166.4</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>168.36</v>
+        <v>167.84</v>
       </c>
       <c r="E26" s="10">
-        <v>168.75</v>
+        <v>168.07</v>
       </c>
       <c r="F26" s="10">
-        <v>178.75</v>
+        <v>178.07</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>163.84</v>
+        <v>163.26</v>
       </c>
       <c r="E27" s="13">
-        <v>163.24</v>
+        <v>162.5</v>
       </c>
       <c r="F27" s="13">
-        <v>172.84</v>
+        <v>172.1</v>
       </c>
       <c r="G27" s="13">
-        <v>164.4</v>
+        <v>163.66</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>169.82</v>
+        <v>169.19</v>
       </c>
       <c r="E28" s="22">
-        <v>168.17</v>
+        <v>167.54</v>
       </c>
       <c r="F28" s="22">
-        <v>178.17</v>
+        <v>177.54</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>169.58</v>
+        <v>168.95</v>
       </c>
       <c r="E29" s="13">
-        <v>168.49</v>
+        <v>167.87</v>
       </c>
       <c r="F29" s="13">
-        <v>178.49</v>
+        <v>177.87</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>170.19</v>
+        <v>169.56</v>
       </c>
       <c r="E30" s="22">
-        <v>167.93</v>
+        <v>167.3</v>
       </c>
       <c r="F30" s="22">
-        <v>177.93</v>
+        <v>177.3</v>
       </c>
       <c r="G30" s="22">
-        <v>167.7</v>
+        <v>167.07</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>168.99</v>
+        <v>168.36</v>
       </c>
       <c r="E31" s="13">
-        <v>169.39</v>
+        <v>168.75</v>
       </c>
       <c r="F31" s="13">
-        <v>179.39</v>
+        <v>178.75</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>162.44</v>
+        <v>161.93</v>
       </c>
       <c r="E35" s="10">
-        <v>160.33000000000001</v>
+        <v>159.66</v>
       </c>
       <c r="F35" s="10">
-        <v>169.33</v>
+        <v>168.66</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>163.06</v>
+        <v>162.44</v>
       </c>
       <c r="E36" s="13">
-        <v>160.94999999999999</v>
+        <v>160.33000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>169.95</v>
+        <v>169.33</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>168.47</v>
+        <v>167.96</v>
       </c>
       <c r="E40" s="10">
-        <v>167.37</v>
+        <v>167.02</v>
       </c>
       <c r="F40" s="10">
-        <v>177.37</v>
+        <v>177.02</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>168.18</v>
+        <v>167.67</v>
       </c>
       <c r="E41" s="13">
-        <v>167.79</v>
+        <v>167.44</v>
       </c>
       <c r="F41" s="13">
-        <v>177.79</v>
+        <v>177.44</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>169.09</v>
+        <v>168.47</v>
       </c>
       <c r="E42" s="10">
-        <v>167.68</v>
+        <v>167.37</v>
       </c>
       <c r="F42" s="10">
-        <v>177.68</v>
+        <v>177.37</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>168.8</v>
+        <v>168.18</v>
       </c>
       <c r="E43" s="13">
-        <v>168.09</v>
+        <v>167.79</v>
       </c>
       <c r="F43" s="13">
-        <v>178.09</v>
+        <v>177.79</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>163.54</v>
+        <v>162.79</v>
       </c>
       <c r="E47" s="10">
-        <v>162.56</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="F47" s="10">
-        <v>172.56</v>
+        <v>171.89</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>163.35</v>
+        <v>162.61000000000001</v>
       </c>
       <c r="E48" s="13">
-        <v>162.65</v>
+        <v>161.97999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>172.65</v>
+        <v>171.98</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>163.65</v>
+        <v>163.54</v>
       </c>
       <c r="E49" s="10">
-        <v>162.9</v>
+        <v>162.56</v>
       </c>
       <c r="F49" s="10">
-        <v>172.9</v>
+        <v>172.56</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>163.47999999999999</v>
+        <v>163.35</v>
       </c>
       <c r="E50" s="13">
-        <v>162.99</v>
+        <v>162.65</v>
       </c>
       <c r="F50" s="13">
-        <v>172.99</v>
+        <v>172.65</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>177.99</v>
+        <v>177.45</v>
       </c>
       <c r="E54" s="10">
-        <v>178.19</v>
+        <v>177.54</v>
       </c>
       <c r="F54" s="10">
-        <v>188.19</v>
+        <v>187.54</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>166.14</v>
+        <v>165.62</v>
       </c>
       <c r="E55" s="13">
-        <v>173.05</v>
+        <v>172.49</v>
       </c>
       <c r="F55" s="13">
-        <v>183.05</v>
+        <v>182.49</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>168.62</v>
+        <v>168.21</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>167.57</v>
+        <v>167.16</v>
       </c>
       <c r="E57" s="13">
-        <v>167.32</v>
+        <v>166.76</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>163.47</v>
+        <v>163.06</v>
       </c>
       <c r="E58" s="10">
-        <v>163.37</v>
+        <v>162.81</v>
       </c>
       <c r="F58" s="10">
-        <v>173.37</v>
+        <v>172.81</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>169.98</v>
+        <v>169.46</v>
       </c>
       <c r="E59" s="13">
-        <v>175.41</v>
+        <v>174.75</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>178.64</v>
+        <v>177.99</v>
       </c>
       <c r="E60" s="10">
-        <v>178.77</v>
+        <v>178.19</v>
       </c>
       <c r="F60" s="10">
-        <v>188.77</v>
+        <v>188.19</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>166.76</v>
+        <v>166.14</v>
       </c>
       <c r="E61" s="13">
-        <v>173.69</v>
+        <v>173.05</v>
       </c>
       <c r="F61" s="13">
-        <v>183.69</v>
+        <v>183.05</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>169.24</v>
+        <v>168.62</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>168.2</v>
+        <v>167.57</v>
       </c>
       <c r="E63" s="13">
-        <v>167.96</v>
+        <v>167.32</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>164.1</v>
+        <v>163.47</v>
       </c>
       <c r="E64" s="10">
-        <v>164.01</v>
+        <v>163.37</v>
       </c>
       <c r="F64" s="10">
-        <v>174.01</v>
+        <v>173.37</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>170.61</v>
+        <v>169.98</v>
       </c>
       <c r="E65" s="13">
-        <v>176.02</v>
+        <v>175.41</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,42 +2134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2161,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Wed Dec 10 03:00:29 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{7984842D-C2DA-490D-99E6-034959EEBF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D56696D0-CB6C-4838-A150-AC92026F8421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentManualCount="8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>161.82</v>
+        <v>160.96</v>
       </c>
       <c r="E8" s="10">
-        <v>160.41999999999999</v>
+        <v>159.43</v>
       </c>
       <c r="F8" s="10">
-        <v>170.42</v>
+        <v>169.43</v>
       </c>
       <c r="G8" s="10">
-        <v>160.54</v>
+        <v>159.54</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>161.82</v>
+        <v>160.96</v>
       </c>
       <c r="E9" s="13">
-        <v>160.41999999999999</v>
+        <v>159.43</v>
       </c>
       <c r="F9" s="13">
-        <v>170.42</v>
+        <v>169.43</v>
       </c>
       <c r="G9" s="13">
-        <v>160.54</v>
+        <v>159.54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>163.65</v>
+        <v>162.79</v>
       </c>
       <c r="E10" s="10">
-        <v>162.63999999999999</v>
+        <v>161.66</v>
       </c>
       <c r="F10" s="10">
-        <v>172.64</v>
+        <v>171.66</v>
       </c>
       <c r="G10" s="10">
-        <v>163.16</v>
+        <v>162.18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>162.22999999999999</v>
+        <v>161.82</v>
       </c>
       <c r="E11" s="13">
-        <v>160.99</v>
+        <v>160.41999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>170.99</v>
+        <v>170.42</v>
       </c>
       <c r="G11" s="13">
-        <v>161.11000000000001</v>
+        <v>160.54</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>162.22999999999999</v>
+        <v>161.82</v>
       </c>
       <c r="E12" s="10">
-        <v>160.99</v>
+        <v>160.41999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>170.99</v>
+        <v>170.42</v>
       </c>
       <c r="G12" s="10">
-        <v>161.11000000000001</v>
+        <v>160.54</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>164.17</v>
+        <v>163.65</v>
       </c>
       <c r="E13" s="13">
-        <v>163.32</v>
+        <v>162.63999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>173.32</v>
+        <v>172.64</v>
       </c>
       <c r="G13" s="13">
-        <v>163.84</v>
+        <v>163.16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>166.56</v>
+        <v>165.73</v>
       </c>
       <c r="E17" s="10">
-        <v>166.32</v>
+        <v>165.36</v>
       </c>
       <c r="F17" s="10">
-        <v>176.32</v>
+        <v>175.36</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>167.08</v>
+        <v>166.56</v>
       </c>
       <c r="E18" s="13">
-        <v>166.69</v>
+        <v>166.32</v>
       </c>
       <c r="F18" s="13">
-        <v>176.69</v>
+        <v>176.32</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>162.85</v>
+        <v>162.1</v>
       </c>
       <c r="E22" s="10">
-        <v>161.72</v>
+        <v>160.97</v>
       </c>
       <c r="F22" s="10">
-        <v>171.32</v>
+        <v>170.57</v>
       </c>
       <c r="G22" s="10">
-        <v>162.88</v>
+        <v>162.13</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>168.67</v>
+        <v>167.82</v>
       </c>
       <c r="E23" s="13">
-        <v>166.86</v>
+        <v>165.88</v>
       </c>
       <c r="F23" s="13">
-        <v>176.86</v>
+        <v>175.88</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>168.44</v>
+        <v>167.59</v>
       </c>
       <c r="E24" s="10">
-        <v>167.19</v>
+        <v>166.2</v>
       </c>
       <c r="F24" s="10">
-        <v>177.19</v>
+        <v>176.2</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>169.05</v>
+        <v>168.2</v>
       </c>
       <c r="E25" s="13">
-        <v>166.63</v>
+        <v>165.63</v>
       </c>
       <c r="F25" s="13">
-        <v>176.63</v>
+        <v>175.63</v>
       </c>
       <c r="G25" s="13">
-        <v>166.4</v>
+        <v>165.4</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>167.84</v>
+        <v>166.99</v>
       </c>
       <c r="E26" s="10">
-        <v>168.07</v>
+        <v>167.07</v>
       </c>
       <c r="F26" s="10">
-        <v>178.07</v>
+        <v>177.07</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>163.26</v>
+        <v>162.85</v>
       </c>
       <c r="E27" s="13">
-        <v>162.5</v>
+        <v>161.72</v>
       </c>
       <c r="F27" s="13">
-        <v>172.1</v>
+        <v>171.32</v>
       </c>
       <c r="G27" s="13">
-        <v>163.66</v>
+        <v>162.88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>169.19</v>
+        <v>168.67</v>
       </c>
       <c r="E28" s="22">
-        <v>167.54</v>
+        <v>166.86</v>
       </c>
       <c r="F28" s="22">
-        <v>177.54</v>
+        <v>176.86</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>168.95</v>
+        <v>168.44</v>
       </c>
       <c r="E29" s="13">
-        <v>167.87</v>
+        <v>167.19</v>
       </c>
       <c r="F29" s="13">
-        <v>177.87</v>
+        <v>177.19</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>169.56</v>
+        <v>169.05</v>
       </c>
       <c r="E30" s="22">
-        <v>167.3</v>
+        <v>166.63</v>
       </c>
       <c r="F30" s="22">
-        <v>177.3</v>
+        <v>176.63</v>
       </c>
       <c r="G30" s="22">
-        <v>167.07</v>
+        <v>166.4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>168.36</v>
+        <v>167.84</v>
       </c>
       <c r="E31" s="13">
-        <v>168.75</v>
+        <v>168.07</v>
       </c>
       <c r="F31" s="13">
-        <v>178.75</v>
+        <v>178.07</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>161.93</v>
+        <v>161.08000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>159.66</v>
+        <v>158.68</v>
       </c>
       <c r="F35" s="10">
-        <v>168.66</v>
+        <v>167.68</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>162.44</v>
+        <v>161.93</v>
       </c>
       <c r="E36" s="13">
-        <v>160.33000000000001</v>
+        <v>159.66</v>
       </c>
       <c r="F36" s="13">
-        <v>169.33</v>
+        <v>168.66</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>167.96</v>
+        <v>167.08</v>
       </c>
       <c r="E40" s="10">
-        <v>167.02</v>
+        <v>166.03</v>
       </c>
       <c r="F40" s="10">
-        <v>177.02</v>
+        <v>176.03</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>167.67</v>
+        <v>166.8</v>
       </c>
       <c r="E41" s="13">
-        <v>167.44</v>
+        <v>166.45</v>
       </c>
       <c r="F41" s="13">
-        <v>177.44</v>
+        <v>176.45</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>168.47</v>
+        <v>167.96</v>
       </c>
       <c r="E42" s="10">
-        <v>167.37</v>
+        <v>167.02</v>
       </c>
       <c r="F42" s="10">
-        <v>177.37</v>
+        <v>177.02</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>168.18</v>
+        <v>167.67</v>
       </c>
       <c r="E43" s="13">
-        <v>167.79</v>
+        <v>167.44</v>
       </c>
       <c r="F43" s="13">
-        <v>177.79</v>
+        <v>177.44</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>162.79</v>
+        <v>162.52000000000001</v>
       </c>
       <c r="E47" s="10">
-        <v>161.88999999999999</v>
+        <v>161.30000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>171.89</v>
+        <v>171.3</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>162.61000000000001</v>
+        <v>162.32</v>
       </c>
       <c r="E48" s="13">
-        <v>161.97999999999999</v>
+        <v>161.38999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>171.98</v>
+        <v>171.39</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>163.54</v>
+        <v>162.79</v>
       </c>
       <c r="E49" s="10">
-        <v>162.56</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="F49" s="10">
-        <v>172.56</v>
+        <v>171.89</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>163.35</v>
+        <v>162.61000000000001</v>
       </c>
       <c r="E50" s="13">
-        <v>162.65</v>
+        <v>161.97999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>172.65</v>
+        <v>171.98</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>177.45</v>
+        <v>176.59</v>
       </c>
       <c r="E54" s="10">
-        <v>177.54</v>
+        <v>176.46</v>
       </c>
       <c r="F54" s="10">
-        <v>187.54</v>
+        <v>186.46</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>165.62</v>
+        <v>164.76</v>
       </c>
       <c r="E55" s="13">
-        <v>172.49</v>
+        <v>171.54</v>
       </c>
       <c r="F55" s="13">
-        <v>182.49</v>
+        <v>181.54</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>168.21</v>
+        <v>167.35</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>167.16</v>
+        <v>166.34</v>
       </c>
       <c r="E57" s="13">
-        <v>166.76</v>
+        <v>165.81</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>163.06</v>
+        <v>162.24</v>
       </c>
       <c r="E58" s="10">
-        <v>162.81</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>172.81</v>
+        <v>171.86</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>169.46</v>
+        <v>168.64</v>
       </c>
       <c r="E59" s="13">
-        <v>174.75</v>
+        <v>173.71</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>177.99</v>
+        <v>177.45</v>
       </c>
       <c r="E60" s="10">
-        <v>178.19</v>
+        <v>177.54</v>
       </c>
       <c r="F60" s="10">
-        <v>188.19</v>
+        <v>187.54</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>166.14</v>
+        <v>165.62</v>
       </c>
       <c r="E61" s="13">
-        <v>173.05</v>
+        <v>172.49</v>
       </c>
       <c r="F61" s="13">
-        <v>183.05</v>
+        <v>182.49</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>168.62</v>
+        <v>168.21</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>167.57</v>
+        <v>167.16</v>
       </c>
       <c r="E63" s="13">
-        <v>167.32</v>
+        <v>166.76</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>163.47</v>
+        <v>163.06</v>
       </c>
       <c r="E64" s="10">
-        <v>163.37</v>
+        <v>162.81</v>
       </c>
       <c r="F64" s="10">
-        <v>173.37</v>
+        <v>172.81</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>169.98</v>
+        <v>169.46</v>
       </c>
       <c r="E65" s="13">
-        <v>175.41</v>
+        <v>174.75</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1864,17 +1864,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,6 +2123,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
@@ -2143,24 +2143,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,6 +2162,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Thu Dec 11 03:03:31 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D56696D0-CB6C-4838-A150-AC92026F8421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{DCB93D3E-9FBA-4F08-A3D4-914B46FC067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>160.96</v>
+        <v>160.38999999999999</v>
       </c>
       <c r="E8" s="10">
-        <v>159.43</v>
+        <v>158.88</v>
       </c>
       <c r="F8" s="10">
-        <v>169.43</v>
+        <v>168.88</v>
       </c>
       <c r="G8" s="10">
-        <v>159.54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>160.96</v>
+        <v>160.38999999999999</v>
       </c>
       <c r="E9" s="13">
-        <v>159.43</v>
+        <v>158.88</v>
       </c>
       <c r="F9" s="13">
-        <v>169.43</v>
+        <v>168.88</v>
       </c>
       <c r="G9" s="13">
-        <v>159.54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>162.79</v>
+        <v>162.18</v>
       </c>
       <c r="E10" s="10">
-        <v>161.66</v>
+        <v>161.29</v>
       </c>
       <c r="F10" s="10">
-        <v>171.66</v>
+        <v>171.29</v>
       </c>
       <c r="G10" s="10">
-        <v>162.18</v>
+        <v>161.81</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>161.82</v>
+        <v>160.96</v>
       </c>
       <c r="E11" s="13">
-        <v>160.41999999999999</v>
+        <v>159.43</v>
       </c>
       <c r="F11" s="13">
-        <v>170.42</v>
+        <v>169.43</v>
       </c>
       <c r="G11" s="13">
-        <v>160.54</v>
+        <v>159.54</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>161.82</v>
+        <v>160.96</v>
       </c>
       <c r="E12" s="10">
-        <v>160.41999999999999</v>
+        <v>159.43</v>
       </c>
       <c r="F12" s="10">
-        <v>170.42</v>
+        <v>169.43</v>
       </c>
       <c r="G12" s="10">
-        <v>160.54</v>
+        <v>159.54</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>163.65</v>
+        <v>162.79</v>
       </c>
       <c r="E13" s="13">
-        <v>162.63999999999999</v>
+        <v>161.66</v>
       </c>
       <c r="F13" s="13">
-        <v>172.64</v>
+        <v>171.66</v>
       </c>
       <c r="G13" s="13">
-        <v>163.16</v>
+        <v>162.18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>165.73</v>
+        <v>165.12</v>
       </c>
       <c r="E17" s="10">
-        <v>165.36</v>
+        <v>164.78</v>
       </c>
       <c r="F17" s="10">
-        <v>175.36</v>
+        <v>174.78</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>166.56</v>
+        <v>165.73</v>
       </c>
       <c r="E18" s="13">
-        <v>166.32</v>
+        <v>165.36</v>
       </c>
       <c r="F18" s="13">
-        <v>176.32</v>
+        <v>175.36</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>162.1</v>
+        <v>161.09</v>
       </c>
       <c r="E22" s="10">
-        <v>160.97</v>
+        <v>160.5</v>
       </c>
       <c r="F22" s="10">
-        <v>170.57</v>
+        <v>170.1</v>
       </c>
       <c r="G22" s="10">
-        <v>162.13</v>
+        <v>161.66</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>167.82</v>
+        <v>167.2</v>
       </c>
       <c r="E23" s="13">
-        <v>165.88</v>
+        <v>165.4</v>
       </c>
       <c r="F23" s="13">
-        <v>175.88</v>
+        <v>175.4</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>167.59</v>
+        <v>166.97</v>
       </c>
       <c r="E24" s="10">
-        <v>166.2</v>
+        <v>165.72</v>
       </c>
       <c r="F24" s="10">
-        <v>176.2</v>
+        <v>175.72</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>168.2</v>
+        <v>167.58</v>
       </c>
       <c r="E25" s="13">
-        <v>165.63</v>
+        <v>165.15</v>
       </c>
       <c r="F25" s="13">
-        <v>175.63</v>
+        <v>175.15</v>
       </c>
       <c r="G25" s="13">
-        <v>165.4</v>
+        <v>164.92</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>166.99</v>
+        <v>166.38</v>
       </c>
       <c r="E26" s="10">
-        <v>167.07</v>
+        <v>166.59</v>
       </c>
       <c r="F26" s="10">
-        <v>177.07</v>
+        <v>176.59</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>162.85</v>
+        <v>162.1</v>
       </c>
       <c r="E27" s="13">
-        <v>161.72</v>
+        <v>160.97</v>
       </c>
       <c r="F27" s="13">
-        <v>171.32</v>
+        <v>170.57</v>
       </c>
       <c r="G27" s="13">
-        <v>162.88</v>
+        <v>162.13</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>168.67</v>
+        <v>167.82</v>
       </c>
       <c r="E28" s="22">
-        <v>166.86</v>
+        <v>165.88</v>
       </c>
       <c r="F28" s="22">
-        <v>176.86</v>
+        <v>175.88</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>168.44</v>
+        <v>167.59</v>
       </c>
       <c r="E29" s="13">
-        <v>167.19</v>
+        <v>166.2</v>
       </c>
       <c r="F29" s="13">
-        <v>177.19</v>
+        <v>176.2</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>169.05</v>
+        <v>168.2</v>
       </c>
       <c r="E30" s="22">
-        <v>166.63</v>
+        <v>165.63</v>
       </c>
       <c r="F30" s="22">
-        <v>176.63</v>
+        <v>175.63</v>
       </c>
       <c r="G30" s="22">
-        <v>166.4</v>
+        <v>165.4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>167.84</v>
+        <v>166.99</v>
       </c>
       <c r="E31" s="13">
-        <v>168.07</v>
+        <v>167.07</v>
       </c>
       <c r="F31" s="13">
-        <v>178.07</v>
+        <v>177.07</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>161.08000000000001</v>
+        <v>160.57</v>
       </c>
       <c r="E35" s="10">
-        <v>158.68</v>
+        <v>158.19999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>167.68</v>
+        <v>167.2</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>161.93</v>
+        <v>161.08000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>159.66</v>
+        <v>158.68</v>
       </c>
       <c r="F36" s="13">
-        <v>168.66</v>
+        <v>167.68</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>167.08</v>
+        <v>166.46</v>
       </c>
       <c r="E40" s="10">
-        <v>166.03</v>
+        <v>165.43</v>
       </c>
       <c r="F40" s="10">
-        <v>176.03</v>
+        <v>175.43</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>166.8</v>
+        <v>166.17</v>
       </c>
       <c r="E41" s="13">
-        <v>166.45</v>
+        <v>165.85</v>
       </c>
       <c r="F41" s="13">
-        <v>176.45</v>
+        <v>175.85</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>167.96</v>
+        <v>167.08</v>
       </c>
       <c r="E42" s="10">
-        <v>167.02</v>
+        <v>166.03</v>
       </c>
       <c r="F42" s="10">
-        <v>177.02</v>
+        <v>176.03</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>167.67</v>
+        <v>166.8</v>
       </c>
       <c r="E43" s="13">
-        <v>167.44</v>
+        <v>166.45</v>
       </c>
       <c r="F43" s="13">
-        <v>177.44</v>
+        <v>176.45</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>162.52000000000001</v>
+        <v>161.61000000000001</v>
       </c>
       <c r="E47" s="10">
-        <v>161.30000000000001</v>
+        <v>160.44</v>
       </c>
       <c r="F47" s="10">
-        <v>171.3</v>
+        <v>170.44</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>162.32</v>
+        <v>161.41999999999999</v>
       </c>
       <c r="E48" s="13">
-        <v>161.38999999999999</v>
+        <v>160.53</v>
       </c>
       <c r="F48" s="13">
-        <v>171.39</v>
+        <v>170.53</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>162.79</v>
+        <v>162.52000000000001</v>
       </c>
       <c r="E49" s="10">
-        <v>161.88999999999999</v>
+        <v>161.30000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>171.89</v>
+        <v>171.3</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>162.61000000000001</v>
+        <v>162.32</v>
       </c>
       <c r="E50" s="13">
-        <v>161.97999999999999</v>
+        <v>161.38999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>171.98</v>
+        <v>171.39</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>176.59</v>
+        <v>175.96</v>
       </c>
       <c r="E54" s="10">
-        <v>176.46</v>
+        <v>175.95</v>
       </c>
       <c r="F54" s="10">
-        <v>186.46</v>
+        <v>185.96</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>164.76</v>
+        <v>164.14</v>
       </c>
       <c r="E55" s="13">
-        <v>171.54</v>
+        <v>171.07</v>
       </c>
       <c r="F55" s="13">
-        <v>181.54</v>
+        <v>181.07</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>167.35</v>
+        <v>166.73</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>166.34</v>
+        <v>165.74</v>
       </c>
       <c r="E57" s="13">
-        <v>165.81</v>
+        <v>165.34</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>162.24</v>
+        <v>161.63999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>161.86000000000001</v>
+        <v>161.38999999999999</v>
       </c>
       <c r="F58" s="10">
-        <v>171.86</v>
+        <v>171.39</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>168.64</v>
+        <v>168.03</v>
       </c>
       <c r="E59" s="13">
-        <v>173.71</v>
+        <v>173.21</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>177.45</v>
+        <v>176.59</v>
       </c>
       <c r="E60" s="10">
-        <v>177.54</v>
+        <v>176.46</v>
       </c>
       <c r="F60" s="10">
-        <v>187.54</v>
+        <v>186.46</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>165.62</v>
+        <v>164.76</v>
       </c>
       <c r="E61" s="13">
-        <v>172.49</v>
+        <v>171.54</v>
       </c>
       <c r="F61" s="13">
-        <v>182.49</v>
+        <v>181.54</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>168.21</v>
+        <v>167.35</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>167.16</v>
+        <v>166.34</v>
       </c>
       <c r="E63" s="13">
-        <v>166.76</v>
+        <v>165.81</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>163.06</v>
+        <v>162.24</v>
       </c>
       <c r="E64" s="10">
-        <v>162.81</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>172.81</v>
+        <v>171.86</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>169.46</v>
+        <v>168.64</v>
       </c>
       <c r="E65" s="13">
-        <v>174.75</v>
+        <v>173.71</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2123,7 +2114,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -2134,15 +2125,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2162,7 +2154,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2180,6 +2172,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Fri Dec 12 03:00:51 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{DCB93D3E-9FBA-4F08-A3D4-914B46FC067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D21B9BAC-3B76-4AAE-AADD-701DDC3D8A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,8 +154,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,7 +331,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>160.38999999999999</v>
+        <v>159.78</v>
       </c>
       <c r="E8" s="10">
-        <v>158.88</v>
+        <v>158.4</v>
       </c>
       <c r="F8" s="10">
-        <v>168.88</v>
+        <v>168.4</v>
       </c>
       <c r="G8" s="10">
-        <v>159</v>
+        <v>158.51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>160.38999999999999</v>
+        <v>159.78</v>
       </c>
       <c r="E9" s="13">
-        <v>158.88</v>
+        <v>158.4</v>
       </c>
       <c r="F9" s="13">
-        <v>168.88</v>
+        <v>168.4</v>
       </c>
       <c r="G9" s="13">
-        <v>159</v>
+        <v>158.51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>162.18</v>
+        <v>161.44</v>
       </c>
       <c r="E10" s="10">
-        <v>161.29</v>
+        <v>161.12</v>
       </c>
       <c r="F10" s="10">
-        <v>171.29</v>
+        <v>171.12</v>
       </c>
       <c r="G10" s="10">
-        <v>161.81</v>
+        <v>161.63999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>160.96</v>
+        <v>160.38999999999999</v>
       </c>
       <c r="E11" s="13">
-        <v>159.43</v>
+        <v>158.88</v>
       </c>
       <c r="F11" s="13">
-        <v>169.43</v>
+        <v>168.88</v>
       </c>
       <c r="G11" s="13">
-        <v>159.54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>160.96</v>
+        <v>160.38999999999999</v>
       </c>
       <c r="E12" s="10">
-        <v>159.43</v>
+        <v>158.88</v>
       </c>
       <c r="F12" s="10">
-        <v>169.43</v>
+        <v>168.88</v>
       </c>
       <c r="G12" s="10">
-        <v>159.54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>162.79</v>
+        <v>162.18</v>
       </c>
       <c r="E13" s="13">
-        <v>161.66</v>
+        <v>161.29</v>
       </c>
       <c r="F13" s="13">
-        <v>171.66</v>
+        <v>171.29</v>
       </c>
       <c r="G13" s="13">
-        <v>162.18</v>
+        <v>161.81</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>165.12</v>
+        <v>164.39</v>
       </c>
       <c r="E17" s="10">
-        <v>164.78</v>
+        <v>164.48</v>
       </c>
       <c r="F17" s="10">
-        <v>174.78</v>
+        <v>174.48</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>165.73</v>
+        <v>165.12</v>
       </c>
       <c r="E18" s="13">
-        <v>165.36</v>
+        <v>164.78</v>
       </c>
       <c r="F18" s="13">
-        <v>175.36</v>
+        <v>174.78</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>161.09</v>
+        <v>160.37</v>
       </c>
       <c r="E22" s="10">
-        <v>160.5</v>
+        <v>160.22</v>
       </c>
       <c r="F22" s="10">
-        <v>170.1</v>
+        <v>169.82</v>
       </c>
       <c r="G22" s="10">
-        <v>161.66</v>
+        <v>161.38999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>167.2</v>
+        <v>166.47</v>
       </c>
       <c r="E23" s="13">
-        <v>165.4</v>
+        <v>165.23</v>
       </c>
       <c r="F23" s="13">
-        <v>175.4</v>
+        <v>175.23</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>166.97</v>
+        <v>166.24</v>
       </c>
       <c r="E24" s="10">
-        <v>165.72</v>
+        <v>165.55</v>
       </c>
       <c r="F24" s="10">
-        <v>175.72</v>
+        <v>175.55</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>167.58</v>
+        <v>166.85</v>
       </c>
       <c r="E25" s="13">
-        <v>165.15</v>
+        <v>164.98</v>
       </c>
       <c r="F25" s="13">
-        <v>175.15</v>
+        <v>174.98</v>
       </c>
       <c r="G25" s="13">
-        <v>164.92</v>
+        <v>164.75</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>166.38</v>
+        <v>165.65</v>
       </c>
       <c r="E26" s="10">
-        <v>166.59</v>
+        <v>166.41</v>
       </c>
       <c r="F26" s="10">
-        <v>176.59</v>
+        <v>176.41</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>162.1</v>
+        <v>161.09</v>
       </c>
       <c r="E27" s="13">
-        <v>160.97</v>
+        <v>160.5</v>
       </c>
       <c r="F27" s="13">
-        <v>170.57</v>
+        <v>170.1</v>
       </c>
       <c r="G27" s="13">
-        <v>162.13</v>
+        <v>161.66</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>167.82</v>
+        <v>167.2</v>
       </c>
       <c r="E28" s="22">
-        <v>165.88</v>
+        <v>165.4</v>
       </c>
       <c r="F28" s="22">
-        <v>175.88</v>
+        <v>175.4</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>167.59</v>
+        <v>166.97</v>
       </c>
       <c r="E29" s="13">
-        <v>166.2</v>
+        <v>165.72</v>
       </c>
       <c r="F29" s="13">
-        <v>176.2</v>
+        <v>175.72</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>168.2</v>
+        <v>167.58</v>
       </c>
       <c r="E30" s="22">
-        <v>165.63</v>
+        <v>165.15</v>
       </c>
       <c r="F30" s="22">
-        <v>175.63</v>
+        <v>175.15</v>
       </c>
       <c r="G30" s="22">
-        <v>165.4</v>
+        <v>164.92</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>166.99</v>
+        <v>166.38</v>
       </c>
       <c r="E31" s="13">
-        <v>167.07</v>
+        <v>166.59</v>
       </c>
       <c r="F31" s="13">
-        <v>177.07</v>
+        <v>176.59</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>160.57</v>
+        <v>159.84</v>
       </c>
       <c r="E35" s="10">
-        <v>158.19999999999999</v>
+        <v>158.03</v>
       </c>
       <c r="F35" s="10">
-        <v>167.2</v>
+        <v>167.04</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>161.08000000000001</v>
+        <v>160.57</v>
       </c>
       <c r="E36" s="13">
-        <v>158.68</v>
+        <v>158.19999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>167.68</v>
+        <v>167.2</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>166.46</v>
+        <v>165.72</v>
       </c>
       <c r="E40" s="10">
-        <v>165.43</v>
+        <v>165.12</v>
       </c>
       <c r="F40" s="10">
-        <v>175.43</v>
+        <v>175.12</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>166.17</v>
+        <v>165.43</v>
       </c>
       <c r="E41" s="13">
-        <v>165.85</v>
+        <v>165.54</v>
       </c>
       <c r="F41" s="13">
-        <v>175.85</v>
+        <v>175.54</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>167.08</v>
+        <v>166.46</v>
       </c>
       <c r="E42" s="10">
-        <v>166.03</v>
+        <v>165.43</v>
       </c>
       <c r="F42" s="10">
-        <v>176.03</v>
+        <v>175.43</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>166.8</v>
+        <v>166.17</v>
       </c>
       <c r="E43" s="13">
-        <v>166.45</v>
+        <v>165.85</v>
       </c>
       <c r="F43" s="13">
-        <v>176.45</v>
+        <v>175.85</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>161.61000000000001</v>
+        <v>160.74</v>
       </c>
       <c r="E47" s="10">
-        <v>160.44</v>
+        <v>159.80000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>170.44</v>
+        <v>169.8</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>161.41999999999999</v>
+        <v>160.55000000000001</v>
       </c>
       <c r="E48" s="13">
-        <v>160.53</v>
+        <v>159.88999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>170.53</v>
+        <v>169.89</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>162.52000000000001</v>
+        <v>161.61000000000001</v>
       </c>
       <c r="E49" s="10">
-        <v>161.30000000000001</v>
+        <v>160.44</v>
       </c>
       <c r="F49" s="10">
-        <v>171.3</v>
+        <v>170.44</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>162.32</v>
+        <v>161.41999999999999</v>
       </c>
       <c r="E50" s="13">
-        <v>161.38999999999999</v>
+        <v>160.53</v>
       </c>
       <c r="F50" s="13">
-        <v>171.39</v>
+        <v>170.53</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>175.96</v>
+        <v>175.23</v>
       </c>
       <c r="E54" s="10">
-        <v>175.95</v>
+        <v>175.76</v>
       </c>
       <c r="F54" s="10">
-        <v>185.96</v>
+        <v>185.76</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>164.14</v>
+        <v>163.41</v>
       </c>
       <c r="E55" s="13">
-        <v>171.07</v>
+        <v>170.91</v>
       </c>
       <c r="F55" s="13">
-        <v>181.07</v>
+        <v>180.91</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>166.73</v>
+        <v>166</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>165.74</v>
+        <v>165.01</v>
       </c>
       <c r="E57" s="13">
-        <v>165.34</v>
+        <v>165.18</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>161.63999999999999</v>
+        <v>160.91999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>161.38999999999999</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="F58" s="10">
-        <v>171.39</v>
+        <v>171.23</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>168.03</v>
+        <v>167.31</v>
       </c>
       <c r="E59" s="13">
-        <v>173.21</v>
+        <v>173.03</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>176.59</v>
+        <v>175.96</v>
       </c>
       <c r="E60" s="10">
-        <v>176.46</v>
+        <v>175.95</v>
       </c>
       <c r="F60" s="10">
-        <v>186.46</v>
+        <v>185.96</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>164.76</v>
+        <v>164.14</v>
       </c>
       <c r="E61" s="13">
-        <v>171.54</v>
+        <v>171.07</v>
       </c>
       <c r="F61" s="13">
-        <v>181.54</v>
+        <v>181.07</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>167.35</v>
+        <v>166.73</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>166.34</v>
+        <v>165.74</v>
       </c>
       <c r="E63" s="13">
-        <v>165.81</v>
+        <v>165.34</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>162.24</v>
+        <v>161.63999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>161.86000000000001</v>
+        <v>161.38999999999999</v>
       </c>
       <c r="F64" s="10">
-        <v>171.86</v>
+        <v>171.39</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>168.64</v>
+        <v>168.03</v>
       </c>
       <c r="E65" s="13">
-        <v>173.71</v>
+        <v>173.21</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,17 +2125,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,6 +2135,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2154,24 +2172,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Mon Dec 15 03:10:26 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D21B9BAC-3B76-4AAE-AADD-701DDC3D8A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{AC0968CC-0ADF-4F12-BE61-94AE10617291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,8 +154,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,7 +331,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>159.78</v>
+        <v>159.01</v>
       </c>
       <c r="E8" s="10">
-        <v>158.4</v>
+        <v>158.24</v>
       </c>
       <c r="F8" s="10">
-        <v>168.4</v>
+        <v>168.24</v>
       </c>
       <c r="G8" s="10">
-        <v>158.51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.36000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>159.78</v>
+        <v>159.01</v>
       </c>
       <c r="E9" s="13">
-        <v>158.4</v>
+        <v>158.24</v>
       </c>
       <c r="F9" s="13">
-        <v>168.4</v>
+        <v>168.24</v>
       </c>
       <c r="G9" s="13">
-        <v>158.51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.36000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>161.44</v>
+        <v>160.69</v>
       </c>
       <c r="E10" s="10">
-        <v>161.12</v>
+        <v>160.87</v>
       </c>
       <c r="F10" s="10">
-        <v>171.12</v>
+        <v>170.87</v>
       </c>
       <c r="G10" s="10">
-        <v>161.63999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.38999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>160.38999999999999</v>
+        <v>159.78</v>
       </c>
       <c r="E11" s="13">
-        <v>158.88</v>
+        <v>158.4</v>
       </c>
       <c r="F11" s="13">
-        <v>168.88</v>
+        <v>168.4</v>
       </c>
       <c r="G11" s="13">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>160.38999999999999</v>
+        <v>159.78</v>
       </c>
       <c r="E12" s="10">
-        <v>158.88</v>
+        <v>158.4</v>
       </c>
       <c r="F12" s="10">
-        <v>168.88</v>
+        <v>168.4</v>
       </c>
       <c r="G12" s="10">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>162.18</v>
+        <v>161.44</v>
       </c>
       <c r="E13" s="13">
-        <v>161.29</v>
+        <v>161.12</v>
       </c>
       <c r="F13" s="13">
-        <v>171.29</v>
+        <v>171.12</v>
       </c>
       <c r="G13" s="13">
-        <v>161.81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.63999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>164.39</v>
+        <v>163.63999999999999</v>
       </c>
       <c r="E17" s="10">
-        <v>164.48</v>
+        <v>164.17</v>
       </c>
       <c r="F17" s="10">
-        <v>174.48</v>
+        <v>174.17</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>165.12</v>
+        <v>164.39</v>
       </c>
       <c r="E18" s="13">
-        <v>164.78</v>
+        <v>164.48</v>
       </c>
       <c r="F18" s="13">
-        <v>174.78</v>
+        <v>174.48</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>160.37</v>
+        <v>159.49</v>
       </c>
       <c r="E22" s="10">
-        <v>160.22</v>
+        <v>159.97999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>169.82</v>
+        <v>169.57</v>
       </c>
       <c r="G22" s="10">
-        <v>161.38999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.13999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>166.47</v>
+        <v>165.72</v>
       </c>
       <c r="E23" s="13">
-        <v>165.23</v>
+        <v>164.98</v>
       </c>
       <c r="F23" s="13">
-        <v>175.23</v>
+        <v>174.98</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>166.24</v>
+        <v>165.49</v>
       </c>
       <c r="E24" s="10">
-        <v>165.55</v>
+        <v>165.3</v>
       </c>
       <c r="F24" s="10">
-        <v>175.55</v>
+        <v>175.3</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>166.85</v>
+        <v>166.1</v>
       </c>
       <c r="E25" s="13">
-        <v>164.98</v>
+        <v>164.73</v>
       </c>
       <c r="F25" s="13">
-        <v>174.98</v>
+        <v>174.73</v>
       </c>
       <c r="G25" s="13">
-        <v>164.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>165.65</v>
+        <v>164.9</v>
       </c>
       <c r="E26" s="10">
-        <v>166.41</v>
+        <v>166.16</v>
       </c>
       <c r="F26" s="10">
-        <v>176.41</v>
+        <v>176.16</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>161.09</v>
+        <v>160.37</v>
       </c>
       <c r="E27" s="13">
-        <v>160.5</v>
+        <v>160.22</v>
       </c>
       <c r="F27" s="13">
-        <v>170.1</v>
+        <v>169.82</v>
       </c>
       <c r="G27" s="13">
-        <v>161.66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.38999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>167.2</v>
+        <v>166.47</v>
       </c>
       <c r="E28" s="22">
-        <v>165.4</v>
+        <v>165.23</v>
       </c>
       <c r="F28" s="22">
-        <v>175.4</v>
+        <v>175.23</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>166.97</v>
+        <v>166.24</v>
       </c>
       <c r="E29" s="13">
-        <v>165.72</v>
+        <v>165.55</v>
       </c>
       <c r="F29" s="13">
-        <v>175.72</v>
+        <v>175.55</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>167.58</v>
+        <v>166.85</v>
       </c>
       <c r="E30" s="22">
-        <v>165.15</v>
+        <v>164.98</v>
       </c>
       <c r="F30" s="22">
-        <v>175.15</v>
+        <v>174.98</v>
       </c>
       <c r="G30" s="22">
-        <v>164.92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>166.38</v>
+        <v>165.65</v>
       </c>
       <c r="E31" s="13">
-        <v>166.59</v>
+        <v>166.41</v>
       </c>
       <c r="F31" s="13">
-        <v>176.59</v>
+        <v>176.41</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>159.84</v>
+        <v>158.87</v>
       </c>
       <c r="E35" s="10">
-        <v>158.03</v>
+        <v>157.79</v>
       </c>
       <c r="F35" s="10">
-        <v>167.04</v>
+        <v>166.79</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>160.57</v>
+        <v>159.84</v>
       </c>
       <c r="E36" s="13">
-        <v>158.19999999999999</v>
+        <v>158.03</v>
       </c>
       <c r="F36" s="13">
-        <v>167.2</v>
+        <v>167.04</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>165.72</v>
+        <v>164.97</v>
       </c>
       <c r="E40" s="10">
-        <v>165.12</v>
+        <v>164.82</v>
       </c>
       <c r="F40" s="10">
-        <v>175.12</v>
+        <v>174.82</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>165.43</v>
+        <v>164.69</v>
       </c>
       <c r="E41" s="13">
-        <v>165.54</v>
+        <v>165.24</v>
       </c>
       <c r="F41" s="13">
-        <v>175.54</v>
+        <v>175.24</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>166.46</v>
+        <v>165.72</v>
       </c>
       <c r="E42" s="10">
-        <v>165.43</v>
+        <v>165.12</v>
       </c>
       <c r="F42" s="10">
-        <v>175.43</v>
+        <v>175.12</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>166.17</v>
+        <v>165.43</v>
       </c>
       <c r="E43" s="13">
-        <v>165.85</v>
+        <v>165.54</v>
       </c>
       <c r="F43" s="13">
-        <v>175.85</v>
+        <v>175.54</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>160.74</v>
+        <v>160.15</v>
       </c>
       <c r="E47" s="10">
-        <v>159.80000000000001</v>
+        <v>159.4</v>
       </c>
       <c r="F47" s="10">
-        <v>169.8</v>
+        <v>169.4</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>160.55000000000001</v>
+        <v>159.96</v>
       </c>
       <c r="E48" s="13">
-        <v>159.88999999999999</v>
+        <v>159.49</v>
       </c>
       <c r="F48" s="13">
-        <v>169.89</v>
+        <v>169.49</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>161.61000000000001</v>
+        <v>160.74</v>
       </c>
       <c r="E49" s="10">
-        <v>160.44</v>
+        <v>159.80000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>170.44</v>
+        <v>169.8</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>161.41999999999999</v>
+        <v>160.55000000000001</v>
       </c>
       <c r="E50" s="13">
-        <v>160.53</v>
+        <v>159.88999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>170.53</v>
+        <v>169.89</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>175.23</v>
+        <v>174.47</v>
       </c>
       <c r="E54" s="10">
-        <v>175.76</v>
+        <v>175.52</v>
       </c>
       <c r="F54" s="10">
-        <v>185.76</v>
+        <v>185.52</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>163.41</v>
+        <v>162.66</v>
       </c>
       <c r="E55" s="13">
-        <v>170.91</v>
+        <v>170.66</v>
       </c>
       <c r="F55" s="13">
-        <v>180.91</v>
+        <v>180.66</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>166</v>
+        <v>165.03</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>165.01</v>
+        <v>164.04</v>
       </c>
       <c r="E57" s="13">
-        <v>165.18</v>
+        <v>164.93</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>160.91999999999999</v>
+        <v>159.94999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>161.22999999999999</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="F58" s="10">
-        <v>171.23</v>
+        <v>170.98</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>167.31</v>
+        <v>166.56</v>
       </c>
       <c r="E59" s="13">
-        <v>173.03</v>
+        <v>172.78</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>175.96</v>
+        <v>175.23</v>
       </c>
       <c r="E60" s="10">
-        <v>175.95</v>
+        <v>175.76</v>
       </c>
       <c r="F60" s="10">
-        <v>185.96</v>
+        <v>185.76</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>164.14</v>
+        <v>163.41</v>
       </c>
       <c r="E61" s="13">
-        <v>171.07</v>
+        <v>170.91</v>
       </c>
       <c r="F61" s="13">
-        <v>181.07</v>
+        <v>180.91</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>166.73</v>
+        <v>166</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>165.74</v>
+        <v>165.01</v>
       </c>
       <c r="E63" s="13">
-        <v>165.34</v>
+        <v>165.18</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>161.63999999999999</v>
+        <v>160.91999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>161.38999999999999</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="F64" s="10">
-        <v>171.39</v>
+        <v>171.23</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46003</v>
+        <v>46004</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>168.03</v>
+        <v>167.31</v>
       </c>
       <c r="E65" s="13">
-        <v>173.21</v>
+        <v>173.03</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,14 +1855,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2126,28 +2124,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2163,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Dec 16 03:01:56 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{AC0968CC-0ADF-4F12-BE61-94AE10617291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{747867EA-CD1B-4BCD-BABF-D12FE85345FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>159.01</v>
+        <v>157.72</v>
       </c>
       <c r="E8" s="10">
-        <v>158.24</v>
+        <v>157.78</v>
       </c>
       <c r="F8" s="10">
-        <v>168.24</v>
+        <v>167.78</v>
       </c>
       <c r="G8" s="10">
-        <v>158.36000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>157.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>159.01</v>
+        <v>157.72</v>
       </c>
       <c r="E9" s="13">
-        <v>158.24</v>
+        <v>157.78</v>
       </c>
       <c r="F9" s="13">
-        <v>168.24</v>
+        <v>167.78</v>
       </c>
       <c r="G9" s="13">
-        <v>158.36000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>157.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>160.69</v>
+        <v>159.65</v>
       </c>
       <c r="E10" s="10">
-        <v>160.87</v>
+        <v>160.22</v>
       </c>
       <c r="F10" s="10">
-        <v>170.87</v>
+        <v>170.23</v>
       </c>
       <c r="G10" s="10">
-        <v>161.38999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>159.78</v>
+        <v>159.01</v>
       </c>
       <c r="E11" s="13">
-        <v>158.4</v>
+        <v>158.24</v>
       </c>
       <c r="F11" s="13">
-        <v>168.4</v>
+        <v>168.24</v>
       </c>
       <c r="G11" s="13">
-        <v>158.51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>158.36000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>159.78</v>
+        <v>159.01</v>
       </c>
       <c r="E12" s="10">
-        <v>158.4</v>
+        <v>158.24</v>
       </c>
       <c r="F12" s="10">
-        <v>168.4</v>
+        <v>168.24</v>
       </c>
       <c r="G12" s="10">
-        <v>158.51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>158.36000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>161.44</v>
+        <v>160.69</v>
       </c>
       <c r="E13" s="13">
-        <v>161.12</v>
+        <v>160.87</v>
       </c>
       <c r="F13" s="13">
-        <v>171.12</v>
+        <v>170.87</v>
       </c>
       <c r="G13" s="13">
-        <v>161.63999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.38999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>163.63999999999999</v>
+        <v>162.6</v>
       </c>
       <c r="E17" s="10">
-        <v>164.17</v>
+        <v>163.76</v>
       </c>
       <c r="F17" s="10">
-        <v>174.17</v>
+        <v>173.76</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>164.39</v>
+        <v>163.63999999999999</v>
       </c>
       <c r="E18" s="13">
-        <v>164.48</v>
+        <v>164.17</v>
       </c>
       <c r="F18" s="13">
-        <v>174.48</v>
+        <v>174.17</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>159.49</v>
+        <v>158.41999999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>159.97999999999999</v>
+        <v>159.44</v>
       </c>
       <c r="F22" s="10">
-        <v>169.57</v>
+        <v>169.04</v>
       </c>
       <c r="G22" s="10">
-        <v>161.13999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>160.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>165.72</v>
+        <v>164.45</v>
       </c>
       <c r="E23" s="13">
-        <v>164.98</v>
+        <v>164.55</v>
       </c>
       <c r="F23" s="13">
-        <v>174.98</v>
+        <v>174.55</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>165.49</v>
+        <v>164.23</v>
       </c>
       <c r="E24" s="10">
-        <v>165.3</v>
+        <v>164.88</v>
       </c>
       <c r="F24" s="10">
-        <v>175.3</v>
+        <v>174.88</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>166.1</v>
+        <v>164.73</v>
       </c>
       <c r="E25" s="13">
-        <v>164.73</v>
+        <v>164.3</v>
       </c>
       <c r="F25" s="13">
-        <v>174.73</v>
+        <v>174.3</v>
       </c>
       <c r="G25" s="13">
-        <v>164.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>164.07</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>164.9</v>
+        <v>163.63</v>
       </c>
       <c r="E26" s="10">
-        <v>166.16</v>
+        <v>165.73</v>
       </c>
       <c r="F26" s="10">
-        <v>176.16</v>
+        <v>175.73</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>160.37</v>
+        <v>159.49</v>
       </c>
       <c r="E27" s="13">
-        <v>160.22</v>
+        <v>159.97999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>169.82</v>
+        <v>169.57</v>
       </c>
       <c r="G27" s="13">
-        <v>161.38999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.13999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>166.47</v>
+        <v>165.72</v>
       </c>
       <c r="E28" s="22">
-        <v>165.23</v>
+        <v>164.98</v>
       </c>
       <c r="F28" s="22">
-        <v>175.23</v>
+        <v>174.98</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>166.24</v>
+        <v>165.49</v>
       </c>
       <c r="E29" s="13">
-        <v>165.55</v>
+        <v>165.3</v>
       </c>
       <c r="F29" s="13">
-        <v>175.55</v>
+        <v>175.3</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>166.85</v>
+        <v>166.1</v>
       </c>
       <c r="E30" s="22">
-        <v>164.98</v>
+        <v>164.73</v>
       </c>
       <c r="F30" s="22">
-        <v>174.98</v>
+        <v>174.73</v>
       </c>
       <c r="G30" s="22">
-        <v>164.75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>164.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>165.65</v>
+        <v>164.9</v>
       </c>
       <c r="E31" s="13">
-        <v>166.41</v>
+        <v>166.16</v>
       </c>
       <c r="F31" s="13">
-        <v>176.41</v>
+        <v>176.16</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>158.87</v>
+        <v>157.83000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>157.79</v>
+        <v>157.36000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>166.79</v>
+        <v>166.36</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>159.84</v>
+        <v>158.87</v>
       </c>
       <c r="E36" s="13">
-        <v>158.03</v>
+        <v>157.79</v>
       </c>
       <c r="F36" s="13">
-        <v>167.04</v>
+        <v>166.79</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>164.97</v>
+        <v>163.93</v>
       </c>
       <c r="E40" s="10">
-        <v>164.82</v>
+        <v>164.42</v>
       </c>
       <c r="F40" s="10">
-        <v>174.82</v>
+        <v>174.42</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>164.69</v>
+        <v>163.65</v>
       </c>
       <c r="E41" s="13">
-        <v>165.24</v>
+        <v>164.84</v>
       </c>
       <c r="F41" s="13">
-        <v>175.24</v>
+        <v>174.84</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>165.72</v>
+        <v>164.97</v>
       </c>
       <c r="E42" s="10">
-        <v>165.12</v>
+        <v>164.82</v>
       </c>
       <c r="F42" s="10">
-        <v>175.12</v>
+        <v>174.82</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>165.43</v>
+        <v>164.69</v>
       </c>
       <c r="E43" s="13">
-        <v>165.54</v>
+        <v>165.24</v>
       </c>
       <c r="F43" s="13">
-        <v>175.54</v>
+        <v>175.24</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>160.15</v>
+        <v>159.24</v>
       </c>
       <c r="E47" s="10">
-        <v>159.4</v>
+        <v>159.1</v>
       </c>
       <c r="F47" s="10">
-        <v>169.4</v>
+        <v>169.1</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>159.96</v>
+        <v>159.05000000000001</v>
       </c>
       <c r="E48" s="13">
-        <v>159.49</v>
+        <v>159.19</v>
       </c>
       <c r="F48" s="13">
-        <v>169.49</v>
+        <v>169.19</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>160.74</v>
+        <v>160.15</v>
       </c>
       <c r="E49" s="10">
-        <v>159.80000000000001</v>
+        <v>159.4</v>
       </c>
       <c r="F49" s="10">
-        <v>169.8</v>
+        <v>169.4</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>160.55000000000001</v>
+        <v>159.96</v>
       </c>
       <c r="E50" s="13">
-        <v>159.88999999999999</v>
+        <v>159.49</v>
       </c>
       <c r="F50" s="13">
-        <v>169.89</v>
+        <v>169.49</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>174.47</v>
+        <v>173.42</v>
       </c>
       <c r="E54" s="10">
-        <v>175.52</v>
+        <v>175.12</v>
       </c>
       <c r="F54" s="10">
-        <v>185.52</v>
+        <v>185.12</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>162.66</v>
+        <v>161.62</v>
       </c>
       <c r="E55" s="13">
-        <v>170.66</v>
+        <v>170.12</v>
       </c>
       <c r="F55" s="13">
-        <v>180.66</v>
+        <v>180.12</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>165.03</v>
+        <v>163.99</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>164.04</v>
+        <v>163</v>
       </c>
       <c r="E57" s="13">
-        <v>164.93</v>
+        <v>164.39</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>159.94999999999999</v>
+        <v>158.9</v>
       </c>
       <c r="E58" s="10">
-        <v>160.97999999999999</v>
+        <v>160.44</v>
       </c>
       <c r="F58" s="10">
-        <v>170.98</v>
+        <v>170.44</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>166.56</v>
+        <v>165.51</v>
       </c>
       <c r="E59" s="13">
-        <v>172.78</v>
+        <v>172.37</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>175.23</v>
+        <v>174.47</v>
       </c>
       <c r="E60" s="10">
-        <v>175.76</v>
+        <v>175.52</v>
       </c>
       <c r="F60" s="10">
-        <v>185.76</v>
+        <v>185.52</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>163.41</v>
+        <v>162.66</v>
       </c>
       <c r="E61" s="13">
-        <v>170.91</v>
+        <v>170.66</v>
       </c>
       <c r="F61" s="13">
-        <v>180.91</v>
+        <v>180.66</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>166</v>
+        <v>165.03</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>165.01</v>
+        <v>164.04</v>
       </c>
       <c r="E63" s="13">
-        <v>165.18</v>
+        <v>164.93</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>160.91999999999999</v>
+        <v>159.94999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>161.22999999999999</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="F64" s="10">
-        <v>171.23</v>
+        <v>170.98</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46004</v>
+        <v>46007</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>167.31</v>
+        <v>166.56</v>
       </c>
       <c r="E65" s="13">
-        <v>173.03</v>
+        <v>172.78</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1864,6 +1864,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2123,17 +2134,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
@@ -2143,6 +2143,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2162,24 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Wed Dec 17 02:58:19 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{747867EA-CD1B-4BCD-BABF-D12FE85345FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D3C4CDFB-8CF2-4FC6-8D1C-2BCBEA1F8145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>157.72</v>
+        <v>156.56</v>
       </c>
       <c r="E8" s="10">
-        <v>157.78</v>
+        <v>156.88999999999999</v>
       </c>
       <c r="F8" s="10">
-        <v>167.78</v>
+        <v>166.89</v>
       </c>
       <c r="G8" s="10">
-        <v>157.9</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>157.72</v>
+        <v>156.56</v>
       </c>
       <c r="E9" s="13">
-        <v>157.78</v>
+        <v>156.88999999999999</v>
       </c>
       <c r="F9" s="13">
-        <v>167.78</v>
+        <v>166.89</v>
       </c>
       <c r="G9" s="13">
-        <v>157.9</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>159.65</v>
+        <v>158.63</v>
       </c>
       <c r="E10" s="10">
-        <v>160.22</v>
+        <v>159.46</v>
       </c>
       <c r="F10" s="10">
-        <v>170.23</v>
+        <v>169.46</v>
       </c>
       <c r="G10" s="10">
-        <v>160.74</v>
+        <v>159.97999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>159.01</v>
+        <v>157.72</v>
       </c>
       <c r="E11" s="13">
-        <v>158.24</v>
+        <v>157.78</v>
       </c>
       <c r="F11" s="13">
-        <v>168.24</v>
+        <v>167.78</v>
       </c>
       <c r="G11" s="13">
-        <v>158.36000000000001</v>
+        <v>157.9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>159.01</v>
+        <v>157.72</v>
       </c>
       <c r="E12" s="10">
-        <v>158.24</v>
+        <v>157.78</v>
       </c>
       <c r="F12" s="10">
-        <v>168.24</v>
+        <v>167.78</v>
       </c>
       <c r="G12" s="10">
-        <v>158.36000000000001</v>
+        <v>157.9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>160.69</v>
+        <v>159.65</v>
       </c>
       <c r="E13" s="13">
-        <v>160.87</v>
+        <v>160.22</v>
       </c>
       <c r="F13" s="13">
-        <v>170.87</v>
+        <v>170.23</v>
       </c>
       <c r="G13" s="13">
-        <v>161.38999999999999</v>
+        <v>160.74</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>162.6</v>
+        <v>161.69</v>
       </c>
       <c r="E17" s="10">
-        <v>163.76</v>
+        <v>163.15</v>
       </c>
       <c r="F17" s="10">
-        <v>173.76</v>
+        <v>173.15</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>163.63999999999999</v>
+        <v>162.6</v>
       </c>
       <c r="E18" s="13">
-        <v>164.17</v>
+        <v>163.76</v>
       </c>
       <c r="F18" s="13">
-        <v>174.17</v>
+        <v>173.76</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>158.41999999999999</v>
+        <v>157.37</v>
       </c>
       <c r="E22" s="10">
-        <v>159.44</v>
+        <v>158.46</v>
       </c>
       <c r="F22" s="10">
-        <v>169.04</v>
+        <v>168.06</v>
       </c>
       <c r="G22" s="10">
-        <v>160.6</v>
+        <v>159.62</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>164.45</v>
+        <v>163.55000000000001</v>
       </c>
       <c r="E23" s="13">
-        <v>164.55</v>
+        <v>163.57</v>
       </c>
       <c r="F23" s="13">
-        <v>174.55</v>
+        <v>173.57</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>164.23</v>
+        <v>163.32</v>
       </c>
       <c r="E24" s="10">
-        <v>164.88</v>
+        <v>163.89</v>
       </c>
       <c r="F24" s="10">
-        <v>174.88</v>
+        <v>173.89</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>164.73</v>
+        <v>163.82</v>
       </c>
       <c r="E25" s="13">
-        <v>164.3</v>
+        <v>163.53</v>
       </c>
       <c r="F25" s="13">
-        <v>174.3</v>
+        <v>173.53</v>
       </c>
       <c r="G25" s="13">
-        <v>164.07</v>
+        <v>163.30000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>163.63</v>
+        <v>162.72999999999999</v>
       </c>
       <c r="E26" s="10">
-        <v>165.73</v>
+        <v>164.96</v>
       </c>
       <c r="F26" s="10">
-        <v>175.73</v>
+        <v>174.96</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>159.49</v>
+        <v>158.41999999999999</v>
       </c>
       <c r="E27" s="13">
-        <v>159.97999999999999</v>
+        <v>159.44</v>
       </c>
       <c r="F27" s="13">
-        <v>169.57</v>
+        <v>169.04</v>
       </c>
       <c r="G27" s="13">
-        <v>161.13999999999999</v>
+        <v>160.6</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>165.72</v>
+        <v>164.45</v>
       </c>
       <c r="E28" s="22">
-        <v>164.98</v>
+        <v>164.55</v>
       </c>
       <c r="F28" s="22">
-        <v>174.98</v>
+        <v>174.55</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>165.49</v>
+        <v>164.23</v>
       </c>
       <c r="E29" s="13">
-        <v>165.3</v>
+        <v>164.88</v>
       </c>
       <c r="F29" s="13">
-        <v>175.3</v>
+        <v>174.88</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>166.1</v>
+        <v>164.73</v>
       </c>
       <c r="E30" s="22">
-        <v>164.73</v>
+        <v>164.3</v>
       </c>
       <c r="F30" s="22">
-        <v>174.73</v>
+        <v>174.3</v>
       </c>
       <c r="G30" s="22">
-        <v>164.5</v>
+        <v>164.07</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>164.9</v>
+        <v>163.63</v>
       </c>
       <c r="E31" s="13">
-        <v>166.16</v>
+        <v>165.73</v>
       </c>
       <c r="F31" s="13">
-        <v>176.16</v>
+        <v>175.73</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>157.83000000000001</v>
+        <v>156.91999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>157.36000000000001</v>
+        <v>156.6</v>
       </c>
       <c r="F35" s="10">
-        <v>166.36</v>
+        <v>165.6</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>158.87</v>
+        <v>157.83000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>157.79</v>
+        <v>157.36000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>166.79</v>
+        <v>166.36</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>163.93</v>
+        <v>163.02000000000001</v>
       </c>
       <c r="E40" s="10">
-        <v>164.42</v>
+        <v>163.81</v>
       </c>
       <c r="F40" s="10">
-        <v>174.42</v>
+        <v>173.81</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>163.65</v>
+        <v>162.74</v>
       </c>
       <c r="E41" s="13">
-        <v>164.84</v>
+        <v>164.23</v>
       </c>
       <c r="F41" s="13">
-        <v>174.84</v>
+        <v>174.23</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>164.97</v>
+        <v>163.93</v>
       </c>
       <c r="E42" s="10">
-        <v>164.82</v>
+        <v>164.42</v>
       </c>
       <c r="F42" s="10">
-        <v>174.82</v>
+        <v>174.42</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>164.69</v>
+        <v>163.65</v>
       </c>
       <c r="E43" s="13">
-        <v>165.24</v>
+        <v>164.84</v>
       </c>
       <c r="F43" s="13">
-        <v>175.24</v>
+        <v>174.84</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>159.24</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="E47" s="10">
-        <v>159.1</v>
+        <v>158.53</v>
       </c>
       <c r="F47" s="10">
-        <v>169.1</v>
+        <v>168.53</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>159.05000000000001</v>
+        <v>157.91999999999999</v>
       </c>
       <c r="E48" s="13">
-        <v>159.19</v>
+        <v>158.62</v>
       </c>
       <c r="F48" s="13">
-        <v>169.19</v>
+        <v>168.62</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>160.15</v>
+        <v>159.24</v>
       </c>
       <c r="E49" s="10">
-        <v>159.4</v>
+        <v>159.1</v>
       </c>
       <c r="F49" s="10">
-        <v>169.4</v>
+        <v>169.1</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>159.96</v>
+        <v>159.05000000000001</v>
       </c>
       <c r="E50" s="13">
-        <v>159.49</v>
+        <v>159.19</v>
       </c>
       <c r="F50" s="13">
-        <v>169.49</v>
+        <v>169.19</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>173.42</v>
+        <v>172.51</v>
       </c>
       <c r="E54" s="10">
-        <v>175.12</v>
+        <v>174.33</v>
       </c>
       <c r="F54" s="10">
-        <v>185.12</v>
+        <v>184.33</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>161.62</v>
+        <v>160.71</v>
       </c>
       <c r="E55" s="13">
-        <v>170.12</v>
+        <v>169.25</v>
       </c>
       <c r="F55" s="13">
-        <v>180.12</v>
+        <v>179.25</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>163.99</v>
+        <v>162.97</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>163</v>
+        <v>161.99</v>
       </c>
       <c r="E57" s="13">
-        <v>164.39</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>158.9</v>
+        <v>157.88999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>160.44</v>
+        <v>159.57</v>
       </c>
       <c r="F58" s="10">
-        <v>170.44</v>
+        <v>169.57</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>165.51</v>
+        <v>164.61</v>
       </c>
       <c r="E59" s="13">
-        <v>172.37</v>
+        <v>171.59</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>174.47</v>
+        <v>173.42</v>
       </c>
       <c r="E60" s="10">
-        <v>175.52</v>
+        <v>175.12</v>
       </c>
       <c r="F60" s="10">
-        <v>185.52</v>
+        <v>185.12</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>162.66</v>
+        <v>161.62</v>
       </c>
       <c r="E61" s="13">
-        <v>170.66</v>
+        <v>170.12</v>
       </c>
       <c r="F61" s="13">
-        <v>180.66</v>
+        <v>180.12</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>165.03</v>
+        <v>163.99</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>164.04</v>
+        <v>163</v>
       </c>
       <c r="E63" s="13">
-        <v>164.93</v>
+        <v>164.39</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>159.94999999999999</v>
+        <v>158.9</v>
       </c>
       <c r="E64" s="10">
-        <v>160.97999999999999</v>
+        <v>160.44</v>
       </c>
       <c r="F64" s="10">
-        <v>170.98</v>
+        <v>170.44</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>166.56</v>
+        <v>165.51</v>
       </c>
       <c r="E65" s="13">
-        <v>172.78</v>
+        <v>172.37</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -1874,7 +1865,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,15 +2125,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2160,7 +2152,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,6 +2172,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Thu Dec 18 02:58:31 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D3C4CDFB-8CF2-4FC6-8D1C-2BCBEA1F8145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{6542A03E-B5EC-420D-81E3-CE3D8B9AD854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>156.56</v>
+        <v>155.34</v>
       </c>
       <c r="E8" s="10">
-        <v>156.88999999999999</v>
+        <v>155.65</v>
       </c>
       <c r="F8" s="10">
-        <v>166.89</v>
+        <v>165.65</v>
       </c>
       <c r="G8" s="10">
-        <v>157</v>
+        <v>155.77000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>156.56</v>
+        <v>155.34</v>
       </c>
       <c r="E9" s="13">
-        <v>156.88999999999999</v>
+        <v>155.65</v>
       </c>
       <c r="F9" s="13">
-        <v>166.89</v>
+        <v>165.65</v>
       </c>
       <c r="G9" s="13">
-        <v>157</v>
+        <v>155.77000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>158.63</v>
+        <v>157.33000000000001</v>
       </c>
       <c r="E10" s="10">
-        <v>159.46</v>
+        <v>158.25</v>
       </c>
       <c r="F10" s="10">
-        <v>169.46</v>
+        <v>168.25</v>
       </c>
       <c r="G10" s="10">
-        <v>159.97999999999999</v>
+        <v>158.77000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>157.72</v>
+        <v>156.56</v>
       </c>
       <c r="E11" s="13">
-        <v>157.78</v>
+        <v>156.88999999999999</v>
       </c>
       <c r="F11" s="13">
-        <v>167.78</v>
+        <v>166.89</v>
       </c>
       <c r="G11" s="13">
-        <v>157.9</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>157.72</v>
+        <v>156.56</v>
       </c>
       <c r="E12" s="10">
-        <v>157.78</v>
+        <v>156.88999999999999</v>
       </c>
       <c r="F12" s="10">
-        <v>167.78</v>
+        <v>166.89</v>
       </c>
       <c r="G12" s="10">
-        <v>157.9</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>159.65</v>
+        <v>158.63</v>
       </c>
       <c r="E13" s="13">
-        <v>160.22</v>
+        <v>159.46</v>
       </c>
       <c r="F13" s="13">
-        <v>170.23</v>
+        <v>169.46</v>
       </c>
       <c r="G13" s="13">
-        <v>160.74</v>
+        <v>159.97999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>161.69</v>
+        <v>160.84</v>
       </c>
       <c r="E17" s="10">
-        <v>163.15</v>
+        <v>162.5</v>
       </c>
       <c r="F17" s="10">
-        <v>173.15</v>
+        <v>172.5</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>162.6</v>
+        <v>161.69</v>
       </c>
       <c r="E18" s="13">
-        <v>163.76</v>
+        <v>163.15</v>
       </c>
       <c r="F18" s="13">
-        <v>173.76</v>
+        <v>173.15</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>157.37</v>
+        <v>156.15</v>
       </c>
       <c r="E22" s="10">
-        <v>158.46</v>
+        <v>157.25</v>
       </c>
       <c r="F22" s="10">
-        <v>168.06</v>
+        <v>166.85</v>
       </c>
       <c r="G22" s="10">
-        <v>159.62</v>
+        <v>158.41</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>163.55000000000001</v>
+        <v>162.68</v>
       </c>
       <c r="E23" s="13">
-        <v>163.57</v>
+        <v>162.57</v>
       </c>
       <c r="F23" s="13">
-        <v>173.57</v>
+        <v>172.57</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>163.32</v>
+        <v>162.44999999999999</v>
       </c>
       <c r="E24" s="10">
-        <v>163.89</v>
+        <v>162.88999999999999</v>
       </c>
       <c r="F24" s="10">
-        <v>173.89</v>
+        <v>172.89</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>163.82</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="E25" s="13">
-        <v>163.53</v>
+        <v>162.53</v>
       </c>
       <c r="F25" s="13">
-        <v>173.53</v>
+        <v>172.53</v>
       </c>
       <c r="G25" s="13">
-        <v>163.30000000000001</v>
+        <v>162.30000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>162.72999999999999</v>
+        <v>161.87</v>
       </c>
       <c r="E26" s="10">
-        <v>164.96</v>
+        <v>163.95</v>
       </c>
       <c r="F26" s="10">
-        <v>174.96</v>
+        <v>173.95</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>158.41999999999999</v>
+        <v>157.37</v>
       </c>
       <c r="E27" s="13">
-        <v>159.44</v>
+        <v>158.46</v>
       </c>
       <c r="F27" s="13">
-        <v>169.04</v>
+        <v>168.06</v>
       </c>
       <c r="G27" s="13">
-        <v>160.6</v>
+        <v>159.62</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>164.45</v>
+        <v>163.55000000000001</v>
       </c>
       <c r="E28" s="22">
-        <v>164.55</v>
+        <v>163.57</v>
       </c>
       <c r="F28" s="22">
-        <v>174.55</v>
+        <v>173.57</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>164.23</v>
+        <v>163.32</v>
       </c>
       <c r="E29" s="13">
-        <v>164.88</v>
+        <v>163.89</v>
       </c>
       <c r="F29" s="13">
-        <v>174.88</v>
+        <v>173.89</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>164.73</v>
+        <v>163.82</v>
       </c>
       <c r="E30" s="22">
-        <v>164.3</v>
+        <v>163.53</v>
       </c>
       <c r="F30" s="22">
-        <v>174.3</v>
+        <v>173.53</v>
       </c>
       <c r="G30" s="22">
-        <v>164.07</v>
+        <v>163.30000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>163.63</v>
+        <v>162.72999999999999</v>
       </c>
       <c r="E31" s="13">
-        <v>165.73</v>
+        <v>164.96</v>
       </c>
       <c r="F31" s="13">
-        <v>175.73</v>
+        <v>174.96</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>156.91999999999999</v>
+        <v>155.84</v>
       </c>
       <c r="E35" s="10">
-        <v>156.6</v>
+        <v>155.6</v>
       </c>
       <c r="F35" s="10">
-        <v>165.6</v>
+        <v>164.6</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>157.83000000000001</v>
+        <v>156.91999999999999</v>
       </c>
       <c r="E36" s="13">
-        <v>157.36000000000001</v>
+        <v>156.6</v>
       </c>
       <c r="F36" s="13">
-        <v>166.36</v>
+        <v>165.6</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>163.02000000000001</v>
+        <v>162.15</v>
       </c>
       <c r="E40" s="10">
-        <v>163.81</v>
+        <v>163.13</v>
       </c>
       <c r="F40" s="10">
-        <v>173.81</v>
+        <v>173.13</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>162.74</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="E41" s="13">
-        <v>164.23</v>
+        <v>163.55000000000001</v>
       </c>
       <c r="F41" s="13">
-        <v>174.23</v>
+        <v>173.55</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>163.93</v>
+        <v>163.02000000000001</v>
       </c>
       <c r="E42" s="10">
-        <v>164.42</v>
+        <v>163.81</v>
       </c>
       <c r="F42" s="10">
-        <v>174.42</v>
+        <v>173.81</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>163.65</v>
+        <v>162.74</v>
       </c>
       <c r="E43" s="13">
-        <v>164.84</v>
+        <v>164.23</v>
       </c>
       <c r="F43" s="13">
-        <v>174.84</v>
+        <v>174.23</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>158.11000000000001</v>
+        <v>157.06</v>
       </c>
       <c r="E47" s="10">
-        <v>158.53</v>
+        <v>157.77000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>168.53</v>
+        <v>167.77</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>157.91999999999999</v>
+        <v>156.87</v>
       </c>
       <c r="E48" s="13">
-        <v>158.62</v>
+        <v>157.86000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>168.62</v>
+        <v>167.86</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>159.24</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="E49" s="10">
-        <v>159.1</v>
+        <v>158.53</v>
       </c>
       <c r="F49" s="10">
-        <v>169.1</v>
+        <v>168.53</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>159.05000000000001</v>
+        <v>157.91999999999999</v>
       </c>
       <c r="E50" s="13">
-        <v>159.19</v>
+        <v>158.62</v>
       </c>
       <c r="F50" s="13">
-        <v>169.19</v>
+        <v>168.62</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>172.51</v>
+        <v>171.66</v>
       </c>
       <c r="E54" s="10">
-        <v>174.33</v>
+        <v>173.28</v>
       </c>
       <c r="F54" s="10">
-        <v>184.33</v>
+        <v>183.28</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>160.71</v>
+        <v>159.84</v>
       </c>
       <c r="E55" s="13">
-        <v>169.25</v>
+        <v>168.05</v>
       </c>
       <c r="F55" s="13">
-        <v>179.25</v>
+        <v>178.05</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>162.97</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>161.99</v>
+        <v>160.93</v>
       </c>
       <c r="E57" s="13">
-        <v>163.52000000000001</v>
+        <v>162.33000000000001</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>157.88999999999999</v>
+        <v>156.83000000000001</v>
       </c>
       <c r="E58" s="10">
-        <v>159.57</v>
+        <v>158.37</v>
       </c>
       <c r="F58" s="10">
-        <v>169.57</v>
+        <v>168.37</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>164.61</v>
+        <v>163.76</v>
       </c>
       <c r="E59" s="13">
-        <v>171.59</v>
+        <v>170.56</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>173.42</v>
+        <v>172.51</v>
       </c>
       <c r="E60" s="10">
-        <v>175.12</v>
+        <v>174.33</v>
       </c>
       <c r="F60" s="10">
-        <v>185.12</v>
+        <v>184.33</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>161.62</v>
+        <v>160.71</v>
       </c>
       <c r="E61" s="13">
-        <v>170.12</v>
+        <v>169.25</v>
       </c>
       <c r="F61" s="13">
-        <v>180.12</v>
+        <v>179.25</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>163.99</v>
+        <v>162.97</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>163</v>
+        <v>161.99</v>
       </c>
       <c r="E63" s="13">
-        <v>164.39</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>158.9</v>
+        <v>157.88999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>160.44</v>
+        <v>159.57</v>
       </c>
       <c r="F64" s="10">
-        <v>170.44</v>
+        <v>169.57</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>165.51</v>
+        <v>164.61</v>
       </c>
       <c r="E65" s="13">
-        <v>172.37</v>
+        <v>171.59</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,14 +1855,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2126,28 +2124,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2163,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fri Dec 19 03:01:46 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{6542A03E-B5EC-420D-81E3-CE3D8B9AD854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{57639887-7CF3-4383-938E-4147EA994A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>155.34</v>
+        <v>154.55000000000001</v>
       </c>
       <c r="E8" s="10">
-        <v>155.65</v>
+        <v>154.31</v>
       </c>
       <c r="F8" s="10">
-        <v>165.65</v>
+        <v>164.31</v>
       </c>
       <c r="G8" s="10">
-        <v>155.77000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>155.34</v>
+        <v>154.55000000000001</v>
       </c>
       <c r="E9" s="13">
-        <v>155.65</v>
+        <v>154.31</v>
       </c>
       <c r="F9" s="13">
-        <v>165.65</v>
+        <v>164.31</v>
       </c>
       <c r="G9" s="13">
-        <v>155.77000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154.43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>157.33000000000001</v>
+        <v>156.56</v>
       </c>
       <c r="E10" s="10">
-        <v>158.25</v>
+        <v>156.91999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>168.25</v>
+        <v>166.92</v>
       </c>
       <c r="G10" s="10">
-        <v>158.77000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>157.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>156.56</v>
+        <v>155.34</v>
       </c>
       <c r="E11" s="13">
-        <v>156.88999999999999</v>
+        <v>155.65</v>
       </c>
       <c r="F11" s="13">
-        <v>166.89</v>
+        <v>165.65</v>
       </c>
       <c r="G11" s="13">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>155.77000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>156.56</v>
+        <v>155.34</v>
       </c>
       <c r="E12" s="10">
-        <v>156.88999999999999</v>
+        <v>155.65</v>
       </c>
       <c r="F12" s="10">
-        <v>166.89</v>
+        <v>165.65</v>
       </c>
       <c r="G12" s="10">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>155.77000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>158.63</v>
+        <v>157.33000000000001</v>
       </c>
       <c r="E13" s="13">
-        <v>159.46</v>
+        <v>158.25</v>
       </c>
       <c r="F13" s="13">
-        <v>169.46</v>
+        <v>168.25</v>
       </c>
       <c r="G13" s="13">
-        <v>159.97999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.77000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>160.84</v>
+        <v>160.41999999999999</v>
       </c>
       <c r="E17" s="10">
-        <v>162.5</v>
+        <v>161.84</v>
       </c>
       <c r="F17" s="10">
-        <v>172.5</v>
+        <v>171.84</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>161.69</v>
+        <v>160.84</v>
       </c>
       <c r="E18" s="13">
-        <v>163.15</v>
+        <v>162.5</v>
       </c>
       <c r="F18" s="13">
-        <v>173.15</v>
+        <v>172.5</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>156.15</v>
+        <v>155.37</v>
       </c>
       <c r="E22" s="10">
-        <v>157.25</v>
+        <v>155.93</v>
       </c>
       <c r="F22" s="10">
-        <v>166.85</v>
+        <v>165.53</v>
       </c>
       <c r="G22" s="10">
-        <v>158.41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>157.09</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>162.68</v>
+        <v>161.69</v>
       </c>
       <c r="E23" s="13">
-        <v>162.57</v>
+        <v>161.58000000000001</v>
       </c>
       <c r="F23" s="13">
-        <v>172.57</v>
+        <v>171.58</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>162.44999999999999</v>
+        <v>161.46</v>
       </c>
       <c r="E24" s="10">
-        <v>162.88999999999999</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="F24" s="10">
-        <v>172.89</v>
+        <v>171.89</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>162.94999999999999</v>
+        <v>161.96</v>
       </c>
       <c r="E25" s="13">
-        <v>162.53</v>
+        <v>161.53</v>
       </c>
       <c r="F25" s="13">
-        <v>172.53</v>
+        <v>171.53</v>
       </c>
       <c r="G25" s="13">
-        <v>162.30000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161.30000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>161.87</v>
+        <v>160.88</v>
       </c>
       <c r="E26" s="10">
-        <v>163.95</v>
+        <v>162.94</v>
       </c>
       <c r="F26" s="10">
-        <v>173.95</v>
+        <v>172.94</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>157.37</v>
+        <v>156.15</v>
       </c>
       <c r="E27" s="13">
-        <v>158.46</v>
+        <v>157.25</v>
       </c>
       <c r="F27" s="13">
-        <v>168.06</v>
+        <v>166.85</v>
       </c>
       <c r="G27" s="13">
-        <v>159.62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>163.55000000000001</v>
+        <v>162.68</v>
       </c>
       <c r="E28" s="22">
-        <v>163.57</v>
+        <v>162.57</v>
       </c>
       <c r="F28" s="22">
-        <v>173.57</v>
+        <v>172.57</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>163.32</v>
+        <v>162.44999999999999</v>
       </c>
       <c r="E29" s="13">
-        <v>163.89</v>
+        <v>162.88999999999999</v>
       </c>
       <c r="F29" s="13">
-        <v>173.89</v>
+        <v>172.89</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>163.82</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="E30" s="22">
-        <v>163.53</v>
+        <v>162.53</v>
       </c>
       <c r="F30" s="22">
-        <v>173.53</v>
+        <v>172.53</v>
       </c>
       <c r="G30" s="22">
-        <v>163.30000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>162.30000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>162.72999999999999</v>
+        <v>161.87</v>
       </c>
       <c r="E31" s="13">
-        <v>164.96</v>
+        <v>163.95</v>
       </c>
       <c r="F31" s="13">
-        <v>174.96</v>
+        <v>173.95</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>155.84</v>
+        <v>154.96</v>
       </c>
       <c r="E35" s="10">
-        <v>155.6</v>
+        <v>154.61000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>164.6</v>
+        <v>163.61000000000001</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>156.91999999999999</v>
+        <v>155.84</v>
       </c>
       <c r="E36" s="13">
-        <v>156.6</v>
+        <v>155.6</v>
       </c>
       <c r="F36" s="13">
-        <v>165.6</v>
+        <v>164.6</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>162.15</v>
+        <v>161.69</v>
       </c>
       <c r="E40" s="10">
-        <v>163.13</v>
+        <v>162.44</v>
       </c>
       <c r="F40" s="10">
-        <v>173.13</v>
+        <v>172.44</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>161.86000000000001</v>
+        <v>161.41</v>
       </c>
       <c r="E41" s="13">
-        <v>163.55000000000001</v>
+        <v>162.86000000000001</v>
       </c>
       <c r="F41" s="13">
-        <v>173.55</v>
+        <v>172.86</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>163.02000000000001</v>
+        <v>162.15</v>
       </c>
       <c r="E42" s="10">
-        <v>163.81</v>
+        <v>163.13</v>
       </c>
       <c r="F42" s="10">
-        <v>173.81</v>
+        <v>173.13</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>162.74</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="E43" s="13">
-        <v>164.23</v>
+        <v>163.55000000000001</v>
       </c>
       <c r="F43" s="13">
-        <v>174.23</v>
+        <v>173.55</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>157.06</v>
+        <v>155.94</v>
       </c>
       <c r="E47" s="10">
-        <v>157.77000000000001</v>
+        <v>156.9</v>
       </c>
       <c r="F47" s="10">
-        <v>167.77</v>
+        <v>166.9</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>156.87</v>
+        <v>155.75</v>
       </c>
       <c r="E48" s="13">
-        <v>157.86000000000001</v>
+        <v>156.99</v>
       </c>
       <c r="F48" s="13">
-        <v>167.86</v>
+        <v>166.99</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>158.11000000000001</v>
+        <v>157.06</v>
       </c>
       <c r="E49" s="10">
-        <v>158.53</v>
+        <v>157.77000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>168.53</v>
+        <v>167.77</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>157.91999999999999</v>
+        <v>156.87</v>
       </c>
       <c r="E50" s="13">
-        <v>158.62</v>
+        <v>157.86000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>168.62</v>
+        <v>167.86</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>171.66</v>
+        <v>171.23</v>
       </c>
       <c r="E54" s="10">
-        <v>173.28</v>
+        <v>172.21</v>
       </c>
       <c r="F54" s="10">
-        <v>183.28</v>
+        <v>182.21</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>159.84</v>
+        <v>159.4</v>
       </c>
       <c r="E55" s="13">
-        <v>168.05</v>
+        <v>166.75</v>
       </c>
       <c r="F55" s="13">
-        <v>178.05</v>
+        <v>176.75</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>161.88999999999999</v>
+        <v>161.11000000000001</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>160.93</v>
+        <v>160.18</v>
       </c>
       <c r="E57" s="13">
-        <v>162.33000000000001</v>
+        <v>161.02000000000001</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>156.83000000000001</v>
+        <v>156.08000000000001</v>
       </c>
       <c r="E58" s="10">
-        <v>158.37</v>
+        <v>157.07</v>
       </c>
       <c r="F58" s="10">
-        <v>168.37</v>
+        <v>167.07</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>163.76</v>
+        <v>163.34</v>
       </c>
       <c r="E59" s="13">
-        <v>170.56</v>
+        <v>169.53</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>172.51</v>
+        <v>171.66</v>
       </c>
       <c r="E60" s="10">
-        <v>174.33</v>
+        <v>173.28</v>
       </c>
       <c r="F60" s="10">
-        <v>184.33</v>
+        <v>183.28</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>160.71</v>
+        <v>159.84</v>
       </c>
       <c r="E61" s="13">
-        <v>169.25</v>
+        <v>168.05</v>
       </c>
       <c r="F61" s="13">
-        <v>179.25</v>
+        <v>178.05</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>162.97</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>161.99</v>
+        <v>160.93</v>
       </c>
       <c r="E63" s="13">
-        <v>163.52000000000001</v>
+        <v>162.33000000000001</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>157.88999999999999</v>
+        <v>156.83000000000001</v>
       </c>
       <c r="E64" s="10">
-        <v>159.57</v>
+        <v>158.37</v>
       </c>
       <c r="F64" s="10">
-        <v>169.57</v>
+        <v>168.37</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>164.61</v>
+        <v>163.76</v>
       </c>
       <c r="E65" s="13">
-        <v>171.59</v>
+        <v>170.56</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1864,6 +1864,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2123,17 +2134,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
@@ -2143,6 +2143,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2162,24 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Mon Dec 22 03:12:40 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{57639887-7CF3-4383-938E-4147EA994A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{18211FC1-ADCD-4577-B851-DB2CAEC7BEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>154.55000000000001</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="E8" s="10">
-        <v>154.31</v>
+        <v>152.87</v>
       </c>
       <c r="F8" s="10">
-        <v>164.31</v>
+        <v>162.87</v>
       </c>
       <c r="G8" s="10">
-        <v>154.43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>152.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>154.55000000000001</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="E9" s="13">
-        <v>154.31</v>
+        <v>152.87</v>
       </c>
       <c r="F9" s="13">
-        <v>164.31</v>
+        <v>162.87</v>
       </c>
       <c r="G9" s="13">
-        <v>154.43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>152.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>156.56</v>
+        <v>155.80000000000001</v>
       </c>
       <c r="E10" s="10">
-        <v>156.91999999999999</v>
+        <v>155.79</v>
       </c>
       <c r="F10" s="10">
-        <v>166.92</v>
+        <v>165.79</v>
       </c>
       <c r="G10" s="10">
-        <v>157.44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>156.31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>155.34</v>
+        <v>154.55000000000001</v>
       </c>
       <c r="E11" s="13">
-        <v>155.65</v>
+        <v>154.31</v>
       </c>
       <c r="F11" s="13">
-        <v>165.65</v>
+        <v>164.31</v>
       </c>
       <c r="G11" s="13">
-        <v>155.77000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>154.43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>155.34</v>
+        <v>154.55000000000001</v>
       </c>
       <c r="E12" s="10">
-        <v>155.65</v>
+        <v>154.31</v>
       </c>
       <c r="F12" s="10">
-        <v>165.65</v>
+        <v>164.31</v>
       </c>
       <c r="G12" s="10">
-        <v>155.77000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>154.43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>157.33000000000001</v>
+        <v>156.56</v>
       </c>
       <c r="E13" s="13">
-        <v>158.25</v>
+        <v>156.91999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>168.25</v>
+        <v>166.92</v>
       </c>
       <c r="G13" s="13">
-        <v>158.77000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>157.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>160.41999999999999</v>
+        <v>159.69</v>
       </c>
       <c r="E17" s="10">
-        <v>161.84</v>
+        <v>160.99</v>
       </c>
       <c r="F17" s="10">
-        <v>171.84</v>
+        <v>171</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>160.84</v>
+        <v>160.41999999999999</v>
       </c>
       <c r="E18" s="13">
-        <v>162.5</v>
+        <v>161.84</v>
       </c>
       <c r="F18" s="13">
-        <v>172.5</v>
+        <v>171.84</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>155.37</v>
+        <v>154.63</v>
       </c>
       <c r="E22" s="10">
-        <v>155.93</v>
+        <v>154.47999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>165.53</v>
+        <v>164.08</v>
       </c>
       <c r="G22" s="10">
-        <v>157.09</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>155.63999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>161.69</v>
+        <v>160.27000000000001</v>
       </c>
       <c r="E23" s="13">
-        <v>161.58000000000001</v>
+        <v>159.88999999999999</v>
       </c>
       <c r="F23" s="13">
-        <v>171.58</v>
+        <v>169.89</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>161.46</v>
+        <v>160.04</v>
       </c>
       <c r="E24" s="10">
-        <v>161.88999999999999</v>
+        <v>160.41</v>
       </c>
       <c r="F24" s="10">
-        <v>171.89</v>
+        <v>170.41</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>161.96</v>
+        <v>160.54</v>
       </c>
       <c r="E25" s="13">
-        <v>161.53</v>
+        <v>160.16</v>
       </c>
       <c r="F25" s="13">
-        <v>171.53</v>
+        <v>170.16</v>
       </c>
       <c r="G25" s="13">
-        <v>161.30000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>159.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>160.88</v>
+        <v>159.47</v>
       </c>
       <c r="E26" s="10">
-        <v>162.94</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="F26" s="10">
-        <v>172.94</v>
+        <v>171.45</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>156.15</v>
+        <v>155.37</v>
       </c>
       <c r="E27" s="13">
-        <v>157.25</v>
+        <v>155.93</v>
       </c>
       <c r="F27" s="13">
-        <v>166.85</v>
+        <v>165.53</v>
       </c>
       <c r="G27" s="13">
-        <v>158.41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>157.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>162.68</v>
+        <v>161.69</v>
       </c>
       <c r="E28" s="22">
-        <v>162.57</v>
+        <v>161.58000000000001</v>
       </c>
       <c r="F28" s="22">
-        <v>172.57</v>
+        <v>171.58</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>162.44999999999999</v>
+        <v>161.46</v>
       </c>
       <c r="E29" s="13">
-        <v>162.88999999999999</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="F29" s="13">
-        <v>172.89</v>
+        <v>171.89</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>162.94999999999999</v>
+        <v>161.96</v>
       </c>
       <c r="E30" s="22">
-        <v>162.53</v>
+        <v>161.53</v>
       </c>
       <c r="F30" s="22">
-        <v>172.53</v>
+        <v>171.53</v>
       </c>
       <c r="G30" s="22">
-        <v>162.30000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>161.30000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>161.87</v>
+        <v>160.88</v>
       </c>
       <c r="E31" s="13">
-        <v>163.95</v>
+        <v>162.94</v>
       </c>
       <c r="F31" s="13">
-        <v>173.95</v>
+        <v>172.94</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>154.96</v>
+        <v>153.63999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>154.61000000000001</v>
+        <v>153.47</v>
       </c>
       <c r="F35" s="10">
-        <v>163.61000000000001</v>
+        <v>162.47</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>155.84</v>
+        <v>154.96</v>
       </c>
       <c r="E36" s="13">
-        <v>155.6</v>
+        <v>154.61000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>164.6</v>
+        <v>163.61000000000001</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>161.69</v>
+        <v>160.9</v>
       </c>
       <c r="E40" s="10">
-        <v>162.44</v>
+        <v>161.54</v>
       </c>
       <c r="F40" s="10">
-        <v>172.44</v>
+        <v>171.54</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>161.41</v>
+        <v>160.62</v>
       </c>
       <c r="E41" s="13">
-        <v>162.86000000000001</v>
+        <v>161.96</v>
       </c>
       <c r="F41" s="13">
-        <v>172.86</v>
+        <v>171.96</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>162.15</v>
+        <v>161.69</v>
       </c>
       <c r="E42" s="10">
-        <v>163.13</v>
+        <v>162.44</v>
       </c>
       <c r="F42" s="10">
-        <v>173.13</v>
+        <v>172.44</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>161.86000000000001</v>
+        <v>161.41</v>
       </c>
       <c r="E43" s="13">
-        <v>163.55000000000001</v>
+        <v>162.86000000000001</v>
       </c>
       <c r="F43" s="13">
-        <v>173.55</v>
+        <v>172.86</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>155.94</v>
+        <v>154.91</v>
       </c>
       <c r="E47" s="10">
-        <v>156.9</v>
+        <v>156.03</v>
       </c>
       <c r="F47" s="10">
-        <v>166.9</v>
+        <v>166.03</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>155.75</v>
+        <v>154.72999999999999</v>
       </c>
       <c r="E48" s="13">
-        <v>156.99</v>
+        <v>156.13</v>
       </c>
       <c r="F48" s="13">
-        <v>166.99</v>
+        <v>166.13</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>157.06</v>
+        <v>155.94</v>
       </c>
       <c r="E49" s="10">
-        <v>157.77000000000001</v>
+        <v>156.9</v>
       </c>
       <c r="F49" s="10">
-        <v>167.77</v>
+        <v>166.9</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>156.87</v>
+        <v>155.75</v>
       </c>
       <c r="E50" s="13">
-        <v>157.86000000000001</v>
+        <v>156.99</v>
       </c>
       <c r="F50" s="13">
-        <v>167.86</v>
+        <v>166.99</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>171.23</v>
+        <v>170.48</v>
       </c>
       <c r="E54" s="10">
-        <v>172.21</v>
+        <v>170.95</v>
       </c>
       <c r="F54" s="10">
-        <v>182.21</v>
+        <v>180.95</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>159.4</v>
+        <v>158.63999999999999</v>
       </c>
       <c r="E55" s="13">
-        <v>166.75</v>
+        <v>165.1</v>
       </c>
       <c r="F55" s="13">
-        <v>176.75</v>
+        <v>175.1</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>161.11000000000001</v>
+        <v>160.01</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>160.18</v>
+        <v>159.12</v>
       </c>
       <c r="E57" s="13">
-        <v>161.02000000000001</v>
+        <v>159.38</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>156.08000000000001</v>
+        <v>155.02000000000001</v>
       </c>
       <c r="E58" s="10">
-        <v>157.07</v>
+        <v>155.41999999999999</v>
       </c>
       <c r="F58" s="10">
-        <v>167.07</v>
+        <v>165.42</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>163.34</v>
+        <v>162.62</v>
       </c>
       <c r="E59" s="13">
-        <v>169.53</v>
+        <v>168.32</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>171.66</v>
+        <v>171.23</v>
       </c>
       <c r="E60" s="10">
-        <v>173.28</v>
+        <v>172.21</v>
       </c>
       <c r="F60" s="10">
-        <v>183.28</v>
+        <v>182.21</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>159.84</v>
+        <v>159.4</v>
       </c>
       <c r="E61" s="13">
-        <v>168.05</v>
+        <v>166.75</v>
       </c>
       <c r="F61" s="13">
-        <v>178.05</v>
+        <v>176.75</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>161.88999999999999</v>
+        <v>161.11000000000001</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>160.93</v>
+        <v>160.18</v>
       </c>
       <c r="E63" s="13">
-        <v>162.33000000000001</v>
+        <v>161.02000000000001</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>156.83000000000001</v>
+        <v>156.08000000000001</v>
       </c>
       <c r="E64" s="10">
-        <v>158.37</v>
+        <v>157.07</v>
       </c>
       <c r="F64" s="10">
-        <v>168.37</v>
+        <v>167.07</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46010</v>
+        <v>46011</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>163.76</v>
+        <v>163.34</v>
       </c>
       <c r="E65" s="13">
-        <v>170.56</v>
+        <v>169.53</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,26 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,10 +2114,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2161,21 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Dec 23 03:07:10 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{18211FC1-ADCD-4577-B851-DB2CAEC7BEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{E59A915B-3D41-4380-ADC3-9CF7BB44A568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentManualCount="8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>153.27000000000001</v>
+        <v>152.34</v>
       </c>
       <c r="E8" s="10">
-        <v>152.87</v>
+        <v>152.05000000000001</v>
       </c>
       <c r="F8" s="10">
-        <v>162.87</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="G8" s="10">
-        <v>152.99</v>
+        <v>152.16999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>153.27000000000001</v>
+        <v>152.34</v>
       </c>
       <c r="E9" s="13">
-        <v>152.87</v>
+        <v>152.05000000000001</v>
       </c>
       <c r="F9" s="13">
-        <v>162.87</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="G9" s="13">
-        <v>152.99</v>
+        <v>152.16999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>155.80000000000001</v>
+        <v>155.07</v>
       </c>
       <c r="E10" s="10">
-        <v>155.79</v>
+        <v>154.18</v>
       </c>
       <c r="F10" s="10">
-        <v>165.79</v>
+        <v>164.18</v>
       </c>
       <c r="G10" s="10">
-        <v>156.31</v>
+        <v>154.69999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>154.55000000000001</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="E11" s="13">
-        <v>154.31</v>
+        <v>152.87</v>
       </c>
       <c r="F11" s="13">
-        <v>164.31</v>
+        <v>162.87</v>
       </c>
       <c r="G11" s="13">
-        <v>154.43</v>
+        <v>152.99</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>154.55000000000001</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="E12" s="10">
-        <v>154.31</v>
+        <v>152.87</v>
       </c>
       <c r="F12" s="10">
-        <v>164.31</v>
+        <v>162.87</v>
       </c>
       <c r="G12" s="10">
-        <v>154.43</v>
+        <v>152.99</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>156.56</v>
+        <v>155.80000000000001</v>
       </c>
       <c r="E13" s="13">
-        <v>156.91999999999999</v>
+        <v>155.79</v>
       </c>
       <c r="F13" s="13">
-        <v>166.92</v>
+        <v>165.79</v>
       </c>
       <c r="G13" s="13">
-        <v>157.44</v>
+        <v>156.31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>159.69</v>
+        <v>159.21</v>
       </c>
       <c r="E17" s="10">
-        <v>160.99</v>
+        <v>160.13999999999999</v>
       </c>
       <c r="F17" s="10">
-        <v>171</v>
+        <v>170.14</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>160.41999999999999</v>
+        <v>159.69</v>
       </c>
       <c r="E18" s="13">
-        <v>161.84</v>
+        <v>160.99</v>
       </c>
       <c r="F18" s="13">
-        <v>171.84</v>
+        <v>171</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>154.63</v>
+        <v>153.93</v>
       </c>
       <c r="E22" s="10">
-        <v>154.47999999999999</v>
+        <v>153.43</v>
       </c>
       <c r="F22" s="10">
-        <v>164.08</v>
+        <v>163.03</v>
       </c>
       <c r="G22" s="10">
-        <v>155.63999999999999</v>
+        <v>154.59</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>160.27000000000001</v>
+        <v>159.53</v>
       </c>
       <c r="E23" s="13">
-        <v>159.88999999999999</v>
+        <v>159.05000000000001</v>
       </c>
       <c r="F23" s="13">
-        <v>169.89</v>
+        <v>169.05</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>160.04</v>
+        <v>159.31</v>
       </c>
       <c r="E24" s="10">
-        <v>160.41</v>
+        <v>159.56</v>
       </c>
       <c r="F24" s="10">
-        <v>170.41</v>
+        <v>169.56</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>160.54</v>
+        <v>159.81</v>
       </c>
       <c r="E25" s="13">
-        <v>160.16</v>
+        <v>159.30000000000001</v>
       </c>
       <c r="F25" s="13">
-        <v>170.16</v>
+        <v>169.3</v>
       </c>
       <c r="G25" s="13">
-        <v>159.93</v>
+        <v>159.07</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>159.47</v>
+        <v>158.74</v>
       </c>
       <c r="E26" s="10">
-        <v>161.44999999999999</v>
+        <v>160.58000000000001</v>
       </c>
       <c r="F26" s="10">
-        <v>171.45</v>
+        <v>170.58</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>155.37</v>
+        <v>154.63</v>
       </c>
       <c r="E27" s="13">
-        <v>155.93</v>
+        <v>154.47999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>165.53</v>
+        <v>164.08</v>
       </c>
       <c r="G27" s="13">
-        <v>157.09</v>
+        <v>155.63999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>161.69</v>
+        <v>160.27000000000001</v>
       </c>
       <c r="E28" s="22">
-        <v>161.58000000000001</v>
+        <v>159.88999999999999</v>
       </c>
       <c r="F28" s="22">
-        <v>171.58</v>
+        <v>169.89</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>161.46</v>
+        <v>160.04</v>
       </c>
       <c r="E29" s="13">
-        <v>161.88999999999999</v>
+        <v>160.41</v>
       </c>
       <c r="F29" s="13">
-        <v>171.89</v>
+        <v>170.41</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>161.96</v>
+        <v>160.54</v>
       </c>
       <c r="E30" s="22">
-        <v>161.53</v>
+        <v>160.16</v>
       </c>
       <c r="F30" s="22">
-        <v>171.53</v>
+        <v>170.16</v>
       </c>
       <c r="G30" s="22">
-        <v>161.30000000000001</v>
+        <v>159.93</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>160.88</v>
+        <v>159.47</v>
       </c>
       <c r="E31" s="13">
-        <v>162.94</v>
+        <v>161.44999999999999</v>
       </c>
       <c r="F31" s="13">
-        <v>172.94</v>
+        <v>171.45</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>153.63999999999999</v>
+        <v>152.58000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>153.47</v>
+        <v>152.63</v>
       </c>
       <c r="F35" s="10">
-        <v>162.47</v>
+        <v>161.63</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>154.96</v>
+        <v>153.63999999999999</v>
       </c>
       <c r="E36" s="13">
-        <v>154.61000000000001</v>
+        <v>153.47</v>
       </c>
       <c r="F36" s="13">
-        <v>163.61000000000001</v>
+        <v>162.47</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>160.9</v>
+        <v>160.37</v>
       </c>
       <c r="E40" s="10">
-        <v>161.54</v>
+        <v>160.63</v>
       </c>
       <c r="F40" s="10">
-        <v>171.54</v>
+        <v>170.63</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>160.62</v>
+        <v>160.09</v>
       </c>
       <c r="E41" s="13">
-        <v>161.96</v>
+        <v>161.05000000000001</v>
       </c>
       <c r="F41" s="13">
-        <v>171.96</v>
+        <v>171.05</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>161.69</v>
+        <v>160.9</v>
       </c>
       <c r="E42" s="10">
-        <v>162.44</v>
+        <v>161.54</v>
       </c>
       <c r="F42" s="10">
-        <v>172.44</v>
+        <v>171.54</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>161.41</v>
+        <v>160.62</v>
       </c>
       <c r="E43" s="13">
-        <v>162.86000000000001</v>
+        <v>161.96</v>
       </c>
       <c r="F43" s="13">
-        <v>172.86</v>
+        <v>171.96</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>154.91</v>
+        <v>154.16999999999999</v>
       </c>
       <c r="E47" s="10">
-        <v>156.03</v>
+        <v>155.25</v>
       </c>
       <c r="F47" s="10">
-        <v>166.03</v>
+        <v>165.25</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>154.72999999999999</v>
+        <v>153.99</v>
       </c>
       <c r="E48" s="13">
-        <v>156.13</v>
+        <v>155.35</v>
       </c>
       <c r="F48" s="13">
-        <v>166.13</v>
+        <v>165.35</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>155.94</v>
+        <v>154.91</v>
       </c>
       <c r="E49" s="10">
-        <v>156.9</v>
+        <v>156.03</v>
       </c>
       <c r="F49" s="10">
-        <v>166.9</v>
+        <v>166.03</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>155.75</v>
+        <v>154.72999999999999</v>
       </c>
       <c r="E50" s="13">
-        <v>156.99</v>
+        <v>156.13</v>
       </c>
       <c r="F50" s="13">
-        <v>166.99</v>
+        <v>166.13</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>170.48</v>
+        <v>169.98</v>
       </c>
       <c r="E54" s="10">
-        <v>170.95</v>
+        <v>169.99</v>
       </c>
       <c r="F54" s="10">
-        <v>180.95</v>
+        <v>179.99</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>158.63999999999999</v>
+        <v>158.13</v>
       </c>
       <c r="E55" s="13">
-        <v>165.1</v>
+        <v>164.62</v>
       </c>
       <c r="F55" s="13">
-        <v>175.1</v>
+        <v>174.62</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>160.01</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>159.12</v>
+        <v>158.97999999999999</v>
       </c>
       <c r="E57" s="13">
-        <v>159.38</v>
+        <v>158.9</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>155.02000000000001</v>
+        <v>154.88</v>
       </c>
       <c r="E58" s="10">
-        <v>155.41999999999999</v>
+        <v>154.94</v>
       </c>
       <c r="F58" s="10">
-        <v>165.42</v>
+        <v>164.94</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>162.62</v>
+        <v>162.13999999999999</v>
       </c>
       <c r="E59" s="13">
-        <v>168.32</v>
+        <v>167.41</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>171.23</v>
+        <v>170.48</v>
       </c>
       <c r="E60" s="10">
-        <v>172.21</v>
+        <v>170.95</v>
       </c>
       <c r="F60" s="10">
-        <v>182.21</v>
+        <v>180.95</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>159.4</v>
+        <v>158.63999999999999</v>
       </c>
       <c r="E61" s="13">
-        <v>166.75</v>
+        <v>165.1</v>
       </c>
       <c r="F61" s="13">
-        <v>176.75</v>
+        <v>175.1</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>161.11000000000001</v>
+        <v>160.01</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>160.18</v>
+        <v>159.12</v>
       </c>
       <c r="E63" s="13">
-        <v>161.02000000000001</v>
+        <v>159.38</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>156.08000000000001</v>
+        <v>155.02000000000001</v>
       </c>
       <c r="E64" s="10">
-        <v>157.07</v>
+        <v>155.41999999999999</v>
       </c>
       <c r="F64" s="10">
-        <v>167.07</v>
+        <v>165.42</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46011</v>
+        <v>46014</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>163.34</v>
+        <v>162.62</v>
       </c>
       <c r="E65" s="13">
-        <v>169.53</v>
+        <v>168.32</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,17 +2125,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,6 +2135,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2154,24 +2172,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Wed Dec 24 03:00:42 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E59A915B-3D41-4380-ADC3-9CF7BB44A568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{F1AB6B2B-885F-4205-8A43-36B4EFB5A3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.34</v>
+        <v>152.16</v>
       </c>
       <c r="E8" s="10">
-        <v>152.05000000000001</v>
+        <v>151.68</v>
       </c>
       <c r="F8" s="10">
-        <v>162.05000000000001</v>
+        <v>161.68</v>
       </c>
       <c r="G8" s="10">
-        <v>152.16999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.34</v>
+        <v>152.16</v>
       </c>
       <c r="E9" s="13">
-        <v>152.05000000000001</v>
+        <v>151.68</v>
       </c>
       <c r="F9" s="13">
-        <v>162.05000000000001</v>
+        <v>161.68</v>
       </c>
       <c r="G9" s="13">
-        <v>152.16999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>155.07</v>
+        <v>154.87</v>
       </c>
       <c r="E10" s="10">
-        <v>154.18</v>
+        <v>153.79</v>
       </c>
       <c r="F10" s="10">
-        <v>164.18</v>
+        <v>163.79</v>
       </c>
       <c r="G10" s="10">
-        <v>154.69999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154.31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>153.27000000000001</v>
+        <v>152.34</v>
       </c>
       <c r="E11" s="13">
-        <v>152.87</v>
+        <v>152.05000000000001</v>
       </c>
       <c r="F11" s="13">
-        <v>162.87</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="G11" s="13">
-        <v>152.99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152.16999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>153.27000000000001</v>
+        <v>152.34</v>
       </c>
       <c r="E12" s="10">
-        <v>152.87</v>
+        <v>152.05000000000001</v>
       </c>
       <c r="F12" s="10">
-        <v>162.87</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="G12" s="10">
-        <v>152.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152.16999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>155.80000000000001</v>
+        <v>155.07</v>
       </c>
       <c r="E13" s="13">
-        <v>155.79</v>
+        <v>154.18</v>
       </c>
       <c r="F13" s="13">
-        <v>165.79</v>
+        <v>164.18</v>
       </c>
       <c r="G13" s="13">
-        <v>156.31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154.69999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>159.21</v>
+        <v>159.04</v>
       </c>
       <c r="E17" s="10">
-        <v>160.13999999999999</v>
+        <v>159.72999999999999</v>
       </c>
       <c r="F17" s="10">
-        <v>170.14</v>
+        <v>169.73</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>159.69</v>
+        <v>159.21</v>
       </c>
       <c r="E18" s="13">
-        <v>160.99</v>
+        <v>160.13999999999999</v>
       </c>
       <c r="F18" s="13">
-        <v>171</v>
+        <v>170.14</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.93</v>
+        <v>153.74</v>
       </c>
       <c r="E22" s="10">
-        <v>153.43</v>
+        <v>153.05000000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>163.03</v>
+        <v>162.65</v>
       </c>
       <c r="G22" s="10">
-        <v>154.59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154.21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>159.53</v>
+        <v>159.33000000000001</v>
       </c>
       <c r="E23" s="13">
-        <v>159.05000000000001</v>
+        <v>158.66</v>
       </c>
       <c r="F23" s="13">
-        <v>169.05</v>
+        <v>168.66</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>159.31</v>
+        <v>159.12</v>
       </c>
       <c r="E24" s="10">
-        <v>159.56</v>
+        <v>159.16</v>
       </c>
       <c r="F24" s="10">
-        <v>169.56</v>
+        <v>169.16</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>159.81</v>
+        <v>159.62</v>
       </c>
       <c r="E25" s="13">
-        <v>159.30000000000001</v>
+        <v>158.9</v>
       </c>
       <c r="F25" s="13">
-        <v>169.3</v>
+        <v>168.9</v>
       </c>
       <c r="G25" s="13">
-        <v>159.07</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.66999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.74</v>
+        <v>158.56</v>
       </c>
       <c r="E26" s="10">
-        <v>160.58000000000001</v>
+        <v>160.18</v>
       </c>
       <c r="F26" s="10">
-        <v>170.58</v>
+        <v>170.18</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>154.63</v>
+        <v>153.93</v>
       </c>
       <c r="E27" s="13">
-        <v>154.47999999999999</v>
+        <v>153.43</v>
       </c>
       <c r="F27" s="13">
-        <v>164.08</v>
+        <v>163.03</v>
       </c>
       <c r="G27" s="13">
-        <v>155.63999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>160.27000000000001</v>
+        <v>159.53</v>
       </c>
       <c r="E28" s="22">
-        <v>159.88999999999999</v>
+        <v>159.05000000000001</v>
       </c>
       <c r="F28" s="22">
-        <v>169.89</v>
+        <v>169.05</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>160.04</v>
+        <v>159.31</v>
       </c>
       <c r="E29" s="13">
-        <v>160.41</v>
+        <v>159.56</v>
       </c>
       <c r="F29" s="13">
-        <v>170.41</v>
+        <v>169.56</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>160.54</v>
+        <v>159.81</v>
       </c>
       <c r="E30" s="22">
-        <v>160.16</v>
+        <v>159.30000000000001</v>
       </c>
       <c r="F30" s="22">
-        <v>170.16</v>
+        <v>169.3</v>
       </c>
       <c r="G30" s="22">
-        <v>159.93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>159.07</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>159.47</v>
+        <v>158.74</v>
       </c>
       <c r="E31" s="13">
-        <v>161.44999999999999</v>
+        <v>160.58000000000001</v>
       </c>
       <c r="F31" s="13">
-        <v>171.45</v>
+        <v>170.58</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.58000000000001</v>
+        <v>152.38999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>152.63</v>
+        <v>152.24</v>
       </c>
       <c r="F35" s="10">
-        <v>161.63</v>
+        <v>161.24</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>153.63999999999999</v>
+        <v>152.58000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>153.47</v>
+        <v>152.63</v>
       </c>
       <c r="F36" s="13">
-        <v>162.47</v>
+        <v>161.63</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>160.37</v>
+        <v>160.15</v>
       </c>
       <c r="E40" s="10">
-        <v>160.63</v>
+        <v>160.18</v>
       </c>
       <c r="F40" s="10">
-        <v>170.63</v>
+        <v>170.18</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>160.09</v>
+        <v>159.87</v>
       </c>
       <c r="E41" s="13">
-        <v>161.05000000000001</v>
+        <v>160.6</v>
       </c>
       <c r="F41" s="13">
-        <v>171.05</v>
+        <v>170.6</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>160.9</v>
+        <v>160.37</v>
       </c>
       <c r="E42" s="10">
-        <v>161.54</v>
+        <v>160.63</v>
       </c>
       <c r="F42" s="10">
-        <v>171.54</v>
+        <v>170.63</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>160.62</v>
+        <v>160.09</v>
       </c>
       <c r="E43" s="13">
-        <v>161.96</v>
+        <v>161.05000000000001</v>
       </c>
       <c r="F43" s="13">
-        <v>171.96</v>
+        <v>171.05</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>154.16999999999999</v>
+        <v>153.63999999999999</v>
       </c>
       <c r="E47" s="10">
-        <v>155.25</v>
+        <v>154.47</v>
       </c>
       <c r="F47" s="10">
-        <v>165.25</v>
+        <v>164.47</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>153.99</v>
+        <v>153.47</v>
       </c>
       <c r="E48" s="13">
-        <v>155.35</v>
+        <v>154.57</v>
       </c>
       <c r="F48" s="13">
-        <v>165.35</v>
+        <v>164.57</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>154.91</v>
+        <v>154.16999999999999</v>
       </c>
       <c r="E49" s="10">
-        <v>156.03</v>
+        <v>155.25</v>
       </c>
       <c r="F49" s="10">
-        <v>166.03</v>
+        <v>165.25</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>154.72999999999999</v>
+        <v>153.99</v>
       </c>
       <c r="E50" s="13">
-        <v>156.13</v>
+        <v>155.35</v>
       </c>
       <c r="F50" s="13">
-        <v>166.13</v>
+        <v>165.35</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>169.98</v>
+        <v>169.79</v>
       </c>
       <c r="E54" s="10">
-        <v>169.99</v>
+        <v>169.5</v>
       </c>
       <c r="F54" s="10">
-        <v>179.99</v>
+        <v>179.5</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>158.13</v>
+        <v>157.93</v>
       </c>
       <c r="E55" s="13">
-        <v>164.62</v>
+        <v>164.26</v>
       </c>
       <c r="F55" s="13">
-        <v>174.62</v>
+        <v>174.26</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>159.83000000000001</v>
+        <v>159.63</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>158.97999999999999</v>
+        <v>158.81</v>
       </c>
       <c r="E57" s="13">
-        <v>158.9</v>
+        <v>158.54</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>154.88</v>
+        <v>154.71</v>
       </c>
       <c r="E58" s="10">
-        <v>154.94</v>
+        <v>154.58000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>164.94</v>
+        <v>164.58</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>162.13999999999999</v>
+        <v>161.97</v>
       </c>
       <c r="E59" s="13">
-        <v>167.41</v>
+        <v>166.97</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>170.48</v>
+        <v>169.98</v>
       </c>
       <c r="E60" s="10">
-        <v>170.95</v>
+        <v>169.99</v>
       </c>
       <c r="F60" s="10">
-        <v>180.95</v>
+        <v>179.99</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>158.63999999999999</v>
+        <v>158.13</v>
       </c>
       <c r="E61" s="13">
-        <v>165.1</v>
+        <v>164.62</v>
       </c>
       <c r="F61" s="13">
-        <v>175.1</v>
+        <v>174.62</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>160.01</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>159.12</v>
+        <v>158.97999999999999</v>
       </c>
       <c r="E63" s="13">
-        <v>159.38</v>
+        <v>158.9</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>155.02000000000001</v>
+        <v>154.88</v>
       </c>
       <c r="E64" s="10">
-        <v>155.41999999999999</v>
+        <v>154.94</v>
       </c>
       <c r="F64" s="10">
-        <v>165.42</v>
+        <v>164.94</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>162.62</v>
+        <v>162.13999999999999</v>
       </c>
       <c r="E65" s="13">
-        <v>168.32</v>
+        <v>167.41</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,14 +1855,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2126,28 +2124,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2163,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Mon Dec 29 03:17:42 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F1AB6B2B-885F-4205-8A43-36B4EFB5A3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{BB4364CA-F29E-4DAF-990A-61E6231A4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.16</v>
+        <v>152.22999999999999</v>
       </c>
       <c r="E8" s="10">
-        <v>151.68</v>
+        <v>151.25</v>
       </c>
       <c r="F8" s="10">
-        <v>161.68</v>
+        <v>161.25</v>
       </c>
       <c r="G8" s="10">
-        <v>151.79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.16</v>
+        <v>152.22999999999999</v>
       </c>
       <c r="E9" s="13">
-        <v>151.68</v>
+        <v>151.25</v>
       </c>
       <c r="F9" s="13">
-        <v>161.68</v>
+        <v>161.25</v>
       </c>
       <c r="G9" s="13">
-        <v>151.79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.87</v>
+        <v>154.88999999999999</v>
       </c>
       <c r="E10" s="10">
-        <v>153.79</v>
+        <v>153.31</v>
       </c>
       <c r="F10" s="10">
-        <v>163.79</v>
+        <v>163.31</v>
       </c>
       <c r="G10" s="10">
-        <v>154.31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>153.83000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.34</v>
+        <v>152.16</v>
       </c>
       <c r="E11" s="13">
-        <v>152.05000000000001</v>
+        <v>151.68</v>
       </c>
       <c r="F11" s="13">
-        <v>162.05000000000001</v>
+        <v>161.68</v>
       </c>
       <c r="G11" s="13">
-        <v>152.16999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.34</v>
+        <v>152.16</v>
       </c>
       <c r="E12" s="10">
-        <v>152.05000000000001</v>
+        <v>151.68</v>
       </c>
       <c r="F12" s="10">
-        <v>162.05000000000001</v>
+        <v>161.68</v>
       </c>
       <c r="G12" s="10">
-        <v>152.16999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>155.07</v>
+        <v>154.87</v>
       </c>
       <c r="E13" s="13">
-        <v>154.18</v>
+        <v>153.79</v>
       </c>
       <c r="F13" s="13">
-        <v>164.18</v>
+        <v>163.79</v>
       </c>
       <c r="G13" s="13">
-        <v>154.69999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>154.31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>159.04</v>
+        <v>159.1</v>
       </c>
       <c r="E17" s="10">
-        <v>159.72999999999999</v>
+        <v>158.53</v>
       </c>
       <c r="F17" s="10">
-        <v>169.73</v>
+        <v>168.53</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>159.21</v>
+        <v>159.04</v>
       </c>
       <c r="E18" s="13">
-        <v>160.13999999999999</v>
+        <v>159.72999999999999</v>
       </c>
       <c r="F18" s="13">
-        <v>170.14</v>
+        <v>169.73</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.74</v>
+        <v>153.82</v>
       </c>
       <c r="E22" s="10">
-        <v>153.05000000000001</v>
+        <v>152.59</v>
       </c>
       <c r="F22" s="10">
-        <v>162.65</v>
+        <v>162.19</v>
       </c>
       <c r="G22" s="10">
-        <v>154.21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>153.76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>159.33000000000001</v>
+        <v>159.35</v>
       </c>
       <c r="E23" s="13">
-        <v>158.66</v>
+        <v>158.19</v>
       </c>
       <c r="F23" s="13">
-        <v>168.66</v>
+        <v>168.19</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>159.12</v>
+        <v>159.15</v>
       </c>
       <c r="E24" s="10">
-        <v>159.16</v>
+        <v>158.66999999999999</v>
       </c>
       <c r="F24" s="10">
-        <v>169.16</v>
+        <v>168.67</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>159.62</v>
+        <v>159.65</v>
       </c>
       <c r="E25" s="13">
-        <v>158.9</v>
+        <v>158.4</v>
       </c>
       <c r="F25" s="13">
-        <v>168.9</v>
+        <v>168.4</v>
       </c>
       <c r="G25" s="13">
-        <v>158.66999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>158.16999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.56</v>
+        <v>158.59</v>
       </c>
       <c r="E26" s="10">
-        <v>160.18</v>
+        <v>159.68</v>
       </c>
       <c r="F26" s="10">
-        <v>170.18</v>
+        <v>169.68</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.93</v>
+        <v>153.74</v>
       </c>
       <c r="E27" s="13">
-        <v>153.43</v>
+        <v>153.05000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>163.03</v>
+        <v>162.65</v>
       </c>
       <c r="G27" s="13">
-        <v>154.59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>154.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>159.53</v>
+        <v>159.33000000000001</v>
       </c>
       <c r="E28" s="22">
-        <v>159.05000000000001</v>
+        <v>158.66</v>
       </c>
       <c r="F28" s="22">
-        <v>169.05</v>
+        <v>168.66</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>159.31</v>
+        <v>159.12</v>
       </c>
       <c r="E29" s="13">
-        <v>159.56</v>
+        <v>159.16</v>
       </c>
       <c r="F29" s="13">
-        <v>169.56</v>
+        <v>169.16</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>159.81</v>
+        <v>159.62</v>
       </c>
       <c r="E30" s="22">
-        <v>159.30000000000001</v>
+        <v>158.9</v>
       </c>
       <c r="F30" s="22">
-        <v>169.3</v>
+        <v>168.9</v>
       </c>
       <c r="G30" s="22">
-        <v>159.07</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>158.66999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.74</v>
+        <v>158.56</v>
       </c>
       <c r="E31" s="13">
-        <v>160.58000000000001</v>
+        <v>160.18</v>
       </c>
       <c r="F31" s="13">
-        <v>170.58</v>
+        <v>170.18</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.38999999999999</v>
+        <v>152.41999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>152.24</v>
+        <v>151.77000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>161.24</v>
+        <v>160.77000000000001</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.58000000000001</v>
+        <v>152.38999999999999</v>
       </c>
       <c r="E36" s="13">
-        <v>152.63</v>
+        <v>152.24</v>
       </c>
       <c r="F36" s="13">
-        <v>161.63</v>
+        <v>161.24</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,28 +1375,28 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>160.15</v>
+        <v>160.13999999999999</v>
       </c>
       <c r="E40" s="10">
-        <v>160.18</v>
+        <v>158.93</v>
       </c>
       <c r="F40" s="10">
-        <v>170.18</v>
+        <v>168.93</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
@@ -1406,52 +1406,52 @@
         <v>159.87</v>
       </c>
       <c r="E41" s="13">
-        <v>160.6</v>
+        <v>159.35</v>
       </c>
       <c r="F41" s="13">
-        <v>170.6</v>
+        <v>169.35</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>160.37</v>
+        <v>160.15</v>
       </c>
       <c r="E42" s="10">
-        <v>160.63</v>
+        <v>160.18</v>
       </c>
       <c r="F42" s="10">
-        <v>170.63</v>
+        <v>170.18</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>160.09</v>
+        <v>159.87</v>
       </c>
       <c r="E43" s="13">
-        <v>161.05000000000001</v>
+        <v>160.6</v>
       </c>
       <c r="F43" s="13">
-        <v>171.05</v>
+        <v>170.6</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>153.63999999999999</v>
+        <v>153.41</v>
       </c>
       <c r="E47" s="10">
-        <v>154.47</v>
+        <v>153.37</v>
       </c>
       <c r="F47" s="10">
-        <v>164.47</v>
+        <v>163.37</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>153.47</v>
+        <v>153.26</v>
       </c>
       <c r="E48" s="13">
-        <v>154.57</v>
+        <v>153.47999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>164.57</v>
+        <v>163.47999999999999</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>154.16999999999999</v>
+        <v>153.63999999999999</v>
       </c>
       <c r="E49" s="10">
-        <v>155.25</v>
+        <v>154.47</v>
       </c>
       <c r="F49" s="10">
-        <v>165.25</v>
+        <v>164.47</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>153.99</v>
+        <v>153.47</v>
       </c>
       <c r="E50" s="13">
-        <v>155.35</v>
+        <v>154.57</v>
       </c>
       <c r="F50" s="13">
-        <v>165.35</v>
+        <v>164.57</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,9 +1605,9 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
@@ -1617,42 +1617,42 @@
         <v>169.79</v>
       </c>
       <c r="E54" s="10">
-        <v>169.5</v>
+        <v>168.88</v>
       </c>
       <c r="F54" s="10">
-        <v>179.5</v>
+        <v>178.88</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>157.93</v>
+        <v>157.94999999999999</v>
       </c>
       <c r="E55" s="13">
-        <v>164.26</v>
+        <v>163.84</v>
       </c>
       <c r="F55" s="13">
-        <v>174.26</v>
+        <v>173.84</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>159.63</v>
+        <v>159.63999999999999</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>158.81</v>
+        <v>158.88999999999999</v>
       </c>
       <c r="E57" s="13">
-        <v>158.54</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>154.71</v>
+        <v>154.79</v>
       </c>
       <c r="E58" s="10">
-        <v>154.58000000000001</v>
+        <v>154.16</v>
       </c>
       <c r="F58" s="10">
-        <v>164.58</v>
+        <v>164.16</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>161.97</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="E59" s="13">
-        <v>166.97</v>
+        <v>166.4</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>169.98</v>
+        <v>169.79</v>
       </c>
       <c r="E60" s="10">
-        <v>169.99</v>
+        <v>169.5</v>
       </c>
       <c r="F60" s="10">
-        <v>179.99</v>
+        <v>179.5</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>158.13</v>
+        <v>157.93</v>
       </c>
       <c r="E61" s="13">
-        <v>164.62</v>
+        <v>164.26</v>
       </c>
       <c r="F61" s="13">
-        <v>174.62</v>
+        <v>174.26</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>159.83000000000001</v>
+        <v>159.63</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>158.97999999999999</v>
+        <v>158.81</v>
       </c>
       <c r="E63" s="13">
-        <v>158.9</v>
+        <v>158.54</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>154.88</v>
+        <v>154.71</v>
       </c>
       <c r="E64" s="10">
-        <v>154.94</v>
+        <v>154.58000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>164.94</v>
+        <v>164.58</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46015</v>
+        <v>46016</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>162.13999999999999</v>
+        <v>161.97</v>
       </c>
       <c r="E65" s="13">
-        <v>167.41</v>
+        <v>166.97</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,15 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2123,6 +2114,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2135,14 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2158,6 +2150,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Dec 30 03:08:00 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{BB4364CA-F29E-4DAF-990A-61E6231A4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{AF0E5E52-27E5-4FEA-809C-A9BCC60A128A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.22999999999999</v>
+        <v>151.83000000000001</v>
       </c>
       <c r="E8" s="10">
-        <v>151.25</v>
+        <v>150.57</v>
       </c>
       <c r="F8" s="10">
-        <v>161.25</v>
+        <v>160.57</v>
       </c>
       <c r="G8" s="10">
-        <v>151.37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150.69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.22999999999999</v>
+        <v>151.83000000000001</v>
       </c>
       <c r="E9" s="13">
-        <v>151.25</v>
+        <v>150.57</v>
       </c>
       <c r="F9" s="13">
-        <v>161.25</v>
+        <v>160.57</v>
       </c>
       <c r="G9" s="13">
-        <v>151.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150.69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.88999999999999</v>
+        <v>154.49</v>
       </c>
       <c r="E10" s="10">
-        <v>153.31</v>
+        <v>152.63</v>
       </c>
       <c r="F10" s="10">
-        <v>163.31</v>
+        <v>162.63</v>
       </c>
       <c r="G10" s="10">
-        <v>153.83000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153.13999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.16</v>
+        <v>152.22999999999999</v>
       </c>
       <c r="E11" s="13">
-        <v>151.68</v>
+        <v>151.25</v>
       </c>
       <c r="F11" s="13">
-        <v>161.68</v>
+        <v>161.25</v>
       </c>
       <c r="G11" s="13">
-        <v>151.79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.16</v>
+        <v>152.22999999999999</v>
       </c>
       <c r="E12" s="10">
-        <v>151.68</v>
+        <v>151.25</v>
       </c>
       <c r="F12" s="10">
-        <v>161.68</v>
+        <v>161.25</v>
       </c>
       <c r="G12" s="10">
-        <v>151.79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.87</v>
+        <v>154.88999999999999</v>
       </c>
       <c r="E13" s="13">
-        <v>153.79</v>
+        <v>153.31</v>
       </c>
       <c r="F13" s="13">
-        <v>163.79</v>
+        <v>163.31</v>
       </c>
       <c r="G13" s="13">
-        <v>154.31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153.83000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>159.1</v>
+        <v>158.71</v>
       </c>
       <c r="E17" s="10">
-        <v>158.53</v>
+        <v>157.65</v>
       </c>
       <c r="F17" s="10">
-        <v>168.53</v>
+        <v>167.65</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>159.04</v>
+        <v>159.1</v>
       </c>
       <c r="E18" s="13">
-        <v>159.72999999999999</v>
+        <v>158.53</v>
       </c>
       <c r="F18" s="13">
-        <v>169.73</v>
+        <v>168.53</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.82</v>
+        <v>153.41</v>
       </c>
       <c r="E22" s="10">
-        <v>152.59</v>
+        <v>151.91999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>162.19</v>
+        <v>161.52000000000001</v>
       </c>
       <c r="G22" s="10">
-        <v>153.76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153.08000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>159.35</v>
+        <v>158.94</v>
       </c>
       <c r="E23" s="13">
-        <v>158.19</v>
+        <v>157.51</v>
       </c>
       <c r="F23" s="13">
-        <v>168.19</v>
+        <v>167.51</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>159.15</v>
+        <v>158.74</v>
       </c>
       <c r="E24" s="10">
-        <v>158.66999999999999</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="F24" s="10">
-        <v>168.67</v>
+        <v>167.98</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>159.65</v>
+        <v>159.24</v>
       </c>
       <c r="E25" s="13">
-        <v>158.4</v>
+        <v>157.71</v>
       </c>
       <c r="F25" s="13">
-        <v>168.4</v>
+        <v>167.71</v>
       </c>
       <c r="G25" s="13">
-        <v>158.16999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>157.47999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.59</v>
+        <v>158.19</v>
       </c>
       <c r="E26" s="10">
-        <v>159.68</v>
+        <v>158.99</v>
       </c>
       <c r="F26" s="10">
-        <v>169.68</v>
+        <v>168.99</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.74</v>
+        <v>153.82</v>
       </c>
       <c r="E27" s="13">
-        <v>153.05000000000001</v>
+        <v>152.59</v>
       </c>
       <c r="F27" s="13">
-        <v>162.65</v>
+        <v>162.19</v>
       </c>
       <c r="G27" s="13">
-        <v>154.21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153.76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>159.33000000000001</v>
+        <v>159.35</v>
       </c>
       <c r="E28" s="22">
-        <v>158.66</v>
+        <v>158.19</v>
       </c>
       <c r="F28" s="22">
-        <v>168.66</v>
+        <v>168.19</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>159.12</v>
+        <v>159.15</v>
       </c>
       <c r="E29" s="13">
-        <v>159.16</v>
+        <v>158.66999999999999</v>
       </c>
       <c r="F29" s="13">
-        <v>169.16</v>
+        <v>168.67</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>159.62</v>
+        <v>159.65</v>
       </c>
       <c r="E30" s="22">
-        <v>158.9</v>
+        <v>158.4</v>
       </c>
       <c r="F30" s="22">
-        <v>168.9</v>
+        <v>168.4</v>
       </c>
       <c r="G30" s="22">
-        <v>158.66999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.16999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.56</v>
+        <v>158.59</v>
       </c>
       <c r="E31" s="13">
-        <v>160.18</v>
+        <v>159.68</v>
       </c>
       <c r="F31" s="13">
-        <v>170.18</v>
+        <v>169.68</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.41999999999999</v>
+        <v>152.02000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>151.77000000000001</v>
+        <v>151.09</v>
       </c>
       <c r="F35" s="10">
-        <v>160.77000000000001</v>
+        <v>160.09</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.38999999999999</v>
+        <v>152.41999999999999</v>
       </c>
       <c r="E36" s="13">
-        <v>152.24</v>
+        <v>151.77000000000001</v>
       </c>
       <c r="F36" s="13">
-        <v>161.24</v>
+        <v>160.77000000000001</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,66 +1375,66 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>160.13999999999999</v>
+        <v>159.72999999999999</v>
       </c>
       <c r="E40" s="10">
-        <v>158.93</v>
+        <v>158.04</v>
       </c>
       <c r="F40" s="10">
-        <v>168.93</v>
+        <v>168.04</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>159.87</v>
+        <v>159.44999999999999</v>
       </c>
       <c r="E41" s="13">
-        <v>159.35</v>
+        <v>158.46</v>
       </c>
       <c r="F41" s="13">
-        <v>169.35</v>
+        <v>168.46</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>160.15</v>
+        <v>160.13999999999999</v>
       </c>
       <c r="E42" s="10">
-        <v>160.18</v>
+        <v>158.93</v>
       </c>
       <c r="F42" s="10">
-        <v>170.18</v>
+        <v>168.93</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
@@ -1444,14 +1444,14 @@
         <v>159.87</v>
       </c>
       <c r="E43" s="13">
-        <v>160.6</v>
+        <v>159.35</v>
       </c>
       <c r="F43" s="13">
-        <v>170.6</v>
+        <v>169.35</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>153.41</v>
+        <v>152.91</v>
       </c>
       <c r="E47" s="10">
-        <v>153.37</v>
+        <v>152.85</v>
       </c>
       <c r="F47" s="10">
-        <v>163.37</v>
+        <v>162.85</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>153.26</v>
+        <v>152.76</v>
       </c>
       <c r="E48" s="13">
-        <v>153.47999999999999</v>
+        <v>152.96</v>
       </c>
       <c r="F48" s="13">
-        <v>163.47999999999999</v>
+        <v>162.96</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>153.63999999999999</v>
+        <v>153.41</v>
       </c>
       <c r="E49" s="10">
-        <v>154.47</v>
+        <v>153.37</v>
       </c>
       <c r="F49" s="10">
-        <v>164.47</v>
+        <v>163.37</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>153.47</v>
+        <v>153.26</v>
       </c>
       <c r="E50" s="13">
-        <v>154.57</v>
+        <v>153.47999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>164.57</v>
+        <v>163.47999999999999</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>169.79</v>
+        <v>169.36</v>
       </c>
       <c r="E54" s="10">
-        <v>168.88</v>
+        <v>168.16</v>
       </c>
       <c r="F54" s="10">
-        <v>178.88</v>
+        <v>178.16</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>157.94999999999999</v>
+        <v>157.54</v>
       </c>
       <c r="E55" s="13">
-        <v>163.84</v>
+        <v>163.16999999999999</v>
       </c>
       <c r="F55" s="13">
-        <v>173.84</v>
+        <v>173.17</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>159.63999999999999</v>
+        <v>159.22999999999999</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,66 +1662,66 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>158.88999999999999</v>
+        <v>158.5</v>
       </c>
       <c r="E57" s="13">
-        <v>158.11000000000001</v>
+        <v>157.44</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>154.79</v>
+        <v>154.4</v>
       </c>
       <c r="E58" s="10">
-        <v>154.16</v>
+        <v>153.49</v>
       </c>
       <c r="F58" s="10">
-        <v>164.16</v>
+        <v>163.49</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>162.05000000000001</v>
+        <v>161.66</v>
       </c>
       <c r="E59" s="13">
-        <v>166.4</v>
+        <v>165.69</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
@@ -1731,42 +1731,42 @@
         <v>169.79</v>
       </c>
       <c r="E60" s="10">
-        <v>169.5</v>
+        <v>168.88</v>
       </c>
       <c r="F60" s="10">
-        <v>179.5</v>
+        <v>178.88</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>157.93</v>
+        <v>157.94999999999999</v>
       </c>
       <c r="E61" s="13">
-        <v>164.26</v>
+        <v>163.84</v>
       </c>
       <c r="F61" s="13">
-        <v>174.26</v>
+        <v>173.84</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>159.63</v>
+        <v>159.63999999999999</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>158.81</v>
+        <v>158.88999999999999</v>
       </c>
       <c r="E63" s="13">
-        <v>158.54</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>154.71</v>
+        <v>154.79</v>
       </c>
       <c r="E64" s="10">
-        <v>154.58000000000001</v>
+        <v>154.16</v>
       </c>
       <c r="F64" s="10">
-        <v>164.58</v>
+        <v>164.16</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46016</v>
+        <v>46021</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>161.97</v>
+        <v>162.05000000000001</v>
       </c>
       <c r="E65" s="13">
-        <v>166.97</v>
+        <v>166.4</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,15 +2123,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2135,6 +2135,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2150,14 +2158,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Wed Dec 31 03:07:13 UTC 2025
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{AF0E5E52-27E5-4FEA-809C-A9BCC60A128A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D32CA7C1-AC53-44C6-AD59-8EC2C582F626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="15540" yWindow="-16380" windowWidth="29016" windowHeight="15696" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.44140625"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>151.83000000000001</v>
+        <v>152.35</v>
       </c>
       <c r="E8" s="10">
-        <v>150.57</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F8" s="10">
-        <v>160.57</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G8" s="10">
-        <v>150.69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>150.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>151.83000000000001</v>
+        <v>152.35</v>
       </c>
       <c r="E9" s="13">
-        <v>150.57</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F9" s="13">
-        <v>160.57</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G9" s="13">
-        <v>150.69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>150.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.49</v>
+        <v>154.63</v>
       </c>
       <c r="E10" s="10">
-        <v>152.63</v>
+        <v>151.97</v>
       </c>
       <c r="F10" s="10">
-        <v>162.63</v>
+        <v>161.97</v>
       </c>
       <c r="G10" s="10">
-        <v>153.13999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>152.37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.22999999999999</v>
+        <v>151.83000000000001</v>
       </c>
       <c r="E11" s="13">
-        <v>151.25</v>
+        <v>150.57</v>
       </c>
       <c r="F11" s="13">
-        <v>161.25</v>
+        <v>160.57</v>
       </c>
       <c r="G11" s="13">
-        <v>151.37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>150.69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.22999999999999</v>
+        <v>151.83000000000001</v>
       </c>
       <c r="E12" s="10">
-        <v>151.25</v>
+        <v>150.57</v>
       </c>
       <c r="F12" s="10">
-        <v>161.25</v>
+        <v>160.57</v>
       </c>
       <c r="G12" s="10">
-        <v>151.37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>150.69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.88999999999999</v>
+        <v>154.49</v>
       </c>
       <c r="E13" s="13">
-        <v>153.31</v>
+        <v>152.63</v>
       </c>
       <c r="F13" s="13">
-        <v>163.31</v>
+        <v>162.63</v>
       </c>
       <c r="G13" s="13">
-        <v>153.83000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>153.13999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>158.71</v>
+        <v>158.54</v>
       </c>
       <c r="E17" s="10">
-        <v>157.65</v>
+        <v>155.61000000000001</v>
       </c>
       <c r="F17" s="10">
-        <v>167.65</v>
+        <v>165.61</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>159.1</v>
+        <v>158.71</v>
       </c>
       <c r="E18" s="13">
-        <v>158.53</v>
+        <v>157.65</v>
       </c>
       <c r="F18" s="13">
-        <v>168.53</v>
+        <v>167.65</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.41</v>
+        <v>154.09</v>
       </c>
       <c r="E22" s="10">
-        <v>151.91999999999999</v>
+        <v>151.32</v>
       </c>
       <c r="F22" s="10">
-        <v>161.52000000000001</v>
+        <v>160.91999999999999</v>
       </c>
       <c r="G22" s="10">
-        <v>153.08000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>152.38999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.94</v>
+        <v>158.93</v>
       </c>
       <c r="E23" s="13">
-        <v>157.51</v>
+        <v>156.88</v>
       </c>
       <c r="F23" s="13">
-        <v>167.51</v>
+        <v>166.88</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.74</v>
+        <v>159.1</v>
       </c>
       <c r="E24" s="10">
-        <v>157.97999999999999</v>
+        <v>157.47</v>
       </c>
       <c r="F24" s="10">
-        <v>167.98</v>
+        <v>167.47</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>159.24</v>
+        <v>159.09</v>
       </c>
       <c r="E25" s="13">
-        <v>157.71</v>
+        <v>156.99</v>
       </c>
       <c r="F25" s="13">
-        <v>167.71</v>
+        <v>166.99</v>
       </c>
       <c r="G25" s="13">
-        <v>157.47999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>157.11000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.19</v>
+        <v>158.74</v>
       </c>
       <c r="E26" s="10">
-        <v>158.99</v>
+        <v>158.61000000000001</v>
       </c>
       <c r="F26" s="10">
-        <v>168.99</v>
+        <v>168.61</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.82</v>
+        <v>153.41</v>
       </c>
       <c r="E27" s="13">
-        <v>152.59</v>
+        <v>151.91999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>162.19</v>
+        <v>161.52000000000001</v>
       </c>
       <c r="G27" s="13">
-        <v>153.76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>153.08000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>159.35</v>
+        <v>158.94</v>
       </c>
       <c r="E28" s="22">
-        <v>158.19</v>
+        <v>157.51</v>
       </c>
       <c r="F28" s="22">
-        <v>168.19</v>
+        <v>167.51</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>159.15</v>
+        <v>158.74</v>
       </c>
       <c r="E29" s="13">
-        <v>158.66999999999999</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="F29" s="13">
-        <v>168.67</v>
+        <v>167.98</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>159.65</v>
+        <v>159.24</v>
       </c>
       <c r="E30" s="22">
-        <v>158.4</v>
+        <v>157.71</v>
       </c>
       <c r="F30" s="22">
-        <v>168.4</v>
+        <v>167.71</v>
       </c>
       <c r="G30" s="22">
-        <v>158.16999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>157.47999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.59</v>
+        <v>158.19</v>
       </c>
       <c r="E31" s="13">
-        <v>159.68</v>
+        <v>158.99</v>
       </c>
       <c r="F31" s="13">
-        <v>169.68</v>
+        <v>168.99</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.02000000000001</v>
+        <v>152.19</v>
       </c>
       <c r="E35" s="10">
-        <v>151.09</v>
+        <v>150.38</v>
       </c>
       <c r="F35" s="10">
-        <v>160.09</v>
+        <v>159.38</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.41999999999999</v>
+        <v>152.02000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>151.77000000000001</v>
+        <v>151.09</v>
       </c>
       <c r="F36" s="13">
-        <v>160.77000000000001</v>
+        <v>160.09</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>159.72999999999999</v>
+        <v>159.61000000000001</v>
       </c>
       <c r="E40" s="10">
-        <v>158.04</v>
+        <v>157.91999999999999</v>
       </c>
       <c r="F40" s="10">
-        <v>168.04</v>
+        <v>167.92</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>159.44999999999999</v>
+        <v>159.33000000000001</v>
       </c>
       <c r="E41" s="13">
-        <v>158.46</v>
+        <v>158.34</v>
       </c>
       <c r="F41" s="13">
-        <v>168.46</v>
+        <v>168.34</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>160.13999999999999</v>
+        <v>159.72999999999999</v>
       </c>
       <c r="E42" s="10">
-        <v>158.93</v>
+        <v>158.04</v>
       </c>
       <c r="F42" s="10">
-        <v>168.93</v>
+        <v>168.04</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>159.87</v>
+        <v>159.44999999999999</v>
       </c>
       <c r="E43" s="13">
-        <v>159.35</v>
+        <v>158.46</v>
       </c>
       <c r="F43" s="13">
-        <v>169.35</v>
+        <v>168.46</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.91</v>
+        <v>153.07</v>
       </c>
       <c r="E47" s="10">
-        <v>152.85</v>
+        <v>152.43</v>
       </c>
       <c r="F47" s="10">
-        <v>162.85</v>
+        <v>162.43</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.76</v>
+        <v>152.74</v>
       </c>
       <c r="E48" s="13">
-        <v>152.96</v>
+        <v>152.38</v>
       </c>
       <c r="F48" s="13">
-        <v>162.96</v>
+        <v>162.38</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>153.41</v>
+        <v>152.91</v>
       </c>
       <c r="E49" s="10">
-        <v>153.37</v>
+        <v>152.85</v>
       </c>
       <c r="F49" s="10">
-        <v>163.37</v>
+        <v>162.85</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>153.26</v>
+        <v>152.76</v>
       </c>
       <c r="E50" s="13">
-        <v>153.47999999999999</v>
+        <v>152.96</v>
       </c>
       <c r="F50" s="13">
-        <v>163.47999999999999</v>
+        <v>162.96</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>169.36</v>
+        <v>168.93</v>
       </c>
       <c r="E54" s="10">
-        <v>168.16</v>
+        <v>165.5</v>
       </c>
       <c r="F54" s="10">
-        <v>178.16</v>
+        <v>175.5</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>157.54</v>
+        <v>161.94</v>
       </c>
       <c r="E55" s="13">
-        <v>163.16999999999999</v>
+        <v>163.68</v>
       </c>
       <c r="F55" s="13">
-        <v>173.17</v>
+        <v>173.68</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>159.22999999999999</v>
+        <v>158.72999999999999</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>158.5</v>
+        <v>159.5</v>
       </c>
       <c r="E57" s="13">
-        <v>157.44</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>154.4</v>
+        <v>155.27000000000001</v>
       </c>
       <c r="E58" s="10">
-        <v>153.49</v>
+        <v>154</v>
       </c>
       <c r="F58" s="10">
-        <v>163.49</v>
+        <v>164</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>161.66</v>
+        <v>161.46</v>
       </c>
       <c r="E59" s="13">
-        <v>165.69</v>
+        <v>164.05</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>169.79</v>
+        <v>169.36</v>
       </c>
       <c r="E60" s="10">
-        <v>168.88</v>
+        <v>168.16</v>
       </c>
       <c r="F60" s="10">
-        <v>178.88</v>
+        <v>178.16</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>157.94999999999999</v>
+        <v>157.54</v>
       </c>
       <c r="E61" s="13">
-        <v>163.84</v>
+        <v>163.16999999999999</v>
       </c>
       <c r="F61" s="13">
-        <v>173.84</v>
+        <v>173.17</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>159.63999999999999</v>
+        <v>159.22999999999999</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>158.88999999999999</v>
+        <v>158.5</v>
       </c>
       <c r="E63" s="13">
-        <v>158.11000000000001</v>
+        <v>157.44</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>154.79</v>
+        <v>154.4</v>
       </c>
       <c r="E64" s="10">
-        <v>154.16</v>
+        <v>153.49</v>
       </c>
       <c r="F64" s="10">
-        <v>164.16</v>
+        <v>163.49</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>162.05000000000001</v>
+        <v>161.66</v>
       </c>
       <c r="E65" s="13">
-        <v>166.4</v>
+        <v>165.69</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,12 +1855,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2124,20 +2126,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2163,19 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fri Jan  2 03:10:38 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D32CA7C1-AC53-44C6-AD59-8EC2C582F626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B1A2A08F-CE2A-4762-9FD9-8AC9B4AF54D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15540" yWindow="-16380" windowWidth="29016" windowHeight="15696" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,8 +154,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,7 +331,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.35</v>
+        <v>152.21</v>
       </c>
       <c r="E8" s="10">
-        <v>150.08000000000001</v>
+        <v>149.96</v>
       </c>
       <c r="F8" s="10">
-        <v>160.08000000000001</v>
+        <v>159.96</v>
       </c>
       <c r="G8" s="10">
-        <v>150.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>149.97999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.35</v>
+        <v>152.21</v>
       </c>
       <c r="E9" s="13">
-        <v>150.08000000000001</v>
+        <v>149.96</v>
       </c>
       <c r="F9" s="13">
-        <v>160.08000000000001</v>
+        <v>159.96</v>
       </c>
       <c r="G9" s="13">
-        <v>150.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>149.97999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.63</v>
+        <v>154.46</v>
       </c>
       <c r="E10" s="10">
-        <v>151.97</v>
+        <v>151.83000000000001</v>
       </c>
       <c r="F10" s="10">
-        <v>161.97</v>
+        <v>161.83000000000001</v>
       </c>
       <c r="G10" s="10">
-        <v>152.37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>152.22999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>151.83000000000001</v>
+        <v>152.35</v>
       </c>
       <c r="E11" s="13">
-        <v>150.57</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F11" s="13">
-        <v>160.57</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G11" s="13">
-        <v>150.69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>150.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>151.83000000000001</v>
+        <v>152.35</v>
       </c>
       <c r="E12" s="10">
-        <v>150.57</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F12" s="10">
-        <v>160.57</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G12" s="10">
-        <v>150.69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>150.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.49</v>
+        <v>154.63</v>
       </c>
       <c r="E13" s="13">
-        <v>152.63</v>
+        <v>151.97</v>
       </c>
       <c r="F13" s="13">
-        <v>162.63</v>
+        <v>161.97</v>
       </c>
       <c r="G13" s="13">
-        <v>153.13999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>152.37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>158.54</v>
+        <v>158.38</v>
       </c>
       <c r="E17" s="10">
-        <v>155.61000000000001</v>
+        <v>155.49</v>
       </c>
       <c r="F17" s="10">
-        <v>165.61</v>
+        <v>165.49</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>158.71</v>
+        <v>158.54</v>
       </c>
       <c r="E18" s="13">
-        <v>157.65</v>
+        <v>155.61000000000001</v>
       </c>
       <c r="F18" s="13">
-        <v>167.65</v>
+        <v>165.61</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>154.09</v>
+        <v>153.94</v>
       </c>
       <c r="E22" s="10">
-        <v>151.32</v>
+        <v>151.19999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>160.91999999999999</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="G22" s="10">
-        <v>152.38999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>152.28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.93</v>
+        <v>158.76</v>
       </c>
       <c r="E23" s="13">
-        <v>156.88</v>
+        <v>156.75</v>
       </c>
       <c r="F23" s="13">
-        <v>166.88</v>
+        <v>166.75</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>159.1</v>
+        <v>158.93</v>
       </c>
       <c r="E24" s="10">
-        <v>157.47</v>
+        <v>157.34</v>
       </c>
       <c r="F24" s="10">
-        <v>167.47</v>
+        <v>167.34</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>159.09</v>
+        <v>158.91999999999999</v>
       </c>
       <c r="E25" s="13">
-        <v>156.99</v>
+        <v>156.85</v>
       </c>
       <c r="F25" s="13">
-        <v>166.99</v>
+        <v>166.85</v>
       </c>
       <c r="G25" s="13">
-        <v>157.11000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>156.97999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.74</v>
+        <v>158.58000000000001</v>
       </c>
       <c r="E26" s="10">
-        <v>158.61000000000001</v>
+        <v>158.47</v>
       </c>
       <c r="F26" s="10">
-        <v>168.61</v>
+        <v>168.47</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.41</v>
+        <v>154.09</v>
       </c>
       <c r="E27" s="13">
-        <v>151.91999999999999</v>
+        <v>151.32</v>
       </c>
       <c r="F27" s="13">
-        <v>161.52000000000001</v>
+        <v>160.91999999999999</v>
       </c>
       <c r="G27" s="13">
-        <v>153.08000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>152.38999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.94</v>
+        <v>158.93</v>
       </c>
       <c r="E28" s="22">
-        <v>157.51</v>
+        <v>156.88</v>
       </c>
       <c r="F28" s="22">
-        <v>167.51</v>
+        <v>166.88</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.74</v>
+        <v>159.1</v>
       </c>
       <c r="E29" s="13">
-        <v>157.97999999999999</v>
+        <v>157.47</v>
       </c>
       <c r="F29" s="13">
-        <v>167.98</v>
+        <v>167.47</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>159.24</v>
+        <v>159.09</v>
       </c>
       <c r="E30" s="22">
-        <v>157.71</v>
+        <v>156.99</v>
       </c>
       <c r="F30" s="22">
-        <v>167.71</v>
+        <v>166.99</v>
       </c>
       <c r="G30" s="22">
-        <v>157.47999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>157.11000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.19</v>
+        <v>158.74</v>
       </c>
       <c r="E31" s="13">
-        <v>158.99</v>
+        <v>158.61000000000001</v>
       </c>
       <c r="F31" s="13">
-        <v>168.99</v>
+        <v>168.61</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.19</v>
+        <v>152.02000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>150.38</v>
+        <v>150.24</v>
       </c>
       <c r="F35" s="10">
-        <v>159.38</v>
+        <v>159.24</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.02000000000001</v>
+        <v>152.19</v>
       </c>
       <c r="E36" s="13">
-        <v>151.09</v>
+        <v>150.38</v>
       </c>
       <c r="F36" s="13">
-        <v>160.09</v>
+        <v>159.38</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>159.61000000000001</v>
+        <v>159.43</v>
       </c>
       <c r="E40" s="10">
-        <v>157.91999999999999</v>
+        <v>157.57</v>
       </c>
       <c r="F40" s="10">
-        <v>167.92</v>
+        <v>167.57</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>159.33000000000001</v>
+        <v>159.15</v>
       </c>
       <c r="E41" s="13">
-        <v>158.34</v>
+        <v>157.99</v>
       </c>
       <c r="F41" s="13">
-        <v>168.34</v>
+        <v>167.99</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>159.72999999999999</v>
+        <v>159.61000000000001</v>
       </c>
       <c r="E42" s="10">
-        <v>158.04</v>
+        <v>157.91999999999999</v>
       </c>
       <c r="F42" s="10">
-        <v>168.04</v>
+        <v>167.92</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>159.44999999999999</v>
+        <v>159.33000000000001</v>
       </c>
       <c r="E43" s="13">
-        <v>158.46</v>
+        <v>158.34</v>
       </c>
       <c r="F43" s="13">
-        <v>168.46</v>
+        <v>168.34</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>153.07</v>
+        <v>153</v>
       </c>
       <c r="E47" s="10">
-        <v>152.43</v>
+        <v>151.9</v>
       </c>
       <c r="F47" s="10">
-        <v>162.43</v>
+        <v>161.9</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.74</v>
+        <v>152.66999999999999</v>
       </c>
       <c r="E48" s="13">
-        <v>152.38</v>
+        <v>151.86000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>162.38</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.91</v>
+        <v>153.07</v>
       </c>
       <c r="E49" s="10">
-        <v>152.85</v>
+        <v>152.43</v>
       </c>
       <c r="F49" s="10">
-        <v>162.85</v>
+        <v>162.43</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.76</v>
+        <v>152.74</v>
       </c>
       <c r="E50" s="13">
-        <v>152.96</v>
+        <v>152.38</v>
       </c>
       <c r="F50" s="13">
-        <v>162.96</v>
+        <v>162.38</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>168.93</v>
+        <v>168.77</v>
       </c>
       <c r="E54" s="10">
-        <v>165.5</v>
+        <v>165.32</v>
       </c>
       <c r="F54" s="10">
-        <v>175.5</v>
+        <v>175.32</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>161.94</v>
+        <v>161.76</v>
       </c>
       <c r="E55" s="13">
-        <v>163.68</v>
+        <v>163.56</v>
       </c>
       <c r="F55" s="13">
-        <v>173.68</v>
+        <v>173.56</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>158.72999999999999</v>
+        <v>158.56</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>159.5</v>
+        <v>159.34</v>
       </c>
       <c r="E57" s="13">
-        <v>158.11000000000001</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>155.27000000000001</v>
+        <v>155.11000000000001</v>
       </c>
       <c r="E58" s="10">
-        <v>154</v>
+        <v>153.88</v>
       </c>
       <c r="F58" s="10">
-        <v>164</v>
+        <v>163.88</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>161.46</v>
+        <v>161.30000000000001</v>
       </c>
       <c r="E59" s="13">
-        <v>164.05</v>
+        <v>163.89</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>169.36</v>
+        <v>168.93</v>
       </c>
       <c r="E60" s="10">
-        <v>168.16</v>
+        <v>165.5</v>
       </c>
       <c r="F60" s="10">
-        <v>178.16</v>
+        <v>175.5</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>157.54</v>
+        <v>161.94</v>
       </c>
       <c r="E61" s="13">
-        <v>163.16999999999999</v>
+        <v>163.68</v>
       </c>
       <c r="F61" s="13">
-        <v>173.17</v>
+        <v>173.68</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>159.22999999999999</v>
+        <v>158.72999999999999</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>158.5</v>
+        <v>159.5</v>
       </c>
       <c r="E63" s="13">
-        <v>157.44</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>154.4</v>
+        <v>155.27000000000001</v>
       </c>
       <c r="E64" s="10">
-        <v>153.49</v>
+        <v>154</v>
       </c>
       <c r="F64" s="10">
-        <v>163.49</v>
+        <v>164</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46022</v>
+        <v>46023</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>161.66</v>
+        <v>161.46</v>
       </c>
       <c r="E65" s="13">
-        <v>165.69</v>
+        <v>164.05</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,17 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2125,6 +2114,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2135,24 +2135,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2172,6 +2154,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Mon Jan  5 03:23:02 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{B1A2A08F-CE2A-4762-9FD9-8AC9B4AF54D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{91860CE4-646F-44FA-964B-AD92B2527E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,8 +154,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,7 +331,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.21</v>
+        <v>152.03</v>
       </c>
       <c r="E8" s="10">
-        <v>149.96</v>
+        <v>149.57</v>
       </c>
       <c r="F8" s="10">
-        <v>159.96</v>
+        <v>159.57</v>
       </c>
       <c r="G8" s="10">
-        <v>149.97999999999999</v>
+        <v>149.59</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.21</v>
+        <v>152.03</v>
       </c>
       <c r="E9" s="13">
-        <v>149.96</v>
+        <v>149.57</v>
       </c>
       <c r="F9" s="13">
-        <v>159.96</v>
+        <v>159.57</v>
       </c>
       <c r="G9" s="13">
-        <v>149.97999999999999</v>
+        <v>149.59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.46</v>
+        <v>154.24</v>
       </c>
       <c r="E10" s="10">
-        <v>151.83000000000001</v>
+        <v>151.4</v>
       </c>
       <c r="F10" s="10">
-        <v>161.83000000000001</v>
+        <v>161.4</v>
       </c>
       <c r="G10" s="10">
-        <v>152.22999999999999</v>
+        <v>151.80000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.35</v>
+        <v>152.21</v>
       </c>
       <c r="E11" s="13">
-        <v>150.08000000000001</v>
+        <v>149.96</v>
       </c>
       <c r="F11" s="13">
-        <v>160.08000000000001</v>
+        <v>159.96</v>
       </c>
       <c r="G11" s="13">
-        <v>150.1</v>
+        <v>149.97999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.35</v>
+        <v>152.21</v>
       </c>
       <c r="E12" s="10">
-        <v>150.08000000000001</v>
+        <v>149.96</v>
       </c>
       <c r="F12" s="10">
-        <v>160.08000000000001</v>
+        <v>159.96</v>
       </c>
       <c r="G12" s="10">
-        <v>150.1</v>
+        <v>149.97999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.63</v>
+        <v>154.46</v>
       </c>
       <c r="E13" s="13">
-        <v>151.97</v>
+        <v>151.83000000000001</v>
       </c>
       <c r="F13" s="13">
-        <v>161.97</v>
+        <v>161.83000000000001</v>
       </c>
       <c r="G13" s="13">
-        <v>152.37</v>
+        <v>152.22999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>158.38</v>
+        <v>158.13999999999999</v>
       </c>
       <c r="E17" s="10">
-        <v>155.49</v>
+        <v>155.03</v>
       </c>
       <c r="F17" s="10">
-        <v>165.49</v>
+        <v>165.03</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>158.54</v>
+        <v>158.38</v>
       </c>
       <c r="E18" s="13">
-        <v>155.61000000000001</v>
+        <v>155.49</v>
       </c>
       <c r="F18" s="13">
-        <v>165.61</v>
+        <v>165.49</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.94</v>
+        <v>153.77000000000001</v>
       </c>
       <c r="E22" s="10">
-        <v>151.19999999999999</v>
+        <v>150.81</v>
       </c>
       <c r="F22" s="10">
-        <v>160.80000000000001</v>
+        <v>160.41</v>
       </c>
       <c r="G22" s="10">
-        <v>152.28</v>
+        <v>151.88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.76</v>
+        <v>158.55000000000001</v>
       </c>
       <c r="E23" s="13">
-        <v>156.75</v>
+        <v>156.31</v>
       </c>
       <c r="F23" s="13">
-        <v>166.75</v>
+        <v>166.31</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.93</v>
+        <v>158.71</v>
       </c>
       <c r="E24" s="10">
-        <v>157.34</v>
+        <v>156.91</v>
       </c>
       <c r="F24" s="10">
-        <v>167.34</v>
+        <v>166.91</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.91999999999999</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="E25" s="13">
-        <v>156.85</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="F25" s="13">
-        <v>166.85</v>
+        <v>166.42</v>
       </c>
       <c r="G25" s="13">
-        <v>156.97999999999999</v>
+        <v>156.55000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.58000000000001</v>
+        <v>158.35</v>
       </c>
       <c r="E26" s="10">
-        <v>158.47</v>
+        <v>158.04</v>
       </c>
       <c r="F26" s="10">
-        <v>168.47</v>
+        <v>168.04</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>154.09</v>
+        <v>153.94</v>
       </c>
       <c r="E27" s="13">
-        <v>151.32</v>
+        <v>151.19999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>160.91999999999999</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="G27" s="13">
-        <v>152.38999999999999</v>
+        <v>152.28</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.93</v>
+        <v>158.76</v>
       </c>
       <c r="E28" s="22">
-        <v>156.88</v>
+        <v>156.75</v>
       </c>
       <c r="F28" s="22">
-        <v>166.88</v>
+        <v>166.75</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>159.1</v>
+        <v>158.93</v>
       </c>
       <c r="E29" s="13">
-        <v>157.47</v>
+        <v>157.34</v>
       </c>
       <c r="F29" s="13">
-        <v>167.47</v>
+        <v>167.34</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>159.09</v>
+        <v>158.91999999999999</v>
       </c>
       <c r="E30" s="22">
-        <v>156.99</v>
+        <v>156.85</v>
       </c>
       <c r="F30" s="22">
-        <v>166.99</v>
+        <v>166.85</v>
       </c>
       <c r="G30" s="22">
-        <v>157.11000000000001</v>
+        <v>156.97999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.74</v>
+        <v>158.58000000000001</v>
       </c>
       <c r="E31" s="13">
-        <v>158.61000000000001</v>
+        <v>158.47</v>
       </c>
       <c r="F31" s="13">
-        <v>168.61</v>
+        <v>168.47</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.02000000000001</v>
+        <v>151.80000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>150.24</v>
+        <v>149.81</v>
       </c>
       <c r="F35" s="10">
-        <v>159.24</v>
+        <v>158.81</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.19</v>
+        <v>152.02000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>150.38</v>
+        <v>150.24</v>
       </c>
       <c r="F36" s="13">
-        <v>159.38</v>
+        <v>159.24</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>159.43</v>
+        <v>159.22999999999999</v>
       </c>
       <c r="E40" s="10">
-        <v>157.57</v>
+        <v>157.4</v>
       </c>
       <c r="F40" s="10">
-        <v>167.57</v>
+        <v>167.4</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>159.15</v>
+        <v>158.94999999999999</v>
       </c>
       <c r="E41" s="13">
-        <v>157.99</v>
+        <v>157.82</v>
       </c>
       <c r="F41" s="13">
-        <v>167.99</v>
+        <v>167.82</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>159.61000000000001</v>
+        <v>159.43</v>
       </c>
       <c r="E42" s="10">
-        <v>157.91999999999999</v>
+        <v>157.57</v>
       </c>
       <c r="F42" s="10">
-        <v>167.92</v>
+        <v>167.57</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>159.33000000000001</v>
+        <v>159.15</v>
       </c>
       <c r="E43" s="13">
-        <v>158.34</v>
+        <v>157.99</v>
       </c>
       <c r="F43" s="13">
-        <v>168.34</v>
+        <v>167.99</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>153</v>
+        <v>152.71</v>
       </c>
       <c r="E47" s="10">
-        <v>151.9</v>
+        <v>151.57</v>
       </c>
       <c r="F47" s="10">
-        <v>161.9</v>
+        <v>161.57</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.66999999999999</v>
+        <v>152.38</v>
       </c>
       <c r="E48" s="13">
-        <v>151.86000000000001</v>
+        <v>151.52000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>161.86000000000001</v>
+        <v>161.52000000000001</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>153.07</v>
+        <v>153</v>
       </c>
       <c r="E49" s="10">
-        <v>152.43</v>
+        <v>151.9</v>
       </c>
       <c r="F49" s="10">
-        <v>162.43</v>
+        <v>161.9</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.74</v>
+        <v>152.66999999999999</v>
       </c>
       <c r="E50" s="13">
-        <v>152.38</v>
+        <v>151.86000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>162.38</v>
+        <v>161.86000000000001</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>168.77</v>
+        <v>168.55</v>
       </c>
       <c r="E54" s="10">
-        <v>165.32</v>
+        <v>164.96</v>
       </c>
       <c r="F54" s="10">
-        <v>175.32</v>
+        <v>174.96</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>161.76</v>
+        <v>161.57</v>
       </c>
       <c r="E55" s="13">
-        <v>163.56</v>
+        <v>163.11000000000001</v>
       </c>
       <c r="F55" s="13">
-        <v>173.56</v>
+        <v>173.11</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>158.56</v>
+        <v>158.34</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>159.34</v>
+        <v>159.1</v>
       </c>
       <c r="E57" s="13">
-        <v>157.97999999999999</v>
+        <v>157.53</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>155.11000000000001</v>
+        <v>154.87</v>
       </c>
       <c r="E58" s="10">
-        <v>153.88</v>
+        <v>153.43</v>
       </c>
       <c r="F58" s="10">
-        <v>163.88</v>
+        <v>163.43</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>161.30000000000001</v>
+        <v>161.06</v>
       </c>
       <c r="E59" s="13">
-        <v>163.89</v>
+        <v>163.5</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>168.93</v>
+        <v>168.77</v>
       </c>
       <c r="E60" s="10">
-        <v>165.5</v>
+        <v>165.32</v>
       </c>
       <c r="F60" s="10">
-        <v>175.5</v>
+        <v>175.32</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>161.94</v>
+        <v>161.76</v>
       </c>
       <c r="E61" s="13">
-        <v>163.68</v>
+        <v>163.56</v>
       </c>
       <c r="F61" s="13">
-        <v>173.68</v>
+        <v>173.56</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>158.72999999999999</v>
+        <v>158.56</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>159.5</v>
+        <v>159.34</v>
       </c>
       <c r="E63" s="13">
-        <v>158.11000000000001</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>155.27000000000001</v>
+        <v>155.11000000000001</v>
       </c>
       <c r="E64" s="10">
-        <v>154</v>
+        <v>153.88</v>
       </c>
       <c r="F64" s="10">
-        <v>164</v>
+        <v>163.88</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>161.46</v>
+        <v>161.30000000000001</v>
       </c>
       <c r="E65" s="13">
-        <v>164.05</v>
+        <v>163.89</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,42 +2134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2161,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tue Jan  6 03:09:18 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{91860CE4-646F-44FA-964B-AD92B2527E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8A73ABDC-C5C5-45A5-8636-21C83A8238DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.03</v>
+        <v>152.5</v>
       </c>
       <c r="E8" s="10">
-        <v>149.57</v>
+        <v>149.77000000000001</v>
       </c>
       <c r="F8" s="10">
-        <v>159.57</v>
+        <v>159.78</v>
       </c>
       <c r="G8" s="10">
-        <v>149.59</v>
+        <v>149.79</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.03</v>
+        <v>152.5</v>
       </c>
       <c r="E9" s="13">
-        <v>149.57</v>
+        <v>149.77000000000001</v>
       </c>
       <c r="F9" s="13">
-        <v>159.57</v>
+        <v>159.78</v>
       </c>
       <c r="G9" s="13">
-        <v>149.59</v>
+        <v>149.79</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.24</v>
+        <v>154.68</v>
       </c>
       <c r="E10" s="10">
-        <v>151.4</v>
+        <v>151.57</v>
       </c>
       <c r="F10" s="10">
-        <v>161.4</v>
+        <v>161.57</v>
       </c>
       <c r="G10" s="10">
-        <v>151.80000000000001</v>
+        <v>151.97</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.21</v>
+        <v>152.03</v>
       </c>
       <c r="E11" s="13">
-        <v>149.96</v>
+        <v>149.57</v>
       </c>
       <c r="F11" s="13">
-        <v>159.96</v>
+        <v>159.57</v>
       </c>
       <c r="G11" s="13">
-        <v>149.97999999999999</v>
+        <v>149.59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.21</v>
+        <v>152.03</v>
       </c>
       <c r="E12" s="10">
-        <v>149.96</v>
+        <v>149.57</v>
       </c>
       <c r="F12" s="10">
-        <v>159.96</v>
+        <v>159.57</v>
       </c>
       <c r="G12" s="10">
-        <v>149.97999999999999</v>
+        <v>149.59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.46</v>
+        <v>154.24</v>
       </c>
       <c r="E13" s="13">
-        <v>151.83000000000001</v>
+        <v>151.4</v>
       </c>
       <c r="F13" s="13">
-        <v>161.83000000000001</v>
+        <v>161.4</v>
       </c>
       <c r="G13" s="13">
-        <v>152.22999999999999</v>
+        <v>151.80000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>158.13999999999999</v>
+        <v>158</v>
       </c>
       <c r="E17" s="10">
-        <v>155.03</v>
+        <v>154.63</v>
       </c>
       <c r="F17" s="10">
-        <v>165.03</v>
+        <v>164.63</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>158.38</v>
+        <v>158.13999999999999</v>
       </c>
       <c r="E18" s="13">
-        <v>155.49</v>
+        <v>155.03</v>
       </c>
       <c r="F18" s="13">
-        <v>165.49</v>
+        <v>165.03</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.77000000000001</v>
+        <v>154.02000000000001</v>
       </c>
       <c r="E22" s="10">
-        <v>150.81</v>
+        <v>151.02000000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>160.41</v>
+        <v>160.62</v>
       </c>
       <c r="G22" s="10">
-        <v>151.88</v>
+        <v>152.09</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.55000000000001</v>
+        <v>158.76</v>
       </c>
       <c r="E23" s="13">
-        <v>156.31</v>
+        <v>156.47999999999999</v>
       </c>
       <c r="F23" s="13">
-        <v>166.31</v>
+        <v>166.48</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.71</v>
+        <v>158.93</v>
       </c>
       <c r="E24" s="10">
-        <v>156.91</v>
+        <v>157.09</v>
       </c>
       <c r="F24" s="10">
-        <v>166.91</v>
+        <v>167.09</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.69999999999999</v>
+        <v>158.91</v>
       </c>
       <c r="E25" s="13">
-        <v>156.41999999999999</v>
+        <v>156.61000000000001</v>
       </c>
       <c r="F25" s="13">
-        <v>166.42</v>
+        <v>166.61</v>
       </c>
       <c r="G25" s="13">
-        <v>156.55000000000001</v>
+        <v>156.72999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.35</v>
+        <v>158.56</v>
       </c>
       <c r="E26" s="10">
-        <v>158.04</v>
+        <v>158.22</v>
       </c>
       <c r="F26" s="10">
-        <v>168.04</v>
+        <v>168.22</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.94</v>
+        <v>153.77000000000001</v>
       </c>
       <c r="E27" s="13">
-        <v>151.19999999999999</v>
+        <v>150.81</v>
       </c>
       <c r="F27" s="13">
-        <v>160.80000000000001</v>
+        <v>160.41</v>
       </c>
       <c r="G27" s="13">
-        <v>152.28</v>
+        <v>151.88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.76</v>
+        <v>158.55000000000001</v>
       </c>
       <c r="E28" s="22">
-        <v>156.75</v>
+        <v>156.31</v>
       </c>
       <c r="F28" s="22">
-        <v>166.75</v>
+        <v>166.31</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.93</v>
+        <v>158.71</v>
       </c>
       <c r="E29" s="13">
-        <v>157.34</v>
+        <v>156.91</v>
       </c>
       <c r="F29" s="13">
-        <v>167.34</v>
+        <v>166.91</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.91999999999999</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="E30" s="22">
-        <v>156.85</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="F30" s="22">
-        <v>166.85</v>
+        <v>166.42</v>
       </c>
       <c r="G30" s="22">
-        <v>156.97999999999999</v>
+        <v>156.55000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.58000000000001</v>
+        <v>158.35</v>
       </c>
       <c r="E31" s="13">
-        <v>158.47</v>
+        <v>158.04</v>
       </c>
       <c r="F31" s="13">
-        <v>168.47</v>
+        <v>168.04</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>151.80000000000001</v>
+        <v>151.69</v>
       </c>
       <c r="E35" s="10">
-        <v>149.81</v>
+        <v>149.43</v>
       </c>
       <c r="F35" s="10">
-        <v>158.81</v>
+        <v>158.43</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.02000000000001</v>
+        <v>151.80000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>150.24</v>
+        <v>149.81</v>
       </c>
       <c r="F36" s="13">
-        <v>159.24</v>
+        <v>158.81</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>159.22999999999999</v>
+        <v>159.13</v>
       </c>
       <c r="E40" s="10">
-        <v>157.4</v>
+        <v>157.28</v>
       </c>
       <c r="F40" s="10">
-        <v>167.4</v>
+        <v>167.28</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>158.94999999999999</v>
+        <v>158.85</v>
       </c>
       <c r="E41" s="13">
-        <v>157.82</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F41" s="13">
-        <v>167.82</v>
+        <v>167.7</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>159.43</v>
+        <v>159.22999999999999</v>
       </c>
       <c r="E42" s="10">
-        <v>157.57</v>
+        <v>157.4</v>
       </c>
       <c r="F42" s="10">
-        <v>167.57</v>
+        <v>167.4</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>159.15</v>
+        <v>158.94999999999999</v>
       </c>
       <c r="E43" s="13">
-        <v>157.99</v>
+        <v>157.82</v>
       </c>
       <c r="F43" s="13">
-        <v>167.99</v>
+        <v>167.82</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.71</v>
+        <v>152.53</v>
       </c>
       <c r="E47" s="10">
-        <v>151.57</v>
+        <v>151.29</v>
       </c>
       <c r="F47" s="10">
-        <v>161.57</v>
+        <v>161.29</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.38</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="E48" s="13">
-        <v>151.52000000000001</v>
+        <v>151.24</v>
       </c>
       <c r="F48" s="13">
-        <v>161.52000000000001</v>
+        <v>161.24</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>153</v>
+        <v>152.71</v>
       </c>
       <c r="E49" s="10">
-        <v>151.9</v>
+        <v>151.57</v>
       </c>
       <c r="F49" s="10">
-        <v>161.9</v>
+        <v>161.57</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.66999999999999</v>
+        <v>152.38</v>
       </c>
       <c r="E50" s="13">
-        <v>151.86000000000001</v>
+        <v>151.52000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>161.86000000000001</v>
+        <v>161.52000000000001</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>168.55</v>
+        <v>168.43</v>
       </c>
       <c r="E54" s="10">
-        <v>164.96</v>
+        <v>164.68</v>
       </c>
       <c r="F54" s="10">
-        <v>174.96</v>
+        <v>174.68</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>161.57</v>
+        <v>161.49</v>
       </c>
       <c r="E55" s="13">
-        <v>163.11000000000001</v>
+        <v>163.26</v>
       </c>
       <c r="F55" s="13">
-        <v>173.11</v>
+        <v>173.26</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>158.34</v>
+        <v>158.56</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>159.1</v>
+        <v>159.29</v>
       </c>
       <c r="E57" s="13">
-        <v>157.53</v>
+        <v>157.68</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>154.87</v>
+        <v>155.05000000000001</v>
       </c>
       <c r="E58" s="10">
-        <v>153.43</v>
+        <v>153.58000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>163.43</v>
+        <v>163.58000000000001</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>161.06</v>
+        <v>160.91</v>
       </c>
       <c r="E59" s="13">
-        <v>163.5</v>
+        <v>163.18</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>168.77</v>
+        <v>168.55</v>
       </c>
       <c r="E60" s="10">
-        <v>165.32</v>
+        <v>164.96</v>
       </c>
       <c r="F60" s="10">
-        <v>175.32</v>
+        <v>174.96</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>161.76</v>
+        <v>161.57</v>
       </c>
       <c r="E61" s="13">
-        <v>163.56</v>
+        <v>163.11000000000001</v>
       </c>
       <c r="F61" s="13">
-        <v>173.56</v>
+        <v>173.11</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>158.56</v>
+        <v>158.34</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>159.34</v>
+        <v>159.1</v>
       </c>
       <c r="E63" s="13">
-        <v>157.97999999999999</v>
+        <v>157.53</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>155.11000000000001</v>
+        <v>154.87</v>
       </c>
       <c r="E64" s="10">
-        <v>153.88</v>
+        <v>153.43</v>
       </c>
       <c r="F64" s="10">
-        <v>163.88</v>
+        <v>163.43</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46025</v>
+        <v>46028</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>161.30000000000001</v>
+        <v>161.06</v>
       </c>
       <c r="E65" s="13">
-        <v>163.89</v>
+        <v>163.5</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,26 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,10 +2114,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2161,21 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Wed Jan  7 03:09:27 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8A73ABDC-C5C5-45A5-8636-21C83A8238DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{4707329D-6E52-4E11-9AC1-E8529D9858D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="27420" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.46484375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.5</v>
+        <v>152.84</v>
       </c>
       <c r="E8" s="10">
-        <v>149.77000000000001</v>
+        <v>149.83000000000001</v>
       </c>
       <c r="F8" s="10">
-        <v>159.78</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="G8" s="10">
-        <v>149.79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.5</v>
+        <v>152.84</v>
       </c>
       <c r="E9" s="13">
-        <v>149.77000000000001</v>
+        <v>149.83000000000001</v>
       </c>
       <c r="F9" s="13">
-        <v>159.78</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="G9" s="13">
-        <v>149.79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.68</v>
+        <v>154.61000000000001</v>
       </c>
       <c r="E10" s="10">
-        <v>151.57</v>
+        <v>151.22999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>161.57</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="G10" s="10">
-        <v>151.97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.03</v>
+        <v>152.5</v>
       </c>
       <c r="E11" s="13">
-        <v>149.57</v>
+        <v>149.77000000000001</v>
       </c>
       <c r="F11" s="13">
-        <v>159.57</v>
+        <v>159.78</v>
       </c>
       <c r="G11" s="13">
-        <v>149.59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.03</v>
+        <v>152.5</v>
       </c>
       <c r="E12" s="10">
-        <v>149.57</v>
+        <v>149.77000000000001</v>
       </c>
       <c r="F12" s="10">
-        <v>159.57</v>
+        <v>159.78</v>
       </c>
       <c r="G12" s="10">
-        <v>149.59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.24</v>
+        <v>154.68</v>
       </c>
       <c r="E13" s="13">
-        <v>151.4</v>
+        <v>151.57</v>
       </c>
       <c r="F13" s="13">
-        <v>161.4</v>
+        <v>161.57</v>
       </c>
       <c r="G13" s="13">
-        <v>151.80000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>158</v>
+        <v>157.91999999999999</v>
       </c>
       <c r="E17" s="10">
-        <v>154.63</v>
+        <v>154.28</v>
       </c>
       <c r="F17" s="10">
-        <v>164.63</v>
+        <v>164.28</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>158.13999999999999</v>
+        <v>158</v>
       </c>
       <c r="E18" s="13">
-        <v>155.03</v>
+        <v>154.63</v>
       </c>
       <c r="F18" s="13">
-        <v>165.03</v>
+        <v>164.63</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>154.02000000000001</v>
+        <v>154.36000000000001</v>
       </c>
       <c r="E22" s="10">
-        <v>151.02000000000001</v>
+        <v>151.08000000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>160.62</v>
+        <v>160.68</v>
       </c>
       <c r="G22" s="10">
-        <v>152.09</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.76</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="E23" s="13">
-        <v>156.47999999999999</v>
+        <v>156.47</v>
       </c>
       <c r="F23" s="13">
-        <v>166.48</v>
+        <v>166.47</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.93</v>
+        <v>158.86000000000001</v>
       </c>
       <c r="E24" s="10">
-        <v>157.09</v>
+        <v>157.08000000000001</v>
       </c>
       <c r="F24" s="10">
-        <v>167.09</v>
+        <v>167.08</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.91</v>
+        <v>158.85</v>
       </c>
       <c r="E25" s="13">
-        <v>156.61000000000001</v>
+        <v>156.6</v>
       </c>
       <c r="F25" s="13">
-        <v>166.61</v>
+        <v>166.6</v>
       </c>
       <c r="G25" s="13">
         <v>156.72999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.56</v>
+        <v>158.49</v>
       </c>
       <c r="E26" s="10">
-        <v>158.22</v>
+        <v>158.21</v>
       </c>
       <c r="F26" s="10">
-        <v>168.22</v>
+        <v>168.21</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.77000000000001</v>
+        <v>154.02000000000001</v>
       </c>
       <c r="E27" s="13">
-        <v>150.81</v>
+        <v>151.02000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>160.41</v>
+        <v>160.62</v>
       </c>
       <c r="G27" s="13">
-        <v>151.88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.55000000000001</v>
+        <v>158.76</v>
       </c>
       <c r="E28" s="22">
-        <v>156.31</v>
+        <v>156.47999999999999</v>
       </c>
       <c r="F28" s="22">
-        <v>166.31</v>
+        <v>166.48</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.71</v>
+        <v>158.93</v>
       </c>
       <c r="E29" s="13">
-        <v>156.91</v>
+        <v>157.09</v>
       </c>
       <c r="F29" s="13">
-        <v>166.91</v>
+        <v>167.09</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.69999999999999</v>
+        <v>158.91</v>
       </c>
       <c r="E30" s="22">
-        <v>156.41999999999999</v>
+        <v>156.61000000000001</v>
       </c>
       <c r="F30" s="22">
-        <v>166.42</v>
+        <v>166.61</v>
       </c>
       <c r="G30" s="22">
-        <v>156.55000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>156.72999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.35</v>
+        <v>158.56</v>
       </c>
       <c r="E31" s="13">
-        <v>158.04</v>
+        <v>158.22</v>
       </c>
       <c r="F31" s="13">
-        <v>168.04</v>
+        <v>168.22</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>151.69</v>
+        <v>152.16999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>149.43</v>
+        <v>149.09</v>
       </c>
       <c r="F35" s="10">
-        <v>158.43</v>
+        <v>158.09</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>151.80000000000001</v>
+        <v>151.69</v>
       </c>
       <c r="E36" s="13">
-        <v>149.81</v>
+        <v>149.43</v>
       </c>
       <c r="F36" s="13">
-        <v>158.81</v>
+        <v>158.43</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>159.13</v>
+        <v>159.07</v>
       </c>
       <c r="E40" s="10">
-        <v>157.28</v>
+        <v>157.13</v>
       </c>
       <c r="F40" s="10">
-        <v>167.28</v>
+        <v>167.13</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>158.85</v>
+        <v>158.79</v>
       </c>
       <c r="E41" s="13">
-        <v>157.69999999999999</v>
+        <v>157.55000000000001</v>
       </c>
       <c r="F41" s="13">
-        <v>167.7</v>
+        <v>167.55</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>159.22999999999999</v>
+        <v>159.13</v>
       </c>
       <c r="E42" s="10">
-        <v>157.4</v>
+        <v>157.28</v>
       </c>
       <c r="F42" s="10">
-        <v>167.4</v>
+        <v>167.28</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>158.94999999999999</v>
+        <v>158.85</v>
       </c>
       <c r="E43" s="13">
-        <v>157.82</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F43" s="13">
-        <v>167.82</v>
+        <v>167.7</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.53</v>
+        <v>152.86000000000001</v>
       </c>
       <c r="E47" s="10">
-        <v>151.29</v>
+        <v>150.9</v>
       </c>
       <c r="F47" s="10">
-        <v>161.29</v>
+        <v>160.9</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.19999999999999</v>
+        <v>152.52000000000001</v>
       </c>
       <c r="E48" s="13">
-        <v>151.24</v>
+        <v>150.85</v>
       </c>
       <c r="F48" s="13">
-        <v>161.24</v>
+        <v>160.85</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.71</v>
+        <v>152.53</v>
       </c>
       <c r="E49" s="10">
-        <v>151.57</v>
+        <v>151.29</v>
       </c>
       <c r="F49" s="10">
-        <v>161.57</v>
+        <v>161.29</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.38</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="E50" s="13">
-        <v>151.52000000000001</v>
+        <v>151.24</v>
       </c>
       <c r="F50" s="13">
-        <v>161.52000000000001</v>
+        <v>161.24</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>168.43</v>
+        <v>168.36</v>
       </c>
       <c r="E54" s="10">
-        <v>164.68</v>
+        <v>164.38</v>
       </c>
       <c r="F54" s="10">
-        <v>174.68</v>
+        <v>174.38</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>161.49</v>
+        <v>161.44</v>
       </c>
       <c r="E55" s="13">
-        <v>163.26</v>
+        <v>163.24</v>
       </c>
       <c r="F55" s="13">
-        <v>173.26</v>
+        <v>173.24</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>158.56</v>
+        <v>158.16999999999999</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>159.29</v>
+        <v>158.88</v>
       </c>
       <c r="E57" s="13">
-        <v>157.68</v>
+        <v>157.66</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>155.05000000000001</v>
+        <v>154.65</v>
       </c>
       <c r="E58" s="10">
-        <v>153.58000000000001</v>
+        <v>153.56</v>
       </c>
       <c r="F58" s="10">
-        <v>163.58000000000001</v>
+        <v>163.56</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>160.91</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="E59" s="13">
-        <v>163.18</v>
+        <v>162.86000000000001</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>168.55</v>
+        <v>168.43</v>
       </c>
       <c r="E60" s="10">
-        <v>164.96</v>
+        <v>164.68</v>
       </c>
       <c r="F60" s="10">
-        <v>174.96</v>
+        <v>174.68</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>161.57</v>
+        <v>161.49</v>
       </c>
       <c r="E61" s="13">
-        <v>163.11000000000001</v>
+        <v>163.26</v>
       </c>
       <c r="F61" s="13">
-        <v>173.11</v>
+        <v>173.26</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>158.34</v>
+        <v>158.56</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>159.1</v>
+        <v>159.29</v>
       </c>
       <c r="E63" s="13">
-        <v>157.53</v>
+        <v>157.68</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>154.87</v>
+        <v>155.05000000000001</v>
       </c>
       <c r="E64" s="10">
-        <v>153.43</v>
+        <v>153.58000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>163.43</v>
+        <v>163.58000000000001</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>161.06</v>
+        <v>160.91</v>
       </c>
       <c r="E65" s="13">
-        <v>163.5</v>
+        <v>163.18</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,42 +2134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,9 +2161,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Thu Jan  8 03:09:22 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{4707329D-6E52-4E11-9AC1-E8529D9858D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{769371DC-F3F3-4631-9343-B52FA7D21208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27420" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.46484375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.84</v>
+        <v>152.74</v>
       </c>
       <c r="E8" s="10">
-        <v>149.83000000000001</v>
+        <v>149.32</v>
       </c>
       <c r="F8" s="10">
-        <v>159.83000000000001</v>
+        <v>159.32</v>
       </c>
       <c r="G8" s="10">
-        <v>149.85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.84</v>
+        <v>152.74</v>
       </c>
       <c r="E9" s="13">
-        <v>149.83000000000001</v>
+        <v>149.32</v>
       </c>
       <c r="F9" s="13">
-        <v>159.83000000000001</v>
+        <v>159.32</v>
       </c>
       <c r="G9" s="13">
-        <v>149.85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.61000000000001</v>
+        <v>153.69</v>
       </c>
       <c r="E10" s="10">
-        <v>151.22999999999999</v>
+        <v>150.22999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>161.22999999999999</v>
+        <v>160.22999999999999</v>
       </c>
       <c r="G10" s="10">
-        <v>151.63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>150.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.5</v>
+        <v>152.84</v>
       </c>
       <c r="E11" s="13">
-        <v>149.77000000000001</v>
+        <v>149.83000000000001</v>
       </c>
       <c r="F11" s="13">
-        <v>159.78</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="G11" s="13">
-        <v>149.79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.5</v>
+        <v>152.84</v>
       </c>
       <c r="E12" s="10">
-        <v>149.77000000000001</v>
+        <v>149.83000000000001</v>
       </c>
       <c r="F12" s="10">
-        <v>159.78</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="G12" s="10">
-        <v>149.79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.68</v>
+        <v>154.61000000000001</v>
       </c>
       <c r="E13" s="13">
-        <v>151.57</v>
+        <v>151.22999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>161.57</v>
+        <v>161.22999999999999</v>
       </c>
       <c r="G13" s="13">
-        <v>151.97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>157.91999999999999</v>
+        <v>156.97999999999999</v>
       </c>
       <c r="E17" s="10">
-        <v>154.28</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="F17" s="10">
-        <v>164.28</v>
+        <v>163.27000000000001</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>158</v>
+        <v>157.91999999999999</v>
       </c>
       <c r="E18" s="13">
-        <v>154.63</v>
+        <v>154.28</v>
       </c>
       <c r="F18" s="13">
-        <v>164.63</v>
+        <v>164.28</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>154.36000000000001</v>
+        <v>153.71</v>
       </c>
       <c r="E22" s="10">
-        <v>151.08000000000001</v>
+        <v>150.34</v>
       </c>
       <c r="F22" s="10">
-        <v>160.68</v>
+        <v>159.94</v>
       </c>
       <c r="G22" s="10">
-        <v>152.15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.41999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.69999999999999</v>
+        <v>158.33000000000001</v>
       </c>
       <c r="E23" s="13">
-        <v>156.47</v>
+        <v>155.91</v>
       </c>
       <c r="F23" s="13">
-        <v>166.47</v>
+        <v>165.91</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.86000000000001</v>
+        <v>158.49</v>
       </c>
       <c r="E24" s="10">
-        <v>157.08000000000001</v>
+        <v>156.53</v>
       </c>
       <c r="F24" s="10">
-        <v>167.08</v>
+        <v>166.53</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.85</v>
+        <v>158.47</v>
       </c>
       <c r="E25" s="13">
-        <v>156.6</v>
+        <v>156.05000000000001</v>
       </c>
       <c r="F25" s="13">
-        <v>166.6</v>
+        <v>166.05</v>
       </c>
       <c r="G25" s="13">
-        <v>156.72999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>156.16999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.49</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="E26" s="10">
-        <v>158.21</v>
+        <v>157.65</v>
       </c>
       <c r="F26" s="10">
-        <v>168.21</v>
+        <v>167.65</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>154.02000000000001</v>
+        <v>154.36000000000001</v>
       </c>
       <c r="E27" s="13">
-        <v>151.02000000000001</v>
+        <v>151.08000000000001</v>
       </c>
       <c r="F27" s="13">
-        <v>160.62</v>
+        <v>160.68</v>
       </c>
       <c r="G27" s="13">
-        <v>152.09</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>152.15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.76</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="E28" s="22">
-        <v>156.47999999999999</v>
+        <v>156.47</v>
       </c>
       <c r="F28" s="22">
-        <v>166.48</v>
+        <v>166.47</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.93</v>
+        <v>158.86000000000001</v>
       </c>
       <c r="E29" s="13">
-        <v>157.09</v>
+        <v>157.08000000000001</v>
       </c>
       <c r="F29" s="13">
-        <v>167.09</v>
+        <v>167.08</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.91</v>
+        <v>158.85</v>
       </c>
       <c r="E30" s="22">
-        <v>156.61000000000001</v>
+        <v>156.6</v>
       </c>
       <c r="F30" s="22">
-        <v>166.61</v>
+        <v>166.6</v>
       </c>
       <c r="G30" s="22">
         <v>156.72999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.56</v>
+        <v>158.49</v>
       </c>
       <c r="E31" s="13">
-        <v>158.22</v>
+        <v>158.21</v>
       </c>
       <c r="F31" s="13">
-        <v>168.22</v>
+        <v>168.21</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.16999999999999</v>
+        <v>151.80000000000001</v>
       </c>
       <c r="E35" s="10">
-        <v>149.09</v>
+        <v>148.1</v>
       </c>
       <c r="F35" s="10">
-        <v>158.09</v>
+        <v>157.1</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>151.69</v>
+        <v>152.16999999999999</v>
       </c>
       <c r="E36" s="13">
-        <v>149.43</v>
+        <v>149.09</v>
       </c>
       <c r="F36" s="13">
-        <v>158.43</v>
+        <v>158.09</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>159.07</v>
+        <v>158.16</v>
       </c>
       <c r="E40" s="10">
-        <v>157.13</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="F40" s="10">
-        <v>167.13</v>
+        <v>166.42</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>158.79</v>
+        <v>157.88</v>
       </c>
       <c r="E41" s="13">
-        <v>157.55000000000001</v>
+        <v>156.84</v>
       </c>
       <c r="F41" s="13">
-        <v>167.55</v>
+        <v>166.84</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>159.13</v>
+        <v>159.07</v>
       </c>
       <c r="E42" s="10">
-        <v>157.28</v>
+        <v>157.13</v>
       </c>
       <c r="F42" s="10">
-        <v>167.28</v>
+        <v>167.13</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>158.85</v>
+        <v>158.79</v>
       </c>
       <c r="E43" s="13">
-        <v>157.69999999999999</v>
+        <v>157.55000000000001</v>
       </c>
       <c r="F43" s="13">
-        <v>167.7</v>
+        <v>167.55</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.86000000000001</v>
+        <v>153.22</v>
       </c>
       <c r="E47" s="10">
-        <v>150.9</v>
+        <v>150.32</v>
       </c>
       <c r="F47" s="10">
-        <v>160.9</v>
+        <v>160.32</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.52000000000001</v>
+        <v>152.87</v>
       </c>
       <c r="E48" s="13">
-        <v>150.85</v>
+        <v>150.27000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>160.85</v>
+        <v>160.27000000000001</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.53</v>
+        <v>152.86000000000001</v>
       </c>
       <c r="E49" s="10">
-        <v>151.29</v>
+        <v>150.9</v>
       </c>
       <c r="F49" s="10">
-        <v>161.29</v>
+        <v>160.9</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.19999999999999</v>
+        <v>152.52000000000001</v>
       </c>
       <c r="E50" s="13">
-        <v>151.24</v>
+        <v>150.85</v>
       </c>
       <c r="F50" s="13">
-        <v>161.24</v>
+        <v>160.85</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>168.36</v>
+        <v>167.41</v>
       </c>
       <c r="E54" s="10">
-        <v>164.38</v>
+        <v>163.47999999999999</v>
       </c>
       <c r="F54" s="10">
-        <v>174.38</v>
+        <v>173.48</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>161.44</v>
+        <v>160.54</v>
       </c>
       <c r="E55" s="13">
-        <v>163.24</v>
+        <v>162.44</v>
       </c>
       <c r="F55" s="13">
-        <v>173.24</v>
+        <v>172.44</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>158.16999999999999</v>
+        <v>157.03</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>158.88</v>
+        <v>157.72</v>
       </c>
       <c r="E57" s="13">
-        <v>157.66</v>
+        <v>156.87</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>154.65</v>
+        <v>153.47999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>153.56</v>
+        <v>152.76</v>
       </c>
       <c r="F58" s="10">
-        <v>163.56</v>
+        <v>162.76</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>160.83000000000001</v>
+        <v>159.88999999999999</v>
       </c>
       <c r="E59" s="13">
-        <v>162.86000000000001</v>
+        <v>161.91</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>168.43</v>
+        <v>168.36</v>
       </c>
       <c r="E60" s="10">
-        <v>164.68</v>
+        <v>164.38</v>
       </c>
       <c r="F60" s="10">
-        <v>174.68</v>
+        <v>174.38</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>161.49</v>
+        <v>161.44</v>
       </c>
       <c r="E61" s="13">
-        <v>163.26</v>
+        <v>163.24</v>
       </c>
       <c r="F61" s="13">
-        <v>173.26</v>
+        <v>173.24</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>158.56</v>
+        <v>158.16999999999999</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>159.29</v>
+        <v>158.88</v>
       </c>
       <c r="E63" s="13">
-        <v>157.68</v>
+        <v>157.66</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>155.05000000000001</v>
+        <v>154.65</v>
       </c>
       <c r="E64" s="10">
-        <v>153.58000000000001</v>
+        <v>153.56</v>
       </c>
       <c r="F64" s="10">
-        <v>163.58000000000001</v>
+        <v>163.56</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>160.91</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="E65" s="13">
-        <v>163.18</v>
+        <v>162.86000000000001</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,26 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,10 +2114,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2161,21 +2173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fri Jan  9 03:11:09 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{769371DC-F3F3-4631-9343-B52FA7D21208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5A563F85-6E37-4C59-8928-0CED01F5C67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="27420" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.74</v>
+        <v>152.83000000000001</v>
       </c>
       <c r="E8" s="10">
-        <v>149.32</v>
+        <v>149.25</v>
       </c>
       <c r="F8" s="10">
-        <v>159.32</v>
+        <v>159.25</v>
       </c>
       <c r="G8" s="10">
-        <v>149.34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.27000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.74</v>
+        <v>152.83000000000001</v>
       </c>
       <c r="E9" s="13">
-        <v>149.32</v>
+        <v>149.25</v>
       </c>
       <c r="F9" s="13">
-        <v>159.32</v>
+        <v>159.25</v>
       </c>
       <c r="G9" s="13">
-        <v>149.34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.27000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>153.69</v>
+        <v>153.76</v>
       </c>
       <c r="E10" s="10">
-        <v>150.22999999999999</v>
+        <v>150.69999999999999</v>
       </c>
       <c r="F10" s="10">
-        <v>160.22999999999999</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="G10" s="10">
-        <v>150.63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.84</v>
+        <v>152.74</v>
       </c>
       <c r="E11" s="13">
-        <v>149.83000000000001</v>
+        <v>149.32</v>
       </c>
       <c r="F11" s="13">
-        <v>159.83000000000001</v>
+        <v>159.32</v>
       </c>
       <c r="G11" s="13">
-        <v>149.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.84</v>
+        <v>152.74</v>
       </c>
       <c r="E12" s="10">
-        <v>149.83000000000001</v>
+        <v>149.32</v>
       </c>
       <c r="F12" s="10">
-        <v>159.83000000000001</v>
+        <v>159.32</v>
       </c>
       <c r="G12" s="10">
-        <v>149.85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.61000000000001</v>
+        <v>153.69</v>
       </c>
       <c r="E13" s="13">
-        <v>151.22999999999999</v>
+        <v>150.22999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>161.22999999999999</v>
+        <v>160.22999999999999</v>
       </c>
       <c r="G13" s="13">
-        <v>151.63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150.63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>156.97999999999999</v>
+        <v>157.26</v>
       </c>
       <c r="E17" s="10">
-        <v>153.27000000000001</v>
+        <v>153.72</v>
       </c>
       <c r="F17" s="10">
-        <v>163.27000000000001</v>
+        <v>163.72</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>157.91999999999999</v>
+        <v>156.97999999999999</v>
       </c>
       <c r="E18" s="13">
-        <v>154.28</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="F18" s="13">
-        <v>164.28</v>
+        <v>163.27000000000001</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.71</v>
+        <v>153.69</v>
       </c>
       <c r="E22" s="10">
-        <v>150.34</v>
+        <v>150.5</v>
       </c>
       <c r="F22" s="10">
-        <v>159.94</v>
+        <v>160.1</v>
       </c>
       <c r="G22" s="10">
-        <v>151.41999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.33000000000001</v>
+        <v>158.28</v>
       </c>
       <c r="E23" s="13">
-        <v>155.91</v>
+        <v>156.15</v>
       </c>
       <c r="F23" s="13">
-        <v>165.91</v>
+        <v>166.15</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.49</v>
+        <v>158.44</v>
       </c>
       <c r="E24" s="10">
-        <v>156.53</v>
+        <v>156.78</v>
       </c>
       <c r="F24" s="10">
-        <v>166.53</v>
+        <v>166.78</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.47</v>
+        <v>158.43</v>
       </c>
       <c r="E25" s="13">
-        <v>156.05000000000001</v>
+        <v>156.29</v>
       </c>
       <c r="F25" s="13">
-        <v>166.05</v>
+        <v>166.29</v>
       </c>
       <c r="G25" s="13">
-        <v>156.16999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>156.41999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.11000000000001</v>
+        <v>158.07</v>
       </c>
       <c r="E26" s="10">
-        <v>157.65</v>
+        <v>157.9</v>
       </c>
       <c r="F26" s="10">
-        <v>167.65</v>
+        <v>167.9</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>154.36000000000001</v>
+        <v>153.71</v>
       </c>
       <c r="E27" s="13">
-        <v>151.08000000000001</v>
+        <v>150.34</v>
       </c>
       <c r="F27" s="13">
-        <v>160.68</v>
+        <v>159.94</v>
       </c>
       <c r="G27" s="13">
-        <v>152.15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151.41999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.69999999999999</v>
+        <v>158.33000000000001</v>
       </c>
       <c r="E28" s="22">
-        <v>156.47</v>
+        <v>155.91</v>
       </c>
       <c r="F28" s="22">
-        <v>166.47</v>
+        <v>165.91</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.86000000000001</v>
+        <v>158.49</v>
       </c>
       <c r="E29" s="13">
-        <v>157.08000000000001</v>
+        <v>156.53</v>
       </c>
       <c r="F29" s="13">
-        <v>167.08</v>
+        <v>166.53</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.85</v>
+        <v>158.47</v>
       </c>
       <c r="E30" s="22">
-        <v>156.6</v>
+        <v>156.05000000000001</v>
       </c>
       <c r="F30" s="22">
-        <v>166.6</v>
+        <v>166.05</v>
       </c>
       <c r="G30" s="22">
-        <v>156.72999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>156.16999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.49</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="E31" s="13">
-        <v>158.21</v>
+        <v>157.65</v>
       </c>
       <c r="F31" s="13">
-        <v>168.21</v>
+        <v>167.65</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>151.80000000000001</v>
+        <v>152.09</v>
       </c>
       <c r="E35" s="10">
-        <v>148.1</v>
+        <v>148.01</v>
       </c>
       <c r="F35" s="10">
-        <v>157.1</v>
+        <v>157.01</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.16999999999999</v>
+        <v>151.80000000000001</v>
       </c>
       <c r="E36" s="13">
-        <v>149.09</v>
+        <v>148.1</v>
       </c>
       <c r="F36" s="13">
-        <v>158.09</v>
+        <v>157.1</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>158.16</v>
+        <v>157.91</v>
       </c>
       <c r="E40" s="10">
-        <v>156.41999999999999</v>
+        <v>156.32</v>
       </c>
       <c r="F40" s="10">
-        <v>166.42</v>
+        <v>166.32</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>157.88</v>
+        <v>157.63</v>
       </c>
       <c r="E41" s="13">
-        <v>156.84</v>
+        <v>156.74</v>
       </c>
       <c r="F41" s="13">
-        <v>166.84</v>
+        <v>166.74</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>159.07</v>
+        <v>158.16</v>
       </c>
       <c r="E42" s="10">
-        <v>157.13</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="F42" s="10">
-        <v>167.13</v>
+        <v>166.42</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>158.79</v>
+        <v>157.88</v>
       </c>
       <c r="E43" s="13">
-        <v>157.55000000000001</v>
+        <v>156.84</v>
       </c>
       <c r="F43" s="13">
-        <v>167.55</v>
+        <v>166.84</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>153.22</v>
+        <v>152.62</v>
       </c>
       <c r="E47" s="10">
-        <v>150.32</v>
+        <v>149.93</v>
       </c>
       <c r="F47" s="10">
-        <v>160.32</v>
+        <v>159.93</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.87</v>
+        <v>152.26</v>
       </c>
       <c r="E48" s="13">
-        <v>150.27000000000001</v>
+        <v>149.87</v>
       </c>
       <c r="F48" s="13">
-        <v>160.27000000000001</v>
+        <v>159.87</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.86000000000001</v>
+        <v>153.22</v>
       </c>
       <c r="E49" s="10">
-        <v>150.9</v>
+        <v>150.32</v>
       </c>
       <c r="F49" s="10">
-        <v>160.9</v>
+        <v>160.32</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.52000000000001</v>
+        <v>152.87</v>
       </c>
       <c r="E50" s="13">
-        <v>150.85</v>
+        <v>150.27000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>160.85</v>
+        <v>160.27000000000001</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>167.41</v>
+        <v>167.15</v>
       </c>
       <c r="E54" s="10">
-        <v>163.47999999999999</v>
+        <v>163.43</v>
       </c>
       <c r="F54" s="10">
-        <v>173.48</v>
+        <v>173.43</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>160.54</v>
+        <v>160.29</v>
       </c>
       <c r="E55" s="13">
-        <v>162.44</v>
+        <v>162.57</v>
       </c>
       <c r="F55" s="13">
-        <v>172.44</v>
+        <v>172.57</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>157.03</v>
+        <v>156.77000000000001</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>157.72</v>
+        <v>157.44</v>
       </c>
       <c r="E57" s="13">
-        <v>156.87</v>
+        <v>156.99</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>153.47999999999999</v>
+        <v>153.21</v>
       </c>
       <c r="E58" s="10">
-        <v>152.76</v>
+        <v>152.88999999999999</v>
       </c>
       <c r="F58" s="10">
-        <v>162.76</v>
+        <v>162.88999999999999</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>159.88999999999999</v>
+        <v>159.62</v>
       </c>
       <c r="E59" s="13">
-        <v>161.91</v>
+        <v>161.85</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>168.36</v>
+        <v>167.41</v>
       </c>
       <c r="E60" s="10">
-        <v>164.38</v>
+        <v>163.47999999999999</v>
       </c>
       <c r="F60" s="10">
-        <v>174.38</v>
+        <v>173.48</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>161.44</v>
+        <v>160.54</v>
       </c>
       <c r="E61" s="13">
-        <v>163.24</v>
+        <v>162.44</v>
       </c>
       <c r="F61" s="13">
-        <v>173.24</v>
+        <v>172.44</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>158.16999999999999</v>
+        <v>157.03</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>158.88</v>
+        <v>157.72</v>
       </c>
       <c r="E63" s="13">
-        <v>157.66</v>
+        <v>156.87</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>154.65</v>
+        <v>153.47999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>153.56</v>
+        <v>152.76</v>
       </c>
       <c r="F64" s="10">
-        <v>163.56</v>
+        <v>162.76</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>160.83000000000001</v>
+        <v>159.88999999999999</v>
       </c>
       <c r="E65" s="13">
-        <v>162.86000000000001</v>
+        <v>161.91</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Mon Jan 12 03:17:17 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5A563F85-6E37-4C59-8928-0CED01F5C67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{81128FA1-9593-4B01-8BBA-E53CE420BD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27420" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentManualCount="8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -716,10 +716,10 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3984375"/>
+    <col min="2" max="2" width="6.46484375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.83000000000001</v>
+        <v>152.91999999999999</v>
       </c>
       <c r="E8" s="10">
-        <v>149.25</v>
+        <v>149.5</v>
       </c>
       <c r="F8" s="10">
-        <v>159.25</v>
+        <v>159.5</v>
       </c>
       <c r="G8" s="10">
-        <v>149.27000000000001</v>
+        <v>149.52000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.83000000000001</v>
+        <v>152.91999999999999</v>
       </c>
       <c r="E9" s="13">
-        <v>149.25</v>
+        <v>149.5</v>
       </c>
       <c r="F9" s="13">
-        <v>159.25</v>
+        <v>159.5</v>
       </c>
       <c r="G9" s="13">
-        <v>149.27000000000001</v>
+        <v>149.52000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>153.76</v>
+        <v>154.04</v>
       </c>
       <c r="E10" s="10">
-        <v>150.69999999999999</v>
+        <v>151.15</v>
       </c>
       <c r="F10" s="10">
-        <v>160.69999999999999</v>
+        <v>161.15</v>
       </c>
       <c r="G10" s="10">
-        <v>151.1</v>
+        <v>151.55000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.74</v>
+        <v>152.83000000000001</v>
       </c>
       <c r="E11" s="13">
-        <v>149.32</v>
+        <v>149.25</v>
       </c>
       <c r="F11" s="13">
-        <v>159.32</v>
+        <v>159.25</v>
       </c>
       <c r="G11" s="13">
-        <v>149.34</v>
+        <v>149.27000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.74</v>
+        <v>152.83000000000001</v>
       </c>
       <c r="E12" s="10">
-        <v>149.32</v>
+        <v>149.25</v>
       </c>
       <c r="F12" s="10">
-        <v>159.32</v>
+        <v>159.25</v>
       </c>
       <c r="G12" s="10">
-        <v>149.34</v>
+        <v>149.27000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>153.69</v>
+        <v>153.76</v>
       </c>
       <c r="E13" s="13">
-        <v>150.22999999999999</v>
+        <v>150.69999999999999</v>
       </c>
       <c r="F13" s="13">
-        <v>160.22999999999999</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="G13" s="13">
-        <v>150.63</v>
+        <v>151.1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>157.26</v>
+        <v>157.32</v>
       </c>
       <c r="E17" s="10">
-        <v>153.72</v>
+        <v>153.83000000000001</v>
       </c>
       <c r="F17" s="10">
-        <v>163.72</v>
+        <v>163.83000000000001</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>156.97999999999999</v>
+        <v>157.26</v>
       </c>
       <c r="E18" s="13">
-        <v>153.27000000000001</v>
+        <v>153.72</v>
       </c>
       <c r="F18" s="13">
-        <v>163.27000000000001</v>
+        <v>163.72</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.69</v>
+        <v>153.88</v>
       </c>
       <c r="E22" s="10">
-        <v>150.5</v>
+        <v>150.63999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>160.1</v>
+        <v>160.24</v>
       </c>
       <c r="G22" s="10">
-        <v>151.57</v>
+        <v>151.71</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.28</v>
+        <v>158.46</v>
       </c>
       <c r="E23" s="13">
-        <v>156.15</v>
+        <v>156.49</v>
       </c>
       <c r="F23" s="13">
-        <v>166.15</v>
+        <v>166.49</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.44</v>
+        <v>158.62</v>
       </c>
       <c r="E24" s="10">
-        <v>156.78</v>
+        <v>157.12</v>
       </c>
       <c r="F24" s="10">
-        <v>166.78</v>
+        <v>167.12</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.43</v>
+        <v>158.61000000000001</v>
       </c>
       <c r="E25" s="13">
-        <v>156.29</v>
+        <v>156.63999999999999</v>
       </c>
       <c r="F25" s="13">
-        <v>166.29</v>
+        <v>166.64</v>
       </c>
       <c r="G25" s="13">
-        <v>156.41999999999999</v>
+        <v>156.77000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.07</v>
+        <v>158.24</v>
       </c>
       <c r="E26" s="10">
-        <v>157.9</v>
+        <v>158.25</v>
       </c>
       <c r="F26" s="10">
-        <v>167.9</v>
+        <v>168.25</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.71</v>
+        <v>153.69</v>
       </c>
       <c r="E27" s="13">
-        <v>150.34</v>
+        <v>150.5</v>
       </c>
       <c r="F27" s="13">
-        <v>159.94</v>
+        <v>160.1</v>
       </c>
       <c r="G27" s="13">
-        <v>151.41999999999999</v>
+        <v>151.57</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.33000000000001</v>
+        <v>158.28</v>
       </c>
       <c r="E28" s="22">
-        <v>155.91</v>
+        <v>156.15</v>
       </c>
       <c r="F28" s="22">
-        <v>165.91</v>
+        <v>166.15</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.49</v>
+        <v>158.44</v>
       </c>
       <c r="E29" s="13">
-        <v>156.53</v>
+        <v>156.78</v>
       </c>
       <c r="F29" s="13">
-        <v>166.53</v>
+        <v>166.78</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.47</v>
+        <v>158.43</v>
       </c>
       <c r="E30" s="22">
-        <v>156.05000000000001</v>
+        <v>156.29</v>
       </c>
       <c r="F30" s="22">
-        <v>166.05</v>
+        <v>166.29</v>
       </c>
       <c r="G30" s="22">
-        <v>156.16999999999999</v>
+        <v>156.41999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.11000000000001</v>
+        <v>158.07</v>
       </c>
       <c r="E31" s="13">
-        <v>157.65</v>
+        <v>157.9</v>
       </c>
       <c r="F31" s="13">
-        <v>167.65</v>
+        <v>167.9</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.09</v>
+        <v>152.49</v>
       </c>
       <c r="E35" s="10">
-        <v>148.01</v>
+        <v>148.13999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>157.01</v>
+        <v>157.13999999999999</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>151.80000000000001</v>
+        <v>152.09</v>
       </c>
       <c r="E36" s="13">
-        <v>148.1</v>
+        <v>148.01</v>
       </c>
       <c r="F36" s="13">
-        <v>157.1</v>
+        <v>157.01</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>157.91</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="E40" s="10">
-        <v>156.32</v>
+        <v>156.43</v>
       </c>
       <c r="F40" s="10">
-        <v>166.32</v>
+        <v>166.43</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>157.63</v>
+        <v>157.71</v>
       </c>
       <c r="E41" s="13">
-        <v>156.74</v>
+        <v>156.85</v>
       </c>
       <c r="F41" s="13">
-        <v>166.74</v>
+        <v>166.85</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>158.16</v>
+        <v>157.91</v>
       </c>
       <c r="E42" s="10">
-        <v>156.41999999999999</v>
+        <v>156.32</v>
       </c>
       <c r="F42" s="10">
-        <v>166.42</v>
+        <v>166.32</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>157.88</v>
+        <v>157.63</v>
       </c>
       <c r="E43" s="13">
-        <v>156.84</v>
+        <v>156.74</v>
       </c>
       <c r="F43" s="13">
-        <v>166.84</v>
+        <v>166.74</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.62</v>
+        <v>152.56</v>
       </c>
       <c r="E47" s="10">
-        <v>149.93</v>
+        <v>149.85</v>
       </c>
       <c r="F47" s="10">
-        <v>159.93</v>
+        <v>159.85</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.26</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="E48" s="13">
-        <v>149.87</v>
+        <v>149.79</v>
       </c>
       <c r="F48" s="13">
-        <v>159.87</v>
+        <v>159.79</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>153.22</v>
+        <v>152.62</v>
       </c>
       <c r="E49" s="10">
-        <v>150.32</v>
+        <v>149.93</v>
       </c>
       <c r="F49" s="10">
-        <v>160.32</v>
+        <v>159.93</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.87</v>
+        <v>152.26</v>
       </c>
       <c r="E50" s="13">
-        <v>150.27000000000001</v>
+        <v>149.87</v>
       </c>
       <c r="F50" s="13">
-        <v>160.27000000000001</v>
+        <v>159.87</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>167.15</v>
+        <v>167.21</v>
       </c>
       <c r="E54" s="10">
-        <v>163.43</v>
+        <v>163.6</v>
       </c>
       <c r="F54" s="10">
-        <v>173.43</v>
+        <v>173.6</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>160.29</v>
+        <v>160.38</v>
       </c>
       <c r="E55" s="13">
-        <v>162.57</v>
+        <v>162.68</v>
       </c>
       <c r="F55" s="13">
-        <v>172.57</v>
+        <v>172.68</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>156.77000000000001</v>
+        <v>156.72999999999999</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>157.44</v>
+        <v>157.38999999999999</v>
       </c>
       <c r="E57" s="13">
-        <v>156.99</v>
+        <v>157.1</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>153.21</v>
+        <v>153.15</v>
       </c>
       <c r="E58" s="10">
-        <v>152.88999999999999</v>
+        <v>153</v>
       </c>
       <c r="F58" s="10">
-        <v>162.88999999999999</v>
+        <v>163</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>159.62</v>
+        <v>159.66999999999999</v>
       </c>
       <c r="E59" s="13">
-        <v>161.85</v>
+        <v>161.99</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>167.41</v>
+        <v>167.15</v>
       </c>
       <c r="E60" s="10">
-        <v>163.47999999999999</v>
+        <v>163.43</v>
       </c>
       <c r="F60" s="10">
-        <v>173.48</v>
+        <v>173.43</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>160.54</v>
+        <v>160.29</v>
       </c>
       <c r="E61" s="13">
-        <v>162.44</v>
+        <v>162.57</v>
       </c>
       <c r="F61" s="13">
-        <v>172.44</v>
+        <v>172.57</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>157.03</v>
+        <v>156.77000000000001</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>157.72</v>
+        <v>157.44</v>
       </c>
       <c r="E63" s="13">
-        <v>156.87</v>
+        <v>156.99</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>153.47999999999999</v>
+        <v>153.21</v>
       </c>
       <c r="E64" s="10">
-        <v>152.76</v>
+        <v>152.88999999999999</v>
       </c>
       <c r="F64" s="10">
-        <v>162.76</v>
+        <v>162.88999999999999</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46031</v>
+        <v>46032</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>159.88999999999999</v>
+        <v>159.62</v>
       </c>
       <c r="E65" s="13">
-        <v>161.91</v>
+        <v>161.85</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -2115,6 +2115,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
@@ -2123,15 +2132,6 @@
     <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2155,6 +2155,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2172,14 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Tue Jan 13 03:08:38 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{81128FA1-9593-4B01-8BBA-E53CE420BD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5DDB2C50-D19E-46EA-ABA4-9BF71A8A48B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.46484375"/>
+    <col min="2" max="2" width="6.42578125"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.91999999999999</v>
+        <v>153.29</v>
       </c>
       <c r="E8" s="10">
-        <v>149.5</v>
+        <v>149.81</v>
       </c>
       <c r="F8" s="10">
-        <v>159.5</v>
+        <v>159.81</v>
       </c>
       <c r="G8" s="10">
-        <v>149.52000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.83000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.91999999999999</v>
+        <v>153.29</v>
       </c>
       <c r="E9" s="13">
-        <v>149.5</v>
+        <v>149.81</v>
       </c>
       <c r="F9" s="13">
-        <v>159.5</v>
+        <v>159.81</v>
       </c>
       <c r="G9" s="13">
-        <v>149.52000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.83000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.04</v>
+        <v>154.4</v>
       </c>
       <c r="E10" s="10">
-        <v>151.15</v>
+        <v>151.43</v>
       </c>
       <c r="F10" s="10">
-        <v>161.15</v>
+        <v>161.43</v>
       </c>
       <c r="G10" s="10">
-        <v>151.55000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.83000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.83000000000001</v>
+        <v>152.91999999999999</v>
       </c>
       <c r="E11" s="13">
-        <v>149.25</v>
+        <v>149.5</v>
       </c>
       <c r="F11" s="13">
-        <v>159.25</v>
+        <v>159.5</v>
       </c>
       <c r="G11" s="13">
-        <v>149.27000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.52000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.83000000000001</v>
+        <v>152.91999999999999</v>
       </c>
       <c r="E12" s="10">
-        <v>149.25</v>
+        <v>149.5</v>
       </c>
       <c r="F12" s="10">
-        <v>159.25</v>
+        <v>159.5</v>
       </c>
       <c r="G12" s="10">
-        <v>149.27000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>149.52000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>153.76</v>
+        <v>154.04</v>
       </c>
       <c r="E13" s="13">
-        <v>150.69999999999999</v>
+        <v>151.15</v>
       </c>
       <c r="F13" s="13">
-        <v>160.69999999999999</v>
+        <v>161.15</v>
       </c>
       <c r="G13" s="13">
-        <v>151.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.55000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>157.32</v>
+        <v>157.66</v>
       </c>
       <c r="E17" s="10">
-        <v>153.83000000000001</v>
+        <v>154.11000000000001</v>
       </c>
       <c r="F17" s="10">
-        <v>163.83000000000001</v>
+        <v>164.11</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>157.26</v>
+        <v>157.32</v>
       </c>
       <c r="E18" s="13">
-        <v>153.72</v>
+        <v>153.83000000000001</v>
       </c>
       <c r="F18" s="13">
-        <v>163.72</v>
+        <v>163.83000000000001</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>153.88</v>
+        <v>154.26</v>
       </c>
       <c r="E22" s="10">
-        <v>150.63999999999999</v>
+        <v>150.94</v>
       </c>
       <c r="F22" s="10">
-        <v>160.24</v>
+        <v>160.54</v>
       </c>
       <c r="G22" s="10">
-        <v>151.71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>152.02000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.46</v>
+        <v>158.82</v>
       </c>
       <c r="E23" s="13">
-        <v>156.49</v>
+        <v>156.77000000000001</v>
       </c>
       <c r="F23" s="13">
-        <v>166.49</v>
+        <v>166.77</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.62</v>
+        <v>158.97999999999999</v>
       </c>
       <c r="E24" s="10">
-        <v>157.12</v>
+        <v>157.41</v>
       </c>
       <c r="F24" s="10">
-        <v>167.12</v>
+        <v>167.41</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.61000000000001</v>
+        <v>158.96</v>
       </c>
       <c r="E25" s="13">
-        <v>156.63999999999999</v>
+        <v>156.93</v>
       </c>
       <c r="F25" s="13">
-        <v>166.64</v>
+        <v>166.93</v>
       </c>
       <c r="G25" s="13">
-        <v>156.77000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>157.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.24</v>
+        <v>158.59</v>
       </c>
       <c r="E26" s="10">
-        <v>158.25</v>
+        <v>158.54</v>
       </c>
       <c r="F26" s="10">
-        <v>168.25</v>
+        <v>168.54</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.69</v>
+        <v>153.88</v>
       </c>
       <c r="E27" s="13">
-        <v>150.5</v>
+        <v>150.63999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>160.1</v>
+        <v>160.24</v>
       </c>
       <c r="G27" s="13">
-        <v>151.57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>151.71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.28</v>
+        <v>158.46</v>
       </c>
       <c r="E28" s="22">
-        <v>156.15</v>
+        <v>156.49</v>
       </c>
       <c r="F28" s="22">
-        <v>166.15</v>
+        <v>166.49</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.44</v>
+        <v>158.62</v>
       </c>
       <c r="E29" s="13">
-        <v>156.78</v>
+        <v>157.12</v>
       </c>
       <c r="F29" s="13">
-        <v>166.78</v>
+        <v>167.12</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.43</v>
+        <v>158.61000000000001</v>
       </c>
       <c r="E30" s="22">
-        <v>156.29</v>
+        <v>156.63999999999999</v>
       </c>
       <c r="F30" s="22">
-        <v>166.29</v>
+        <v>166.64</v>
       </c>
       <c r="G30" s="22">
-        <v>156.41999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>156.77000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.07</v>
+        <v>158.24</v>
       </c>
       <c r="E31" s="13">
-        <v>157.9</v>
+        <v>158.25</v>
       </c>
       <c r="F31" s="13">
-        <v>167.9</v>
+        <v>168.25</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.49</v>
+        <v>152.84</v>
       </c>
       <c r="E35" s="10">
-        <v>148.13999999999999</v>
+        <v>148.41999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>157.13999999999999</v>
+        <v>157.41999999999999</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.09</v>
+        <v>152.49</v>
       </c>
       <c r="E36" s="13">
-        <v>148.01</v>
+        <v>148.13999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>157.01</v>
+        <v>157.13999999999999</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>157.97999999999999</v>
+        <v>158.34</v>
       </c>
       <c r="E40" s="10">
-        <v>156.43</v>
+        <v>156.74</v>
       </c>
       <c r="F40" s="10">
-        <v>166.43</v>
+        <v>166.74</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>157.71</v>
+        <v>158.06</v>
       </c>
       <c r="E41" s="13">
-        <v>156.85</v>
+        <v>157.16</v>
       </c>
       <c r="F41" s="13">
-        <v>166.85</v>
+        <v>167.16</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>157.91</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="E42" s="10">
-        <v>156.32</v>
+        <v>156.43</v>
       </c>
       <c r="F42" s="10">
-        <v>166.32</v>
+        <v>166.43</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>157.63</v>
+        <v>157.71</v>
       </c>
       <c r="E43" s="13">
-        <v>156.74</v>
+        <v>156.85</v>
       </c>
       <c r="F43" s="13">
-        <v>166.74</v>
+        <v>166.85</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.56</v>
+        <v>152.82</v>
       </c>
       <c r="E47" s="10">
-        <v>149.85</v>
+        <v>150.05000000000001</v>
       </c>
       <c r="F47" s="10">
-        <v>159.85</v>
+        <v>160.05000000000001</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.19999999999999</v>
+        <v>152.46</v>
       </c>
       <c r="E48" s="13">
-        <v>149.79</v>
+        <v>149.97999999999999</v>
       </c>
       <c r="F48" s="13">
-        <v>159.79</v>
+        <v>159.97999999999999</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.62</v>
+        <v>152.56</v>
       </c>
       <c r="E49" s="10">
-        <v>149.93</v>
+        <v>149.85</v>
       </c>
       <c r="F49" s="10">
-        <v>159.93</v>
+        <v>159.85</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.26</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="E50" s="13">
-        <v>149.87</v>
+        <v>149.79</v>
       </c>
       <c r="F50" s="13">
-        <v>159.87</v>
+        <v>159.79</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>167.21</v>
+        <v>167.56</v>
       </c>
       <c r="E54" s="10">
-        <v>163.6</v>
+        <v>163.92</v>
       </c>
       <c r="F54" s="10">
-        <v>173.6</v>
+        <v>173.92</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>160.38</v>
+        <v>160.74</v>
       </c>
       <c r="E55" s="13">
-        <v>162.68</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="F55" s="13">
-        <v>172.68</v>
+        <v>172.95</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>156.72999999999999</v>
+        <v>156.97999999999999</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>157.38999999999999</v>
+        <v>157.62</v>
       </c>
       <c r="E57" s="13">
-        <v>157.1</v>
+        <v>157.37</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>153.15</v>
+        <v>153.38999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>153</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>163</v>
+        <v>163.27000000000001</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>159.66999999999999</v>
+        <v>160.02000000000001</v>
       </c>
       <c r="E59" s="13">
-        <v>161.99</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>167.15</v>
+        <v>167.21</v>
       </c>
       <c r="E60" s="10">
-        <v>163.43</v>
+        <v>163.6</v>
       </c>
       <c r="F60" s="10">
-        <v>173.43</v>
+        <v>173.6</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>160.29</v>
+        <v>160.38</v>
       </c>
       <c r="E61" s="13">
-        <v>162.57</v>
+        <v>162.68</v>
       </c>
       <c r="F61" s="13">
-        <v>172.57</v>
+        <v>172.68</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>156.77000000000001</v>
+        <v>156.72999999999999</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>157.44</v>
+        <v>157.38999999999999</v>
       </c>
       <c r="E63" s="13">
-        <v>156.99</v>
+        <v>157.1</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>153.21</v>
+        <v>153.15</v>
       </c>
       <c r="E64" s="10">
-        <v>152.88999999999999</v>
+        <v>153</v>
       </c>
       <c r="F64" s="10">
-        <v>162.88999999999999</v>
+        <v>163</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>159.62</v>
+        <v>159.66999999999999</v>
       </c>
       <c r="E65" s="13">
-        <v>161.85</v>
+        <v>161.99</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,6 +1855,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2114,27 +2134,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2154,32 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Wed Jan 14 03:15:56 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5DDB2C50-D19E-46EA-ABA4-9BF71A8A48B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{48EBF6DC-BB15-46D7-9C9B-615175E3F7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>153.29</v>
+        <v>152.66999999999999</v>
       </c>
       <c r="E8" s="10">
-        <v>149.81</v>
+        <v>149.22</v>
       </c>
       <c r="F8" s="10">
-        <v>159.81</v>
+        <v>159.22</v>
       </c>
       <c r="G8" s="10">
-        <v>149.83000000000001</v>
+        <v>149.22999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>153.29</v>
+        <v>152.66999999999999</v>
       </c>
       <c r="E9" s="13">
-        <v>149.81</v>
+        <v>149.22</v>
       </c>
       <c r="F9" s="13">
-        <v>159.81</v>
+        <v>159.22</v>
       </c>
       <c r="G9" s="13">
-        <v>149.83000000000001</v>
+        <v>149.22999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.4</v>
+        <v>154.32</v>
       </c>
       <c r="E10" s="10">
-        <v>151.43</v>
+        <v>151.72</v>
       </c>
       <c r="F10" s="10">
-        <v>161.43</v>
+        <v>161.72</v>
       </c>
       <c r="G10" s="10">
-        <v>151.83000000000001</v>
+        <v>152.12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.91999999999999</v>
+        <v>153.29</v>
       </c>
       <c r="E11" s="13">
-        <v>149.5</v>
+        <v>149.81</v>
       </c>
       <c r="F11" s="13">
-        <v>159.5</v>
+        <v>159.81</v>
       </c>
       <c r="G11" s="13">
-        <v>149.52000000000001</v>
+        <v>149.83000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.91999999999999</v>
+        <v>153.29</v>
       </c>
       <c r="E12" s="10">
-        <v>149.5</v>
+        <v>149.81</v>
       </c>
       <c r="F12" s="10">
-        <v>159.5</v>
+        <v>159.81</v>
       </c>
       <c r="G12" s="10">
-        <v>149.52000000000001</v>
+        <v>149.83000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.04</v>
+        <v>154.4</v>
       </c>
       <c r="E13" s="13">
-        <v>151.15</v>
+        <v>151.43</v>
       </c>
       <c r="F13" s="13">
-        <v>161.15</v>
+        <v>161.43</v>
       </c>
       <c r="G13" s="13">
-        <v>151.55000000000001</v>
+        <v>151.83000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>157.66</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="E17" s="10">
-        <v>154.11000000000001</v>
+        <v>154.37</v>
       </c>
       <c r="F17" s="10">
-        <v>164.11</v>
+        <v>164.37</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>157.32</v>
+        <v>157.66</v>
       </c>
       <c r="E18" s="13">
-        <v>153.83000000000001</v>
+        <v>154.11000000000001</v>
       </c>
       <c r="F18" s="13">
-        <v>163.83000000000001</v>
+        <v>164.11</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>154.26</v>
+        <v>154.08000000000001</v>
       </c>
       <c r="E22" s="10">
-        <v>150.94</v>
+        <v>151.22999999999999</v>
       </c>
       <c r="F22" s="10">
-        <v>160.54</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="G22" s="10">
-        <v>152.02000000000001</v>
+        <v>152.30000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>158.82</v>
+        <v>159.29</v>
       </c>
       <c r="E23" s="13">
-        <v>156.77000000000001</v>
+        <v>157.06</v>
       </c>
       <c r="F23" s="13">
-        <v>166.77</v>
+        <v>167.06</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>158.97999999999999</v>
+        <v>159.44999999999999</v>
       </c>
       <c r="E24" s="10">
-        <v>157.41</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F24" s="10">
-        <v>167.41</v>
+        <v>167.7</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>158.96</v>
+        <v>159.43</v>
       </c>
       <c r="E25" s="13">
-        <v>156.93</v>
+        <v>157.22999999999999</v>
       </c>
       <c r="F25" s="13">
-        <v>166.93</v>
+        <v>167.23</v>
       </c>
       <c r="G25" s="13">
-        <v>157.06</v>
+        <v>157.36000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>158.59</v>
+        <v>159.06</v>
       </c>
       <c r="E26" s="10">
-        <v>158.54</v>
+        <v>158.84</v>
       </c>
       <c r="F26" s="10">
-        <v>168.54</v>
+        <v>168.84</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>153.88</v>
+        <v>154.26</v>
       </c>
       <c r="E27" s="13">
-        <v>150.63999999999999</v>
+        <v>150.94</v>
       </c>
       <c r="F27" s="13">
-        <v>160.24</v>
+        <v>160.54</v>
       </c>
       <c r="G27" s="13">
-        <v>151.71</v>
+        <v>152.02000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.46</v>
+        <v>158.82</v>
       </c>
       <c r="E28" s="22">
-        <v>156.49</v>
+        <v>156.77000000000001</v>
       </c>
       <c r="F28" s="22">
-        <v>166.49</v>
+        <v>166.77</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.62</v>
+        <v>158.97999999999999</v>
       </c>
       <c r="E29" s="13">
-        <v>157.12</v>
+        <v>157.41</v>
       </c>
       <c r="F29" s="13">
-        <v>167.12</v>
+        <v>167.41</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.61000000000001</v>
+        <v>158.96</v>
       </c>
       <c r="E30" s="22">
-        <v>156.63999999999999</v>
+        <v>156.93</v>
       </c>
       <c r="F30" s="22">
-        <v>166.64</v>
+        <v>166.93</v>
       </c>
       <c r="G30" s="22">
-        <v>156.77000000000001</v>
+        <v>157.06</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.24</v>
+        <v>158.59</v>
       </c>
       <c r="E31" s="13">
-        <v>158.25</v>
+        <v>158.54</v>
       </c>
       <c r="F31" s="13">
-        <v>168.25</v>
+        <v>168.54</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.84</v>
+        <v>152.21</v>
       </c>
       <c r="E35" s="10">
-        <v>148.41999999999999</v>
+        <v>148.69999999999999</v>
       </c>
       <c r="F35" s="10">
-        <v>157.41999999999999</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.49</v>
+        <v>152.84</v>
       </c>
       <c r="E36" s="13">
-        <v>148.13999999999999</v>
+        <v>148.41999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>157.13999999999999</v>
+        <v>157.41999999999999</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>158.34</v>
+        <v>158.84</v>
       </c>
       <c r="E40" s="10">
-        <v>156.74</v>
+        <v>157.1</v>
       </c>
       <c r="F40" s="10">
-        <v>166.74</v>
+        <v>167.1</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>158.06</v>
+        <v>158.56</v>
       </c>
       <c r="E41" s="13">
-        <v>157.16</v>
+        <v>157.52000000000001</v>
       </c>
       <c r="F41" s="13">
-        <v>167.16</v>
+        <v>167.52</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>157.97999999999999</v>
+        <v>158.34</v>
       </c>
       <c r="E42" s="10">
-        <v>156.43</v>
+        <v>156.74</v>
       </c>
       <c r="F42" s="10">
-        <v>166.43</v>
+        <v>166.74</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>157.71</v>
+        <v>158.06</v>
       </c>
       <c r="E43" s="13">
-        <v>156.85</v>
+        <v>157.16</v>
       </c>
       <c r="F43" s="13">
-        <v>166.85</v>
+        <v>167.16</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.82</v>
+        <v>152.34</v>
       </c>
       <c r="E47" s="10">
-        <v>150.05000000000001</v>
+        <v>150.18</v>
       </c>
       <c r="F47" s="10">
-        <v>160.05000000000001</v>
+        <v>160.18</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.46</v>
+        <v>151.97</v>
       </c>
       <c r="E48" s="13">
-        <v>149.97999999999999</v>
+        <v>150.11000000000001</v>
       </c>
       <c r="F48" s="13">
-        <v>159.97999999999999</v>
+        <v>160.11000000000001</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.56</v>
+        <v>152.82</v>
       </c>
       <c r="E49" s="10">
-        <v>149.85</v>
+        <v>150.05000000000001</v>
       </c>
       <c r="F49" s="10">
-        <v>159.85</v>
+        <v>160.05000000000001</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.19999999999999</v>
+        <v>152.46</v>
       </c>
       <c r="E50" s="13">
-        <v>149.79</v>
+        <v>149.97999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>159.79</v>
+        <v>159.97999999999999</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>167.56</v>
+        <v>168.03</v>
       </c>
       <c r="E54" s="10">
-        <v>163.92</v>
+        <v>164.32</v>
       </c>
       <c r="F54" s="10">
-        <v>173.92</v>
+        <v>174.32</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>160.74</v>
+        <v>160.49</v>
       </c>
       <c r="E55" s="13">
-        <v>162.94999999999999</v>
+        <v>162.44</v>
       </c>
       <c r="F55" s="13">
-        <v>172.95</v>
+        <v>172.44</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>156.97999999999999</v>
+        <v>156.91</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>157.62</v>
+        <v>157.51</v>
       </c>
       <c r="E57" s="13">
-        <v>157.37</v>
+        <v>156.86000000000001</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>153.38999999999999</v>
+        <v>153.28</v>
       </c>
       <c r="E58" s="10">
-        <v>153.27000000000001</v>
+        <v>152.76</v>
       </c>
       <c r="F58" s="10">
-        <v>163.27000000000001</v>
+        <v>162.76</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>160.02000000000001</v>
+        <v>160.46</v>
       </c>
       <c r="E59" s="13">
-        <v>162.30000000000001</v>
+        <v>162.65</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>167.21</v>
+        <v>167.56</v>
       </c>
       <c r="E60" s="10">
-        <v>163.6</v>
+        <v>163.92</v>
       </c>
       <c r="F60" s="10">
-        <v>173.6</v>
+        <v>173.92</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>160.38</v>
+        <v>160.74</v>
       </c>
       <c r="E61" s="13">
-        <v>162.68</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="F61" s="13">
-        <v>172.68</v>
+        <v>172.95</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>156.72999999999999</v>
+        <v>156.97999999999999</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>157.38999999999999</v>
+        <v>157.62</v>
       </c>
       <c r="E63" s="13">
-        <v>157.1</v>
+        <v>157.37</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>153.15</v>
+        <v>153.38999999999999</v>
       </c>
       <c r="E64" s="10">
-        <v>153</v>
+        <v>153.27000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>163</v>
+        <v>163.27000000000001</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>159.66999999999999</v>
+        <v>160.02000000000001</v>
       </c>
       <c r="E65" s="13">
-        <v>161.99</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Thu Jan 15 03:11:04 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{48EBF6DC-BB15-46D7-9C9B-615175E3F7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5CD28510-F1DD-4A25-BEEA-857DEC5F7BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>152.66999999999999</v>
+        <v>154.25</v>
       </c>
       <c r="E8" s="10">
-        <v>149.22</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F8" s="10">
-        <v>159.22</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G8" s="10">
-        <v>149.22999999999999</v>
+        <v>150.1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>152.66999999999999</v>
+        <v>154.25</v>
       </c>
       <c r="E9" s="13">
-        <v>149.22</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F9" s="13">
-        <v>159.22</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G9" s="13">
-        <v>149.22999999999999</v>
+        <v>150.1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>154.32</v>
+        <v>155.62</v>
       </c>
       <c r="E10" s="10">
-        <v>151.72</v>
+        <v>152.53</v>
       </c>
       <c r="F10" s="10">
-        <v>161.72</v>
+        <v>162.53</v>
       </c>
       <c r="G10" s="10">
-        <v>152.12</v>
+        <v>152.93</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>153.29</v>
+        <v>152.66999999999999</v>
       </c>
       <c r="E11" s="13">
-        <v>149.81</v>
+        <v>149.22</v>
       </c>
       <c r="F11" s="13">
-        <v>159.81</v>
+        <v>159.22</v>
       </c>
       <c r="G11" s="13">
-        <v>149.83000000000001</v>
+        <v>149.22999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>153.29</v>
+        <v>152.66999999999999</v>
       </c>
       <c r="E12" s="10">
-        <v>149.81</v>
+        <v>149.22</v>
       </c>
       <c r="F12" s="10">
-        <v>159.81</v>
+        <v>159.22</v>
       </c>
       <c r="G12" s="10">
-        <v>149.83000000000001</v>
+        <v>149.22999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.4</v>
+        <v>154.32</v>
       </c>
       <c r="E13" s="13">
-        <v>151.43</v>
+        <v>151.72</v>
       </c>
       <c r="F13" s="13">
-        <v>161.43</v>
+        <v>161.72</v>
       </c>
       <c r="G13" s="13">
-        <v>151.83000000000001</v>
+        <v>152.12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>158.11000000000001</v>
+        <v>159.38</v>
       </c>
       <c r="E17" s="10">
-        <v>154.37</v>
+        <v>155.16</v>
       </c>
       <c r="F17" s="10">
-        <v>164.37</v>
+        <v>165.16</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>157.66</v>
+        <v>158.11000000000001</v>
       </c>
       <c r="E18" s="13">
-        <v>154.11000000000001</v>
+        <v>154.37</v>
       </c>
       <c r="F18" s="13">
-        <v>164.11</v>
+        <v>164.37</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>154.08000000000001</v>
+        <v>155.66</v>
       </c>
       <c r="E22" s="10">
-        <v>151.22999999999999</v>
+        <v>152.09</v>
       </c>
       <c r="F22" s="10">
-        <v>160.83000000000001</v>
+        <v>161.69</v>
       </c>
       <c r="G22" s="10">
-        <v>152.30000000000001</v>
+        <v>153.16999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>159.29</v>
+        <v>160.6</v>
       </c>
       <c r="E23" s="13">
-        <v>157.06</v>
+        <v>157.87</v>
       </c>
       <c r="F23" s="13">
-        <v>167.06</v>
+        <v>167.87</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>159.44999999999999</v>
+        <v>160.75</v>
       </c>
       <c r="E24" s="10">
-        <v>157.69999999999999</v>
+        <v>158.53</v>
       </c>
       <c r="F24" s="10">
-        <v>167.7</v>
+        <v>168.53</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>159.43</v>
+        <v>160.72999999999999</v>
       </c>
       <c r="E25" s="13">
-        <v>157.22999999999999</v>
+        <v>158.05000000000001</v>
       </c>
       <c r="F25" s="13">
-        <v>167.23</v>
+        <v>168.05</v>
       </c>
       <c r="G25" s="13">
-        <v>157.36000000000001</v>
+        <v>158.18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>159.06</v>
+        <v>160.35</v>
       </c>
       <c r="E26" s="10">
-        <v>158.84</v>
+        <v>159.66999999999999</v>
       </c>
       <c r="F26" s="10">
-        <v>168.84</v>
+        <v>169.67</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>154.26</v>
+        <v>154.08000000000001</v>
       </c>
       <c r="E27" s="13">
-        <v>150.94</v>
+        <v>151.22999999999999</v>
       </c>
       <c r="F27" s="13">
-        <v>160.54</v>
+        <v>160.83000000000001</v>
       </c>
       <c r="G27" s="13">
-        <v>152.02000000000001</v>
+        <v>152.30000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>158.82</v>
+        <v>159.29</v>
       </c>
       <c r="E28" s="22">
-        <v>156.77000000000001</v>
+        <v>157.06</v>
       </c>
       <c r="F28" s="22">
-        <v>166.77</v>
+        <v>167.06</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>158.97999999999999</v>
+        <v>159.44999999999999</v>
       </c>
       <c r="E29" s="13">
-        <v>157.41</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="F29" s="13">
-        <v>167.41</v>
+        <v>167.7</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>158.96</v>
+        <v>159.43</v>
       </c>
       <c r="E30" s="22">
-        <v>156.93</v>
+        <v>157.22999999999999</v>
       </c>
       <c r="F30" s="22">
-        <v>166.93</v>
+        <v>167.23</v>
       </c>
       <c r="G30" s="22">
-        <v>157.06</v>
+        <v>157.36000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>158.59</v>
+        <v>159.06</v>
       </c>
       <c r="E31" s="13">
-        <v>158.54</v>
+        <v>158.84</v>
       </c>
       <c r="F31" s="13">
-        <v>168.54</v>
+        <v>168.84</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>152.21</v>
+        <v>154.06</v>
       </c>
       <c r="E35" s="10">
-        <v>148.69999999999999</v>
+        <v>149.51</v>
       </c>
       <c r="F35" s="10">
-        <v>157.69999999999999</v>
+        <v>158.51</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.84</v>
+        <v>152.21</v>
       </c>
       <c r="E36" s="13">
-        <v>148.41999999999999</v>
+        <v>148.69999999999999</v>
       </c>
       <c r="F36" s="13">
-        <v>157.41999999999999</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>158.84</v>
+        <v>160.16</v>
       </c>
       <c r="E40" s="10">
-        <v>157.1</v>
+        <v>157.82</v>
       </c>
       <c r="F40" s="10">
-        <v>167.1</v>
+        <v>167.82</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>158.56</v>
+        <v>159.88</v>
       </c>
       <c r="E41" s="13">
-        <v>157.52000000000001</v>
+        <v>158.24</v>
       </c>
       <c r="F41" s="13">
-        <v>167.52</v>
+        <v>168.24</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>158.34</v>
+        <v>158.84</v>
       </c>
       <c r="E42" s="10">
-        <v>156.74</v>
+        <v>157.1</v>
       </c>
       <c r="F42" s="10">
-        <v>166.74</v>
+        <v>167.1</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>158.06</v>
+        <v>158.56</v>
       </c>
       <c r="E43" s="13">
-        <v>157.16</v>
+        <v>157.52000000000001</v>
       </c>
       <c r="F43" s="13">
-        <v>167.16</v>
+        <v>167.52</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>152.34</v>
+        <v>153.09</v>
       </c>
       <c r="E47" s="10">
-        <v>150.18</v>
+        <v>150.47</v>
       </c>
       <c r="F47" s="10">
-        <v>160.18</v>
+        <v>160.47</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>151.97</v>
+        <v>152.72</v>
       </c>
       <c r="E48" s="13">
-        <v>150.11000000000001</v>
+        <v>150.41</v>
       </c>
       <c r="F48" s="13">
-        <v>160.11000000000001</v>
+        <v>160.41</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.82</v>
+        <v>152.34</v>
       </c>
       <c r="E49" s="10">
-        <v>150.05000000000001</v>
+        <v>150.18</v>
       </c>
       <c r="F49" s="10">
-        <v>160.05000000000001</v>
+        <v>160.18</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.46</v>
+        <v>151.97</v>
       </c>
       <c r="E50" s="13">
-        <v>149.97999999999999</v>
+        <v>150.11000000000001</v>
       </c>
       <c r="F50" s="13">
-        <v>159.97999999999999</v>
+        <v>160.11000000000001</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>168.03</v>
+        <v>169.33</v>
       </c>
       <c r="E54" s="10">
-        <v>164.32</v>
+        <v>165.24</v>
       </c>
       <c r="F54" s="10">
-        <v>174.32</v>
+        <v>175.24</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>160.49</v>
+        <v>161.84</v>
       </c>
       <c r="E55" s="13">
-        <v>162.44</v>
+        <v>163.55000000000001</v>
       </c>
       <c r="F55" s="13">
-        <v>172.44</v>
+        <v>173.55</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>156.91</v>
+        <v>158.54</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>157.51</v>
+        <v>159.1</v>
       </c>
       <c r="E57" s="13">
-        <v>156.86000000000001</v>
+        <v>157.97</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>153.28</v>
+        <v>154.87</v>
       </c>
       <c r="E58" s="10">
-        <v>152.76</v>
+        <v>153.87</v>
       </c>
       <c r="F58" s="10">
-        <v>162.76</v>
+        <v>163.87</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>160.46</v>
+        <v>161.72</v>
       </c>
       <c r="E59" s="13">
-        <v>162.65</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>167.56</v>
+        <v>168.03</v>
       </c>
       <c r="E60" s="10">
-        <v>163.92</v>
+        <v>164.32</v>
       </c>
       <c r="F60" s="10">
-        <v>173.92</v>
+        <v>174.32</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>160.74</v>
+        <v>160.49</v>
       </c>
       <c r="E61" s="13">
-        <v>162.94999999999999</v>
+        <v>162.44</v>
       </c>
       <c r="F61" s="13">
-        <v>172.95</v>
+        <v>172.44</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>156.97999999999999</v>
+        <v>156.91</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>157.62</v>
+        <v>157.51</v>
       </c>
       <c r="E63" s="13">
-        <v>157.37</v>
+        <v>156.86000000000001</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>153.38999999999999</v>
+        <v>153.28</v>
       </c>
       <c r="E64" s="10">
-        <v>153.27000000000001</v>
+        <v>152.76</v>
       </c>
       <c r="F64" s="10">
-        <v>163.27000000000001</v>
+        <v>162.76</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>160.02000000000001</v>
+        <v>160.46</v>
       </c>
       <c r="E65" s="13">
-        <v>162.30000000000001</v>
+        <v>162.65</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>
@@ -1855,17 +1855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1874,7 +1863,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3632DF5622958439304627C030B0427" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c2ecbce386d6bac497f8eb2d8f0fb7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87276d81-85f4-4ef2-9e6e-55066304288f" xmlns:ns3="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad" xmlns:ns4="b23b8984-eafa-4e79-985e-54f52f3da58e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cfd0c2f651c1ce156ad4fcb44ea61dd" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="87276d81-85f4-4ef2-9e6e-55066304288f"/>
@@ -2134,25 +2123,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
-    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87276d81-85f4-4ef2-9e6e-55066304288f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b23b8984-eafa-4e79-985e-54f52f3da58e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60519E9-FD90-4339-869C-BC2F85719BB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2160,7 +2142,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44E1863-2778-41F9-ACBA-48420F931671}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,6 +2162,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57A83D98-2BAE-4D83-823A-D31C464B620C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b23b8984-eafa-4e79-985e-54f52f3da58e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39e1dda6-d1d8-4c88-a3b9-f1abc1284bad"/>
+    <ds:schemaRef ds:uri="87276d81-85f4-4ef2-9e6e-55066304288f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{569bf4a9-87bd-4dbf-a36c-1db5158e5def}" enabled="1" method="Privileged" siteId="{ea80952e-a476-42d4-aaf4-5457852b0f7e}" removed="0"/>

</xml_diff>

<commit_message>
Fri Jan 16 03:10:55 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5CD28510-F1DD-4A25-BEEA-857DEC5F7BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{CD2AC9F3-A42B-4658-BEFA-A266F84FA416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125"/>
+    <col min="2" max="2" width="6.3984375"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="22.15" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -742,7 +742,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -773,7 +773,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,133 +805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>154.25</v>
+        <v>156.03</v>
       </c>
       <c r="E8" s="10">
-        <v>150.08000000000001</v>
+        <v>150.84</v>
       </c>
       <c r="F8" s="10">
-        <v>160.08000000000001</v>
+        <v>160.84</v>
       </c>
       <c r="G8" s="10">
-        <v>150.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>154.25</v>
+        <v>156.03</v>
       </c>
       <c r="E9" s="13">
-        <v>150.08000000000001</v>
+        <v>150.84</v>
       </c>
       <c r="F9" s="13">
-        <v>160.08000000000001</v>
+        <v>160.84</v>
       </c>
       <c r="G9" s="13">
-        <v>150.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>155.62</v>
+        <v>157.01</v>
       </c>
       <c r="E10" s="10">
-        <v>152.53</v>
+        <v>153.01</v>
       </c>
       <c r="F10" s="10">
-        <v>162.53</v>
+        <v>163.01</v>
       </c>
       <c r="G10" s="10">
-        <v>152.93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153.41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>152.66999999999999</v>
+        <v>154.25</v>
       </c>
       <c r="E11" s="13">
-        <v>149.22</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F11" s="13">
-        <v>159.22</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G11" s="13">
-        <v>149.22999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>152.66999999999999</v>
+        <v>154.25</v>
       </c>
       <c r="E12" s="10">
-        <v>149.22</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="F12" s="10">
-        <v>159.22</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G12" s="10">
-        <v>149.22999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>154.32</v>
+        <v>155.62</v>
       </c>
       <c r="E13" s="13">
-        <v>151.72</v>
+        <v>152.53</v>
       </c>
       <c r="F13" s="13">
-        <v>161.72</v>
+        <v>162.53</v>
       </c>
       <c r="G13" s="13">
-        <v>152.12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152.93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -940,7 +940,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>13</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -970,45 +970,45 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>159.38</v>
+        <v>160.51</v>
       </c>
       <c r="E17" s="10">
-        <v>155.16</v>
+        <v>155.6</v>
       </c>
       <c r="F17" s="10">
-        <v>165.16</v>
+        <v>165.6</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>158.11000000000001</v>
+        <v>159.38</v>
       </c>
       <c r="E18" s="13">
-        <v>154.37</v>
+        <v>155.16</v>
       </c>
       <c r="F18" s="13">
-        <v>164.37</v>
+        <v>165.16</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1017,7 +1017,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,217 +1049,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>155.66</v>
+        <v>157.11000000000001</v>
       </c>
       <c r="E22" s="10">
-        <v>152.09</v>
+        <v>152.63</v>
       </c>
       <c r="F22" s="10">
-        <v>161.69</v>
+        <v>162.22999999999999</v>
       </c>
       <c r="G22" s="10">
-        <v>153.16999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153.69999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>160.6</v>
+        <v>161.78</v>
       </c>
       <c r="E23" s="13">
-        <v>157.87</v>
+        <v>158.35</v>
       </c>
       <c r="F23" s="13">
-        <v>167.87</v>
+        <v>168.35</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>160.75</v>
+        <v>161.91999999999999</v>
       </c>
       <c r="E24" s="10">
-        <v>158.53</v>
+        <v>159.02000000000001</v>
       </c>
       <c r="F24" s="10">
-        <v>168.53</v>
+        <v>169.02</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>160.72999999999999</v>
+        <v>161.9</v>
       </c>
       <c r="E25" s="13">
-        <v>158.05000000000001</v>
+        <v>158.56</v>
       </c>
       <c r="F25" s="13">
-        <v>168.05</v>
+        <v>168.56</v>
       </c>
       <c r="G25" s="13">
-        <v>158.18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>160.35</v>
+        <v>161.51</v>
       </c>
       <c r="E26" s="10">
-        <v>159.66999999999999</v>
+        <v>160.18</v>
       </c>
       <c r="F26" s="10">
-        <v>169.67</v>
+        <v>170.18</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>154.08000000000001</v>
+        <v>155.66</v>
       </c>
       <c r="E27" s="13">
-        <v>151.22999999999999</v>
+        <v>152.09</v>
       </c>
       <c r="F27" s="13">
-        <v>160.83000000000001</v>
+        <v>161.69</v>
       </c>
       <c r="G27" s="13">
-        <v>152.30000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153.16999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>159.29</v>
+        <v>160.6</v>
       </c>
       <c r="E28" s="22">
-        <v>157.06</v>
+        <v>157.87</v>
       </c>
       <c r="F28" s="22">
-        <v>167.06</v>
+        <v>167.87</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>159.44999999999999</v>
+        <v>160.75</v>
       </c>
       <c r="E29" s="13">
-        <v>157.69999999999999</v>
+        <v>158.53</v>
       </c>
       <c r="F29" s="13">
-        <v>167.7</v>
+        <v>168.53</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>159.43</v>
+        <v>160.72999999999999</v>
       </c>
       <c r="E30" s="22">
-        <v>157.22999999999999</v>
+        <v>158.05000000000001</v>
       </c>
       <c r="F30" s="22">
-        <v>167.23</v>
+        <v>168.05</v>
       </c>
       <c r="G30" s="22">
-        <v>157.36000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>159.06</v>
+        <v>160.35</v>
       </c>
       <c r="E31" s="13">
-        <v>158.84</v>
+        <v>159.66999999999999</v>
       </c>
       <c r="F31" s="13">
-        <v>168.84</v>
+        <v>169.67</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1268,7 +1268,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1298,45 +1298,45 @@
       </c>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>154.06</v>
+        <v>155.88999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>149.51</v>
+        <v>149.99</v>
       </c>
       <c r="F35" s="10">
-        <v>158.51</v>
+        <v>158.99</v>
       </c>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>152.21</v>
+        <v>154.06</v>
       </c>
       <c r="E36" s="13">
-        <v>148.69999999999999</v>
+        <v>149.51</v>
       </c>
       <c r="F36" s="13">
-        <v>157.69999999999999</v>
+        <v>158.51</v>
       </c>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1345,7 +1345,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="23" t="s">
         <v>4</v>
       </c>
@@ -1375,83 +1375,83 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>160.16</v>
+        <v>161.37</v>
       </c>
       <c r="E40" s="10">
-        <v>157.82</v>
+        <v>158.36000000000001</v>
       </c>
       <c r="F40" s="10">
-        <v>167.82</v>
+        <v>168.36</v>
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>159.88</v>
+        <v>161.09</v>
       </c>
       <c r="E41" s="13">
-        <v>158.24</v>
+        <v>158.78</v>
       </c>
       <c r="F41" s="13">
-        <v>168.24</v>
+        <v>168.78</v>
       </c>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>158.84</v>
+        <v>160.16</v>
       </c>
       <c r="E42" s="10">
-        <v>157.1</v>
+        <v>157.82</v>
       </c>
       <c r="F42" s="10">
-        <v>167.1</v>
+        <v>167.82</v>
       </c>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>158.56</v>
+        <v>159.88</v>
       </c>
       <c r="E43" s="13">
-        <v>157.52000000000001</v>
+        <v>158.24</v>
       </c>
       <c r="F43" s="13">
-        <v>167.52</v>
+        <v>168.24</v>
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="24"/>
       <c r="C44" s="15"/>
@@ -1460,7 +1460,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="25" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>4</v>
       </c>
@@ -1490,83 +1490,83 @@
       </c>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>153.09</v>
+        <v>154.4</v>
       </c>
       <c r="E47" s="10">
-        <v>150.47</v>
+        <v>150.66999999999999</v>
       </c>
       <c r="F47" s="10">
-        <v>160.47</v>
+        <v>160.66999999999999</v>
       </c>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>152.72</v>
+        <v>154.02000000000001</v>
       </c>
       <c r="E48" s="13">
-        <v>150.41</v>
+        <v>150.6</v>
       </c>
       <c r="F48" s="13">
-        <v>160.41</v>
+        <v>160.6</v>
       </c>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>152.34</v>
+        <v>153.09</v>
       </c>
       <c r="E49" s="10">
-        <v>150.18</v>
+        <v>150.47</v>
       </c>
       <c r="F49" s="10">
-        <v>160.18</v>
+        <v>160.47</v>
       </c>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>151.97</v>
+        <v>152.72</v>
       </c>
       <c r="E50" s="13">
-        <v>150.11000000000001</v>
+        <v>150.41</v>
       </c>
       <c r="F50" s="13">
-        <v>160.11000000000001</v>
+        <v>160.41</v>
       </c>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
@@ -1575,7 +1575,7 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A52" s="27" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23" t="s">
         <v>4</v>
       </c>
@@ -1605,54 +1605,54 @@
       </c>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>169.33</v>
+        <v>170.5</v>
       </c>
       <c r="E54" s="10">
-        <v>165.24</v>
+        <v>165.91</v>
       </c>
       <c r="F54" s="10">
-        <v>175.24</v>
+        <v>175.91</v>
       </c>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>161.84</v>
+        <v>163.09</v>
       </c>
       <c r="E55" s="13">
-        <v>163.55000000000001</v>
+        <v>164.2</v>
       </c>
       <c r="F55" s="13">
-        <v>173.55</v>
+        <v>174.2</v>
       </c>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>158.54</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1662,111 +1662,111 @@
       </c>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>159.1</v>
+        <v>160.32</v>
       </c>
       <c r="E57" s="13">
-        <v>157.97</v>
+        <v>158.62</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>154.87</v>
+        <v>156.09</v>
       </c>
       <c r="E58" s="10">
-        <v>153.87</v>
+        <v>154.52000000000001</v>
       </c>
       <c r="F58" s="10">
-        <v>163.87</v>
+        <v>164.52</v>
       </c>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>161.72</v>
+        <v>162.84</v>
       </c>
       <c r="E59" s="13">
-        <v>163.52000000000001</v>
+        <v>164.11</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>168.03</v>
+        <v>169.33</v>
       </c>
       <c r="E60" s="10">
-        <v>164.32</v>
+        <v>165.24</v>
       </c>
       <c r="F60" s="10">
-        <v>174.32</v>
+        <v>175.24</v>
       </c>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>160.49</v>
+        <v>161.84</v>
       </c>
       <c r="E61" s="13">
-        <v>162.44</v>
+        <v>163.55000000000001</v>
       </c>
       <c r="F61" s="13">
-        <v>172.44</v>
+        <v>173.55</v>
       </c>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>156.91</v>
+        <v>158.54</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1776,57 +1776,57 @@
       </c>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>157.51</v>
+        <v>159.1</v>
       </c>
       <c r="E63" s="13">
-        <v>156.86000000000001</v>
+        <v>157.97</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>153.28</v>
+        <v>154.87</v>
       </c>
       <c r="E64" s="10">
-        <v>152.76</v>
+        <v>153.87</v>
       </c>
       <c r="F64" s="10">
-        <v>162.76</v>
+        <v>163.87</v>
       </c>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>160.46</v>
+        <v>161.72</v>
       </c>
       <c r="E65" s="13">
-        <v>162.65</v>
+        <v>163.52000000000001</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Mon Jan 19 03:17:59 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{CD2AC9F3-A42B-4658-BEFA-A266F84FA416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{743C7B9A-EDF1-42CE-B615-5D62C5AC1D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
+    <workbookView xWindow="-10215" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,8 +154,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,7 +331,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -807,128 +807,128 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="10">
-        <v>156.03</v>
+        <v>156.52000000000001</v>
       </c>
       <c r="E8" s="10">
+        <v>150.82</v>
+      </c>
+      <c r="F8" s="10">
+        <v>160.82</v>
+      </c>
+      <c r="G8" s="10">
         <v>150.84</v>
-      </c>
-      <c r="F8" s="10">
-        <v>160.84</v>
-      </c>
-      <c r="G8" s="10">
-        <v>150.85</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>156.03</v>
+        <v>156.52000000000001</v>
       </c>
       <c r="E9" s="13">
+        <v>150.82</v>
+      </c>
+      <c r="F9" s="13">
+        <v>160.82</v>
+      </c>
+      <c r="G9" s="13">
         <v>150.84</v>
-      </c>
-      <c r="F9" s="13">
-        <v>160.84</v>
-      </c>
-      <c r="G9" s="13">
-        <v>150.85</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>157.01</v>
+        <v>157.54</v>
       </c>
       <c r="E10" s="10">
-        <v>153.01</v>
+        <v>152.82</v>
       </c>
       <c r="F10" s="10">
-        <v>163.01</v>
+        <v>162.82</v>
       </c>
       <c r="G10" s="10">
-        <v>153.41</v>
+        <v>153.22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="13">
-        <v>154.25</v>
+        <v>156.03</v>
       </c>
       <c r="E11" s="13">
-        <v>150.08000000000001</v>
+        <v>150.84</v>
       </c>
       <c r="F11" s="13">
-        <v>160.08000000000001</v>
+        <v>160.84</v>
       </c>
       <c r="G11" s="13">
-        <v>150.1</v>
+        <v>150.85</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="10">
-        <v>154.25</v>
+        <v>156.03</v>
       </c>
       <c r="E12" s="10">
-        <v>150.08000000000001</v>
+        <v>150.84</v>
       </c>
       <c r="F12" s="10">
-        <v>160.08000000000001</v>
+        <v>160.84</v>
       </c>
       <c r="G12" s="10">
-        <v>150.1</v>
+        <v>150.85</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13">
-        <v>155.62</v>
+        <v>157.01</v>
       </c>
       <c r="E13" s="13">
-        <v>152.53</v>
+        <v>153.01</v>
       </c>
       <c r="F13" s="13">
-        <v>162.53</v>
+        <v>163.01</v>
       </c>
       <c r="G13" s="13">
-        <v>152.93</v>
+        <v>153.41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -972,39 +972,39 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>160.51</v>
+        <v>160.99</v>
       </c>
       <c r="E17" s="10">
-        <v>155.6</v>
+        <v>155.37</v>
       </c>
       <c r="F17" s="10">
-        <v>165.6</v>
+        <v>165.37</v>
       </c>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>159.38</v>
+        <v>160.51</v>
       </c>
       <c r="E18" s="13">
-        <v>155.16</v>
+        <v>155.6</v>
       </c>
       <c r="F18" s="13">
-        <v>165.16</v>
+        <v>165.6</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1051,41 +1051,41 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="10">
-        <v>157.11000000000001</v>
+        <v>157.71</v>
       </c>
       <c r="E22" s="10">
-        <v>152.63</v>
+        <v>152.51</v>
       </c>
       <c r="F22" s="10">
-        <v>162.22999999999999</v>
+        <v>162.11000000000001</v>
       </c>
       <c r="G22" s="10">
-        <v>153.69999999999999</v>
+        <v>153.58000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="13">
-        <v>161.78</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="E23" s="13">
-        <v>158.35</v>
+        <v>158.15</v>
       </c>
       <c r="F23" s="13">
-        <v>168.35</v>
+        <v>168.15</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>18</v>
@@ -1093,20 +1093,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="10">
-        <v>161.91999999999999</v>
+        <v>162.44</v>
       </c>
       <c r="E24" s="10">
-        <v>159.02000000000001</v>
+        <v>158.85</v>
       </c>
       <c r="F24" s="10">
-        <v>169.02</v>
+        <v>168.85</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>18</v>
@@ -1114,41 +1114,41 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="13">
-        <v>161.9</v>
+        <v>162.43</v>
       </c>
       <c r="E25" s="13">
-        <v>158.56</v>
+        <v>158.38</v>
       </c>
       <c r="F25" s="13">
-        <v>168.56</v>
+        <v>168.38</v>
       </c>
       <c r="G25" s="13">
-        <v>158.68</v>
+        <v>158.51</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="10">
-        <v>161.51</v>
+        <v>162.03</v>
       </c>
       <c r="E26" s="10">
-        <v>160.18</v>
+        <v>160.01</v>
       </c>
       <c r="F26" s="10">
-        <v>170.18</v>
+        <v>170.01</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1156,41 +1156,41 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="13">
-        <v>155.66</v>
+        <v>157.11000000000001</v>
       </c>
       <c r="E27" s="13">
-        <v>152.09</v>
+        <v>152.63</v>
       </c>
       <c r="F27" s="13">
-        <v>161.69</v>
+        <v>162.22999999999999</v>
       </c>
       <c r="G27" s="13">
-        <v>153.16999999999999</v>
+        <v>153.69999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="10">
-        <v>160.6</v>
+        <v>161.78</v>
       </c>
       <c r="E28" s="22">
-        <v>157.87</v>
+        <v>158.35</v>
       </c>
       <c r="F28" s="22">
-        <v>167.87</v>
+        <v>168.35</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>18</v>
@@ -1198,20 +1198,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="13">
-        <v>160.75</v>
+        <v>161.91999999999999</v>
       </c>
       <c r="E29" s="13">
-        <v>158.53</v>
+        <v>159.02000000000001</v>
       </c>
       <c r="F29" s="13">
-        <v>168.53</v>
+        <v>169.02</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>18</v>
@@ -1219,41 +1219,41 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10">
-        <v>160.72999999999999</v>
+        <v>161.9</v>
       </c>
       <c r="E30" s="22">
-        <v>158.05000000000001</v>
+        <v>158.56</v>
       </c>
       <c r="F30" s="22">
-        <v>168.05</v>
+        <v>168.56</v>
       </c>
       <c r="G30" s="22">
-        <v>158.18</v>
+        <v>158.68</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="13">
-        <v>160.35</v>
+        <v>161.51</v>
       </c>
       <c r="E31" s="13">
-        <v>159.66999999999999</v>
+        <v>160.18</v>
       </c>
       <c r="F31" s="13">
-        <v>169.67</v>
+        <v>170.18</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>18</v>
@@ -1300,39 +1300,39 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="10">
-        <v>155.88999999999999</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>149.99</v>
+        <v>149.81</v>
       </c>
       <c r="F35" s="10">
-        <v>158.99</v>
+        <v>158.81</v>
       </c>
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="13">
-        <v>154.06</v>
+        <v>155.88999999999999</v>
       </c>
       <c r="E36" s="13">
-        <v>149.51</v>
+        <v>149.99</v>
       </c>
       <c r="F36" s="13">
-        <v>158.51</v>
+        <v>158.99</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -1377,77 +1377,77 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="10">
-        <v>161.37</v>
+        <v>161.91999999999999</v>
       </c>
       <c r="E40" s="10">
-        <v>158.36000000000001</v>
+        <v>158.16</v>
       </c>
       <c r="F40" s="10">
-        <v>168.36</v>
+        <v>168.16</v>
       </c>
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="13">
-        <v>161.09</v>
+        <v>161.63999999999999</v>
       </c>
       <c r="E41" s="13">
-        <v>158.78</v>
+        <v>158.58000000000001</v>
       </c>
       <c r="F41" s="13">
-        <v>168.78</v>
+        <v>168.58</v>
       </c>
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="10">
-        <v>160.16</v>
+        <v>161.37</v>
       </c>
       <c r="E42" s="10">
-        <v>157.82</v>
+        <v>158.36000000000001</v>
       </c>
       <c r="F42" s="10">
-        <v>167.82</v>
+        <v>168.36</v>
       </c>
       <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="13">
-        <v>159.88</v>
+        <v>161.09</v>
       </c>
       <c r="E43" s="13">
-        <v>158.24</v>
+        <v>158.78</v>
       </c>
       <c r="F43" s="13">
-        <v>168.24</v>
+        <v>168.78</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -1492,77 +1492,77 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="10">
-        <v>154.4</v>
+        <v>155.81</v>
       </c>
       <c r="E47" s="10">
-        <v>150.66999999999999</v>
+        <v>151.04</v>
       </c>
       <c r="F47" s="10">
-        <v>160.66999999999999</v>
+        <v>161.04</v>
       </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13">
-        <v>154.02000000000001</v>
+        <v>155.41</v>
       </c>
       <c r="E48" s="13">
-        <v>150.6</v>
+        <v>150.96</v>
       </c>
       <c r="F48" s="13">
-        <v>160.6</v>
+        <v>160.96</v>
       </c>
       <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="10">
-        <v>153.09</v>
+        <v>154.4</v>
       </c>
       <c r="E49" s="10">
-        <v>150.47</v>
+        <v>150.66999999999999</v>
       </c>
       <c r="F49" s="10">
-        <v>160.47</v>
+        <v>160.66999999999999</v>
       </c>
       <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13">
-        <v>152.72</v>
+        <v>154.02000000000001</v>
       </c>
       <c r="E50" s="13">
-        <v>150.41</v>
+        <v>150.6</v>
       </c>
       <c r="F50" s="13">
-        <v>160.41</v>
+        <v>160.6</v>
       </c>
       <c r="G50" s="17"/>
     </row>
@@ -1607,52 +1607,52 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="10">
-        <v>170.5</v>
+        <v>171</v>
       </c>
       <c r="E54" s="10">
-        <v>165.91</v>
+        <v>165.89</v>
       </c>
       <c r="F54" s="10">
-        <v>175.91</v>
+        <v>175.89</v>
       </c>
       <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="13">
-        <v>163.09</v>
+        <v>163.68</v>
       </c>
       <c r="E55" s="13">
-        <v>164.2</v>
+        <v>164.08</v>
       </c>
       <c r="F55" s="13">
-        <v>174.2</v>
+        <v>174.08</v>
       </c>
       <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10">
-        <v>159.83000000000001</v>
+        <v>160.47</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>18</v>
@@ -1664,17 +1664,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="13">
-        <v>160.32</v>
+        <v>160.91</v>
       </c>
       <c r="E57" s="13">
-        <v>158.62</v>
+        <v>158.5</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>18</v>
@@ -1683,36 +1683,36 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="7">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="10">
-        <v>156.09</v>
+        <v>156.66999999999999</v>
       </c>
       <c r="E58" s="10">
-        <v>154.52000000000001</v>
+        <v>154.4</v>
       </c>
       <c r="F58" s="10">
-        <v>164.52</v>
+        <v>164.4</v>
       </c>
       <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="11">
-        <v>46039</v>
+        <v>46042</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D59" s="13">
-        <v>162.84</v>
+        <v>163.31</v>
       </c>
       <c r="E59" s="13">
-        <v>164.11</v>
+        <v>164.01</v>
       </c>
       <c r="F59" s="13" t="s">
         <v>18</v>
@@ -1721,52 +1721,52 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="20" t="s">
         <v>31</v>
       </c>
       <c r="D60" s="10">
-        <v>169.33</v>
+        <v>170.5</v>
       </c>
       <c r="E60" s="10">
-        <v>165.24</v>
+        <v>165.91</v>
       </c>
       <c r="F60" s="10">
-        <v>175.24</v>
+        <v>175.91</v>
       </c>
       <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D61" s="13">
-        <v>161.84</v>
+        <v>163.09</v>
       </c>
       <c r="E61" s="13">
-        <v>163.55000000000001</v>
+        <v>164.2</v>
       </c>
       <c r="F61" s="13">
-        <v>173.55</v>
+        <v>174.2</v>
       </c>
       <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="10">
-        <v>158.54</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>18</v>
@@ -1778,17 +1778,17 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="13">
-        <v>159.1</v>
+        <v>160.32</v>
       </c>
       <c r="E63" s="13">
-        <v>157.97</v>
+        <v>158.62</v>
       </c>
       <c r="F63" s="13" t="s">
         <v>18</v>
@@ -1797,36 +1797,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="7">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D64" s="10">
-        <v>154.87</v>
+        <v>156.09</v>
       </c>
       <c r="E64" s="10">
-        <v>153.87</v>
+        <v>154.52000000000001</v>
       </c>
       <c r="F64" s="10">
-        <v>163.87</v>
+        <v>164.52</v>
       </c>
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="11">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="13">
-        <v>161.72</v>
+        <v>162.84</v>
       </c>
       <c r="E65" s="13">
-        <v>163.52000000000001</v>
+        <v>164.11</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Tue Jan 20 03:13:29 UTC 2026
</commit_message>
<xml_diff>
--- a/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
+++ b/bp.com-content-dam-bp-country-sites-en_au-australia-home-products-services-pricing-tgp-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bp365.sharepoint.com/sites/WholesalePricing/Shared Documents/B2C/TGP/Daily TGP/Web TGP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{743C7B9A-EDF1-42CE-B615-5D62C5AC1D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B5C523F2-61E6-4B2D-A600-EA0DD6FE660A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10215" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1B412EEF-F96D-4DF4-A4E9-C7F0F183C2FB}"/>
   </bookViews>
@@ 